<commit_message>
Adjusting the H-TESSEL comment for the 9 involved variables.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="633">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (200) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (204) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t xml:space="preserve">siflfwbot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siflfwdrain</t>
   </si>
   <si>
     <t xml:space="preserve">siflsaltbot</t>
@@ -2031,8 +2034,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A242" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A260" activeCellId="0" sqref="A260:A390"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A248" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F255" activeCellId="0" sqref="F255:F256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4849,2144 +4852,2144 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B260" s="0" t="s">
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C256" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="C260" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="D260" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="E260" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F260" s="2" t="s">
-        <v>265</v>
+      <c r="E256" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F256" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D261" s="0" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E261" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F261" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C262" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="D262" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D262" s="0" t="s">
-        <v>269</v>
-      </c>
       <c r="E262" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F262" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D263" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="C263" s="0" t="s">
+      <c r="E263" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F263" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B264" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="D263" s="0" t="s">
+      <c r="C264" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E263" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F263" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B265" s="0" t="s">
+      <c r="D264" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="C265" s="0" t="s">
+      <c r="E264" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F264" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B266" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="D265" s="0" t="s">
+      <c r="C266" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="E265" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F265" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B267" s="0" t="s">
+      <c r="D266" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="C267" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="D267" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="E267" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F267" s="0" t="s">
-        <v>265</v>
+      <c r="E266" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F266" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C268" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="D268" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="D268" s="0" t="s">
-        <v>280</v>
-      </c>
       <c r="E268" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F268" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C269" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D269" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="D269" s="0" t="s">
+      <c r="E269" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F269" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B270" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C270" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="E269" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F269" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B271" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C271" s="0" t="s">
+      <c r="D270" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="D271" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="E271" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F271" s="0" t="s">
-        <v>265</v>
+      <c r="E270" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F270" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C272" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="D272" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="C272" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="D272" s="0" t="s">
-        <v>287</v>
-      </c>
       <c r="E272" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F272" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C273" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D273" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="D273" s="0" t="s">
-        <v>289</v>
-      </c>
       <c r="E273" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F273" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="0" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C274" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D274" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="D274" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="E274" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F274" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C275" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="D275" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="D275" s="0" t="s">
-        <v>293</v>
-      </c>
       <c r="E275" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F275" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C276" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="D276" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="D276" s="0" t="s">
-        <v>295</v>
-      </c>
       <c r="E276" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F276" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C277" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D277" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="D277" s="0" t="s">
-        <v>297</v>
-      </c>
       <c r="E277" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F277" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C278" s="0" t="s">
-        <v>268</v>
+        <v>297</v>
       </c>
       <c r="D278" s="0" t="s">
         <v>298</v>
       </c>
       <c r="E278" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F278" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C279" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D279" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="D279" s="0" t="s">
-        <v>300</v>
-      </c>
       <c r="E279" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F279" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C280" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="D280" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="D280" s="0" t="s">
-        <v>302</v>
-      </c>
       <c r="E280" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F280" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C281" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D281" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="D281" s="0" t="s">
-        <v>304</v>
-      </c>
       <c r="E281" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F281" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="0" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C282" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="D282" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="D282" s="0" t="s">
-        <v>306</v>
-      </c>
       <c r="E282" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F282" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
       <c r="D283" s="0" t="s">
         <v>307</v>
       </c>
       <c r="E283" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F283" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C284" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="D284" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="D284" s="0" t="s">
-        <v>309</v>
-      </c>
       <c r="E284" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F284" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C285" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D285" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="D285" s="0" t="s">
-        <v>311</v>
-      </c>
       <c r="E285" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F285" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C286" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="D286" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="D286" s="0" t="s">
-        <v>313</v>
-      </c>
       <c r="E286" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F286" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C287" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="D287" s="0" t="s">
         <v>314</v>
       </c>
-      <c r="D287" s="0" t="s">
-        <v>315</v>
-      </c>
       <c r="E287" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F287" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C288" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="D288" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="D288" s="0" t="s">
-        <v>317</v>
-      </c>
       <c r="E288" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F288" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C289" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="D289" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="D289" s="0" t="s">
-        <v>319</v>
-      </c>
       <c r="E289" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F289" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C290" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="D290" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="D290" s="0" t="s">
-        <v>321</v>
-      </c>
       <c r="E290" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F290" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C291" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D291" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="D291" s="0" t="s">
-        <v>323</v>
-      </c>
       <c r="E291" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F291" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B292" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C292" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="D292" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="D292" s="0" t="s">
-        <v>325</v>
-      </c>
       <c r="E292" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F292" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C293" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="D293" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="D293" s="0" t="s">
-        <v>327</v>
-      </c>
       <c r="E293" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F293" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C294" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D294" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="D294" s="0" t="s">
-        <v>329</v>
-      </c>
       <c r="E294" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F294" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C295" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="D295" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="D295" s="0" t="s">
-        <v>331</v>
-      </c>
       <c r="E295" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F295" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C296" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="D296" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="D296" s="0" t="s">
-        <v>333</v>
-      </c>
       <c r="E296" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F296" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B297" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C297" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="D297" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="D297" s="0" t="s">
-        <v>335</v>
-      </c>
       <c r="E297" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F297" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B298" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C298" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="D298" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="D298" s="0" t="s">
-        <v>337</v>
-      </c>
       <c r="E298" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F298" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C299" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="D299" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="D299" s="0" t="s">
-        <v>339</v>
-      </c>
       <c r="E299" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F299" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="0" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C300" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="D300" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D300" s="0" t="s">
-        <v>341</v>
-      </c>
       <c r="E300" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F300" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C301" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="D301" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="D301" s="0" t="s">
-        <v>343</v>
-      </c>
       <c r="E301" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F301" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C302" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="D302" s="0" t="s">
         <v>344</v>
       </c>
-      <c r="D302" s="0" t="s">
-        <v>345</v>
-      </c>
       <c r="E302" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F302" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C303" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="D303" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="D303" s="0" t="s">
-        <v>347</v>
-      </c>
       <c r="E303" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F303" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B304" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C304" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="D304" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="D304" s="0" t="s">
-        <v>349</v>
-      </c>
       <c r="E304" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F304" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B305" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C305" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="D305" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="D305" s="0" t="s">
-        <v>351</v>
-      </c>
       <c r="E305" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F305" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C306" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="D306" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="D306" s="0" t="s">
-        <v>353</v>
-      </c>
       <c r="E306" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F306" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="0" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C307" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="D307" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="D307" s="0" t="s">
-        <v>355</v>
-      </c>
       <c r="E307" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F307" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C308" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="D308" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="D308" s="0" t="s">
-        <v>357</v>
-      </c>
       <c r="E308" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F308" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B309" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C309" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="D309" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="D309" s="0" t="s">
-        <v>359</v>
-      </c>
       <c r="E309" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F309" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C310" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="D310" s="0" t="s">
         <v>360</v>
       </c>
-      <c r="D310" s="0" t="s">
-        <v>361</v>
-      </c>
       <c r="E310" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F310" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B311" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C311" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="D311" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="D311" s="0" t="s">
-        <v>363</v>
-      </c>
       <c r="E311" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F311" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C312" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="D312" s="0" t="s">
         <v>364</v>
       </c>
-      <c r="D312" s="0" t="s">
-        <v>365</v>
-      </c>
       <c r="E312" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F312" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C313" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="D313" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="D313" s="0" t="s">
-        <v>367</v>
-      </c>
       <c r="E313" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F313" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C314" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="D314" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="D314" s="0" t="s">
-        <v>369</v>
-      </c>
       <c r="E314" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F314" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C315" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="D315" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="D315" s="0" t="s">
-        <v>371</v>
-      </c>
       <c r="E315" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F315" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B316" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C316" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="D316" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="D316" s="0" t="s">
-        <v>373</v>
-      </c>
       <c r="E316" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F316" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C317" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="D317" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="D317" s="0" t="s">
-        <v>375</v>
-      </c>
       <c r="E317" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F317" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C318" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="D318" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="D318" s="0" t="s">
-        <v>377</v>
-      </c>
       <c r="E318" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F318" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B319" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C319" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="D319" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="D319" s="0" t="s">
-        <v>379</v>
-      </c>
       <c r="E319" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F319" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C320" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="D320" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="D320" s="0" t="s">
-        <v>381</v>
-      </c>
       <c r="E320" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F320" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C321" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="D321" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="D321" s="0" t="s">
-        <v>383</v>
-      </c>
       <c r="E321" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F321" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B322" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C322" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="D322" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="D322" s="0" t="s">
-        <v>385</v>
-      </c>
       <c r="E322" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F322" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C323" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="D323" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="D323" s="0" t="s">
-        <v>387</v>
-      </c>
       <c r="E323" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F323" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B324" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C324" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="D324" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="D324" s="0" t="s">
-        <v>389</v>
-      </c>
       <c r="E324" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F324" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C325" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="D325" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="D325" s="0" t="s">
-        <v>391</v>
-      </c>
       <c r="E325" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F325" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B326" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>262</v>
+        <v>391</v>
       </c>
       <c r="D326" s="0" t="s">
         <v>392</v>
       </c>
       <c r="E326" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F326" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C327" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="D327" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="D327" s="0" t="s">
-        <v>394</v>
-      </c>
       <c r="E327" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F327" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C328" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="D328" s="0" t="s">
         <v>395</v>
       </c>
-      <c r="D328" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E328" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F328" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B329" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C329" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="D329" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="D329" s="0" t="s">
-        <v>398</v>
-      </c>
       <c r="E329" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F329" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B330" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C330" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="D330" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="D330" s="0" t="s">
-        <v>400</v>
-      </c>
       <c r="E330" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F330" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B331" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C331" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="D331" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="D331" s="0" t="s">
-        <v>396</v>
-      </c>
       <c r="E331" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F331" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B332" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C332" s="0" t="s">
         <v>402</v>
       </c>
       <c r="D332" s="0" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E332" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F332" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B333" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C333" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="D333" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="D333" s="0" t="s">
-        <v>405</v>
-      </c>
       <c r="E333" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F333" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B334" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C334" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="D334" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="D334" s="0" t="s">
-        <v>407</v>
-      </c>
       <c r="E334" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F334" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B335" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C335" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="D335" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="D335" s="0" t="s">
-        <v>409</v>
-      </c>
       <c r="E335" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F335" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B336" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C336" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="D336" s="0" t="s">
         <v>410</v>
       </c>
-      <c r="D336" s="0" t="s">
-        <v>411</v>
-      </c>
       <c r="E336" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F336" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B337" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C337" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="D337" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="D337" s="0" t="s">
-        <v>413</v>
-      </c>
       <c r="E337" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F337" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B338" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C338" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="D338" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="D338" s="0" t="s">
-        <v>415</v>
-      </c>
       <c r="E338" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F338" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B339" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C339" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="D339" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="D339" s="0" t="s">
-        <v>417</v>
-      </c>
       <c r="E339" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F339" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B340" s="0" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C340" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="D340" s="0" t="s">
         <v>418</v>
       </c>
-      <c r="D340" s="0" t="s">
-        <v>419</v>
-      </c>
       <c r="E340" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F340" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B341" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C341" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="D341" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="D341" s="0" t="s">
-        <v>421</v>
-      </c>
       <c r="E341" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F341" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B342" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="D342" s="0" t="s">
         <v>422</v>
       </c>
-      <c r="C342" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="D342" s="0" t="s">
-        <v>272</v>
-      </c>
       <c r="E342" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F342" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B343" s="0" t="s">
-        <v>276</v>
+        <v>423</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>423</v>
+        <v>272</v>
       </c>
       <c r="D343" s="0" t="s">
-        <v>424</v>
+        <v>273</v>
       </c>
       <c r="E343" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F343" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B344" s="0" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C344" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="D344" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="D344" s="0" t="s">
-        <v>426</v>
-      </c>
       <c r="E344" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F344" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B345" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C345" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="D345" s="0" t="s">
         <v>427</v>
       </c>
-      <c r="D345" s="0" t="s">
-        <v>428</v>
-      </c>
       <c r="E345" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F345" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B346" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C346" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D346" s="0" t="s">
         <v>429</v>
       </c>
-      <c r="D346" s="0" t="s">
-        <v>430</v>
-      </c>
       <c r="E346" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F346" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B347" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C347" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="D347" s="0" t="s">
         <v>431</v>
       </c>
-      <c r="D347" s="0" t="s">
-        <v>432</v>
-      </c>
       <c r="E347" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F347" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B348" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C348" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="D348" s="0" t="s">
         <v>433</v>
       </c>
-      <c r="D348" s="0" t="s">
-        <v>434</v>
-      </c>
       <c r="E348" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F348" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B349" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C349" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="D349" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="D349" s="0" t="s">
-        <v>436</v>
-      </c>
       <c r="E349" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F349" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B350" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C350" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="D350" s="0" t="s">
         <v>437</v>
       </c>
-      <c r="D350" s="0" t="s">
-        <v>438</v>
-      </c>
       <c r="E350" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F350" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B351" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C351" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="D351" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="D351" s="0" t="s">
-        <v>440</v>
-      </c>
       <c r="E351" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F351" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B352" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C352" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="D352" s="0" t="s">
         <v>441</v>
       </c>
-      <c r="D352" s="0" t="s">
-        <v>442</v>
-      </c>
       <c r="E352" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F352" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B353" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C353" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="D353" s="0" t="s">
         <v>443</v>
       </c>
-      <c r="D353" s="0" t="s">
-        <v>444</v>
-      </c>
       <c r="E353" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F353" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B354" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C354" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="D354" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="D354" s="0" t="s">
-        <v>446</v>
-      </c>
       <c r="E354" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F354" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B355" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C355" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="D355" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="D355" s="0" t="s">
-        <v>448</v>
-      </c>
       <c r="E355" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F355" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B356" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C356" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="D356" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="D356" s="0" t="s">
-        <v>450</v>
-      </c>
       <c r="E356" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F356" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B357" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C357" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="D357" s="0" t="s">
         <v>451</v>
       </c>
-      <c r="D357" s="0" t="s">
+      <c r="E357" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F357" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B358" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C358" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="E357" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F357" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B359" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C359" s="0" t="s">
+      <c r="D358" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="D359" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="E359" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F359" s="0" t="s">
-        <v>265</v>
+      <c r="E358" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F358" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B360" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C360" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="D360" s="0" t="s">
         <v>455</v>
       </c>
-      <c r="D360" s="0" t="s">
-        <v>456</v>
-      </c>
       <c r="E360" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F360" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B361" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>395</v>
+        <v>456</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>396</v>
+        <v>457</v>
       </c>
       <c r="E361" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F361" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B362" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>457</v>
+        <v>396</v>
       </c>
       <c r="D362" s="0" t="s">
-        <v>458</v>
+        <v>397</v>
       </c>
       <c r="E362" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F362" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B363" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>429</v>
+        <v>458</v>
       </c>
       <c r="D363" s="0" t="s">
         <v>459</v>
       </c>
       <c r="E363" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F363" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B365" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B364" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C364" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="D364" s="0" t="s">
         <v>460</v>
       </c>
-      <c r="C365" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="D365" s="0" t="s">
+      <c r="E364" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F364" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B366" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="C366" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E365" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F365" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B367" s="0" t="s">
-        <v>461</v>
-      </c>
-      <c r="C367" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="D367" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="E367" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F367" s="0" t="s">
-        <v>265</v>
+      <c r="D366" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E366" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F366" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B368" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>354</v>
+        <v>269</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>355</v>
+        <v>299</v>
       </c>
       <c r="E368" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F368" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B369" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C369" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="D369" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="D369" s="0" t="s">
-        <v>357</v>
-      </c>
       <c r="E369" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F369" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>462</v>
+        <v>357</v>
       </c>
       <c r="D370" s="0" t="s">
-        <v>463</v>
+        <v>358</v>
       </c>
       <c r="E370" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F370" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C371" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D371" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="D371" s="0" t="s">
-        <v>465</v>
-      </c>
       <c r="E371" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F371" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B372" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>262</v>
+        <v>465</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>392</v>
+        <v>466</v>
       </c>
       <c r="E372" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F372" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>418</v>
+        <v>263</v>
       </c>
       <c r="D373" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="E373" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F373" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B374" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C374" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="E373" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F373" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B375" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C375" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="D375" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="E375" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F375" s="0" t="s">
-        <v>265</v>
+      <c r="D374" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="E374" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F374" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B376" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C376" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D376" s="0" t="s">
         <v>468</v>
       </c>
-      <c r="D376" s="0" t="s">
+      <c r="E376" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F376" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B377" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C377" s="0" t="s">
         <v>469</v>
       </c>
-      <c r="E376" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F376" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B378" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C378" s="0" t="s">
+      <c r="D377" s="0" t="s">
         <v>470</v>
       </c>
-      <c r="D378" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="E378" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="F378" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H378" s="0" t="s">
-        <v>473</v>
+      <c r="E377" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F377" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B379" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C379" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D379" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="E379" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F379" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="H379" s="0" t="s">
         <v>474</v>
-      </c>
-      <c r="D379" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="E379" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="F379" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H379" s="0" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B380" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C380" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D380" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="E380" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F380" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="H380" s="0" t="s">
         <v>477</v>
-      </c>
-      <c r="D380" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="E380" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="F380" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H380" s="0" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C381" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="D381" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="E381" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F381" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="H381" s="0" t="s">
         <v>480</v>
-      </c>
-      <c r="C381" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="D381" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="E381" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="F381" s="0" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B382" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C382" s="0" t="s">
         <v>482</v>
       </c>
       <c r="D382" s="0" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E382" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F382" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C383" s="0" t="s">
         <v>483</v>
       </c>
-      <c r="C383" s="0" t="s">
-        <v>484</v>
-      </c>
       <c r="D383" s="0" t="s">
-        <v>485</v>
+        <v>268</v>
       </c>
       <c r="E383" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F383" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H383" s="0" t="s">
-        <v>486</v>
+        <v>266</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B384" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C384" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="D384" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="E384" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F384" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="H384" s="0" t="s">
         <v>487</v>
-      </c>
-      <c r="C384" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="D384" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E384" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="F384" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H384" s="0" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B385" s="0" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="C385" s="0" t="s">
         <v>489</v>
       </c>
       <c r="D385" s="0" t="s">
-        <v>269</v>
+        <v>486</v>
       </c>
       <c r="E385" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F385" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
+      </c>
+      <c r="H385" s="0" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B386" s="0" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C386" s="0" t="s">
         <v>490</v>
       </c>
       <c r="D386" s="0" t="s">
-        <v>491</v>
+        <v>270</v>
       </c>
       <c r="E386" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F386" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H386" s="0" t="s">
-        <v>491</v>
+        <v>266</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B387" s="0" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C387" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D387" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="D387" s="0" t="s">
-        <v>491</v>
-      </c>
       <c r="E387" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F387" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H387" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="0" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="C388" s="0" t="s">
         <v>493</v>
       </c>
       <c r="D388" s="0" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E388" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F388" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
+      </c>
+      <c r="H388" s="0" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B389" s="0" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C389" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D389" s="0" t="s">
         <v>495</v>
       </c>
-      <c r="D389" s="0" t="s">
-        <v>496</v>
-      </c>
       <c r="E389" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F389" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H389" s="0" t="s">
-        <v>497</v>
+        <v>266</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B390" s="0" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C390" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D390" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="E390" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F390" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="H390" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="D390" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="E390" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="F390" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H390" s="0" t="s">
+    </row>
+    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B391" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C391" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="D391" s="0" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C394" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="E394" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="F394" s="0" t="s">
-        <v>501</v>
+      <c r="E391" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="F391" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="H391" s="0" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C395" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E395" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F395" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6994,43 +6997,43 @@
         <v>503</v>
       </c>
       <c r="E396" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F396" s="0" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C398" s="0" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C397" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="E398" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="F398" s="0" t="s">
-        <v>501</v>
+      <c r="E397" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="F397" s="0" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C399" s="0" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="E399" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F399" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C400" s="0" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E400" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F400" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7038,10 +7041,10 @@
         <v>506</v>
       </c>
       <c r="E401" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F401" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7049,10 +7052,10 @@
         <v>507</v>
       </c>
       <c r="E402" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F402" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7060,10 +7063,10 @@
         <v>508</v>
       </c>
       <c r="E403" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F403" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7071,10 +7074,10 @@
         <v>509</v>
       </c>
       <c r="E404" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F404" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7082,10 +7085,10 @@
         <v>510</v>
       </c>
       <c r="E405" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F405" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7093,10 +7096,10 @@
         <v>511</v>
       </c>
       <c r="E406" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F406" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7104,10 +7107,10 @@
         <v>512</v>
       </c>
       <c r="E407" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F407" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7115,10 +7118,10 @@
         <v>513</v>
       </c>
       <c r="E408" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F408" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7126,10 +7129,10 @@
         <v>514</v>
       </c>
       <c r="E409" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F409" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7137,10 +7140,10 @@
         <v>515</v>
       </c>
       <c r="E410" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F410" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7148,10 +7151,10 @@
         <v>516</v>
       </c>
       <c r="E411" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F411" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7159,10 +7162,10 @@
         <v>517</v>
       </c>
       <c r="E412" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F412" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7170,10 +7173,10 @@
         <v>518</v>
       </c>
       <c r="E413" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F413" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7181,10 +7184,10 @@
         <v>519</v>
       </c>
       <c r="E414" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F414" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7192,10 +7195,10 @@
         <v>520</v>
       </c>
       <c r="E415" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F415" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7203,10 +7206,10 @@
         <v>521</v>
       </c>
       <c r="E416" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F416" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7214,10 +7217,10 @@
         <v>522</v>
       </c>
       <c r="E417" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F417" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7225,10 +7228,10 @@
         <v>523</v>
       </c>
       <c r="E418" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F418" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7236,10 +7239,10 @@
         <v>524</v>
       </c>
       <c r="E419" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F419" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7247,10 +7250,10 @@
         <v>525</v>
       </c>
       <c r="E420" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F420" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7258,10 +7261,10 @@
         <v>526</v>
       </c>
       <c r="E421" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F421" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7269,10 +7272,10 @@
         <v>527</v>
       </c>
       <c r="E422" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F422" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7280,10 +7283,10 @@
         <v>528</v>
       </c>
       <c r="E423" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F423" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7291,10 +7294,10 @@
         <v>529</v>
       </c>
       <c r="E424" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F424" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7302,10 +7305,10 @@
         <v>530</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F425" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7313,10 +7316,10 @@
         <v>531</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F426" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7324,10 +7327,10 @@
         <v>532</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F427" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7335,10 +7338,10 @@
         <v>533</v>
       </c>
       <c r="E428" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F428" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7346,10 +7349,10 @@
         <v>534</v>
       </c>
       <c r="E429" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F429" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7357,10 +7360,10 @@
         <v>535</v>
       </c>
       <c r="E430" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F430" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7368,10 +7371,10 @@
         <v>536</v>
       </c>
       <c r="E431" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F431" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7379,10 +7382,10 @@
         <v>537</v>
       </c>
       <c r="E432" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F432" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7390,10 +7393,10 @@
         <v>538</v>
       </c>
       <c r="E433" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F433" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7401,10 +7404,10 @@
         <v>539</v>
       </c>
       <c r="E434" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F434" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7412,10 +7415,10 @@
         <v>540</v>
       </c>
       <c r="E435" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F435" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7423,10 +7426,10 @@
         <v>541</v>
       </c>
       <c r="E436" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F436" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7434,10 +7437,10 @@
         <v>542</v>
       </c>
       <c r="E437" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F437" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7445,10 +7448,10 @@
         <v>543</v>
       </c>
       <c r="E438" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F438" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7456,10 +7459,10 @@
         <v>544</v>
       </c>
       <c r="E439" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F439" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7467,10 +7470,10 @@
         <v>545</v>
       </c>
       <c r="E440" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F440" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7478,10 +7481,10 @@
         <v>546</v>
       </c>
       <c r="E441" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F441" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7489,10 +7492,10 @@
         <v>547</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7500,10 +7503,10 @@
         <v>548</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7511,10 +7514,10 @@
         <v>549</v>
       </c>
       <c r="E444" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7522,10 +7525,10 @@
         <v>550</v>
       </c>
       <c r="E445" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F445" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7533,10 +7536,10 @@
         <v>551</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7544,10 +7547,10 @@
         <v>552</v>
       </c>
       <c r="E447" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F447" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7555,10 +7558,10 @@
         <v>553</v>
       </c>
       <c r="E448" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F448" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7566,10 +7569,10 @@
         <v>554</v>
       </c>
       <c r="E449" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F449" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7577,10 +7580,10 @@
         <v>555</v>
       </c>
       <c r="E450" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F450" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7588,10 +7591,10 @@
         <v>556</v>
       </c>
       <c r="E451" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F451" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7599,10 +7602,10 @@
         <v>557</v>
       </c>
       <c r="E452" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F452" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7610,10 +7613,10 @@
         <v>558</v>
       </c>
       <c r="E453" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F453" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7621,10 +7624,10 @@
         <v>559</v>
       </c>
       <c r="E454" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F454" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7632,10 +7635,10 @@
         <v>560</v>
       </c>
       <c r="E455" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F455" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7643,10 +7646,10 @@
         <v>561</v>
       </c>
       <c r="E456" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F456" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7654,10 +7657,10 @@
         <v>562</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F457" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7665,10 +7668,10 @@
         <v>563</v>
       </c>
       <c r="E458" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F458" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7676,10 +7679,10 @@
         <v>564</v>
       </c>
       <c r="E459" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F459" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7687,10 +7690,10 @@
         <v>565</v>
       </c>
       <c r="E460" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F460" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7698,10 +7701,10 @@
         <v>566</v>
       </c>
       <c r="E461" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F461" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7709,10 +7712,10 @@
         <v>567</v>
       </c>
       <c r="E462" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F462" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7720,10 +7723,10 @@
         <v>568</v>
       </c>
       <c r="E463" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F463" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7731,10 +7734,10 @@
         <v>569</v>
       </c>
       <c r="E464" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F464" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7742,10 +7745,10 @@
         <v>570</v>
       </c>
       <c r="E465" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F465" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7753,10 +7756,10 @@
         <v>571</v>
       </c>
       <c r="E466" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F466" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7764,10 +7767,10 @@
         <v>572</v>
       </c>
       <c r="E467" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F467" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7775,10 +7778,10 @@
         <v>573</v>
       </c>
       <c r="E468" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F468" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7786,10 +7789,10 @@
         <v>574</v>
       </c>
       <c r="E469" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F469" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7797,10 +7800,10 @@
         <v>575</v>
       </c>
       <c r="E470" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F470" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7808,10 +7811,10 @@
         <v>576</v>
       </c>
       <c r="E471" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F471" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7819,10 +7822,10 @@
         <v>577</v>
       </c>
       <c r="E472" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F472" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7830,10 +7833,10 @@
         <v>578</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7841,10 +7844,10 @@
         <v>579</v>
       </c>
       <c r="E474" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F474" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7852,10 +7855,10 @@
         <v>580</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7863,10 +7866,10 @@
         <v>581</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F476" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7874,10 +7877,10 @@
         <v>582</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F477" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7885,10 +7888,10 @@
         <v>583</v>
       </c>
       <c r="E478" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F478" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7896,10 +7899,10 @@
         <v>584</v>
       </c>
       <c r="E479" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F479" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7907,10 +7910,10 @@
         <v>585</v>
       </c>
       <c r="E480" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F480" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7918,10 +7921,10 @@
         <v>586</v>
       </c>
       <c r="E481" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F481" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7929,10 +7932,10 @@
         <v>587</v>
       </c>
       <c r="E482" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F482" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7940,10 +7943,10 @@
         <v>588</v>
       </c>
       <c r="E483" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F483" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7951,10 +7954,10 @@
         <v>589</v>
       </c>
       <c r="E484" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F484" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7962,10 +7965,10 @@
         <v>590</v>
       </c>
       <c r="E485" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F485" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7973,10 +7976,10 @@
         <v>591</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F486" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7984,10 +7987,10 @@
         <v>592</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F487" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7995,10 +7998,10 @@
         <v>593</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8006,21 +8009,21 @@
         <v>594</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C491" s="0" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C490" s="0" t="s">
         <v>595</v>
       </c>
-      <c r="E491" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="F491" s="0" t="s">
-        <v>501</v>
+      <c r="E490" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="F490" s="0" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8028,32 +8031,32 @@
         <v>596</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F492" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C493" s="0" t="s">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F493" s="0" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C495" s="0" t="s">
-        <v>597</v>
-      </c>
-      <c r="E495" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="F495" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C494" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="E494" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="F494" s="0" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8061,10 +8064,10 @@
         <v>598</v>
       </c>
       <c r="E496" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F496" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8072,10 +8075,10 @@
         <v>599</v>
       </c>
       <c r="E497" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F497" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8083,10 +8086,10 @@
         <v>600</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F498" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8094,10 +8097,10 @@
         <v>601</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8105,10 +8108,10 @@
         <v>602</v>
       </c>
       <c r="E500" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F500" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8116,10 +8119,10 @@
         <v>603</v>
       </c>
       <c r="E501" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F501" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8127,32 +8130,32 @@
         <v>604</v>
       </c>
       <c r="E502" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F502" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="0" t="s">
-        <v>503</v>
+        <v>605</v>
       </c>
       <c r="E503" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F503" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C504" s="0" t="s">
-        <v>605</v>
+        <v>504</v>
       </c>
       <c r="E504" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F504" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8160,10 +8163,10 @@
         <v>606</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F505" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8171,21 +8174,21 @@
         <v>607</v>
       </c>
       <c r="E506" s="0" t="s">
-        <v>608</v>
+        <v>501</v>
       </c>
       <c r="F506" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C507" s="0" t="s">
+        <v>608</v>
+      </c>
+      <c r="E507" s="0" t="s">
         <v>609</v>
       </c>
-      <c r="E507" s="0" t="s">
-        <v>500</v>
-      </c>
       <c r="F507" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8193,10 +8196,10 @@
         <v>610</v>
       </c>
       <c r="E508" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F508" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8204,10 +8207,10 @@
         <v>611</v>
       </c>
       <c r="E509" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F509" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8215,10 +8218,10 @@
         <v>612</v>
       </c>
       <c r="E510" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F510" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8226,10 +8229,10 @@
         <v>613</v>
       </c>
       <c r="E511" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F511" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8237,10 +8240,10 @@
         <v>614</v>
       </c>
       <c r="E512" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F512" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8248,32 +8251,32 @@
         <v>615</v>
       </c>
       <c r="E513" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F513" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="0" t="s">
-        <v>499</v>
+        <v>616</v>
       </c>
       <c r="E514" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F514" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="0" t="s">
-        <v>616</v>
+        <v>500</v>
       </c>
       <c r="E515" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F515" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8281,10 +8284,10 @@
         <v>617</v>
       </c>
       <c r="E516" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F516" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8292,10 +8295,10 @@
         <v>618</v>
       </c>
       <c r="E517" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F517" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8303,10 +8306,10 @@
         <v>619</v>
       </c>
       <c r="E518" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F518" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8314,10 +8317,10 @@
         <v>620</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8325,10 +8328,10 @@
         <v>621</v>
       </c>
       <c r="E520" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8336,10 +8339,10 @@
         <v>622</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8347,10 +8350,10 @@
         <v>623</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8358,10 +8361,10 @@
         <v>624</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8369,10 +8372,10 @@
         <v>625</v>
       </c>
       <c r="E524" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8380,10 +8383,10 @@
         <v>626</v>
       </c>
       <c r="E525" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F525" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8391,10 +8394,10 @@
         <v>627</v>
       </c>
       <c r="E526" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F526" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8402,10 +8405,10 @@
         <v>628</v>
       </c>
       <c r="E527" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F527" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8413,10 +8416,10 @@
         <v>629</v>
       </c>
       <c r="E528" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F528" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8424,10 +8427,10 @@
         <v>630</v>
       </c>
       <c r="E529" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F529" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8435,13 +8438,23 @@
         <v>631</v>
       </c>
       <c r="E530" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F530" s="0" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="1047818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C531" s="0" t="s">
+        <v>632</v>
+      </c>
+      <c r="E531" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="F531" s="0" t="s">
+        <v>502</v>
+      </c>
+    </row>
     <row r="1047819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1047820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1047821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update the pre identified missing file for the ping -file update of shaconemo revision 211. And add some comment to step 3 in update procedure.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (210) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (211) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -2079,8 +2079,8 @@
   </sheetPr>
   <dimension ref="A1:H552"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A249" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B267" activeCellId="0" sqref="B267"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A254" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updating the pre identified missing file for shaconemo update - in fact only the comment column has changed for revision 212.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (211) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (212) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -2079,7 +2079,7 @@
   </sheetPr>
   <dimension ref="A1:H552"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A254" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A240" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E265"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update pre identified file for Shaconemo r215 update, and adding some forgotten NEMO code names
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="652">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (212) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (215) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -1963,7 +1963,19 @@
     <t xml:space="preserve">landCoverFrac</t>
   </si>
   <si>
+    <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expfe</t>
+  </si>
+  <si>
     <t xml:space="preserve">David Warlind, Raffaele Bernardello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expcal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: PPPHY2</t>
   </si>
 </sst>
 </file>
@@ -2077,10 +2089,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H552"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A240" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E265"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E552" activeCellId="0" sqref="E552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8625,42 +8637,63 @@
       <c r="C548" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="E548" s="2" t="s">
+        <v>647</v>
+      </c>
       <c r="F548" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C549" s="0" t="s">
         <v>141</v>
       </c>
+      <c r="E549" s="0" t="s">
+        <v>649</v>
+      </c>
       <c r="F549" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C550" s="0" t="s">
         <v>139</v>
       </c>
+      <c r="E550" s="0" t="s">
+        <v>650</v>
+      </c>
       <c r="F550" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C551" s="0" t="s">
         <v>194</v>
       </c>
+      <c r="E551" s="0" t="s">
+        <v>651</v>
+      </c>
       <c r="F551" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C552" s="0" t="s">
         <v>195</v>
       </c>
+      <c r="E552" s="0" t="s">
+        <v>651</v>
+      </c>
       <c r="F552" s="0" t="s">
-        <v>647</v>
-      </c>
-    </row>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update for Shaconemo r216 - ping files not affected.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (215) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (216) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -2091,8 +2091,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E552" activeCellId="0" sqref="E552"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A245" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
The variables wfcorr and hfcorr are moved form the pre ignored to the pre identified missing file. #133
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="657">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -848,6 +848,21 @@
   </si>
   <si>
     <t xml:space="preserve">Available in PISCES: Alkalini in upper layer (Alkalini in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but radiative forcing sees historical+future atmospheric CO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wfcorr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA.  Torben: &lt;field field_ref="erp"    name="wfcorr"   long_name="water_flux_correction" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raffaele, Torben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfcorr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in NEMO-OPA.  Torben: &lt;field field_ref="qrp"     name="hfcorr"      long_name="heat_flux_correction"</t>
   </si>
   <si>
     <t xml:space="preserve">longitude latitude plev19 time</t>
@@ -2092,7 +2107,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A245" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E265"/>
+      <selection pane="topLeft" activeCell="A271" activeCellId="0" sqref="271:271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5041,60 +5056,48 @@
         <v>273</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B276" s="0" t="s">
+    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C269" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="C276" s="0" t="s">
+      <c r="E269" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="D276" s="0" t="s">
+      <c r="F269" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="E276" s="0" t="s">
+    </row>
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C270" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="F276" s="2" t="s">
+      <c r="E270" s="0" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B277" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C277" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="D277" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="E277" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F277" s="2" t="s">
-        <v>280</v>
+      <c r="F270" s="0" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C278" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D278" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="D278" s="0" t="s">
-        <v>284</v>
-      </c>
       <c r="E278" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F278" s="2" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C279" s="0" t="s">
         <v>286</v>
@@ -5103,117 +5106,117 @@
         <v>287</v>
       </c>
       <c r="E279" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F279" s="2" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B280" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="C280" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="D280" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="E280" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F280" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D281" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E281" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F281" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
+      </c>
+      <c r="F281" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D283" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E283" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F283" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B284" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="C284" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="D284" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="E284" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F284" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C285" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="D285" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="E285" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F285" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B286" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="D285" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="E285" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F285" s="0" t="s">
-        <v>280</v>
+      <c r="C286" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="D286" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="E286" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F286" s="0" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C287" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D287" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E287" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F287" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B288" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="C288" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="D288" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="E288" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F288" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C289" s="0" t="s">
         <v>303</v>
@@ -5222,1861 +5225,1858 @@
         <v>304</v>
       </c>
       <c r="E289" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F289" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C290" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D290" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E290" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F290" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E291" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F291" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B292" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D292" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E292" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F292" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C293" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D293" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E293" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F293" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="D294" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E294" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F294" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D295" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E295" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F295" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>316</v>
+        <v>288</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E296" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F296" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B297" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E297" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F297" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B298" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C298" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D298" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E298" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F298" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
       <c r="D299" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E299" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F299" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C300" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D300" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E300" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F300" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>325</v>
+        <v>286</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E301" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F301" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C302" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D302" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E302" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F302" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C303" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D303" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E303" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F303" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B304" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C304" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D304" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E304" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F304" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B305" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C305" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D305" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E305" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F305" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C306" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D306" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E306" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F306" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C307" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D307" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E307" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F307" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C308" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D308" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E308" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F308" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B309" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C309" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D309" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E309" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F309" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C310" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D310" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E310" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F310" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B311" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C311" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E311" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F311" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D312" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E312" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F312" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C313" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D313" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E313" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F313" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C314" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D314" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E314" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F314" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C315" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D315" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E315" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F315" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B316" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C316" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D316" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E316" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F316" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C317" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E317" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F317" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D318" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E318" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F318" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B319" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C319" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D319" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E319" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F319" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C320" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D320" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E320" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F320" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E321" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F321" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B322" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D322" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E322" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F322" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B323" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D323" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E323" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F323" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B324" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D324" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E324" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F324" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B325" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D325" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E325" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F325" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B326" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D326" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E326" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F326" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D327" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E327" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F327" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B328" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D328" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E328" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F328" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B329" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D329" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E329" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F329" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B330" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D330" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E330" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F330" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B331" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D331" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E331" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F331" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B332" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D332" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E332" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F332" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B333" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D333" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E333" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F333" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B334" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D334" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E334" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F334" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B335" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E335" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F335" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B336" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D336" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E336" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F336" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B337" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D337" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E337" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F337" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B338" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D338" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E338" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F338" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B339" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D339" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E339" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F339" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B340" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D340" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E340" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F340" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B341" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D341" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E341" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F341" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B342" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>277</v>
+        <v>408</v>
       </c>
       <c r="D342" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E342" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F342" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B343" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D343" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E343" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F343" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B344" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>410</v>
+        <v>282</v>
       </c>
       <c r="D344" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E344" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F344" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B345" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D345" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E345" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F345" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B346" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D346" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E346" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F346" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B347" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D347" s="0" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="E347" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F347" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B348" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D348" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E348" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F348" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B349" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E349" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F349" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B350" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E350" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F350" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B351" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D351" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E351" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F351" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B352" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D352" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E352" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F352" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B353" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D353" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E353" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F353" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B354" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D354" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E354" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F354" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B355" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D355" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E355" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F355" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B356" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D356" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E356" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F356" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B357" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D357" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E357" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F357" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B358" s="0" t="s">
-        <v>437</v>
+        <v>305</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>286</v>
+        <v>438</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>287</v>
+        <v>439</v>
       </c>
       <c r="E358" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F358" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B359" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D359" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="E359" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F359" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B360" s="0" t="s">
-        <v>300</v>
+        <v>442</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>440</v>
+        <v>291</v>
       </c>
       <c r="D360" s="0" t="s">
-        <v>441</v>
+        <v>292</v>
       </c>
       <c r="E360" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F360" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B361" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D361" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E361" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F361" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B362" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D362" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E362" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F362" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B363" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D363" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E363" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F363" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B364" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D364" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E364" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F364" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B365" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D365" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E365" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F365" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B366" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D366" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E366" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F366" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B367" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D367" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E367" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F367" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B368" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E368" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F368" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B369" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D369" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E369" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F369" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D370" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E370" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F370" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B371" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D371" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E371" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F371" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B372" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E372" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F372" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B373" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D373" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E373" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F373" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B374" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C374" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D374" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="E374" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F374" s="0" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B375" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D375" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="E375" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F375" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B376" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="C376" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="D376" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="E376" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F376" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B377" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>410</v>
+        <v>473</v>
       </c>
       <c r="D377" s="0" t="s">
-        <v>411</v>
+        <v>474</v>
       </c>
       <c r="E377" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F377" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B378" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="D378" s="0" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="E378" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F378" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B379" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>444</v>
+        <v>415</v>
       </c>
       <c r="D379" s="0" t="s">
-        <v>474</v>
+        <v>416</v>
       </c>
       <c r="E379" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F379" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B380" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C380" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="D380" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="E380" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F380" s="0" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B381" s="0" t="s">
-        <v>475</v>
+        <v>296</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>286</v>
+        <v>449</v>
       </c>
       <c r="D381" s="0" t="s">
-        <v>287</v>
+        <v>479</v>
       </c>
       <c r="E381" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F381" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="0" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D383" s="0" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="E383" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F383" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B384" s="0" t="s">
-        <v>476</v>
-      </c>
-      <c r="C384" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="D384" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="E384" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F384" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B385" s="0" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>371</v>
+        <v>288</v>
       </c>
       <c r="D385" s="0" t="s">
-        <v>372</v>
+        <v>318</v>
       </c>
       <c r="E385" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F385" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B386" s="0" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C386" s="0" t="s">
-        <v>477</v>
+        <v>374</v>
       </c>
       <c r="D386" s="0" t="s">
-        <v>478</v>
+        <v>375</v>
       </c>
       <c r="E386" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F386" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B387" s="0" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>479</v>
+        <v>376</v>
       </c>
       <c r="D387" s="0" t="s">
-        <v>480</v>
+        <v>377</v>
       </c>
       <c r="E387" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F387" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B388" s="0" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C388" s="0" t="s">
-        <v>277</v>
+        <v>482</v>
       </c>
       <c r="D388" s="0" t="s">
-        <v>407</v>
+        <v>483</v>
       </c>
       <c r="E388" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F388" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B389" s="0" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C389" s="0" t="s">
-        <v>433</v>
+        <v>484</v>
       </c>
       <c r="D389" s="0" t="s">
-        <v>434</v>
+        <v>485</v>
       </c>
       <c r="E389" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F389" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B390" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C390" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D390" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="E390" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F390" s="0" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B391" s="0" t="s">
-        <v>291</v>
+        <v>481</v>
       </c>
       <c r="C391" s="0" t="s">
-        <v>481</v>
+        <v>438</v>
       </c>
       <c r="D391" s="0" t="s">
-        <v>482</v>
+        <v>439</v>
       </c>
       <c r="E391" s="0" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F391" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B392" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="C392" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="D392" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="E392" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F392" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B393" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C393" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="D393" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="E393" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F393" s="0" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B394" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C394" s="0" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="D394" s="0" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="E394" s="0" t="s">
-        <v>487</v>
+        <v>284</v>
       </c>
       <c r="F394" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H394" s="0" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B395" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="C395" s="0" t="s">
-        <v>489</v>
-      </c>
-      <c r="D395" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="E395" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="F395" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H395" s="0" t="s">
-        <v>491</v>
+        <v>285</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B396" s="0" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C396" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D396" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="E396" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="D396" s="0" t="s">
+      <c r="F396" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="H396" s="0" t="s">
         <v>493</v>
-      </c>
-      <c r="E396" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="F396" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H396" s="0" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B397" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C397" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D397" s="0" t="s">
         <v>495</v>
       </c>
-      <c r="C397" s="0" t="s">
+      <c r="E397" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="F397" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="H397" s="0" t="s">
         <v>496</v>
-      </c>
-      <c r="D397" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="E397" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="F397" s="0" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B398" s="0" t="s">
-        <v>495</v>
+        <v>296</v>
       </c>
       <c r="C398" s="0" t="s">
         <v>497</v>
       </c>
       <c r="D398" s="0" t="s">
-        <v>282</v>
+        <v>498</v>
       </c>
       <c r="E398" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F398" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+      <c r="H398" s="0" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B399" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C399" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D399" s="0" t="s">
-        <v>500</v>
+        <v>283</v>
       </c>
       <c r="E399" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F399" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H399" s="0" t="s">
-        <v>501</v>
+        <v>285</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B400" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="C400" s="0" t="s">
         <v>502</v>
       </c>
-      <c r="C400" s="0" t="s">
-        <v>503</v>
-      </c>
       <c r="D400" s="0" t="s">
-        <v>500</v>
+        <v>287</v>
       </c>
       <c r="E400" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F400" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H400" s="0" t="s">
-        <v>501</v>
+        <v>285</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B401" s="0" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="C401" s="0" t="s">
         <v>504</v>
       </c>
       <c r="D401" s="0" t="s">
-        <v>284</v>
+        <v>505</v>
       </c>
       <c r="E401" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F401" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+      <c r="H401" s="0" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B402" s="0" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
       <c r="C402" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="D402" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="D402" s="0" t="s">
-        <v>506</v>
-      </c>
       <c r="E402" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F402" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="H402" s="0" t="s">
         <v>506</v>
@@ -7084,1612 +7084,1647 @@
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B403" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C403" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D403" s="0" t="s">
-        <v>506</v>
+        <v>289</v>
       </c>
       <c r="E403" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F403" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H403" s="0" t="s">
-        <v>506</v>
+        <v>285</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B404" s="0" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="C404" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="D404" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E404" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F404" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
+      </c>
+      <c r="H404" s="0" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B405" s="0" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
       <c r="C405" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D405" s="0" t="s">
         <v>511</v>
       </c>
       <c r="E405" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F405" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="H405" s="0" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B406" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C406" s="0" t="s">
         <v>513</v>
       </c>
       <c r="D406" s="0" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="E406" s="0" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F406" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="H406" s="0" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C410" s="0" t="s">
-        <v>514</v>
-      </c>
-      <c r="E410" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B407" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="C407" s="0" t="s">
         <v>515</v>
       </c>
-      <c r="F410" s="0" t="s">
+      <c r="D407" s="0" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C411" s="0" t="s">
+      <c r="E407" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="F407" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="H407" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="E411" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="F411" s="0" t="s">
+    </row>
+    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B408" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="C408" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="D408" s="0" t="s">
         <v>516</v>
+      </c>
+      <c r="E408" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="F408" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="H408" s="0" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C412" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E412" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F412" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C413" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="E413" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F413" s="0" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C414" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="E414" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F414" s="0" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C415" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="E415" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="F415" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C416" s="0" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="E416" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F416" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C417" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E417" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F417" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C418" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="E418" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F418" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C419" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E419" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F419" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C420" s="0" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="E420" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F420" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C421" s="0" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E421" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F421" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C422" s="0" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="E422" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F422" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C423" s="0" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E423" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F423" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C424" s="0" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="E424" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F424" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C425" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F425" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C426" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F426" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C427" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F427" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C428" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="E428" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F428" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C429" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="E429" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F429" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C430" s="0" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="E430" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F430" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C431" s="0" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E431" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F431" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C432" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="E432" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F432" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C433" s="0" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="E433" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F433" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C434" s="0" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="E434" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F434" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C435" s="0" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="E435" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F435" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C436" s="0" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="E436" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F436" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C437" s="0" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="E437" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F437" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C438" s="0" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="E438" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F438" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C439" s="0" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="E439" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F439" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C440" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="E440" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F440" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C441" s="0" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="E441" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F441" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C442" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C443" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C444" s="0" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="E444" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C445" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="E445" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F445" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C446" s="0" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C447" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="E447" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F447" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C448" s="0" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="E448" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F448" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C449" s="0" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="E449" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F449" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C450" s="0" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="E450" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F450" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C451" s="0" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="E451" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F451" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C452" s="0" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="E452" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F452" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C453" s="0" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="E453" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F453" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C454" s="0" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="E454" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F454" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C455" s="0" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="E455" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F455" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C456" s="0" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="E456" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F456" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C457" s="0" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F457" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C458" s="0" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="E458" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F458" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C459" s="0" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="E459" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F459" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C460" s="0" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="E460" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F460" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C461" s="0" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="E461" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F461" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C462" s="0" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="E462" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F462" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C463" s="0" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="E463" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F463" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C464" s="0" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="E464" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F464" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C465" s="0" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E465" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F465" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C466" s="0" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="E466" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F466" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C467" s="0" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="E467" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F467" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C468" s="0" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="E468" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F468" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C469" s="0" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="E469" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F469" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C470" s="0" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="E470" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F470" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C471" s="0" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="E471" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F471" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C472" s="0" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="E472" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F472" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C473" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C474" s="0" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="E474" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F474" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C475" s="0" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C476" s="0" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F476" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C477" s="0" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F477" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C478" s="0" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="E478" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F478" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C479" s="0" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="E479" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F479" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C480" s="0" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="E480" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F480" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C481" s="0" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="E481" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F481" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C482" s="0" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="E482" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F482" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C483" s="0" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="E483" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F483" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C484" s="0" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="E484" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F484" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C485" s="0" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="E485" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F485" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C486" s="0" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F486" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C487" s="0" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F487" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C488" s="0" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C489" s="0" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C490" s="0" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="E490" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F490" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C491" s="0" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F491" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C492" s="0" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F492" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C493" s="0" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F493" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C494" s="0" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="E494" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F494" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C495" s="0" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="E495" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F495" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C496" s="0" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="E496" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F496" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C497" s="0" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="E497" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F497" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C498" s="0" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F498" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C499" s="0" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C500" s="0" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="E500" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F500" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C501" s="0" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="E501" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F501" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C502" s="0" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="E502" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F502" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="0" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="E503" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F503" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C504" s="0" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="E504" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F504" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C505" s="0" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F505" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C506" s="0" t="s">
+        <v>613</v>
+      </c>
+      <c r="E506" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F506" s="0" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C507" s="0" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="E507" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F507" s="0" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C508" s="0" t="s">
-        <v>611</v>
-      </c>
-      <c r="E508" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="F508" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C509" s="0" t="s">
-        <v>600</v>
+        <v>615</v>
       </c>
       <c r="E509" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F509" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C510" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="E510" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F510" s="0" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C511" s="0" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="E511" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F511" s="0" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C512" s="0" t="s">
-        <v>613</v>
-      </c>
-      <c r="E512" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="F512" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C513" s="0" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="E513" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F513" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="0" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="E514" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F514" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="0" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="E515" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F515" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="0" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="E516" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F516" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C517" s="0" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="E517" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F517" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C518" s="0" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="E518" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F518" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C519" s="0" t="s">
-        <v>518</v>
+        <v>623</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C520" s="0" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="E520" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C521" s="0" t="s">
-        <v>621</v>
+        <v>523</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C522" s="0" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>623</v>
+        <v>520</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="0" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="0" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="E524" s="0" t="s">
-        <v>515</v>
+        <v>628</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C525" s="0" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="E525" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F525" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C526" s="0" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="E526" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F526" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C527" s="0" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="E527" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F527" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C528" s="0" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="E528" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F528" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C529" s="0" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="E529" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F529" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C530" s="0" t="s">
-        <v>514</v>
+        <v>634</v>
       </c>
       <c r="E530" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F530" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C531" s="0" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="E531" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F531" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="0" t="s">
-        <v>632</v>
+        <v>519</v>
       </c>
       <c r="E532" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F532" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C533" s="0" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="E533" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F533" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C534" s="0" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="E534" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F534" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C535" s="0" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="E535" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F535" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C536" s="0" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="E536" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F536" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C537" s="0" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="E537" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F537" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="0" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="E538" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F538" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="0" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="E539" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F539" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="0" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="E540" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F540" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C541" s="0" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="E541" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F541" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C542" s="0" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="E542" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F542" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C543" s="0" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="E543" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F543" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C544" s="0" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="E544" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F544" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C545" s="0" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="E545" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F545" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C546" s="0" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="E546" s="0" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F546" s="0" t="s">
-        <v>516</v>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C547" s="0" t="s">
+        <v>650</v>
+      </c>
+      <c r="E547" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F547" s="0" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C548" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E548" s="2" t="s">
-        <v>647</v>
+        <v>651</v>
+      </c>
+      <c r="E548" s="0" t="s">
+        <v>520</v>
       </c>
       <c r="F548" s="0" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C549" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E549" s="0" t="s">
-        <v>649</v>
-      </c>
-      <c r="F549" s="0" t="s">
-        <v>648</v>
+        <v>521</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C550" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="E550" s="0" t="s">
-        <v>650</v>
+        <v>140</v>
+      </c>
+      <c r="E550" s="2" t="s">
+        <v>652</v>
       </c>
       <c r="F550" s="0" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C551" s="0" t="s">
-        <v>194</v>
+        <v>141</v>
       </c>
       <c r="E551" s="0" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="F551" s="0" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C552" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E552" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="F552" s="0" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C553" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E553" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="F553" s="0" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C554" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="E552" s="0" t="s">
-        <v>651</v>
-      </c>
-      <c r="F552" s="0" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E554" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="F554" s="0" t="s">
+        <v>653</v>
+      </c>
+    </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update pre basic ignored file for shaconemo revision 235.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (224) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (235) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -2109,8 +2109,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A248" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F265" activeCellId="0" sqref="F265:F266"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A253" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Adding a bunch of "step 2" variables to the pre basic ignored and the pre basic identified missing files. #141
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="692">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1597,7 +1597,7 @@
     <t xml:space="preserve">Available in LPJ-GUESS, will be cmorized by Peter Anthoni &amp; Lars Nieradzik</t>
   </si>
   <si>
-    <t xml:space="preserve">David Warlind</t>
+    <t xml:space="preserve">David Wårlind</t>
   </si>
   <si>
     <t xml:space="preserve">mrsol</t>
@@ -1990,10 +1990,22 @@
     <t xml:space="preserve">landCoverFrac</t>
   </si>
   <si>
+    <t xml:space="preserve">cSoilLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cVegLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cLitterLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cProductLut</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expfe</t>
   </si>
   <si>
-    <t xml:space="preserve">David Warlind, Raffaele Bernardello</t>
+    <t xml:space="preserve">David Wårlind, Raffaele Bernardello</t>
   </si>
   <si>
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expsi</t>
@@ -2003,6 +2015,87 @@
   </si>
   <si>
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: PPPHY2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SImon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siflswdtop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable qsr_ice (solar heat flux at ice surface, W/m²),     &lt;field id="qsr_ice"   long_name="solar heat flux at ice surface: sum over categories"    standard_name="surface_downwelling_shortwave_flux_in_air"    unit="W/m2" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Docquier, Torben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areacellg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shuting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large-scale precipitation (rain+snow) + Convective precipitation (rain+snow) - Snowfall: grib 128.142 + 128.143 - 128.144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shuting, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrroLi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP: ISCCP total cloud area, CVEXTRA(5)='94 ISCCP_TOTALCLDAREA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">albisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP: ISCCP cloud albedo, CVEXTRA(7)='96 ISCCP_MEANALBEDOCLD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pctisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP: ISCCP cloud top pressure, CVEXTRA(6)='95 ISCCP_MEANPTOP'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP: CALIPSO total cloud cover, CVEXTRA(4)='93 CALIPSO_CLDLAYER TOTAL'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cllcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP: CALIPSO low cloud cover, CVEXTRA(1)='90 CALIPSO_CLDLAYER LOW'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clmcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP: CALIPSO mid cloud cover, CVEXTRA(2)='91 CALIPSO_CLDLAYER MID'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clhcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP: CALIPSO high cloud cover, CVEXTRA(3)='92 CALIPSO_CLDLAYER HIGH'</t>
   </si>
 </sst>
 </file>
@@ -2012,7 +2105,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2043,13 +2136,39 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2086,7 +2205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2096,6 +2215,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2116,10 +2247,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H560"/>
+  <dimension ref="A1:H584"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A245" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F266" activeCellId="0" sqref="F266:F269"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B547" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I568" activeCellId="0" sqref="I568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8728,57 +8859,227 @@
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C556" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E556" s="2" t="s">
         <v>656</v>
       </c>
+      <c r="E556" s="0" t="s">
+        <v>524</v>
+      </c>
       <c r="F556" s="0" t="s">
-        <v>657</v>
+        <v>525</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C557" s="0" t="s">
-        <v>142</v>
+        <v>657</v>
       </c>
       <c r="E557" s="0" t="s">
-        <v>658</v>
+        <v>524</v>
       </c>
       <c r="F557" s="0" t="s">
-        <v>657</v>
+        <v>525</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C558" s="0" t="s">
-        <v>140</v>
+        <v>658</v>
       </c>
       <c r="E558" s="0" t="s">
-        <v>659</v>
+        <v>524</v>
       </c>
       <c r="F558" s="0" t="s">
-        <v>657</v>
+        <v>525</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C559" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="E559" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="F559" s="0" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C562" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E562" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="F562" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C563" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E563" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="F563" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C564" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E564" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="F564" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C565" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="E559" s="0" t="s">
-        <v>660</v>
-      </c>
-      <c r="F559" s="0" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C560" s="0" t="s">
+      <c r="E565" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="F565" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C566" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="E560" s="0" t="s">
-        <v>660</v>
-      </c>
-      <c r="F560" s="0" t="s">
-        <v>657</v>
+      <c r="E566" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="F566" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="568" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A568" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="C568" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E568" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="F568" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="G568" s="3"/>
+      <c r="H568" s="3"/>
+    </row>
+    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C570" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="E570" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="F570" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C571" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="E571" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="F571" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C572" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="E572" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="F572" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C578" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="E578" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="F578" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C579" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="E579" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="F579" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C580" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="E580" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="F580" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C581" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="E581" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="F581" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C582" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="E582" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="F582" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C583" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="E583" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="F583" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C584" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="E584" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="F584" s="3" t="s">
+        <v>679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding more "step 2" variables to the pre basic ignored and the pre identified missing files #141.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="707">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1513,27 +1513,18 @@
     <t xml:space="preserve">Not available in the AOGCM, but will be added by Tommi  in the ESM in TM5 with its cmor name.</t>
   </si>
   <si>
-    <t xml:space="preserve">This is requested only for the emission-driven coupled carbon climate model runs.  Does not include natural fire sources but, includes all anthropogenic sources, including fossil fuel use, cement production, agricultural burning, and sources associated with anthropogenic land use change excluding forest regrowth.</t>
-  </si>
-  <si>
     <t xml:space="preserve">fco2fos</t>
   </si>
   <si>
     <t xml:space="preserve">Carbon Mass Flux into Atmosphere Due to Fossil Fuel Emissions of CO2</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the prescribed anthropogenic CO2 flux from fossil fuel use, including cement production, and flaring (but not from land-use changes, agricultural burning, forest regrowth, etc.)</t>
-  </si>
-  <si>
     <t xml:space="preserve">fco2nat</t>
   </si>
   <si>
     <t xml:space="preserve">Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources</t>
   </si>
   <si>
-    <t xml:space="preserve">This is what the atmosphere sees (on its own grid).  This field should be equivalent to the combined natural fluxes of carbon  that account for natural exchanges between the atmosphere and land (nep) or ocean (fgco2) reservoirs.</t>
-  </si>
-  <si>
     <t xml:space="preserve">longitude latitude plev19 time2</t>
   </si>
   <si>
@@ -1552,9 +1543,6 @@
     <t xml:space="preserve">Total Atmospheric Mass of CO2</t>
   </si>
   <si>
-    <t xml:space="preserve">Total atmospheric mass of Carbon Dioxide</t>
-  </si>
-  <si>
     <t xml:space="preserve">time2</t>
   </si>
   <si>
@@ -1585,10 +1573,67 @@
     <t xml:space="preserve">Global Mean Mole Fraction of N2O</t>
   </si>
   <si>
-    <t xml:space="preserve">Global mean Nitrous Oxide (N2O)</t>
-  </si>
-  <si>
     <t xml:space="preserve">n2oglobalClim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AERmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lossch4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in TM5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twan &amp; Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lossco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pod0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in TM5??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flashrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in TM5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depdust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sedustCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od443dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in TM5?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od865dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loaddust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concdust</t>
   </si>
   <si>
     <t xml:space="preserve">lai</t>
@@ -2247,10 +2292,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H584"/>
+  <dimension ref="A1:H599"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B547" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I568" activeCellId="0" sqref="I568"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A400" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H402" activeCellId="0" sqref="H402:H414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7151,28 +7196,22 @@
       <c r="F402" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H402" s="0" t="s">
-        <v>497</v>
-      </c>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B403" s="0" t="s">
         <v>300</v>
       </c>
       <c r="C403" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D403" s="0" t="s">
         <v>498</v>
-      </c>
-      <c r="D403" s="0" t="s">
-        <v>499</v>
       </c>
       <c r="E403" s="0" t="s">
         <v>496</v>
       </c>
       <c r="F403" s="0" t="s">
         <v>289</v>
-      </c>
-      <c r="H403" s="0" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7180,10 +7219,10 @@
         <v>300</v>
       </c>
       <c r="C404" s="0" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D404" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E404" s="0" t="s">
         <v>496</v>
@@ -7191,16 +7230,13 @@
       <c r="F404" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H404" s="0" t="s">
-        <v>503</v>
-      </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B405" s="0" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C405" s="0" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D405" s="0" t="s">
         <v>287</v>
@@ -7214,10 +7250,10 @@
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B406" s="0" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C406" s="0" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D406" s="0" t="s">
         <v>291</v>
@@ -7231,13 +7267,13 @@
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B407" s="0" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C407" s="0" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D407" s="0" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E407" s="0" t="s">
         <v>496</v>
@@ -7245,19 +7281,16 @@
       <c r="F407" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H407" s="0" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B408" s="0" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C408" s="0" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D408" s="0" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E408" s="0" t="s">
         <v>496</v>
@@ -7265,16 +7298,13 @@
       <c r="F408" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H408" s="0" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B409" s="0" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C409" s="0" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D409" s="0" t="s">
         <v>293</v>
@@ -7288,13 +7318,13 @@
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B410" s="0" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C410" s="0" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D410" s="0" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E410" s="0" t="s">
         <v>496</v>
@@ -7302,19 +7332,16 @@
       <c r="F410" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H410" s="0" t="s">
-        <v>515</v>
-      </c>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B411" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="C411" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D411" s="0" t="s">
         <v>511</v>
-      </c>
-      <c r="C411" s="0" t="s">
-        <v>516</v>
-      </c>
-      <c r="D411" s="0" t="s">
-        <v>515</v>
       </c>
       <c r="E411" s="0" t="s">
         <v>496</v>
@@ -7322,19 +7349,16 @@
       <c r="F411" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H411" s="0" t="s">
-        <v>515</v>
-      </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B412" s="0" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C412" s="0" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D412" s="0" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="E412" s="0" t="s">
         <v>496</v>
@@ -7345,13 +7369,13 @@
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B413" s="0" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C413" s="0" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D413" s="0" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E413" s="0" t="s">
         <v>496</v>
@@ -7359,19 +7383,16 @@
       <c r="F413" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H413" s="0" t="s">
-        <v>521</v>
-      </c>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B414" s="0" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="D414" s="0" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E414" s="0" t="s">
         <v>496</v>
@@ -7379,162 +7400,187 @@
       <c r="F414" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="H414" s="0" t="s">
+    </row>
+    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C416" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="E416" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F416" s="0" t="s">
         <v>521</v>
       </c>
     </row>
+    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C417" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="E417" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F417" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="0" t="s">
+        <v>518</v>
+      </c>
       <c r="C418" s="0" t="s">
         <v>523</v>
       </c>
       <c r="E418" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F418" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A419" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C419" s="0" t="s">
         <v>524</v>
       </c>
-      <c r="F418" s="0" t="s">
+      <c r="E419" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="F419" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A420" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C420" s="0" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C419" s="0" t="s">
+      <c r="E420" s="0" t="s">
         <v>526</v>
       </c>
-      <c r="E419" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F419" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C420" s="0" t="s">
+      <c r="F420" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="0" t="s">
         <v>527</v>
       </c>
-      <c r="E420" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F420" s="0" t="s">
-        <v>525</v>
+      <c r="C421" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="E421" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="F421" s="0" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="0" t="s">
+        <v>527</v>
+      </c>
       <c r="C422" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E422" s="0" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="F422" s="0" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="0" t="s">
+        <v>527</v>
+      </c>
       <c r="C423" s="0" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="E423" s="0" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F423" s="0" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A424" s="0" t="s">
+        <v>527</v>
+      </c>
       <c r="C424" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="E424" s="0" t="s">
         <v>529</v>
       </c>
-      <c r="E424" s="0" t="s">
-        <v>524</v>
-      </c>
       <c r="F424" s="0" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="0" t="s">
+        <v>527</v>
+      </c>
       <c r="C425" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>524</v>
+        <v>534</v>
       </c>
       <c r="F425" s="0" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="0" t="s">
+        <v>527</v>
+      </c>
       <c r="C426" s="0" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>524</v>
+        <v>534</v>
       </c>
       <c r="F426" s="0" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="0" t="s">
+        <v>527</v>
+      </c>
       <c r="C427" s="0" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="F427" s="0" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="0" t="s">
+        <v>527</v>
+      </c>
       <c r="C428" s="0" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="E428" s="0" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="F428" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C429" s="0" t="s">
-        <v>534</v>
-      </c>
-      <c r="E429" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F429" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="0" t="s">
-        <v>535</v>
-      </c>
-      <c r="E430" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F430" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C431" s="0" t="s">
-        <v>536</v>
-      </c>
-      <c r="E431" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F431" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C432" s="0" t="s">
-        <v>537</v>
-      </c>
-      <c r="E432" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F432" s="0" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7542,65 +7588,54 @@
         <v>538</v>
       </c>
       <c r="E433" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F433" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C434" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E434" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F434" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C435" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E435" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F435" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C436" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="E436" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F436" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C437" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E437" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F437" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C438" s="0" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E438" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F438" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7608,10 +7643,10 @@
         <v>544</v>
       </c>
       <c r="E439" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F439" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7619,10 +7654,10 @@
         <v>545</v>
       </c>
       <c r="E440" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F440" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7630,10 +7665,10 @@
         <v>546</v>
       </c>
       <c r="E441" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F441" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7641,10 +7676,10 @@
         <v>547</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7652,10 +7687,10 @@
         <v>548</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7663,10 +7698,10 @@
         <v>549</v>
       </c>
       <c r="E444" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7674,10 +7709,10 @@
         <v>550</v>
       </c>
       <c r="E445" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F445" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7685,10 +7720,10 @@
         <v>551</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7696,10 +7731,10 @@
         <v>552</v>
       </c>
       <c r="E447" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F447" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7707,10 +7742,10 @@
         <v>553</v>
       </c>
       <c r="E448" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F448" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7718,10 +7753,10 @@
         <v>554</v>
       </c>
       <c r="E449" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F449" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7729,10 +7764,10 @@
         <v>555</v>
       </c>
       <c r="E450" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F450" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7740,10 +7775,10 @@
         <v>556</v>
       </c>
       <c r="E451" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F451" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7751,10 +7786,10 @@
         <v>557</v>
       </c>
       <c r="E452" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F452" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7762,10 +7797,10 @@
         <v>558</v>
       </c>
       <c r="E453" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F453" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7773,10 +7808,10 @@
         <v>559</v>
       </c>
       <c r="E454" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F454" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7784,10 +7819,10 @@
         <v>560</v>
       </c>
       <c r="E455" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F455" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7795,10 +7830,10 @@
         <v>561</v>
       </c>
       <c r="E456" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F456" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7806,10 +7841,10 @@
         <v>562</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F457" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7817,10 +7852,10 @@
         <v>563</v>
       </c>
       <c r="E458" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F458" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7828,10 +7863,10 @@
         <v>564</v>
       </c>
       <c r="E459" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F459" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7839,10 +7874,10 @@
         <v>565</v>
       </c>
       <c r="E460" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F460" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7850,10 +7885,10 @@
         <v>566</v>
       </c>
       <c r="E461" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F461" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7861,10 +7896,10 @@
         <v>567</v>
       </c>
       <c r="E462" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F462" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7872,10 +7907,10 @@
         <v>568</v>
       </c>
       <c r="E463" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F463" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7883,10 +7918,10 @@
         <v>569</v>
       </c>
       <c r="E464" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F464" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7894,10 +7929,10 @@
         <v>570</v>
       </c>
       <c r="E465" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F465" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7905,10 +7940,10 @@
         <v>571</v>
       </c>
       <c r="E466" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F466" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7916,10 +7951,10 @@
         <v>572</v>
       </c>
       <c r="E467" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F467" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7927,10 +7962,10 @@
         <v>573</v>
       </c>
       <c r="E468" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F468" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7938,10 +7973,10 @@
         <v>574</v>
       </c>
       <c r="E469" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F469" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7949,10 +7984,10 @@
         <v>575</v>
       </c>
       <c r="E470" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F470" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7960,10 +7995,10 @@
         <v>576</v>
       </c>
       <c r="E471" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F471" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7971,10 +8006,10 @@
         <v>577</v>
       </c>
       <c r="E472" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F472" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7982,10 +8017,10 @@
         <v>578</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7993,10 +8028,10 @@
         <v>579</v>
       </c>
       <c r="E474" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F474" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8004,10 +8039,10 @@
         <v>580</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8015,10 +8050,10 @@
         <v>581</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F476" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8026,10 +8061,10 @@
         <v>582</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F477" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8037,10 +8072,10 @@
         <v>583</v>
       </c>
       <c r="E478" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F478" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8048,10 +8083,10 @@
         <v>584</v>
       </c>
       <c r="E479" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F479" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8059,10 +8094,10 @@
         <v>585</v>
       </c>
       <c r="E480" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F480" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8070,10 +8105,10 @@
         <v>586</v>
       </c>
       <c r="E481" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F481" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8081,10 +8116,10 @@
         <v>587</v>
       </c>
       <c r="E482" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F482" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8092,10 +8127,10 @@
         <v>588</v>
       </c>
       <c r="E483" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F483" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8103,10 +8138,10 @@
         <v>589</v>
       </c>
       <c r="E484" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F484" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8114,10 +8149,10 @@
         <v>590</v>
       </c>
       <c r="E485" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F485" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8125,10 +8160,10 @@
         <v>591</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F486" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8136,10 +8171,10 @@
         <v>592</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F487" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8147,10 +8182,10 @@
         <v>593</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8158,10 +8193,10 @@
         <v>594</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8169,10 +8204,10 @@
         <v>595</v>
       </c>
       <c r="E490" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F490" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8180,10 +8215,10 @@
         <v>596</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F491" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8191,10 +8226,10 @@
         <v>597</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F492" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8202,10 +8237,10 @@
         <v>598</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F493" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8213,10 +8248,10 @@
         <v>599</v>
       </c>
       <c r="E494" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F494" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8224,10 +8259,10 @@
         <v>600</v>
       </c>
       <c r="E495" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F495" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8235,10 +8270,10 @@
         <v>601</v>
       </c>
       <c r="E496" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F496" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8246,10 +8281,10 @@
         <v>602</v>
       </c>
       <c r="E497" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F497" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8257,10 +8292,10 @@
         <v>603</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F498" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8268,10 +8303,10 @@
         <v>604</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8279,10 +8314,10 @@
         <v>605</v>
       </c>
       <c r="E500" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F500" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8290,10 +8325,10 @@
         <v>606</v>
       </c>
       <c r="E501" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F501" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8301,10 +8336,10 @@
         <v>607</v>
       </c>
       <c r="E502" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F502" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8312,10 +8347,10 @@
         <v>608</v>
       </c>
       <c r="E503" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F503" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8323,10 +8358,10 @@
         <v>609</v>
       </c>
       <c r="E504" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F504" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8334,10 +8369,10 @@
         <v>610</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F505" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8345,10 +8380,10 @@
         <v>611</v>
       </c>
       <c r="E506" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F506" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8356,10 +8391,10 @@
         <v>612</v>
       </c>
       <c r="E507" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F507" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8367,10 +8402,10 @@
         <v>613</v>
       </c>
       <c r="E508" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F508" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8378,10 +8413,10 @@
         <v>614</v>
       </c>
       <c r="E509" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F509" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8389,10 +8424,10 @@
         <v>615</v>
       </c>
       <c r="E510" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F510" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8400,10 +8435,10 @@
         <v>616</v>
       </c>
       <c r="E511" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F511" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8411,10 +8446,10 @@
         <v>617</v>
       </c>
       <c r="E512" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F512" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8422,208 +8457,208 @@
         <v>618</v>
       </c>
       <c r="E513" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F513" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C514" s="0" t="s">
+        <v>619</v>
+      </c>
+      <c r="E514" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F514" s="0" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E515" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F515" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="E516" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F516" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C517" s="0" t="s">
-        <v>609</v>
+        <v>622</v>
       </c>
       <c r="E517" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F517" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C518" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="E518" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F518" s="0" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C519" s="0" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C520" s="0" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="E520" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C521" s="0" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C522" s="0" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="0" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="0" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="E524" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C525" s="0" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="E525" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F525" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C526" s="0" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="E526" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F526" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C527" s="0" t="s">
-        <v>527</v>
+        <v>632</v>
       </c>
       <c r="E527" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F527" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C528" s="0" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="E528" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F528" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C529" s="0" t="s">
-        <v>630</v>
-      </c>
-      <c r="E529" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F529" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C530" s="0" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="E530" s="0" t="s">
-        <v>632</v>
+        <v>539</v>
       </c>
       <c r="F530" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C531" s="0" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="E531" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F531" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="0" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="E532" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F532" s="0" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C533" s="0" t="s">
-        <v>635</v>
-      </c>
-      <c r="E533" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="F533" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8631,10 +8666,10 @@
         <v>636</v>
       </c>
       <c r="E534" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F534" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8642,10 +8677,10 @@
         <v>637</v>
       </c>
       <c r="E535" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F535" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8653,10 +8688,10 @@
         <v>638</v>
       </c>
       <c r="E536" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F536" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8664,65 +8699,65 @@
         <v>639</v>
       </c>
       <c r="E537" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F537" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="0" t="s">
-        <v>523</v>
+        <v>640</v>
       </c>
       <c r="E538" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F538" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E539" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F539" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E540" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F540" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C541" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E541" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F541" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C542" s="0" t="s">
-        <v>643</v>
+        <v>542</v>
       </c>
       <c r="E542" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F542" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8730,10 +8765,10 @@
         <v>644</v>
       </c>
       <c r="E543" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F543" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8741,10 +8776,10 @@
         <v>645</v>
       </c>
       <c r="E544" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F544" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8752,98 +8787,98 @@
         <v>646</v>
       </c>
       <c r="E545" s="0" t="s">
-        <v>524</v>
+        <v>647</v>
       </c>
       <c r="F545" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C546" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E546" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F546" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C547" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E547" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F547" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C548" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E548" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F548" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C549" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="E549" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F549" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C550" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E550" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F550" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C551" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E551" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F551" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C552" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E552" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F552" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C553" s="0" t="s">
-        <v>654</v>
+        <v>538</v>
       </c>
       <c r="E553" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F553" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8851,235 +8886,400 @@
         <v>655</v>
       </c>
       <c r="E554" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F554" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C555" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="E555" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F555" s="0" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C556" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E556" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F556" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C557" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E557" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F557" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C558" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E558" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F558" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C559" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E559" s="0" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="F559" s="0" t="s">
-        <v>525</v>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C560" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="E560" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F560" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C561" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="E561" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F561" s="0" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C562" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E562" s="2" t="s">
-        <v>660</v>
+        <v>663</v>
+      </c>
+      <c r="E562" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="F562" s="0" t="s">
-        <v>661</v>
+        <v>540</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C563" s="0" t="s">
-        <v>142</v>
+        <v>664</v>
       </c>
       <c r="E563" s="0" t="s">
-        <v>662</v>
+        <v>539</v>
       </c>
       <c r="F563" s="0" t="s">
-        <v>661</v>
+        <v>540</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C564" s="0" t="s">
-        <v>140</v>
+        <v>665</v>
       </c>
       <c r="E564" s="0" t="s">
-        <v>663</v>
+        <v>539</v>
       </c>
       <c r="F564" s="0" t="s">
-        <v>661</v>
+        <v>540</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C565" s="0" t="s">
-        <v>195</v>
+        <v>666</v>
       </c>
       <c r="E565" s="0" t="s">
-        <v>664</v>
+        <v>539</v>
       </c>
       <c r="F565" s="0" t="s">
-        <v>661</v>
+        <v>540</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C566" s="0" t="s">
-        <v>196</v>
+        <v>667</v>
       </c>
       <c r="E566" s="0" t="s">
-        <v>664</v>
+        <v>539</v>
       </c>
       <c r="F566" s="0" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="568" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A568" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="C568" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="E568" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="F568" s="3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C567" s="0" t="s">
         <v>668</v>
       </c>
-      <c r="G568" s="3"/>
-      <c r="H568" s="3"/>
-    </row>
-    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C570" s="2" t="s">
+      <c r="E567" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F567" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C568" s="0" t="s">
         <v>669</v>
       </c>
-      <c r="E570" s="3" t="s">
+      <c r="E568" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F568" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C569" s="0" t="s">
         <v>670</v>
       </c>
-      <c r="F570" s="4" t="s">
-        <v>671</v>
+      <c r="E569" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F569" s="0" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C571" s="0" t="s">
-        <v>672</v>
-      </c>
-      <c r="E571" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="F571" s="4" t="s">
-        <v>674</v>
+        <v>671</v>
+      </c>
+      <c r="E571" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F571" s="0" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C572" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="E572" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F572" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C573" s="0" t="s">
+        <v>673</v>
+      </c>
+      <c r="E573" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F573" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C574" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="E574" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="F574" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C577" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E577" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="E572" s="3" t="s">
+      <c r="F577" s="0" t="s">
         <v>676</v>
-      </c>
-      <c r="F572" s="4" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C578" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E578" s="0" t="s">
         <v>677</v>
       </c>
-      <c r="E578" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="F578" s="3" t="s">
-        <v>679</v>
+      <c r="F578" s="0" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C579" s="0" t="s">
-        <v>680</v>
-      </c>
-      <c r="E579" s="5" t="s">
-        <v>681</v>
-      </c>
-      <c r="F579" s="3" t="s">
-        <v>679</v>
+        <v>140</v>
+      </c>
+      <c r="E579" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="F579" s="0" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C580" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="E580" s="5" t="s">
-        <v>683</v>
-      </c>
-      <c r="F580" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E580" s="0" t="s">
         <v>679</v>
+      </c>
+      <c r="F580" s="0" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C581" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E581" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="F581" s="0" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="583" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A583" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="C583" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="E583" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F583" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="G583" s="3"/>
+      <c r="H583" s="3"/>
+    </row>
+    <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C585" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="E581" s="3" t="s">
+      <c r="E585" s="3" t="s">
         <v>685</v>
       </c>
-      <c r="F581" s="3" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C582" s="0" t="s">
+      <c r="F585" s="4" t="s">
         <v>686</v>
       </c>
-      <c r="E582" s="3" t="s">
+    </row>
+    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C586" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="F582" s="3" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C583" s="0" t="s">
+      <c r="E586" s="3" t="s">
         <v>688</v>
       </c>
-      <c r="E583" s="3" t="s">
+      <c r="F586" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="F583" s="3" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C584" s="0" t="s">
+    </row>
+    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C587" s="0" t="s">
         <v>690</v>
       </c>
-      <c r="E584" s="3" t="s">
+      <c r="E587" s="3" t="s">
         <v>691</v>
       </c>
-      <c r="F584" s="3" t="s">
-        <v>679</v>
+      <c r="F587" s="4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C593" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="E593" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="F593" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C594" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="E594" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="F594" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C595" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="E595" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="F595" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C596" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="E596" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="F596" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C597" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="E597" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="F597" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C598" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="E598" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="F598" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C599" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="E599" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="F599" s="3" t="s">
+        <v>694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving those LPJ-GUESS variables which have fields which are the same as other available variables from the basic ignored to the missing identified file. And add one such variable from the step 2 file. #141
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="725">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2045,6 +2045,60 @@
   </si>
   <si>
     <t xml:space="preserve">cProductLut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrsll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same as mrsol because: No frozen fraction of water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">netAtmosLandCO2Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same as nbp in Lmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fFire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same as fFireNat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fHarvest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same as fHarvestToAtmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cCwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same as cLitterCwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rGrowth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same as raOther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rMaint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same as r*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prCrop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same precipitation over crops as for the rest of the gridcell. Available in LPJ-GUESS, but the field will be the same precipitation over crops as for the rest of the gridcell.</t>
   </si>
   <si>
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expfe</t>
@@ -2150,7 +2204,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2184,6 +2238,13 @@
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="&quot;normal arial&quot;"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -2250,7 +2311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2275,6 +2336,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2292,10 +2357,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H599"/>
+  <dimension ref="A1:H609"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A400" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H402" activeCellId="0" sqref="H402:H414"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B562" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B585" activeCellId="0" sqref="B585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9101,185 +9166,289 @@
         <v>540</v>
       </c>
     </row>
+    <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C576" s="0" t="s">
+        <v>675</v>
+      </c>
+      <c r="E576" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="F576" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C577" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E577" s="2" t="s">
-        <v>675</v>
+        <v>677</v>
+      </c>
+      <c r="E577" s="0" t="s">
+        <v>678</v>
       </c>
       <c r="F577" s="0" t="s">
-        <v>676</v>
+        <v>540</v>
       </c>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C578" s="0" t="s">
-        <v>142</v>
+        <v>679</v>
       </c>
       <c r="E578" s="0" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="F578" s="0" t="s">
-        <v>676</v>
+        <v>540</v>
       </c>
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C579" s="0" t="s">
-        <v>140</v>
+        <v>680</v>
       </c>
       <c r="E579" s="0" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="F579" s="0" t="s">
-        <v>676</v>
+        <v>540</v>
       </c>
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C580" s="0" t="s">
-        <v>195</v>
+        <v>682</v>
       </c>
       <c r="E580" s="0" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="F580" s="0" t="s">
-        <v>676</v>
+        <v>540</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C581" s="0" t="s">
-        <v>196</v>
+        <v>684</v>
       </c>
       <c r="E581" s="0" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="F581" s="0" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="583" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A583" s="2" t="s">
-        <v>680</v>
-      </c>
-      <c r="C583" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="E583" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="F583" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="G583" s="3"/>
-      <c r="H583" s="3"/>
-    </row>
-    <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C585" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="E585" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="F585" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C582" s="0" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C586" s="0" t="s">
+      <c r="E582" s="0" t="s">
         <v>687</v>
       </c>
-      <c r="E586" s="3" t="s">
+      <c r="F582" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C583" s="0" t="s">
         <v>688</v>
       </c>
-      <c r="F586" s="4" t="s">
+      <c r="E583" s="0" t="s">
         <v>689</v>
       </c>
+      <c r="F583" s="0" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A584" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="C584" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E584" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="F584" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="G584" s="3"/>
+      <c r="H584" s="4"/>
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C587" s="0" t="s">
-        <v>690</v>
-      </c>
-      <c r="E587" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="F587" s="4" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C593" s="0" t="s">
-        <v>692</v>
+        <v>141</v>
+      </c>
+      <c r="E587" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="F587" s="0" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C588" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E588" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="F588" s="0" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C589" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E589" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="F589" s="0" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C590" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E590" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="F590" s="0" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C591" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E591" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="F591" s="0" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="593" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A593" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C593" s="2" t="s">
+        <v>699</v>
       </c>
       <c r="E593" s="3" t="s">
-        <v>693</v>
+        <v>700</v>
       </c>
       <c r="F593" s="3" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C594" s="0" t="s">
-        <v>695</v>
-      </c>
-      <c r="E594" s="5" t="s">
-        <v>696</v>
-      </c>
-      <c r="F594" s="3" t="s">
-        <v>694</v>
-      </c>
+        <v>701</v>
+      </c>
+      <c r="G593" s="3"/>
+      <c r="H593" s="3"/>
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C595" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="E595" s="5" t="s">
-        <v>698</v>
-      </c>
-      <c r="F595" s="3" t="s">
-        <v>694</v>
+      <c r="C595" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="E595" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="F595" s="5" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C596" s="0" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
       <c r="E596" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="F596" s="3" t="s">
-        <v>694</v>
+        <v>706</v>
+      </c>
+      <c r="F596" s="5" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C597" s="0" t="s">
-        <v>701</v>
+        <v>708</v>
       </c>
       <c r="E597" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="F597" s="3" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C598" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="E598" s="3" t="s">
-        <v>704</v>
-      </c>
-      <c r="F598" s="3" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C599" s="0" t="s">
-        <v>705</v>
-      </c>
-      <c r="E599" s="3" t="s">
-        <v>706</v>
-      </c>
-      <c r="F599" s="3" t="s">
-        <v>694</v>
+        <v>709</v>
+      </c>
+      <c r="F597" s="5" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C603" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="E603" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="F603" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C604" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="E604" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="F604" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C605" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="E605" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="F605" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C606" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="E606" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="F606" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C607" s="0" t="s">
+        <v>719</v>
+      </c>
+      <c r="E607" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="F607" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C608" s="0" t="s">
+        <v>721</v>
+      </c>
+      <c r="E608" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="F608" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C609" s="0" t="s">
+        <v>723</v>
+      </c>
+      <c r="E609" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="F609" s="3" t="s">
+        <v>712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the pre basic identified missing file for shaconemo revision 238.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in one of the shaconemo (236) ping files. </t>
+    <t xml:space="preserve">Identified in one of the shaconemo (238) ping files. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -2359,8 +2359,8 @@
   </sheetPr>
   <dimension ref="A1:H609"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B562" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B585" activeCellId="0" sqref="B585"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B236" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Adding more "step 2" variables to the pre identified missing files #141.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="752">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1636,6 +1636,12 @@
     <t xml:space="preserve">concdust</t>
   </si>
   <si>
+    <t xml:space="preserve">od550aerso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determined by CMIP6 stratospheric aerosol forcing data set</t>
+  </si>
+  <si>
     <t xml:space="preserve">lai</t>
   </si>
   <si>
@@ -2195,6 +2201,81 @@
   </si>
   <si>
     <t xml:space="preserve">COSP: CALIPSO high cloud cover, CVEXTRA(3)='92 CALIPSO_CLDLAYER HIGH'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3hrPt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the IFS code we found: A CALL TO SUBROUTINE *SOLANG* GIVES FIELDS OF SOLAR ZENITH. Best would be to copy the IFS routine/formula to ece2cmor3 and produce this field off-line.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gijs &amp; Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tauupbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: Eastward turbulent surface stress: grib 128.180 maybe the Eastward gravity wave surface stress grib 128.195 has to be added. This needs to be checked with ECMWF people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tauvpbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: Northward turbulent surface stress: grib 128.181 maybe the Northward gravity wave surface stress grib 128.196 has to be added. This needs to be checked with ECMWF people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prrc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availlable in IFS: Precip. flux from convection liquid grib 128.107, this is a 3D field so the surface field has to be extracted from this. So only level 91 needs to be outputted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prhmax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaialbe in IFS by postprocessing hourly data into maximum for the month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uqint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS, via postprocessing the vertical integral can be taken of the following grib 128.131 * 128.133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vqint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS, via postprocessing the vertical integral can be taken of the following grib 128.132 * 128.133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the U component of wind (grib 128.131) and this needs to be vertically integrated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intvaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the V component of wind (grib 128.132) and this needs to be vertically integrated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuadse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the V component of wind (grib 128.132) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intvadse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the U component of wind (grib 128.131) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
   </si>
 </sst>
 </file>
@@ -2204,7 +2285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2262,6 +2343,27 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF007FFF"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF007FFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2311,7 +2413,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2340,6 +2442,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2349,6 +2463,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF007FFF"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -2357,10 +2531,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H609"/>
+  <dimension ref="A1:H624"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B236" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E269"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A593" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C616" activeCellId="0" sqref="C616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7648,1624 +7822,1640 @@
         <v>521</v>
       </c>
     </row>
+    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C430" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="E430" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="F430" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G430" s="3"/>
+      <c r="H430" s="3"/>
+    </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C433" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E433" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F433" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C434" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E434" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F434" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C435" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E435" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F435" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C437" s="0" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E437" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F437" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C438" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E438" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F438" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C439" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="E439" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F439" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C440" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E440" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F440" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C441" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E441" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F441" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C442" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C443" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C444" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E444" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C445" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E445" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F445" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C446" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C447" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E447" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F447" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C448" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="E448" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F448" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C449" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="E449" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F449" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C450" s="0" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="E450" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F450" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C451" s="0" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="E451" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F451" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C452" s="0" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E452" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F452" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C453" s="0" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="E453" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F453" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C454" s="0" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="E454" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F454" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C455" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="E455" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F455" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C456" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="E456" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F456" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C457" s="0" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F457" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C458" s="0" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E458" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F458" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C459" s="0" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="E459" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F459" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C460" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E460" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F460" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C461" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="E461" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F461" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C462" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="E462" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F462" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C463" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E463" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F463" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C464" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="E464" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F464" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C465" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="E465" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F465" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C466" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="E466" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F466" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C467" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="E467" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F467" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C468" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="E468" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F468" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C469" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="E469" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F469" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C470" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="E470" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F470" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C471" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="E471" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F471" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C472" s="0" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="E472" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F472" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C473" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C474" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="E474" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F474" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C475" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C476" s="0" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F476" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C477" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F477" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C478" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="E478" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F478" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C479" s="0" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="E479" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F479" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C480" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="E480" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F480" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C481" s="0" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E481" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F481" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C482" s="0" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="E482" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F482" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C483" s="0" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="E483" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F483" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C484" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="E484" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F484" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C485" s="0" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="E485" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F485" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C486" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F486" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C487" s="0" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F487" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C488" s="0" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C489" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C490" s="0" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="E490" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F490" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C491" s="0" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F491" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C492" s="0" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F492" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C493" s="0" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F493" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C494" s="0" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="E494" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F494" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C495" s="0" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="E495" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F495" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C496" s="0" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="E496" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F496" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C497" s="0" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="E497" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F497" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C498" s="0" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F498" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C499" s="0" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C500" s="0" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="E500" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F500" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C501" s="0" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="E501" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F501" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C502" s="0" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="E502" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F502" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="0" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="E503" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F503" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C504" s="0" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="E504" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F504" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C505" s="0" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F505" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C506" s="0" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="E506" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F506" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C507" s="0" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="E507" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F507" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C508" s="0" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="E508" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F508" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C509" s="0" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="E509" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F509" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C510" s="0" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="E510" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F510" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C511" s="0" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="E511" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F511" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C512" s="0" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="E512" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F512" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C513" s="0" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="E513" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F513" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="0" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="E514" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F514" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="0" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="E515" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F515" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="0" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="E516" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F516" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C517" s="0" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="E517" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F517" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C518" s="0" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="E518" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F518" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C519" s="0" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C520" s="0" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="E520" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C521" s="0" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C522" s="0" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="0" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="0" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="E524" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C525" s="0" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="E525" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F525" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C526" s="0" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="E526" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F526" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C527" s="0" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="E527" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F527" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C528" s="0" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="E528" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F528" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C530" s="0" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="E530" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F530" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C531" s="0" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="E531" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F531" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="0" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="E532" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F532" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C534" s="0" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="E534" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F534" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C535" s="0" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="E535" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F535" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C536" s="0" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="E536" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F536" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C537" s="0" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="E537" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F537" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="0" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="E538" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F538" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="0" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E539" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F539" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="0" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="E540" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F540" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C541" s="0" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="E541" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F541" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C542" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E542" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F542" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C543" s="0" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="E543" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F543" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C544" s="0" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="E544" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F544" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C545" s="0" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="E545" s="0" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="F545" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C546" s="0" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="E546" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F546" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C547" s="0" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="E547" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F547" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C548" s="0" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="E548" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F548" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C549" s="0" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="E549" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F549" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C550" s="0" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="E550" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F550" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C551" s="0" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="E551" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F551" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C552" s="0" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="E552" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F552" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C553" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E553" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F553" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C554" s="0" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="E554" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F554" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C555" s="0" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="E555" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F555" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C556" s="0" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="E556" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F556" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C557" s="0" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="E557" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F557" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C558" s="0" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="E558" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F558" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C559" s="0" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E559" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F559" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C560" s="0" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="E560" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F560" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C561" s="0" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="E561" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F561" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C562" s="0" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="E562" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F562" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C563" s="0" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="E563" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F563" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C564" s="0" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="E564" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F564" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C565" s="0" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="E565" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F565" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C566" s="0" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="E566" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F566" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C567" s="0" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="E567" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F567" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C568" s="0" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="E568" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F568" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C569" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="E569" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F569" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C571" s="0" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="E571" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F571" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C572" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E572" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F572" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C573" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="E573" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F573" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C574" s="0" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="E574" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F574" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C576" s="0" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="E576" s="0" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="F576" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C577" s="0" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="E577" s="0" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="F577" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C578" s="0" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="E578" s="0" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="F578" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C579" s="0" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E579" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="F579" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C580" s="0" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="E580" s="0" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="F580" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C581" s="0" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E581" s="0" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="F581" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C582" s="0" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E582" s="0" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="F582" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C583" s="0" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="E583" s="0" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="F583" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="0" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C584" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E584" s="3" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="F584" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="G584" s="3"/>
       <c r="H584" s="4"/>
@@ -9275,10 +9465,10 @@
         <v>141</v>
       </c>
       <c r="E587" s="2" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="F587" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9286,10 +9476,10 @@
         <v>142</v>
       </c>
       <c r="E588" s="0" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="F588" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9297,10 +9487,10 @@
         <v>140</v>
       </c>
       <c r="E589" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="F589" s="0" t="s">
         <v>696</v>
-      </c>
-      <c r="F589" s="0" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9308,10 +9498,10 @@
         <v>195</v>
       </c>
       <c r="E590" s="0" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F590" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9319,137 +9509,313 @@
         <v>196</v>
       </c>
       <c r="E591" s="0" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F591" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="593" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="2" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C593" s="2" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="E593" s="3" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="F593" s="3" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="G593" s="3"/>
       <c r="H593" s="3"/>
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C595" s="2" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="E595" s="3" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="F595" s="5" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C596" s="0" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="E596" s="3" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="F596" s="5" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C597" s="0" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="E597" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="F597" s="5" t="s">
         <v>709</v>
-      </c>
-      <c r="F597" s="5" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C603" s="0" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="E603" s="3" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="F603" s="3" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C604" s="0" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="E604" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="F604" s="3" t="s">
         <v>714</v>
-      </c>
-      <c r="F604" s="3" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C605" s="0" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="E605" s="6" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="F605" s="3" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C606" s="0" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="E606" s="3" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="F606" s="3" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C607" s="0" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="E607" s="3" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="F607" s="3" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C608" s="0" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="E608" s="3" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="F608" s="3" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C609" s="0" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E609" s="3" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="F609" s="3" t="s">
-        <v>712</v>
-      </c>
+        <v>714</v>
+      </c>
+    </row>
+    <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A614" s="0" t="s">
+        <v>727</v>
+      </c>
+      <c r="C614" s="0" t="s">
+        <v>728</v>
+      </c>
+      <c r="E614" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="F614" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G614" s="7"/>
+      <c r="H614" s="5"/>
+    </row>
+    <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A615" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="C615" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="E615" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="F615" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G615" s="7"/>
+      <c r="H615" s="5"/>
+    </row>
+    <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A616" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="C616" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="E616" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="F616" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G616" s="7"/>
+      <c r="H616" s="5"/>
+    </row>
+    <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A617" s="0" t="s">
+        <v>735</v>
+      </c>
+      <c r="C617" s="0" t="s">
+        <v>736</v>
+      </c>
+      <c r="E617" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="F617" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G617" s="7"/>
+      <c r="H617" s="3"/>
+    </row>
+    <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A618" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C618" s="0" t="s">
+        <v>738</v>
+      </c>
+      <c r="E618" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="F618" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G618" s="7"/>
+      <c r="H618" s="3"/>
+    </row>
+    <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A619" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C619" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="E619" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="F619" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G619" s="7"/>
+      <c r="H619" s="5"/>
+    </row>
+    <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A620" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C620" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="E620" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="F620" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G620" s="7"/>
+      <c r="H620" s="5"/>
+    </row>
+    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A621" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C621" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="E621" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="F621" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="G621" s="7"/>
+      <c r="H621" s="3"/>
+    </row>
+    <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A622" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C622" s="0" t="s">
+        <v>746</v>
+      </c>
+      <c r="E622" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="F622" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="G622" s="7"/>
+      <c r="H622" s="3"/>
+    </row>
+    <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A623" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C623" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="E623" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="F623" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="G623" s="9"/>
+      <c r="H623" s="3"/>
+    </row>
+    <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A624" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C624" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="E624" s="9" t="s">
+        <v>751</v>
+      </c>
+      <c r="F624" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="G624" s="9"/>
+      <c r="H624" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Adding "step 2" double radiation call variables to the pre identified missing files #141.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="762">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2276,6 +2276,36 @@
   </si>
   <si>
     <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the U component of wind (grib 128.131) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlutaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlutcsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsutaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #403   aerosol free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsutcsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsdscsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsuscsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #405</t>
   </si>
 </sst>
 </file>
@@ -2531,10 +2561,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H624"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A593" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C616" activeCellId="0" sqref="C616"/>
+      <selection pane="topLeft" activeCell="I626" activeCellId="0" sqref="I626:I631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9817,6 +9847,103 @@
       <c r="G624" s="9"/>
       <c r="H624" s="3"/>
     </row>
+    <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A626" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C626" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="E626" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="F626" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G626" s="3"/>
+      <c r="H626" s="3"/>
+    </row>
+    <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A627" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C627" s="0" t="s">
+        <v>754</v>
+      </c>
+      <c r="E627" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="F627" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G627" s="3"/>
+      <c r="H627" s="3"/>
+    </row>
+    <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A628" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C628" s="0" t="s">
+        <v>756</v>
+      </c>
+      <c r="E628" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="F628" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G628" s="3"/>
+      <c r="H628" s="3"/>
+    </row>
+    <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A629" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C629" s="0" t="s">
+        <v>758</v>
+      </c>
+      <c r="E629" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="F629" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G629" s="3"/>
+      <c r="H629" s="3"/>
+    </row>
+    <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A630" s="0" t="s">
+        <v>727</v>
+      </c>
+      <c r="C630" s="0" t="s">
+        <v>759</v>
+      </c>
+      <c r="E630" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="F630" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G630" s="3"/>
+      <c r="H630" s="3"/>
+    </row>
+    <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A631" s="0" t="s">
+        <v>727</v>
+      </c>
+      <c r="C631" s="0" t="s">
+        <v>760</v>
+      </c>
+      <c r="E631" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="F631" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G631" s="3"/>
+      <c r="H631" s="3"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adding the "step 2" IFS variables with a grib code to the pre identified missing files #141.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2176" uniqueCount="830">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2388,6 +2388,177 @@
   <si>
     <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #405</t>
   </si>
+  <si>
+    <t xml:space="preserve">LImon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tasIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2M as in IFS (grib code 128.167)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tsIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use soil layer 1 temeperature as the proxy (grib 128.139)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tsnIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is Grib 128.238. But we never test it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsnIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prraIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.(142+143-144)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sblIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snmIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.45 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrroIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hflsIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfssIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsdsIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsusIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.(169-176)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rldsIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlusIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.(175-177)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: T-tendency from radiation: grib 128.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: T-tendency from convection : grib 128.105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: q-tendency from convection: grib 128.106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmonZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hrPlev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wsgmax10m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: 10 metre wind gust in the 6 hours: grib 128.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: convective cloud cover ccc: grib 128.185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lwp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: Total column liquid water: grib 128.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS:Vertical velocity:w: grib 128.135 requires unit conversion from Pa.s-1 to m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zmla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: Boundary layer height: grib 128.159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: Surface net thermal radiation: grib 128.177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: Surface net solar radiation: grib 128.176</t>
+  </si>
 </sst>
 </file>
 
@@ -2396,7 +2567,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2475,6 +2646,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2524,7 +2702,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2563,6 +2741,10 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2642,10 +2824,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H636"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A248" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E276" activeCellId="0" sqref="E276"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A628" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D639" activeCellId="0" sqref="D639:D665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10094,6 +10276,444 @@
       <c r="G636" s="3"/>
       <c r="H636" s="3"/>
     </row>
+    <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A639" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C639" s="0" t="s">
+        <v>774</v>
+      </c>
+      <c r="E639" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="F639" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G639" s="3"/>
+      <c r="H639" s="3"/>
+    </row>
+    <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A640" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C640" s="0" t="s">
+        <v>776</v>
+      </c>
+      <c r="E640" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="F640" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G640" s="3"/>
+      <c r="H640" s="3"/>
+      <c r="I640" s="3"/>
+    </row>
+    <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A641" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C641" s="0" t="s">
+        <v>778</v>
+      </c>
+      <c r="E641" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="F641" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G641" s="3"/>
+      <c r="H641" s="3"/>
+    </row>
+    <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A642" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C642" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="E642" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="F642" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G642" s="3"/>
+      <c r="H642" s="3"/>
+    </row>
+    <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A643" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C643" s="0" t="s">
+        <v>782</v>
+      </c>
+      <c r="E643" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="F643" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G643" s="3"/>
+      <c r="H643" s="3"/>
+    </row>
+    <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A644" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C644" s="0" t="s">
+        <v>784</v>
+      </c>
+      <c r="E644" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="F644" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G644" s="3"/>
+      <c r="H644" s="3"/>
+    </row>
+    <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A645" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C645" s="0" t="s">
+        <v>786</v>
+      </c>
+      <c r="E645" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="F645" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G645" s="3"/>
+      <c r="H645" s="3"/>
+    </row>
+    <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A646" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C646" s="0" t="s">
+        <v>788</v>
+      </c>
+      <c r="E646" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="F646" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G646" s="3"/>
+      <c r="H646" s="3"/>
+      <c r="I646" s="3"/>
+    </row>
+    <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A647" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C647" s="0" t="s">
+        <v>790</v>
+      </c>
+      <c r="E647" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="F647" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G647" s="3"/>
+      <c r="H647" s="3"/>
+    </row>
+    <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A648" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C648" s="0" t="s">
+        <v>792</v>
+      </c>
+      <c r="E648" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="F648" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G648" s="3"/>
+      <c r="H648" s="3"/>
+    </row>
+    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A649" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C649" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="E649" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="F649" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G649" s="3"/>
+      <c r="H649" s="3"/>
+    </row>
+    <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A650" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C650" s="0" t="s">
+        <v>796</v>
+      </c>
+      <c r="E650" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="F650" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G650" s="3"/>
+      <c r="H650" s="3"/>
+      <c r="I650" s="3"/>
+    </row>
+    <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A651" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C651" s="0" t="s">
+        <v>798</v>
+      </c>
+      <c r="E651" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="F651" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G651" s="3"/>
+      <c r="H651" s="3"/>
+    </row>
+    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A652" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C652" s="0" t="s">
+        <v>800</v>
+      </c>
+      <c r="E652" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="F652" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G652" s="3"/>
+      <c r="H652" s="3"/>
+    </row>
+    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A653" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="C653" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="E653" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="F653" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G653" s="3"/>
+      <c r="H653" s="3"/>
+    </row>
+    <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A654" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="C654" s="0" t="s">
+        <v>806</v>
+      </c>
+      <c r="E654" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="F654" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G654" s="3"/>
+      <c r="H654" s="3"/>
+    </row>
+    <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A655" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="C655" s="0" t="s">
+        <v>808</v>
+      </c>
+      <c r="E655" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="F655" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G655" s="3"/>
+      <c r="H655" s="3"/>
+    </row>
+    <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A656" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="C656" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="E656" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="F656" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G656" s="3"/>
+      <c r="H656" s="3"/>
+    </row>
+    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A657" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="C657" s="0" t="s">
+        <v>812</v>
+      </c>
+      <c r="E657" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F657" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G657" s="3"/>
+      <c r="H657" s="3"/>
+    </row>
+    <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A658" s="0" t="s">
+        <v>814</v>
+      </c>
+      <c r="C658" s="0" t="s">
+        <v>806</v>
+      </c>
+      <c r="E658" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="F658" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G658" s="3"/>
+      <c r="H658" s="3"/>
+    </row>
+    <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A659" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="C659" s="0" t="s">
+        <v>816</v>
+      </c>
+      <c r="E659" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="F659" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G659" s="3"/>
+      <c r="H659" s="3"/>
+    </row>
+    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A660" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="C660" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="E660" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="F660" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="G660" s="3"/>
+      <c r="H660" s="5"/>
+    </row>
+    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A661" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="C661" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="E661" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="F661" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G661" s="3"/>
+      <c r="H661" s="3"/>
+    </row>
+    <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A662" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="C662" s="0" t="s">
+        <v>822</v>
+      </c>
+      <c r="E662" s="10" t="s">
+        <v>823</v>
+      </c>
+      <c r="G662" s="10"/>
+    </row>
+    <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A663" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="C663" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="E663" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="F663" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="G663" s="3"/>
+      <c r="H663" s="5"/>
+    </row>
+    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A664" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="C664" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="E664" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="F664" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="G664" s="3"/>
+      <c r="H664" s="3"/>
+    </row>
+    <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A665" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="C665" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="E665" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="F665" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="G665" s="3"/>
+      <c r="H665" s="3"/>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adding available "step 2" IFS variables which have no grib code (but which can be produced in other ways) to the pre identified missing files #141.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2176" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="852">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2299,13 +2299,51 @@
     <t xml:space="preserve">tauupbl</t>
   </si>
   <si>
-    <t xml:space="preserve">Available in IFS: Eastward turbulent surface stress: grib 128.180 maybe the Eastward gravity wave surface stress grib 128.195 has to be added. This needs to be checked with ECMWF people.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF007FFF"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Available in IFS: Eastward turbulent surface stress: grib 128.180 maybe the Eastward gravity wave surface stress grib 128.195 has to be added. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This needs to be checked with ECMWF people.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">tauvpbl</t>
   </si>
   <si>
-    <t xml:space="preserve">Available in IFS: Northward turbulent surface stress: grib 128.181 maybe the Northward gravity wave surface stress grib 128.196 has to be added. This needs to be checked with ECMWF people.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF007FFF"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Available in IFS: Northward turbulent surface stress: grib 128.181 maybe the Northward gravity wave surface stress grib 128.196 has to be added. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This needs to be checked with ECMWF people.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">E3hr</t>
@@ -2407,7 +2445,25 @@
     <t xml:space="preserve">tsnIs</t>
   </si>
   <si>
-    <t xml:space="preserve">This is Grib 128.238. But we never test it</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This is Grib 128.238. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">But we never test it</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">prsnIs</t>
@@ -2558,6 +2614,99 @@
   </si>
   <si>
     <t xml:space="preserve">Available in IFS: Surface net solar radiation: grib 128.176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ksat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture  (not in the output; no grib code associated).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea &amp; Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rootdsl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture (not in the output, no grib code associated).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slthick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: independent of lon, lat. Top soil layer: 0-7 cm, Soil layer 2: 7-28 cm, Soil layer 3: 28-100 cm, Soil layer 4: 100-289 cm, added as issue #126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sncIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in IFS. Although it could be calculated from tile fractions and written out as extra output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sftgif</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This is the land ice mask and will be an extra variable in IFS (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">thomas: via PEXTRA?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">sftgrf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Greenland this is the same as above sftgif. We do not have Antarctic ice sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orogIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is grib 128.129 at surface. But be aware not missing up with the grib 128.129 for free atmospehre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternatively, just estimating the delta T per month. No direct grib code for the totoal T-tendency found. In IFS from Cycle 39R1: add all the T-Tendencies: grib 128.93 + 128.95 + 128.98 + 128.102 + 128.105 + 128.109. But with IFS cycle 36 the T-tendency of gravity wave drag grib 128.102 is bugged until Cycle 39R1. This has been checked by Gijs with ECMWF: https://software.ecmwf.int/wiki/pages/viewpage.action?pageId=97384581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFsubhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This site lon,lat is specifed by the experiment we guess, and should be available in the netcdf file. So far it doesn't seem to be specified in the data request: in the CMIP6_coordinate.json table file the requested": "" is empty for site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
   </si>
 </sst>
 </file>
@@ -2567,7 +2716,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2635,6 +2784,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF007FFF"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -2739,11 +2895,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2826,8 +2982,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A628" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D639" activeCellId="0" sqref="D639:D665"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A649" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D667" activeCellId="0" sqref="D667:D676"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10020,7 +10176,7 @@
       <c r="G619" s="7"/>
       <c r="H619" s="5"/>
     </row>
-    <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="620" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="0" t="s">
         <v>704</v>
       </c>
@@ -10036,7 +10192,7 @@
       <c r="G620" s="7"/>
       <c r="H620" s="5"/>
     </row>
-    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="621" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="0" t="s">
         <v>704</v>
       </c>
@@ -10309,7 +10465,7 @@
       <c r="H640" s="3"/>
       <c r="I640" s="3"/>
     </row>
-    <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="641" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="0" t="s">
         <v>773</v>
       </c>
@@ -10707,6 +10863,170 @@
       <c r="G665" s="3"/>
       <c r="H665" s="3"/>
     </row>
+    <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A667" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C667" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="E667" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="F667" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="G667" s="3"/>
+      <c r="H667" s="3"/>
+    </row>
+    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A668" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C668" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="E668" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="F668" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="G668" s="3"/>
+      <c r="H668" s="3"/>
+    </row>
+    <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A669" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C669" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="E669" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="F669" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="G669" s="3"/>
+      <c r="H669" s="3"/>
+    </row>
+    <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A670" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C670" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="E670" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="F670" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G670" s="3"/>
+      <c r="H670" s="3"/>
+    </row>
+    <row r="671" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A671" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C671" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="E671" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="F671" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G671" s="3"/>
+      <c r="H671" s="3"/>
+    </row>
+    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A672" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C672" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="E672" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="F672" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G672" s="3"/>
+      <c r="H672" s="3"/>
+    </row>
+    <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A673" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="C673" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="E673" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="F673" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="G673" s="3"/>
+      <c r="H673" s="3"/>
+    </row>
+    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A674" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="C674" s="0" t="s">
+        <v>846</v>
+      </c>
+      <c r="E674" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="F674" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G674" s="3"/>
+      <c r="H674" s="3"/>
+    </row>
+    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A675" s="0" t="s">
+        <v>848</v>
+      </c>
+      <c r="C675" s="0" t="s">
+        <v>849</v>
+      </c>
+      <c r="E675" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="F675" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="G675" s="3"/>
+      <c r="H675" s="5"/>
+    </row>
+    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A676" s="0" t="s">
+        <v>848</v>
+      </c>
+      <c r="C676" s="0" t="s">
+        <v>851</v>
+      </c>
+      <c r="E676" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="F676" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="G676" s="3"/>
+      <c r="H676" s="5"/>
+    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Few comment adjustements for two "step 2" IFS variables with a grib code to the pre identified missing files #141.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -2307,7 +2307,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Available in IFS: Eastward turbulent surface stress: grib 128.180 maybe the Eastward gravity wave surface stress grib 128.195 has to be added. </t>
+      <t xml:space="preserve">Available in IFS: Eastward turbulent surface stress (grib 128.180) plus the Eastward gravity wave surface stress (grib 128.195).  </t>
     </r>
     <r>
       <rPr>
@@ -2317,7 +2317,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">This needs to be checked with ECMWF people.</t>
+      <t xml:space="preserve">Check with data request or DynVar people if this is indeed what is asked here.</t>
     </r>
   </si>
   <si>
@@ -2332,7 +2332,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Available in IFS: Northward turbulent surface stress: grib 128.181 maybe the Northward gravity wave surface stress grib 128.196 has to be added. </t>
+      <t xml:space="preserve">Available in IFS: Northward turbulent surface stress (grib 128.181) plus the Northward gravity wave surface stress (grib 128.196).  </t>
     </r>
     <r>
       <rPr>
@@ -2342,7 +2342,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">This needs to be checked with ECMWF people.</t>
+      <t xml:space="preserve">Check with data request or DynVar people if this is indeed what is asked here.</t>
     </r>
   </si>
   <si>
@@ -2982,8 +2982,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A649" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D667" activeCellId="0" sqref="D667:D676"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A607" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E621" activeCellId="0" sqref="E621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10159,6 +10159,9 @@
       <c r="F614" s="3" t="s">
         <v>725</v>
       </c>
+    </row>
+    <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E618" s="7"/>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="0" t="s">

</xml_diff>

<commit_message>
Adding Efx "step 2" IFS variables to the pre basic ignored and pre basic identified missing files #141.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="862">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2707,6 +2707,36 @@
   </si>
   <si>
     <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wilt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilting point is defined in HTESSEL as a fraction (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128) of field capacity. (Alessandri A.: an Effective Wilting Point can be defined ... same as below discussion for the field capacity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fldcapacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum amount of water the soil can hold (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128). It is constant map in time in H-TESSEL (Alessandri A.: an Effective Field Capacity can be defined for coupling analysis pourpouses that will change with the effective vegetation cover; as soon as we have daily effective vegetation cover in the outputs we can compute as well the Effective Field capacity).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clayfrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): very fine (&amp; fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siltfrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): medium (&amp; medium fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandfrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): coarse in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
   </si>
 </sst>
 </file>
@@ -2982,8 +3012,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A607" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E621" activeCellId="0" sqref="E621"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A665" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E680" activeCellId="0" sqref="E680:F684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11025,6 +11055,86 @@
       </c>
       <c r="G676" s="3"/>
       <c r="H676" s="5"/>
+    </row>
+    <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A680" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C680" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="E680" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="F680" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="G680" s="3"/>
+      <c r="H680" s="3"/>
+    </row>
+    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A681" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C681" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="E681" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="F681" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="G681" s="3"/>
+      <c r="H681" s="3"/>
+    </row>
+    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A682" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C682" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E682" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="F682" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="G682" s="3"/>
+      <c r="H682" s="3"/>
+    </row>
+    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A683" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C683" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="E683" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="F683" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="G683" s="3"/>
+      <c r="H683" s="3"/>
+    </row>
+    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A684" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="C684" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="E684" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="F684" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="G684" s="3"/>
+      <c r="H684" s="3"/>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Remove a special character from in the pre basic files, correction on #141 edits.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -1732,7 +1732,7 @@
     <t xml:space="preserve">Available in LPJ-GUESS, will be cmorized by Peter Anthoni &amp; Lars Nieradzik</t>
   </si>
   <si>
-    <t xml:space="preserve">David Wårlind</t>
+    <t xml:space="preserve">David Warlind</t>
   </si>
   <si>
     <t xml:space="preserve">mrsol</t>
@@ -2194,7 +2194,7 @@
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expfe</t>
   </si>
   <si>
-    <t xml:space="preserve">David Wårlind, Raffaele Bernardello</t>
+    <t xml:space="preserve">David Warlind, Raffaele Bernardello</t>
   </si>
   <si>
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expsi</t>
@@ -3012,8 +3012,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A665" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E680" activeCellId="0" sqref="E680:F684"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A418" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F438" activeCellId="0" sqref="F438:F440 F442:F533 F535:F537 F539:F574 F576:F579 F581:F589 F592:F596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Removing a special character in the comment column, so the writing of the ascii identified file is fine again
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -2212,7 +2212,7 @@
     <t xml:space="preserve">siflswdtop</t>
   </si>
   <si>
-    <t xml:space="preserve">Variable qsr_ice (solar heat flux at ice surface, W/m²),     &lt;field id="qsr_ice"   long_name="solar heat flux at ice surface: sum over categories"    standard_name="surface_downwelling_shortwave_flux_in_air"    unit="W/m2" </t>
+    <t xml:space="preserve">Variable qsr_ice (solar heat flux at ice surface, W/m2),     &lt;field id="qsr_ice"   long_name="solar heat flux at ice surface: sum over categories"    standard_name="surface_downwelling_shortwave_flux_in_air"    unit="W/m2" </t>
   </si>
   <si>
     <t xml:space="preserve">David Docquier, Torben</t>
@@ -3012,8 +3012,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E3:E269"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A578" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D600" activeCellId="0" sqref="D600"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Move the TM5? markend variables from the pre identified missing to the pre ignored file.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="857">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1681,12 +1681,6 @@
     <t xml:space="preserve">o3prod</t>
   </si>
   <si>
-    <t xml:space="preserve">pod0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in TM5??</t>
-  </si>
-  <si>
     <t xml:space="preserve">Emon</t>
   </si>
   <si>
@@ -1703,15 +1697,6 @@
   </si>
   <si>
     <t xml:space="preserve">md</t>
-  </si>
-  <si>
-    <t xml:space="preserve">od443dust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in TM5?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">od865dust</t>
   </si>
   <si>
     <t xml:space="preserve">loaddust</t>
@@ -3012,8 +2997,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A578" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D600" activeCellId="0" sqref="D600"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A409" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A429" activeCellId="0" sqref="A429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8247,13 +8232,13 @@
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="C425" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F425" s="0" t="s">
         <v>533</v>
@@ -8261,13 +8246,13 @@
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C426" s="0" t="s">
         <v>540</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F426" s="0" t="s">
         <v>533</v>
@@ -8275,13 +8260,13 @@
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C427" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="F427" s="0" t="s">
         <v>533</v>
@@ -8289,13 +8274,13 @@
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="C428" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="E428" s="0" t="s">
         <v>539</v>
-      </c>
-      <c r="C428" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="E428" s="0" t="s">
-        <v>532</v>
       </c>
       <c r="F428" s="0" t="s">
         <v>533</v>
@@ -8303,13 +8288,13 @@
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="C429" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="E429" s="0" t="s">
         <v>539</v>
-      </c>
-      <c r="C429" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="E429" s="0" t="s">
-        <v>541</v>
       </c>
       <c r="F429" s="0" t="s">
         <v>533</v>
@@ -8317,118 +8302,109 @@
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="C430" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="E430" s="0" t="s">
         <v>539</v>
-      </c>
-      <c r="C430" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="E430" s="0" t="s">
-        <v>546</v>
       </c>
       <c r="F430" s="0" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="C431" s="0" t="s">
-        <v>547</v>
-      </c>
-      <c r="E431" s="0" t="s">
-        <v>546</v>
-      </c>
-      <c r="F431" s="0" t="s">
-        <v>533</v>
-      </c>
-    </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C432" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E432" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="F432" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="E432" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="F432" s="3" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="C433" s="0" t="s">
-        <v>549</v>
-      </c>
-      <c r="E433" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="F433" s="0" t="s">
-        <v>533</v>
-      </c>
+      <c r="G432" s="3"/>
+      <c r="H432" s="3"/>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="0" t="s">
-        <v>539</v>
-      </c>
       <c r="C435" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="E435" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F435" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C436" s="0" t="s">
         <v>550</v>
       </c>
-      <c r="E435" s="3" t="s">
+      <c r="E436" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F436" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C437" s="0" t="s">
         <v>551</v>
       </c>
-      <c r="F435" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="G435" s="3"/>
-      <c r="H435" s="3"/>
-    </row>
-    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C438" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="E438" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="F438" s="0" t="s">
-        <v>554</v>
+      <c r="E437" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F437" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C439" s="0" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E439" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F439" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C440" s="0" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="E440" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F440" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C441" s="0" t="s">
         <v>553</v>
       </c>
-      <c r="F440" s="0" t="s">
-        <v>554</v>
+      <c r="E441" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F441" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C442" s="0" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8436,1473 +8412,1473 @@
         <v>555</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C444" s="0" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E444" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C445" s="0" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E445" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F445" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C446" s="0" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C447" s="0" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E447" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F447" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C448" s="0" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E448" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F448" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C449" s="0" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E449" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F449" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C450" s="0" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E450" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F450" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C451" s="0" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E451" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F451" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C452" s="0" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E452" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F452" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C453" s="0" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E453" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F453" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C454" s="0" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E454" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F454" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C455" s="0" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E455" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F455" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C456" s="0" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E456" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F456" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C457" s="0" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F457" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C458" s="0" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E458" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F458" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C459" s="0" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E459" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F459" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C460" s="0" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E460" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F460" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C461" s="0" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E461" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F461" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C462" s="0" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E462" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F462" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C463" s="0" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E463" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F463" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C464" s="0" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E464" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F464" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C465" s="0" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E465" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F465" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C466" s="0" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E466" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F466" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C467" s="0" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E467" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F467" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C468" s="0" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E468" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F468" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C469" s="0" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E469" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F469" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C470" s="0" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E470" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F470" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C471" s="0" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E471" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F471" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C472" s="0" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E472" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F472" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C473" s="0" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C474" s="0" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E474" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F474" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C475" s="0" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C476" s="0" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F476" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C477" s="0" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F477" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C478" s="0" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E478" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F478" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C479" s="0" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E479" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F479" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C480" s="0" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E480" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F480" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C481" s="0" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E481" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F481" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C482" s="0" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E482" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F482" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C483" s="0" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E483" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F483" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C484" s="0" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E484" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F484" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C485" s="0" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E485" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F485" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C486" s="0" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F486" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C487" s="0" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F487" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C488" s="0" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C489" s="0" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C490" s="0" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E490" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F490" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C491" s="0" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F491" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C492" s="0" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F492" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C493" s="0" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F493" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C494" s="0" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E494" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F494" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C495" s="0" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E495" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F495" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C496" s="0" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E496" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F496" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C497" s="0" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E497" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F497" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C498" s="0" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F498" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C499" s="0" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C500" s="0" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E500" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F500" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C501" s="0" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E501" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F501" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C502" s="0" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E502" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F502" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="0" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E503" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F503" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C504" s="0" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E504" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F504" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C505" s="0" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F505" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C506" s="0" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E506" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F506" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C507" s="0" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E507" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F507" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C508" s="0" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E508" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F508" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C509" s="0" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E509" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F509" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C510" s="0" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E510" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F510" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C511" s="0" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E511" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F511" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C512" s="0" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E512" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F512" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C513" s="0" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E513" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F513" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="0" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E514" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F514" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="0" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E515" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F515" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="0" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E516" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F516" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C517" s="0" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E517" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F517" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C518" s="0" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E518" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F518" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C519" s="0" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C520" s="0" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E520" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C521" s="0" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C522" s="0" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="0" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="0" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E524" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C525" s="0" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E525" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F525" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C526" s="0" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E526" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F526" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C527" s="0" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E527" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F527" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C528" s="0" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E528" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F528" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C529" s="0" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E529" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F529" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C530" s="0" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E530" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F530" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C531" s="0" t="s">
-        <v>645</v>
-      </c>
-      <c r="E531" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="F531" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="0" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E532" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F532" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C533" s="0" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E533" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F533" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C535" s="0" t="s">
-        <v>648</v>
-      </c>
-      <c r="E535" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="F535" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C534" s="0" t="s">
+        <v>633</v>
+      </c>
+      <c r="E534" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F534" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C536" s="0" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="E536" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F536" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C537" s="0" t="s">
-        <v>638</v>
+        <v>646</v>
       </c>
       <c r="E537" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F537" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C538" s="0" t="s">
+        <v>647</v>
+      </c>
+      <c r="E538" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F538" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="0" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E539" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F539" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="0" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E540" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F540" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C541" s="0" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E541" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F541" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C542" s="0" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E542" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F542" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C543" s="0" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E543" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F543" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C544" s="0" t="s">
-        <v>655</v>
+        <v>551</v>
       </c>
       <c r="E544" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F544" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C545" s="0" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="E545" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F545" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C546" s="0" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="E546" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F546" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C547" s="0" t="s">
-        <v>556</v>
+        <v>655</v>
       </c>
       <c r="E547" s="0" t="s">
-        <v>553</v>
+        <v>656</v>
       </c>
       <c r="F547" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C548" s="0" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E548" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F548" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C549" s="0" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E549" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F549" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C550" s="0" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E550" s="0" t="s">
-        <v>661</v>
+        <v>548</v>
       </c>
       <c r="F550" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C551" s="0" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E551" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F551" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C552" s="0" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E552" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F552" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C553" s="0" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E553" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F553" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C554" s="0" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="E554" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F554" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C555" s="0" t="s">
-        <v>666</v>
+        <v>547</v>
       </c>
       <c r="E555" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F555" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C556" s="0" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="E556" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F556" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C557" s="0" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E557" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F557" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C558" s="0" t="s">
-        <v>552</v>
+        <v>666</v>
       </c>
       <c r="E558" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F558" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C559" s="0" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E559" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F559" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C560" s="0" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E560" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F560" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C561" s="0" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="E561" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F561" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C562" s="0" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E562" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F562" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C563" s="0" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E563" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F563" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C564" s="0" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E564" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F564" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C565" s="0" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E565" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F565" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C566" s="0" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E566" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F566" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C567" s="0" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="E567" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F567" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C568" s="0" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E568" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F568" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C569" s="0" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="E569" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F569" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C570" s="0" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E570" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F570" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C571" s="0" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="E571" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F571" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C572" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="E572" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="F572" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C573" s="0" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="E573" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F573" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C574" s="0" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="E574" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F574" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C575" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="E575" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="F575" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C576" s="0" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E576" s="0" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F576" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C577" s="0" t="s">
-        <v>686</v>
-      </c>
-      <c r="E577" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="F577" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C578" s="0" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E578" s="0" t="s">
-        <v>553</v>
+        <v>685</v>
       </c>
       <c r="F578" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C579" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="E579" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="F579" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C580" s="0" t="s">
         <v>688</v>
       </c>
-      <c r="E579" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="F579" s="0" t="s">
-        <v>554</v>
+      <c r="E580" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="F580" s="0" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9913,7 +9889,7 @@
         <v>690</v>
       </c>
       <c r="F581" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9924,7 +9900,7 @@
         <v>692</v>
       </c>
       <c r="F582" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9932,452 +9908,467 @@
         <v>693</v>
       </c>
       <c r="E583" s="0" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="F583" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C584" s="0" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E584" s="0" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="F584" s="0" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C585" s="0" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E585" s="0" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="F585" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="586" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A586" s="0" t="s">
+        <v>699</v>
+      </c>
       <c r="C586" s="0" t="s">
-        <v>698</v>
-      </c>
-      <c r="E586" s="0" t="s">
-        <v>699</v>
+        <v>700</v>
+      </c>
+      <c r="E586" s="3" t="s">
+        <v>701</v>
       </c>
       <c r="F586" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C587" s="0" t="s">
-        <v>700</v>
-      </c>
-      <c r="E587" s="0" t="s">
-        <v>701</v>
-      </c>
-      <c r="F587" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C588" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="G586" s="3"/>
+      <c r="H586" s="4"/>
+    </row>
+    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C589" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E589" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="E588" s="0" t="s">
+      <c r="F589" s="0" t="s">
         <v>703</v>
       </c>
-      <c r="F588" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A589" s="0" t="s">
+    </row>
+    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C590" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E590" s="0" t="s">
         <v>704</v>
       </c>
-      <c r="C589" s="0" t="s">
+      <c r="F590" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C591" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E591" s="0" t="s">
         <v>705</v>
       </c>
-      <c r="E589" s="3" t="s">
-        <v>706</v>
-      </c>
-      <c r="F589" s="0" t="s">
-        <v>554</v>
-      </c>
-      <c r="G589" s="3"/>
-      <c r="H589" s="4"/>
+      <c r="F591" s="0" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C592" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E592" s="2" t="s">
-        <v>707</v>
+        <v>195</v>
+      </c>
+      <c r="E592" s="0" t="s">
+        <v>706</v>
       </c>
       <c r="F592" s="0" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C593" s="0" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="E593" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="F593" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="595" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A595" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C595" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="E595" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="F593" s="0" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C594" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E594" s="0" t="s">
+      <c r="F595" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="F594" s="0" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C595" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="E595" s="0" t="s">
+      <c r="G595" s="3"/>
+      <c r="H595" s="3"/>
+    </row>
+    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C597" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="F595" s="0" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C596" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E596" s="0" t="s">
-        <v>711</v>
-      </c>
-      <c r="F596" s="0" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="598" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A598" s="2" t="s">
+      <c r="E597" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="C598" s="2" t="s">
+      <c r="F597" s="5" t="s">
         <v>713</v>
+      </c>
+    </row>
+    <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C598" s="0" t="s">
+        <v>286</v>
       </c>
       <c r="E598" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="F598" s="3" t="s">
+      <c r="F598" s="5" t="s">
         <v>715</v>
       </c>
-      <c r="G598" s="3"/>
-      <c r="H598" s="3"/>
-    </row>
-    <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C600" s="2" t="s">
+    </row>
+    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C599" s="0" t="s">
         <v>716</v>
       </c>
-      <c r="E600" s="3" t="s">
+      <c r="E599" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="F600" s="5" t="s">
+      <c r="F599" s="5" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C605" s="0" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C601" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="E601" s="3" t="s">
+      <c r="E605" s="3" t="s">
         <v>719</v>
       </c>
-      <c r="F601" s="5" t="s">
+      <c r="F605" s="3" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C602" s="0" t="s">
+    <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C606" s="0" t="s">
         <v>721</v>
       </c>
-      <c r="E602" s="3" t="s">
+      <c r="E606" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="F602" s="5" t="s">
+      <c r="F606" s="3" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C607" s="0" t="s">
+        <v>723</v>
+      </c>
+      <c r="E607" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="F607" s="3" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C608" s="0" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="E608" s="3" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="F608" s="3" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C609" s="0" t="s">
-        <v>726</v>
-      </c>
-      <c r="E609" s="6" t="s">
         <v>727</v>
       </c>
+      <c r="E609" s="3" t="s">
+        <v>728</v>
+      </c>
       <c r="F609" s="3" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C610" s="0" t="s">
-        <v>728</v>
-      </c>
-      <c r="E610" s="6" t="s">
         <v>729</v>
       </c>
+      <c r="E610" s="3" t="s">
+        <v>730</v>
+      </c>
       <c r="F610" s="3" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C611" s="0" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="E611" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F611" s="3" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C612" s="0" t="s">
-        <v>732</v>
-      </c>
-      <c r="E612" s="3" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E615" s="7"/>
+    </row>
+    <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A616" s="0" t="s">
         <v>733</v>
       </c>
-      <c r="F612" s="3" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C613" s="0" t="s">
+      <c r="C616" s="0" t="s">
         <v>734</v>
       </c>
-      <c r="E613" s="3" t="s">
+      <c r="E616" s="7" t="s">
         <v>735</v>
       </c>
-      <c r="F613" s="3" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C614" s="0" t="s">
+      <c r="F616" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="E614" s="3" t="s">
+      <c r="G616" s="7"/>
+      <c r="H616" s="5"/>
+    </row>
+    <row r="617" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A617" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="C617" s="8" t="s">
         <v>737</v>
       </c>
-      <c r="F614" s="3" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E618" s="7"/>
+      <c r="E617" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="F617" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="G617" s="7"/>
+      <c r="H617" s="5"/>
+    </row>
+    <row r="618" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A618" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="C618" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="E618" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="F618" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="G618" s="7"/>
+      <c r="H618" s="5"/>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="0" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="C619" s="0" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="E619" s="7" t="s">
-        <v>740</v>
-      </c>
-      <c r="F619" s="5" t="s">
-        <v>741</v>
+        <v>743</v>
+      </c>
+      <c r="F619" s="3" t="s">
+        <v>533</v>
       </c>
       <c r="G619" s="7"/>
-      <c r="H619" s="5"/>
-    </row>
-    <row r="620" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H619" s="3"/>
+    </row>
+    <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="C620" s="8" t="s">
-        <v>742</v>
+        <v>537</v>
+      </c>
+      <c r="C620" s="0" t="s">
+        <v>744</v>
       </c>
       <c r="E620" s="7" t="s">
-        <v>743</v>
-      </c>
-      <c r="F620" s="5" t="s">
-        <v>741</v>
+        <v>745</v>
+      </c>
+      <c r="F620" s="3" t="s">
+        <v>533</v>
       </c>
       <c r="G620" s="7"/>
-      <c r="H620" s="5"/>
-    </row>
-    <row r="621" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H620" s="3"/>
+    </row>
+    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="C621" s="8" t="s">
-        <v>744</v>
+        <v>537</v>
+      </c>
+      <c r="C621" s="0" t="s">
+        <v>746</v>
       </c>
       <c r="E621" s="7" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="F621" s="5" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="G621" s="7"/>
       <c r="H621" s="5"/>
     </row>
     <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="0" t="s">
-        <v>746</v>
+        <v>537</v>
       </c>
       <c r="C622" s="0" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="E622" s="7" t="s">
-        <v>748</v>
-      </c>
-      <c r="F622" s="3" t="s">
-        <v>533</v>
+        <v>749</v>
+      </c>
+      <c r="F622" s="5" t="s">
+        <v>736</v>
       </c>
       <c r="G622" s="7"/>
-      <c r="H622" s="3"/>
+      <c r="H622" s="5"/>
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C623" s="0" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="E623" s="7" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="F623" s="3" t="s">
-        <v>533</v>
+        <v>736</v>
       </c>
       <c r="G623" s="7"/>
       <c r="H623" s="3"/>
     </row>
     <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C624" s="0" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="E624" s="7" t="s">
-        <v>752</v>
-      </c>
-      <c r="F624" s="5" t="s">
-        <v>741</v>
+        <v>753</v>
+      </c>
+      <c r="F624" s="3" t="s">
+        <v>736</v>
       </c>
       <c r="G624" s="7"/>
-      <c r="H624" s="5"/>
+      <c r="H624" s="3"/>
     </row>
     <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C625" s="0" t="s">
-        <v>753</v>
-      </c>
-      <c r="E625" s="7" t="s">
         <v>754</v>
       </c>
-      <c r="F625" s="5" t="s">
-        <v>741</v>
-      </c>
-      <c r="G625" s="7"/>
-      <c r="H625" s="5"/>
+      <c r="E625" s="9" t="s">
+        <v>755</v>
+      </c>
+      <c r="F625" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="G625" s="9"/>
+      <c r="H625" s="3"/>
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="0" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C626" s="0" t="s">
-        <v>755</v>
-      </c>
-      <c r="E626" s="7" t="s">
         <v>756</v>
       </c>
+      <c r="E626" s="9" t="s">
+        <v>757</v>
+      </c>
       <c r="F626" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="G626" s="7"/>
+        <v>736</v>
+      </c>
+      <c r="G626" s="9"/>
       <c r="H626" s="3"/>
-    </row>
-    <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A627" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="C627" s="0" t="s">
-        <v>757</v>
-      </c>
-      <c r="E627" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="F627" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="G627" s="7"/>
-      <c r="H627" s="3"/>
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="0" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="C628" s="0" t="s">
+        <v>758</v>
+      </c>
+      <c r="E628" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="E628" s="9" t="s">
-        <v>760</v>
-      </c>
       <c r="F628" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="G628" s="9"/>
+        <v>533</v>
+      </c>
+      <c r="G628" s="3"/>
       <c r="H628" s="3"/>
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="0" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="C629" s="0" t="s">
+        <v>760</v>
+      </c>
+      <c r="E629" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="E629" s="9" t="s">
+      <c r="F629" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G629" s="3"/>
+      <c r="H629" s="3"/>
+    </row>
+    <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A630" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="C630" s="0" t="s">
         <v>762</v>
       </c>
-      <c r="F629" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="G629" s="9"/>
-      <c r="H629" s="3"/>
+      <c r="E630" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="F630" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G630" s="3"/>
+      <c r="H630" s="3"/>
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="0" t="s">
         <v>530</v>
       </c>
       <c r="C631" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="E631" s="3" t="s">
         <v>763</v>
-      </c>
-      <c r="E631" s="3" t="s">
-        <v>764</v>
       </c>
       <c r="F631" s="3" t="s">
         <v>533</v>
@@ -10387,13 +10378,13 @@
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="0" t="s">
-        <v>530</v>
+        <v>733</v>
       </c>
       <c r="C632" s="0" t="s">
         <v>765</v>
       </c>
       <c r="E632" s="3" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="F632" s="3" t="s">
         <v>533</v>
@@ -10403,13 +10394,13 @@
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="0" t="s">
-        <v>530</v>
+        <v>733</v>
       </c>
       <c r="C633" s="0" t="s">
+        <v>766</v>
+      </c>
+      <c r="E633" s="3" t="s">
         <v>767</v>
-      </c>
-      <c r="E633" s="3" t="s">
-        <v>768</v>
       </c>
       <c r="F633" s="3" t="s">
         <v>533</v>
@@ -10417,370 +10408,370 @@
       <c r="G633" s="3"/>
       <c r="H633" s="3"/>
     </row>
-    <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A634" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="C634" s="0" t="s">
-        <v>769</v>
-      </c>
-      <c r="E634" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="F634" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="G634" s="3"/>
-      <c r="H634" s="3"/>
-    </row>
-    <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A635" s="0" t="s">
-        <v>738</v>
-      </c>
-      <c r="C635" s="0" t="s">
-        <v>770</v>
-      </c>
-      <c r="E635" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="F635" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="G635" s="3"/>
-      <c r="H635" s="3"/>
-    </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="0" t="s">
-        <v>738</v>
+        <v>768</v>
       </c>
       <c r="C636" s="0" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E636" s="3" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F636" s="3" t="s">
-        <v>533</v>
+        <v>713</v>
       </c>
       <c r="G636" s="3"/>
       <c r="H636" s="3"/>
     </row>
+    <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A637" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="C637" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="E637" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="F637" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="G637" s="3"/>
+      <c r="H637" s="3"/>
+      <c r="I637" s="3"/>
+    </row>
+    <row r="638" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A638" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="C638" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="E638" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F638" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="G638" s="3"/>
+      <c r="H638" s="3"/>
+    </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C639" s="0" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E639" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="F639" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G639" s="3"/>
       <c r="H639" s="3"/>
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C640" s="0" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="E640" s="3" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F640" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G640" s="3"/>
       <c r="H640" s="3"/>
-      <c r="I640" s="3"/>
-    </row>
-    <row r="641" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C641" s="0" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="E641" s="3" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F641" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G641" s="3"/>
       <c r="H641" s="3"/>
     </row>
     <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C642" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="E642" s="3" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F642" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G642" s="3"/>
       <c r="H642" s="3"/>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C643" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="E643" s="3" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="F643" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G643" s="3"/>
       <c r="H643" s="3"/>
+      <c r="I643" s="3"/>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C644" s="0" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="E644" s="3" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F644" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G644" s="3"/>
       <c r="H644" s="3"/>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C645" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="E645" s="3" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="F645" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G645" s="3"/>
       <c r="H645" s="3"/>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C646" s="0" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="E646" s="3" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="F646" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G646" s="3"/>
       <c r="H646" s="3"/>
-      <c r="I646" s="3"/>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C647" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="E647" s="3" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F647" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G647" s="3"/>
       <c r="H647" s="3"/>
+      <c r="I647" s="3"/>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C648" s="0" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E648" s="3" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F648" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G648" s="3"/>
       <c r="H648" s="3"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C649" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="E649" s="3" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="F649" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G649" s="3"/>
       <c r="H649" s="3"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
-        <v>773</v>
+        <v>797</v>
       </c>
       <c r="C650" s="0" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="E650" s="3" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="F650" s="3" t="s">
-        <v>718</v>
+        <v>800</v>
       </c>
       <c r="G650" s="3"/>
       <c r="H650" s="3"/>
-      <c r="I650" s="3"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
-        <v>773</v>
+        <v>797</v>
       </c>
       <c r="C651" s="0" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="E651" s="3" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="F651" s="3" t="s">
-        <v>718</v>
+        <v>800</v>
       </c>
       <c r="G651" s="3"/>
       <c r="H651" s="3"/>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="0" t="s">
-        <v>773</v>
+        <v>797</v>
       </c>
       <c r="C652" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="E652" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="F652" s="3" t="s">
         <v>800</v>
-      </c>
-      <c r="E652" s="3" t="s">
-        <v>801</v>
-      </c>
-      <c r="F652" s="3" t="s">
-        <v>718</v>
       </c>
       <c r="G652" s="3"/>
       <c r="H652" s="3"/>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="0" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="C653" s="0" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="E653" s="3" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="F653" s="3" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="G653" s="3"/>
       <c r="H653" s="3"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="C654" s="0" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E654" s="3" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="F654" s="3" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="G654" s="3"/>
       <c r="H654" s="3"/>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="0" t="s">
+        <v>809</v>
+      </c>
+      <c r="C655" s="0" t="s">
+        <v>801</v>
+      </c>
+      <c r="E655" s="3" t="s">
         <v>802</v>
       </c>
-      <c r="C655" s="0" t="s">
-        <v>808</v>
-      </c>
-      <c r="E655" s="3" t="s">
-        <v>809</v>
-      </c>
       <c r="F655" s="3" t="s">
-        <v>805</v>
+        <v>533</v>
       </c>
       <c r="G655" s="3"/>
       <c r="H655" s="3"/>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
-        <v>802</v>
+        <v>810</v>
       </c>
       <c r="C656" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="E656" s="3" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="F656" s="3" t="s">
-        <v>805</v>
+        <v>533</v>
       </c>
       <c r="G656" s="3"/>
       <c r="H656" s="3"/>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="0" t="s">
-        <v>802</v>
+        <v>530</v>
       </c>
       <c r="C657" s="0" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="E657" s="3" t="s">
-        <v>813</v>
-      </c>
-      <c r="F657" s="3" t="s">
-        <v>805</v>
+        <v>814</v>
+      </c>
+      <c r="F657" s="5" t="s">
+        <v>736</v>
       </c>
       <c r="G657" s="3"/>
-      <c r="H657" s="3"/>
+      <c r="H657" s="5"/>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
-        <v>814</v>
+        <v>530</v>
       </c>
       <c r="C658" s="0" t="s">
-        <v>806</v>
+        <v>815</v>
       </c>
       <c r="E658" s="3" t="s">
-        <v>807</v>
+        <v>816</v>
       </c>
       <c r="F658" s="3" t="s">
         <v>533</v>
@@ -10790,83 +10781,67 @@
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>815</v>
+        <v>530</v>
       </c>
       <c r="C659" s="0" t="s">
-        <v>816</v>
-      </c>
-      <c r="E659" s="3" t="s">
         <v>817</v>
       </c>
-      <c r="F659" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="G659" s="3"/>
-      <c r="H659" s="3"/>
+      <c r="E659" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="G659" s="10"/>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="0" t="s">
-        <v>530</v>
+        <v>699</v>
       </c>
       <c r="C660" s="0" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="E660" s="3" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="F660" s="5" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="G660" s="3"/>
       <c r="H660" s="5"/>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="0" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="C661" s="0" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="E661" s="3" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="F661" s="3" t="s">
-        <v>533</v>
+        <v>736</v>
       </c>
       <c r="G661" s="3"/>
       <c r="H661" s="3"/>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="C662" s="0" t="s">
-        <v>822</v>
-      </c>
-      <c r="E662" s="10" t="s">
         <v>823</v>
       </c>
-      <c r="G662" s="10"/>
-    </row>
-    <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A663" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="C663" s="0" t="s">
+      <c r="E662" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="E663" s="3" t="s">
-        <v>825</v>
-      </c>
-      <c r="F663" s="5" t="s">
-        <v>741</v>
-      </c>
-      <c r="G663" s="3"/>
-      <c r="H663" s="5"/>
+      <c r="F662" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="G662" s="3"/>
+      <c r="H662" s="3"/>
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="0" t="s">
-        <v>539</v>
+        <v>825</v>
       </c>
       <c r="C664" s="0" t="s">
         <v>826</v>
@@ -10875,267 +10850,238 @@
         <v>827</v>
       </c>
       <c r="F664" s="3" t="s">
-        <v>741</v>
+        <v>828</v>
       </c>
       <c r="G664" s="3"/>
       <c r="H664" s="3"/>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="s">
-        <v>539</v>
+        <v>825</v>
       </c>
       <c r="C665" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="E665" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="F665" s="3" t="s">
         <v>828</v>
-      </c>
-      <c r="E665" s="3" t="s">
-        <v>829</v>
-      </c>
-      <c r="F665" s="3" t="s">
-        <v>741</v>
       </c>
       <c r="G665" s="3"/>
       <c r="H665" s="3"/>
     </row>
+    <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A666" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="C666" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="E666" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="F666" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="G666" s="3"/>
+      <c r="H666" s="3"/>
+    </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
-        <v>830</v>
+        <v>768</v>
       </c>
       <c r="C667" s="0" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="E667" s="3" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="F667" s="3" t="s">
-        <v>833</v>
+        <v>713</v>
       </c>
       <c r="G667" s="3"/>
       <c r="H667" s="3"/>
     </row>
-    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="668" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="0" t="s">
-        <v>830</v>
+        <v>768</v>
       </c>
       <c r="C668" s="0" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E668" s="3" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F668" s="3" t="s">
-        <v>833</v>
+        <v>713</v>
       </c>
       <c r="G668" s="3"/>
       <c r="H668" s="3"/>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>830</v>
+        <v>768</v>
       </c>
       <c r="C669" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E669" s="3" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="F669" s="3" t="s">
-        <v>741</v>
+        <v>713</v>
       </c>
       <c r="G669" s="3"/>
       <c r="H669" s="3"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="C670" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E670" s="3" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="F670" s="3" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="G670" s="3"/>
       <c r="H670" s="3"/>
     </row>
-    <row r="671" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>773</v>
+        <v>797</v>
       </c>
       <c r="C671" s="0" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E671" s="3" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F671" s="3" t="s">
-        <v>718</v>
+        <v>800</v>
       </c>
       <c r="G671" s="3"/>
       <c r="H671" s="3"/>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>773</v>
+        <v>843</v>
       </c>
       <c r="C672" s="0" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="E672" s="3" t="s">
-        <v>843</v>
-      </c>
-      <c r="F672" s="3" t="s">
-        <v>718</v>
+        <v>845</v>
+      </c>
+      <c r="F672" s="5" t="s">
+        <v>736</v>
       </c>
       <c r="G672" s="3"/>
-      <c r="H672" s="3"/>
+      <c r="H672" s="5"/>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
-        <v>773</v>
+        <v>843</v>
       </c>
       <c r="C673" s="0" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="E673" s="3" t="s">
         <v>845</v>
       </c>
-      <c r="F673" s="3" t="s">
-        <v>718</v>
+      <c r="F673" s="5" t="s">
+        <v>736</v>
       </c>
       <c r="G673" s="3"/>
-      <c r="H673" s="3"/>
-    </row>
-    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A674" s="0" t="s">
-        <v>802</v>
-      </c>
-      <c r="C674" s="0" t="s">
-        <v>846</v>
-      </c>
-      <c r="E674" s="3" t="s">
+      <c r="H673" s="5"/>
+    </row>
+    <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A677" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="C677" s="0" t="s">
         <v>847</v>
       </c>
-      <c r="F674" s="3" t="s">
-        <v>805</v>
-      </c>
-      <c r="G674" s="3"/>
-      <c r="H674" s="3"/>
-    </row>
-    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A675" s="0" t="s">
+      <c r="E677" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="C675" s="0" t="s">
+      <c r="F677" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="G677" s="3"/>
+      <c r="H677" s="3"/>
+    </row>
+    <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A678" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="C678" s="0" t="s">
         <v>849</v>
       </c>
-      <c r="E675" s="3" t="s">
+      <c r="E678" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="F675" s="5" t="s">
-        <v>741</v>
-      </c>
-      <c r="G675" s="3"/>
-      <c r="H675" s="5"/>
-    </row>
-    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A676" s="0" t="s">
-        <v>848</v>
-      </c>
-      <c r="C676" s="0" t="s">
+      <c r="F678" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="G678" s="3"/>
+      <c r="H678" s="3"/>
+    </row>
+    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A679" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="C679" s="0" t="s">
         <v>851</v>
       </c>
-      <c r="E676" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="F676" s="5" t="s">
-        <v>741</v>
-      </c>
-      <c r="G676" s="3"/>
-      <c r="H676" s="5"/>
+      <c r="E679" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="F679" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="G679" s="3"/>
+      <c r="H679" s="3"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="C680" s="0" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="E680" s="3" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="F680" s="3" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="G680" s="3"/>
       <c r="H680" s="3"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="C681" s="0" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="E681" s="3" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="F681" s="3" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="G681" s="3"/>
       <c r="H681" s="3"/>
     </row>
-    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A682" s="0" t="s">
-        <v>830</v>
-      </c>
-      <c r="C682" s="0" t="s">
-        <v>856</v>
-      </c>
-      <c r="E682" s="3" t="s">
-        <v>857</v>
-      </c>
-      <c r="F682" s="3" t="s">
-        <v>833</v>
-      </c>
-      <c r="G682" s="3"/>
-      <c r="H682" s="3"/>
-    </row>
-    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A683" s="0" t="s">
-        <v>830</v>
-      </c>
-      <c r="C683" s="0" t="s">
-        <v>858</v>
-      </c>
-      <c r="E683" s="3" t="s">
-        <v>859</v>
-      </c>
-      <c r="F683" s="3" t="s">
-        <v>833</v>
-      </c>
-      <c r="G683" s="3"/>
-      <c r="H683" s="3"/>
-    </row>
-    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A684" s="0" t="s">
-        <v>830</v>
-      </c>
-      <c r="C684" s="0" t="s">
-        <v>860</v>
-      </c>
-      <c r="E684" s="3" t="s">
-        <v>861</v>
-      </c>
-      <c r="F684" s="3" t="s">
-        <v>833</v>
-      </c>
-      <c r="G684" s="3"/>
-      <c r="H684" s="3"/>
-    </row>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update for identification of some LS3MIP step 3 variables.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="870">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2195,6 +2195,24 @@
   </si>
   <si>
     <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same precipitation over crops as for the rest of the gridcell. Available in LPJ-GUESS, but the field will be the same precipitation over crops as for the rest of the gridcell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">et</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS. Is now implemented as a monthly output from LPJ-GUESS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS.  Already exist as - evspsblveg - Total Evaporation of intercepted water from Canopy [kg m-2 s-1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS.  Already exist as - tran - Transpiration [kg m-2 s-1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS.  Is now implemented as a monthly output from LPJ-GUESS.</t>
   </si>
   <si>
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expfe</t>
@@ -3022,8 +3040,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A420" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D433" activeCellId="0" sqref="D433"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A569" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A591" activeCellId="0" sqref="591:591"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9995,314 +10013,312 @@
       <c r="G586" s="4"/>
       <c r="H586" s="5"/>
     </row>
-    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A587" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="C587" s="0" t="s">
+        <v>709</v>
+      </c>
+      <c r="E587" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="F587" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="G587" s="4"/>
+      <c r="H587" s="5"/>
+    </row>
+    <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A588" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="C588" s="0" t="s">
+        <v>711</v>
+      </c>
+      <c r="E588" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="F588" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="G588" s="4"/>
+      <c r="H588" s="5"/>
+    </row>
+    <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A589" s="0" t="s">
+        <v>706</v>
+      </c>
       <c r="C589" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E589" s="2" t="s">
-        <v>709</v>
+        <v>659</v>
+      </c>
+      <c r="E589" s="4" t="s">
+        <v>713</v>
       </c>
       <c r="F589" s="0" t="s">
-        <v>710</v>
-      </c>
+        <v>556</v>
+      </c>
+      <c r="G589" s="4"/>
+      <c r="H589" s="5"/>
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A590" s="0" t="s">
+        <v>706</v>
+      </c>
       <c r="C590" s="0" t="s">
-        <v>142</v>
+        <v>551</v>
       </c>
       <c r="E590" s="0" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="F590" s="0" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C591" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E591" s="0" t="s">
-        <v>712</v>
-      </c>
-      <c r="F591" s="0" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C592" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="E592" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="F592" s="0" t="s">
-        <v>710</v>
+        <v>556</v>
       </c>
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C593" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E593" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="F593" s="0" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C594" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E594" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="F594" s="0" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C595" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E595" s="0" t="s">
+        <v>718</v>
+      </c>
+      <c r="F595" s="0" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C596" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E596" s="0" t="s">
+        <v>719</v>
+      </c>
+      <c r="F596" s="0" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C597" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="E593" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="F593" s="0" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="595" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A595" s="2" t="s">
-        <v>714</v>
-      </c>
-      <c r="C595" s="2" t="s">
-        <v>715</v>
-      </c>
-      <c r="E595" s="4" t="s">
+      <c r="E597" s="0" t="s">
+        <v>719</v>
+      </c>
+      <c r="F597" s="0" t="s">
         <v>716</v>
       </c>
-      <c r="F595" s="4" t="s">
-        <v>717</v>
-      </c>
-      <c r="G595" s="4"/>
-      <c r="H595" s="4"/>
-    </row>
-    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C597" s="2" t="s">
-        <v>718</v>
-      </c>
-      <c r="E597" s="4" t="s">
-        <v>719</v>
-      </c>
-      <c r="F597" s="6" t="s">
+    </row>
+    <row r="599" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A599" s="2" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C598" s="0" t="s">
+      <c r="C599" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="E599" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="F599" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="G599" s="4"/>
+      <c r="H599" s="4"/>
+    </row>
+    <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C601" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="E601" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="F601" s="6" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C602" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E598" s="4" t="s">
-        <v>721</v>
-      </c>
-      <c r="F598" s="6" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C599" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="E599" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="F599" s="6" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C605" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="E605" s="4" t="s">
-        <v>726</v>
-      </c>
-      <c r="F605" s="4" t="s">
+      <c r="E602" s="4" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C606" s="0" t="s">
+      <c r="F602" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="E606" s="7" t="s">
+    </row>
+    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C603" s="0" t="s">
         <v>729</v>
       </c>
-      <c r="F606" s="4" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C607" s="0" t="s">
+      <c r="E603" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="E607" s="7" t="s">
-        <v>731</v>
-      </c>
-      <c r="F607" s="4" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C608" s="0" t="s">
-        <v>732</v>
-      </c>
-      <c r="E608" s="4" t="s">
-        <v>733</v>
-      </c>
-      <c r="F608" s="4" t="s">
-        <v>727</v>
+      <c r="F603" s="6" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C609" s="0" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E609" s="4" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="F609" s="4" t="s">
-        <v>727</v>
+        <v>733</v>
       </c>
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C610" s="0" t="s">
-        <v>736</v>
-      </c>
-      <c r="E610" s="4" t="s">
-        <v>737</v>
+        <v>734</v>
+      </c>
+      <c r="E610" s="7" t="s">
+        <v>735</v>
       </c>
       <c r="F610" s="4" t="s">
-        <v>727</v>
+        <v>733</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C611" s="0" t="s">
+        <v>736</v>
+      </c>
+      <c r="E611" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="F611" s="4" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C612" s="0" t="s">
         <v>738</v>
       </c>
-      <c r="E611" s="4" t="s">
+      <c r="E612" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="F611" s="4" t="s">
-        <v>727</v>
+      <c r="F612" s="4" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C613" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="E613" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="F613" s="4" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C614" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="E614" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="F614" s="4" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E615" s="8"/>
-    </row>
-    <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A616" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="C616" s="0" t="s">
-        <v>741</v>
-      </c>
-      <c r="E616" s="8" t="s">
-        <v>742</v>
-      </c>
-      <c r="F616" s="6" t="s">
-        <v>743</v>
-      </c>
-      <c r="G616" s="8"/>
-      <c r="H616" s="6"/>
-    </row>
-    <row r="617" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A617" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="C617" s="9" t="s">
+      <c r="C615" s="0" t="s">
         <v>744</v>
       </c>
-      <c r="E617" s="8" t="s">
+      <c r="E615" s="4" t="s">
         <v>745</v>
       </c>
-      <c r="F617" s="6" t="s">
-        <v>743</v>
-      </c>
-      <c r="G617" s="8"/>
-      <c r="H617" s="6"/>
-    </row>
-    <row r="618" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A618" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="C618" s="9" t="s">
-        <v>746</v>
-      </c>
-      <c r="E618" s="8" t="s">
-        <v>747</v>
-      </c>
-      <c r="F618" s="6" t="s">
-        <v>743</v>
-      </c>
-      <c r="G618" s="8"/>
-      <c r="H618" s="6"/>
+      <c r="F615" s="4" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A619" s="0" t="s">
-        <v>748</v>
-      </c>
-      <c r="C619" s="0" t="s">
-        <v>749</v>
-      </c>
-      <c r="E619" s="8" t="s">
-        <v>750</v>
-      </c>
-      <c r="F619" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G619" s="8"/>
-      <c r="H619" s="4"/>
+      <c r="E619" s="8"/>
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="0" t="s">
-        <v>541</v>
+        <v>746</v>
       </c>
       <c r="C620" s="0" t="s">
+        <v>747</v>
+      </c>
+      <c r="E620" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="F620" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="G620" s="8"/>
+      <c r="H620" s="6"/>
+    </row>
+    <row r="621" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A621" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="C621" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="E621" s="8" t="s">
         <v>751</v>
       </c>
-      <c r="E620" s="8" t="s">
-        <v>752</v>
-      </c>
-      <c r="F620" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G620" s="8"/>
-      <c r="H620" s="4"/>
-    </row>
-    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A621" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="C621" s="0" t="s">
-        <v>753</v>
-      </c>
-      <c r="E621" s="8" t="s">
-        <v>754</v>
-      </c>
       <c r="F621" s="6" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="G621" s="8"/>
       <c r="H621" s="6"/>
     </row>
-    <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="622" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="C622" s="0" t="s">
-        <v>755</v>
+        <v>706</v>
+      </c>
+      <c r="C622" s="9" t="s">
+        <v>752</v>
       </c>
       <c r="E622" s="8" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="F622" s="6" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="G622" s="8"/>
       <c r="H622" s="6"/>
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="0" t="s">
-        <v>541</v>
+        <v>754</v>
       </c>
       <c r="C623" s="0" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E623" s="8" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F623" s="4" t="s">
-        <v>743</v>
+        <v>496</v>
       </c>
       <c r="G623" s="8"/>
       <c r="H623" s="4"/>
@@ -10312,13 +10328,13 @@
         <v>541</v>
       </c>
       <c r="C624" s="0" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E624" s="8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F624" s="4" t="s">
-        <v>743</v>
+        <v>496</v>
       </c>
       <c r="G624" s="8"/>
       <c r="H624" s="4"/>
@@ -10328,106 +10344,106 @@
         <v>541</v>
       </c>
       <c r="C625" s="0" t="s">
-        <v>761</v>
-      </c>
-      <c r="E625" s="10" t="s">
-        <v>762</v>
-      </c>
-      <c r="F625" s="4" t="s">
-        <v>743</v>
-      </c>
-      <c r="G625" s="10"/>
-      <c r="H625" s="4"/>
+        <v>759</v>
+      </c>
+      <c r="E625" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="F625" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="G625" s="8"/>
+      <c r="H625" s="6"/>
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="0" t="s">
         <v>541</v>
       </c>
       <c r="C626" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="E626" s="8" t="s">
+        <v>762</v>
+      </c>
+      <c r="F626" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="G626" s="8"/>
+      <c r="H626" s="6"/>
+    </row>
+    <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A627" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="C627" s="0" t="s">
         <v>763</v>
       </c>
-      <c r="E626" s="10" t="s">
+      <c r="E627" s="8" t="s">
         <v>764</v>
       </c>
-      <c r="F626" s="4" t="s">
-        <v>743</v>
-      </c>
-      <c r="G626" s="10"/>
-      <c r="H626" s="4"/>
+      <c r="F627" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="G627" s="8"/>
+      <c r="H627" s="4"/>
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="0" t="s">
-        <v>458</v>
+        <v>541</v>
       </c>
       <c r="C628" s="0" t="s">
         <v>765</v>
       </c>
-      <c r="E628" s="4" t="s">
+      <c r="E628" s="8" t="s">
         <v>766</v>
       </c>
       <c r="F628" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G628" s="4"/>
+        <v>749</v>
+      </c>
+      <c r="G628" s="8"/>
       <c r="H628" s="4"/>
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="0" t="s">
-        <v>458</v>
+        <v>541</v>
       </c>
       <c r="C629" s="0" t="s">
         <v>767</v>
       </c>
-      <c r="E629" s="4" t="s">
+      <c r="E629" s="10" t="s">
         <v>768</v>
       </c>
       <c r="F629" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G629" s="4"/>
+        <v>749</v>
+      </c>
+      <c r="G629" s="10"/>
       <c r="H629" s="4"/>
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="0" t="s">
-        <v>458</v>
+        <v>541</v>
       </c>
       <c r="C630" s="0" t="s">
         <v>769</v>
       </c>
-      <c r="E630" s="4" t="s">
+      <c r="E630" s="10" t="s">
         <v>770</v>
       </c>
       <c r="F630" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G630" s="4"/>
+        <v>749</v>
+      </c>
+      <c r="G630" s="10"/>
       <c r="H630" s="4"/>
-    </row>
-    <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A631" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="C631" s="0" t="s">
-        <v>771</v>
-      </c>
-      <c r="E631" s="4" t="s">
-        <v>770</v>
-      </c>
-      <c r="F631" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="G631" s="4"/>
-      <c r="H631" s="4"/>
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="0" t="s">
-        <v>740</v>
+        <v>458</v>
       </c>
       <c r="C632" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="E632" s="4" t="s">
         <v>772</v>
-      </c>
-      <c r="E632" s="4" t="s">
-        <v>768</v>
       </c>
       <c r="F632" s="4" t="s">
         <v>496</v>
@@ -10437,7 +10453,7 @@
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="0" t="s">
-        <v>740</v>
+        <v>458</v>
       </c>
       <c r="C633" s="0" t="s">
         <v>773</v>
@@ -10451,196 +10467,195 @@
       <c r="G633" s="4"/>
       <c r="H633" s="4"/>
     </row>
+    <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A634" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C634" s="0" t="s">
+        <v>775</v>
+      </c>
+      <c r="E634" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F634" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="G634" s="4"/>
+      <c r="H634" s="4"/>
+    </row>
+    <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A635" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C635" s="0" t="s">
+        <v>777</v>
+      </c>
+      <c r="E635" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F635" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="G635" s="4"/>
+      <c r="H635" s="4"/>
+    </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="0" t="s">
-        <v>775</v>
+        <v>746</v>
       </c>
       <c r="C636" s="0" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="E636" s="4" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="F636" s="4" t="s">
-        <v>720</v>
+        <v>496</v>
       </c>
       <c r="G636" s="4"/>
       <c r="H636" s="4"/>
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="0" t="s">
-        <v>775</v>
+        <v>746</v>
       </c>
       <c r="C637" s="0" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="E637" s="4" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F637" s="4" t="s">
-        <v>720</v>
+        <v>496</v>
       </c>
       <c r="G637" s="4"/>
       <c r="H637" s="4"/>
-      <c r="I637" s="4"/>
-    </row>
-    <row r="638" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A638" s="0" t="s">
-        <v>775</v>
-      </c>
-      <c r="C638" s="0" t="s">
-        <v>780</v>
-      </c>
-      <c r="E638" s="4" t="s">
-        <v>781</v>
-      </c>
-      <c r="F638" s="4" t="s">
-        <v>720</v>
-      </c>
-      <c r="G638" s="4"/>
-      <c r="H638" s="4"/>
-    </row>
-    <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A639" s="0" t="s">
-        <v>775</v>
-      </c>
-      <c r="C639" s="0" t="s">
-        <v>782</v>
-      </c>
-      <c r="E639" s="4" t="s">
-        <v>783</v>
-      </c>
-      <c r="F639" s="4" t="s">
-        <v>720</v>
-      </c>
-      <c r="G639" s="4"/>
-      <c r="H639" s="4"/>
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C640" s="0" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E640" s="4" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F640" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G640" s="4"/>
       <c r="H640" s="4"/>
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C641" s="0" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E641" s="4" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F641" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G641" s="4"/>
       <c r="H641" s="4"/>
-    </row>
-    <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I641" s="4"/>
+    </row>
+    <row r="642" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C642" s="0" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E642" s="4" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F642" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G642" s="4"/>
       <c r="H642" s="4"/>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C643" s="0" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E643" s="4" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F643" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G643" s="4"/>
       <c r="H643" s="4"/>
-      <c r="I643" s="4"/>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C644" s="0" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E644" s="4" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F644" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G644" s="4"/>
       <c r="H644" s="4"/>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C645" s="0" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E645" s="4" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F645" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G645" s="4"/>
       <c r="H645" s="4"/>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C646" s="0" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="E646" s="4" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F646" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G646" s="4"/>
       <c r="H646" s="4"/>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C647" s="0" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E647" s="4" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F647" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G647" s="4"/>
       <c r="H647" s="4"/>
@@ -10648,484 +10663,545 @@
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C648" s="0" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E648" s="4" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F648" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G648" s="4"/>
       <c r="H648" s="4"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C649" s="0" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E649" s="4" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F649" s="4" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="G649" s="4"/>
       <c r="H649" s="4"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
-        <v>804</v>
+        <v>781</v>
       </c>
       <c r="C650" s="0" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="E650" s="4" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="F650" s="4" t="s">
-        <v>807</v>
+        <v>726</v>
       </c>
       <c r="G650" s="4"/>
       <c r="H650" s="4"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="C651" s="0" t="s">
         <v>804</v>
       </c>
-      <c r="C651" s="0" t="s">
-        <v>808</v>
-      </c>
       <c r="E651" s="4" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="F651" s="4" t="s">
-        <v>807</v>
+        <v>726</v>
       </c>
       <c r="G651" s="4"/>
       <c r="H651" s="4"/>
+      <c r="I651" s="4"/>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="0" t="s">
-        <v>804</v>
+        <v>781</v>
       </c>
       <c r="C652" s="0" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="E652" s="4" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="F652" s="4" t="s">
-        <v>807</v>
+        <v>726</v>
       </c>
       <c r="G652" s="4"/>
       <c r="H652" s="4"/>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="0" t="s">
-        <v>804</v>
+        <v>781</v>
       </c>
       <c r="C653" s="0" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="E653" s="4" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="F653" s="4" t="s">
-        <v>807</v>
+        <v>726</v>
       </c>
       <c r="G653" s="4"/>
       <c r="H653" s="4"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>804</v>
+        <v>810</v>
       </c>
       <c r="C654" s="0" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="E654" s="4" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="F654" s="4" t="s">
-        <v>807</v>
+        <v>813</v>
       </c>
       <c r="G654" s="4"/>
       <c r="H654" s="4"/>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="0" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="C655" s="0" t="s">
-        <v>808</v>
+        <v>814</v>
       </c>
       <c r="E655" s="4" t="s">
-        <v>809</v>
+        <v>815</v>
       </c>
       <c r="F655" s="4" t="s">
-        <v>496</v>
+        <v>813</v>
       </c>
       <c r="G655" s="4"/>
       <c r="H655" s="4"/>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="C656" s="0" t="s">
+        <v>816</v>
+      </c>
+      <c r="E656" s="4" t="s">
         <v>817</v>
       </c>
-      <c r="C656" s="0" t="s">
-        <v>818</v>
-      </c>
-      <c r="E656" s="4" t="s">
-        <v>819</v>
-      </c>
       <c r="F656" s="4" t="s">
-        <v>496</v>
+        <v>813</v>
       </c>
       <c r="G656" s="4"/>
       <c r="H656" s="4"/>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="0" t="s">
-        <v>458</v>
+        <v>810</v>
       </c>
       <c r="C657" s="0" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E657" s="4" t="s">
-        <v>821</v>
-      </c>
-      <c r="F657" s="6" t="s">
-        <v>743</v>
+        <v>819</v>
+      </c>
+      <c r="F657" s="4" t="s">
+        <v>813</v>
       </c>
       <c r="G657" s="4"/>
-      <c r="H657" s="6"/>
+      <c r="H657" s="4"/>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
-        <v>458</v>
+        <v>810</v>
       </c>
       <c r="C658" s="0" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="E658" s="4" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="F658" s="4" t="s">
-        <v>496</v>
+        <v>813</v>
       </c>
       <c r="G658" s="4"/>
       <c r="H658" s="4"/>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>458</v>
+        <v>822</v>
       </c>
       <c r="C659" s="0" t="s">
-        <v>824</v>
-      </c>
-      <c r="E659" s="11" t="s">
-        <v>825</v>
-      </c>
-      <c r="G659" s="11"/>
+        <v>814</v>
+      </c>
+      <c r="E659" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="F659" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="G659" s="4"/>
+      <c r="H659" s="4"/>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="0" t="s">
-        <v>706</v>
+        <v>823</v>
       </c>
       <c r="C660" s="0" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="E660" s="4" t="s">
-        <v>827</v>
-      </c>
-      <c r="F660" s="6" t="s">
-        <v>743</v>
+        <v>825</v>
+      </c>
+      <c r="F660" s="4" t="s">
+        <v>496</v>
       </c>
       <c r="G660" s="4"/>
-      <c r="H660" s="6"/>
+      <c r="H660" s="4"/>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="0" t="s">
-        <v>541</v>
+        <v>458</v>
       </c>
       <c r="C661" s="0" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E661" s="4" t="s">
-        <v>829</v>
-      </c>
-      <c r="F661" s="4" t="s">
-        <v>743</v>
+        <v>827</v>
+      </c>
+      <c r="F661" s="6" t="s">
+        <v>749</v>
       </c>
       <c r="G661" s="4"/>
-      <c r="H661" s="4"/>
+      <c r="H661" s="6"/>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
-        <v>541</v>
+        <v>458</v>
       </c>
       <c r="C662" s="0" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="E662" s="4" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="F662" s="4" t="s">
-        <v>743</v>
+        <v>496</v>
       </c>
       <c r="G662" s="4"/>
       <c r="H662" s="4"/>
     </row>
+    <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A663" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C663" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="E663" s="11" t="s">
+        <v>831</v>
+      </c>
+      <c r="G663" s="11"/>
+    </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="C664" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="C664" s="0" t="s">
+      <c r="E664" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="E664" s="4" t="s">
-        <v>834</v>
-      </c>
-      <c r="F664" s="4" t="s">
-        <v>835</v>
+      <c r="F664" s="6" t="s">
+        <v>749</v>
       </c>
       <c r="G664" s="4"/>
-      <c r="H664" s="4"/>
+      <c r="H664" s="6"/>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="s">
-        <v>832</v>
+        <v>541</v>
       </c>
       <c r="C665" s="0" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E665" s="4" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="F665" s="4" t="s">
-        <v>835</v>
+        <v>749</v>
       </c>
       <c r="G665" s="4"/>
       <c r="H665" s="4"/>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
-        <v>832</v>
+        <v>541</v>
       </c>
       <c r="C666" s="0" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="E666" s="4" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="F666" s="4" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="G666" s="4"/>
       <c r="H666" s="4"/>
     </row>
-    <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A667" s="0" t="s">
-        <v>775</v>
-      </c>
-      <c r="C667" s="0" t="s">
+    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A668" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="C668" s="0" t="s">
+        <v>839</v>
+      </c>
+      <c r="E668" s="4" t="s">
         <v>840</v>
       </c>
-      <c r="E667" s="4" t="s">
+      <c r="F668" s="4" t="s">
         <v>841</v>
-      </c>
-      <c r="F667" s="4" t="s">
-        <v>720</v>
-      </c>
-      <c r="G667" s="4"/>
-      <c r="H667" s="4"/>
-    </row>
-    <row r="668" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A668" s="0" t="s">
-        <v>775</v>
-      </c>
-      <c r="C668" s="0" t="s">
-        <v>842</v>
-      </c>
-      <c r="E668" s="4" t="s">
-        <v>843</v>
-      </c>
-      <c r="F668" s="4" t="s">
-        <v>720</v>
       </c>
       <c r="G668" s="4"/>
       <c r="H668" s="4"/>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>775</v>
+        <v>838</v>
       </c>
       <c r="C669" s="0" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="E669" s="4" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="F669" s="4" t="s">
-        <v>720</v>
+        <v>841</v>
       </c>
       <c r="G669" s="4"/>
       <c r="H669" s="4"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>775</v>
+        <v>838</v>
       </c>
       <c r="C670" s="0" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E670" s="4" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="F670" s="4" t="s">
-        <v>720</v>
+        <v>749</v>
       </c>
       <c r="G670" s="4"/>
       <c r="H670" s="4"/>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>804</v>
+        <v>781</v>
       </c>
       <c r="C671" s="0" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E671" s="4" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="F671" s="4" t="s">
-        <v>807</v>
+        <v>726</v>
       </c>
       <c r="G671" s="4"/>
       <c r="H671" s="4"/>
     </row>
-    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="672" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>850</v>
+        <v>781</v>
       </c>
       <c r="C672" s="0" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="E672" s="4" t="s">
-        <v>852</v>
-      </c>
-      <c r="F672" s="6" t="s">
-        <v>743</v>
+        <v>849</v>
+      </c>
+      <c r="F672" s="4" t="s">
+        <v>726</v>
       </c>
       <c r="G672" s="4"/>
-      <c r="H672" s="6"/>
+      <c r="H672" s="4"/>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="C673" s="0" t="s">
         <v>850</v>
       </c>
-      <c r="C673" s="0" t="s">
+      <c r="E673" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="F673" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="G673" s="4"/>
+      <c r="H673" s="4"/>
+    </row>
+    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A674" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="C674" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="E674" s="4" t="s">
         <v>853</v>
       </c>
-      <c r="E673" s="4" t="s">
-        <v>852</v>
-      </c>
-      <c r="F673" s="6" t="s">
-        <v>743</v>
-      </c>
-      <c r="G673" s="4"/>
-      <c r="H673" s="6"/>
+      <c r="F674" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="G674" s="4"/>
+      <c r="H674" s="4"/>
+    </row>
+    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A675" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="C675" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="E675" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="F675" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="G675" s="4"/>
+      <c r="H675" s="4"/>
+    </row>
+    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A676" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="C676" s="0" t="s">
+        <v>857</v>
+      </c>
+      <c r="E676" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="F676" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="G676" s="4"/>
+      <c r="H676" s="6"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>832</v>
+        <v>856</v>
       </c>
       <c r="C677" s="0" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
       <c r="E677" s="4" t="s">
-        <v>855</v>
-      </c>
-      <c r="F677" s="4" t="s">
-        <v>835</v>
+        <v>858</v>
+      </c>
+      <c r="F677" s="6" t="s">
+        <v>749</v>
       </c>
       <c r="G677" s="4"/>
-      <c r="H677" s="4"/>
-    </row>
-    <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A678" s="0" t="s">
-        <v>832</v>
-      </c>
-      <c r="C678" s="0" t="s">
-        <v>856</v>
-      </c>
-      <c r="E678" s="4" t="s">
-        <v>857</v>
-      </c>
-      <c r="F678" s="4" t="s">
-        <v>835</v>
-      </c>
-      <c r="G678" s="4"/>
-      <c r="H678" s="4"/>
-    </row>
-    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A679" s="0" t="s">
-        <v>832</v>
-      </c>
-      <c r="C679" s="0" t="s">
-        <v>858</v>
-      </c>
-      <c r="E679" s="4" t="s">
-        <v>859</v>
-      </c>
-      <c r="F679" s="4" t="s">
-        <v>835</v>
-      </c>
-      <c r="G679" s="4"/>
-      <c r="H679" s="4"/>
-    </row>
-    <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A680" s="0" t="s">
-        <v>832</v>
-      </c>
-      <c r="C680" s="0" t="s">
-        <v>860</v>
-      </c>
-      <c r="E680" s="4" t="s">
-        <v>861</v>
-      </c>
-      <c r="F680" s="4" t="s">
-        <v>835</v>
-      </c>
-      <c r="G680" s="4"/>
-      <c r="H680" s="4"/>
+      <c r="H677" s="6"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
-        <v>832</v>
+        <v>838</v>
       </c>
       <c r="C681" s="0" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E681" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F681" s="4" t="s">
-        <v>835</v>
+        <v>841</v>
       </c>
       <c r="G681" s="4"/>
       <c r="H681" s="4"/>
     </row>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A682" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="C682" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="E682" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="F682" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="G682" s="4"/>
+      <c r="H682" s="4"/>
+    </row>
+    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A683" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="C683" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="E683" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="F683" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="G683" s="4"/>
+      <c r="H683" s="4"/>
+    </row>
+    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A684" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="C684" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="E684" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="F684" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="G684" s="4"/>
+      <c r="H684" s="4"/>
+    </row>
+    <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A685" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="C685" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="E685" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="F685" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="G685" s="4"/>
+      <c r="H685" s="4"/>
+    </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update the comment for fco2antt and fco2nat: available now in LPJ-GUESS #188.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="1125">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2380,7 +2380,39 @@
     <t xml:space="preserve">Carbon Mass Flux into Atmosphere Due to All Anthropogenic Emissions of CO2</t>
   </si>
   <si>
-    <t xml:space="preserve">Not available in the AOGCM, neither in TM5. TM5 can only provide total fluxes. Maybe sum the land use in LPJ-GUESS + fossil fuel from CEDS? This means it then has to be added in an additional post processing step.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Available in LPJ-GUESS, will be cmorized by Peter Anthoni &amp; Lars Nieradzik.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Previous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Not available in the AOGCM, neither in TM5. TM5 can only provide total fluxes. Maybe sum the land use in LPJ-GUESS + fossil fuel from CEDS? This means it then has to be added in an additional post processing step.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind, Tommi Bergman</t>
   </si>
   <si>
     <t xml:space="preserve">fco2fos</t>
@@ -2398,7 +2430,36 @@
     <t xml:space="preserve">Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources</t>
   </si>
   <si>
-    <t xml:space="preserve">Not available in the AOGCM, neither in TM5. TM5 can only provide total fluxes. It is not clear to us if this variable includes the contribution from land use. This variable can be calculated from the total CO2 flux provided by TM5 and the contributions from CEDS and land use from LPJ-GUESS. This "Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources" could be provided by LPJ-GUESS but its definition is very vague... Should we include emissions from managed forests? Cropland? Pasture? Any managed land? If a land has a history of being managed, but now is "natural"?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Available in LPJ-GUESS, will be cmorized by Peter Anthoni &amp; Lars Nieradzik.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Previous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: Not available in the AOGCM, neither in TM5. TM5 can only provide total fluxes. It is not clear to us if this variable includes the contribution from land use. This variable can be calculated from the total CO2 flux provided by TM5 and the contributions from CEDS and land use from LPJ-GUESS. This "Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources" could be provided by LPJ-GUESS but its definition is very vague... Should we include emissions from managed forests? Cropland? Pasture? Any managed land? If a land has a history of being managed, but now is "natural"?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">longitude latitude plev19 time2</t>
@@ -3802,13 +3863,13 @@
   </sheetPr>
   <dimension ref="A1:I687"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B255" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C269"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C403" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C414" activeCellId="0" sqref="414:414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.66"/>
@@ -8813,7 +8874,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B412" s="0" t="s">
         <v>566</v>
       </c>
@@ -8827,7 +8888,7 @@
         <v>770</v>
       </c>
       <c r="F412" s="0" t="s">
-        <v>555</v>
+        <v>771</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8835,47 +8896,47 @@
         <v>566</v>
       </c>
       <c r="C413" s="0" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D413" s="0" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="E413" s="0" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="F413" s="0" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B414" s="0" t="s">
         <v>566</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D414" s="0" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="E414" s="0" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F414" s="0" t="s">
-        <v>555</v>
+        <v>771</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B415" s="0" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C415" s="0" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="D415" s="0" t="s">
         <v>553</v>
       </c>
       <c r="E415" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F415" s="0" t="s">
         <v>555</v>
@@ -8883,16 +8944,16 @@
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B416" s="0" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C416" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D416" s="0" t="s">
         <v>557</v>
       </c>
       <c r="E416" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F416" s="0" t="s">
         <v>555</v>
@@ -8900,16 +8961,16 @@
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B417" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C417" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D417" s="0" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E417" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F417" s="0" t="s">
         <v>555</v>
@@ -8917,16 +8978,16 @@
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B418" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="C418" s="0" t="s">
+        <v>786</v>
+      </c>
+      <c r="D418" s="0" t="s">
         <v>784</v>
       </c>
-      <c r="C418" s="0" t="s">
-        <v>785</v>
-      </c>
-      <c r="D418" s="0" t="s">
-        <v>783</v>
-      </c>
       <c r="E418" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F418" s="0" t="s">
         <v>555</v>
@@ -8934,16 +8995,16 @@
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B419" s="0" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C419" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="D419" s="0" t="s">
         <v>559</v>
       </c>
       <c r="E419" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F419" s="0" t="s">
         <v>555</v>
@@ -8951,16 +9012,16 @@
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B420" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C420" s="0" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="D420" s="0" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="E420" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F420" s="0" t="s">
         <v>555</v>
@@ -8968,16 +9029,16 @@
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B421" s="0" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C421" s="0" t="s">
+        <v>790</v>
+      </c>
+      <c r="D421" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="D421" s="0" t="s">
-        <v>788</v>
-      </c>
       <c r="E421" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F421" s="0" t="s">
         <v>555</v>
@@ -8988,10 +9049,10 @@
         <v>712</v>
       </c>
       <c r="C423" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="E423" s="0" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F423" s="0" t="s">
         <v>750</v>
@@ -9002,10 +9063,10 @@
         <v>712</v>
       </c>
       <c r="C424" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="E424" s="0" t="s">
         <v>792</v>
-      </c>
-      <c r="E424" s="0" t="s">
-        <v>791</v>
       </c>
       <c r="F424" s="0" t="s">
         <v>750</v>
@@ -9016,10 +9077,10 @@
         <v>712</v>
       </c>
       <c r="C425" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F425" s="0" t="s">
         <v>750</v>
@@ -9030,10 +9091,10 @@
         <v>712</v>
       </c>
       <c r="C426" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F426" s="0" t="s">
         <v>750</v>
@@ -9041,13 +9102,13 @@
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C427" s="0" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F427" s="0" t="s">
         <v>750</v>
@@ -9055,13 +9116,13 @@
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C428" s="0" t="s">
+        <v>799</v>
+      </c>
+      <c r="E428" s="0" t="s">
         <v>798</v>
-      </c>
-      <c r="E428" s="0" t="s">
-        <v>797</v>
       </c>
       <c r="F428" s="0" t="s">
         <v>750</v>
@@ -9069,13 +9130,13 @@
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C429" s="0" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="E429" s="0" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F429" s="0" t="s">
         <v>750</v>
@@ -9083,13 +9144,13 @@
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C430" s="0" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="E430" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F430" s="0" t="s">
         <v>750</v>
@@ -9097,13 +9158,13 @@
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C431" s="0" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="E431" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F431" s="0" t="s">
         <v>750</v>
@@ -9111,13 +9172,13 @@
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C432" s="0" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E432" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F432" s="0" t="s">
         <v>750</v>
@@ -9125,13 +9186,13 @@
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C434" s="0" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E434" s="4" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="F434" s="4" t="s">
         <v>750</v>
@@ -9141,1700 +9202,1700 @@
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C435" s="0" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E435" s="0" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="F435" s="0" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C437" s="0" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="E437" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F437" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C438" s="0" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="E438" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F438" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C439" s="0" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="E439" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F439" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C441" s="0" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="E441" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F441" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C442" s="0" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="E442" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F442" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C443" s="0" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="E443" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F443" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C444" s="0" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="E444" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F444" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C445" s="0" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="E445" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F445" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C446" s="0" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="E446" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F446" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C447" s="0" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="E447" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F447" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C448" s="0" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="E448" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F448" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C449" s="0" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="E449" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F449" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C450" s="0" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="E450" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F450" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C451" s="0" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="E451" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F451" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C452" s="0" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="E452" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F452" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C453" s="0" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="E453" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F453" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C454" s="0" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="E454" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F454" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C455" s="0" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="E455" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F455" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C456" s="0" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="E456" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F456" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C457" s="0" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F457" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C458" s="0" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E458" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F458" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C459" s="0" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="E459" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F459" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C460" s="0" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E460" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F460" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C461" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E461" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F461" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C462" s="0" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="E462" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F462" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C463" s="0" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E463" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F463" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C464" s="0" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="E464" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F464" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C465" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E465" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F465" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C466" s="0" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="E466" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F466" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C467" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E467" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F467" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C468" s="0" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E468" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F468" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C469" s="0" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E469" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F469" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C470" s="0" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="E470" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F470" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C471" s="0" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="E471" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F471" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C472" s="0" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="E472" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F472" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C473" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="E473" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F473" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C474" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="E474" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F474" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C475" s="0" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="E475" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F475" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C476" s="0" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F476" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C477" s="0" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F477" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C478" s="0" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="E478" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F478" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C479" s="0" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="E479" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F479" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C480" s="0" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="E480" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F480" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C481" s="0" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="E481" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F481" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C482" s="0" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E482" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F482" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C483" s="0" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="E483" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F483" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C484" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="E484" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F484" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C485" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="E485" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F485" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C486" s="0" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E486" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F486" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C487" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E487" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F487" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C488" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E488" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F488" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C489" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E489" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F489" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C490" s="0" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E490" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F490" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C491" s="0" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="E491" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F491" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C492" s="0" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E492" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F492" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C493" s="0" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="E493" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F493" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C494" s="0" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E494" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F494" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C495" s="0" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="E495" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F495" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C496" s="0" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E496" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F496" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C497" s="0" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="E497" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F497" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C498" s="0" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E498" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F498" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C499" s="0" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="E499" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F499" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C500" s="0" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="E500" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F500" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C501" s="0" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="E501" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F501" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C502" s="0" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="E502" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F502" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="0" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="E503" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F503" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C504" s="0" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E504" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F504" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C505" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="E505" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F505" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C506" s="0" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="E506" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F506" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C507" s="0" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="E507" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F507" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C508" s="0" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="E508" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F508" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C509" s="0" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="E509" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F509" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C510" s="0" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="E510" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F510" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C511" s="0" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="E511" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F511" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C512" s="0" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="E512" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F512" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C513" s="0" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="E513" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F513" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="0" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="E514" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F514" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="0" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="E515" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F515" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="0" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="E516" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F516" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C517" s="0" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="E517" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F517" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C518" s="0" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E518" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F518" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C519" s="0" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F519" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C520" s="0" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="E520" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F520" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C521" s="0" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C522" s="0" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="E522" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="0" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="0" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E524" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F524" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C525" s="0" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E525" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F525" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C526" s="0" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E526" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F526" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C527" s="0" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="E527" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F527" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C528" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E528" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F528" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C529" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="E529" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F529" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C530" s="0" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E530" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F530" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C531" s="0" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="E531" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F531" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="0" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E532" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F532" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C534" s="0" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="E534" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F534" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C535" s="0" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="E535" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F535" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C536" s="0" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="E536" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F536" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="0" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="E538" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F538" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="0" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E539" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F539" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="0" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="E540" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F540" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C541" s="0" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E541" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F541" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C542" s="0" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="E542" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F542" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C543" s="0" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E543" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F543" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C544" s="0" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="E544" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F544" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C545" s="0" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="E545" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F545" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C546" s="0" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="E546" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F546" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C547" s="0" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="E547" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F547" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C548" s="0" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E548" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F548" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C549" s="0" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="E549" s="0" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="F549" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C550" s="0" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="E550" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F550" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C551" s="0" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="E551" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F551" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C552" s="0" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="E552" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F552" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C553" s="0" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="E553" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F553" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C554" s="0" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="E554" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F554" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C555" s="0" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E555" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F555" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C556" s="0" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="E556" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F556" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C557" s="0" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="E557" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F557" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C558" s="0" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="E558" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F558" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C559" s="0" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="E559" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F559" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C560" s="0" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E560" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F560" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C561" s="0" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="E561" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F561" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C562" s="0" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="E562" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F562" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C563" s="0" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="E563" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F563" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C564" s="0" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E564" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F564" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C565" s="0" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E565" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F565" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C566" s="0" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="E566" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F566" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C567" s="0" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E567" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F567" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C568" s="0" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="E568" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F568" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="569" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C569" s="0" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E569" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F569" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C570" s="0" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="E570" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F570" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C571" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E571" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F571" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="572" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C572" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="E572" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F572" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C573" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="E573" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F573" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="575" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C575" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="E575" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F575" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C576" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E576" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F576" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C577" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="E577" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F577" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="578" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C578" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="E578" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F578" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C580" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E580" s="0" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="F580" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C581" s="0" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="E581" s="0" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="F581" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C582" s="0" t="s">
+        <v>950</v>
+      </c>
+      <c r="E582" s="0" t="s">
         <v>949</v>
       </c>
-      <c r="E582" s="0" t="s">
-        <v>948</v>
-      </c>
       <c r="F582" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C583" s="0" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="E583" s="0" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="F583" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C584" s="0" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E584" s="0" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="F584" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C585" s="0" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="E585" s="0" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="F585" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="586" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C586" s="0" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E586" s="0" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="F586" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C587" s="0" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="E587" s="0" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="F587" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="588" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C588" s="0" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="E588" s="4" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="F588" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="G588" s="4"/>
       <c r="H588" s="5"/>
     </row>
     <row r="589" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C589" s="0" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="E589" s="4" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="F589" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="G589" s="4"/>
       <c r="H589" s="5"/>
     </row>
     <row r="590" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C590" s="0" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="E590" s="4" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="F590" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="G590" s="4"/>
       <c r="H590" s="5"/>
     </row>
     <row r="591" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C591" s="0" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="E591" s="4" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="F591" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="G591" s="4"/>
       <c r="H591" s="5"/>
     </row>
     <row r="592" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C592" s="0" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E592" s="0" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="F592" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="595" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10842,10 +10903,10 @@
         <v>268</v>
       </c>
       <c r="E595" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="F595" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="596" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10853,10 +10914,10 @@
         <v>270</v>
       </c>
       <c r="E596" s="0" t="s">
+        <v>972</v>
+      </c>
+      <c r="F596" s="0" t="s">
         <v>971</v>
-      </c>
-      <c r="F596" s="0" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10864,10 +10925,10 @@
         <v>266</v>
       </c>
       <c r="E597" s="0" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="F597" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="598" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10875,10 +10936,10 @@
         <v>371</v>
       </c>
       <c r="E598" s="0" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F598" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10886,37 +10947,37 @@
         <v>372</v>
       </c>
       <c r="E599" s="0" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F599" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="601" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C601" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="E601" s="4" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F601" s="4" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="G601" s="4"/>
       <c r="H601" s="4"/>
     </row>
     <row r="603" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C603" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="E603" s="4" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="F603" s="6" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="604" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10924,98 +10985,98 @@
         <v>540</v>
       </c>
       <c r="E604" s="4" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="F604" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C605" s="0" t="s">
+        <v>984</v>
+      </c>
+      <c r="E605" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="F605" s="6" t="s">
         <v>983</v>
-      </c>
-      <c r="E605" s="4" t="s">
-        <v>984</v>
-      </c>
-      <c r="F605" s="6" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C611" s="0" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="E611" s="4" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F611" s="4" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="612" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C612" s="0" t="s">
+        <v>989</v>
+      </c>
+      <c r="E612" s="7" t="s">
+        <v>990</v>
+      </c>
+      <c r="F612" s="4" t="s">
         <v>988</v>
-      </c>
-      <c r="E612" s="7" t="s">
-        <v>989</v>
-      </c>
-      <c r="F612" s="4" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C613" s="0" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="E613" s="7" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="F613" s="4" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C614" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E614" s="4" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F614" s="4" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C615" s="0" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="E615" s="4" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="F615" s="4" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C616" s="0" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="E616" s="4" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="F616" s="4" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C617" s="0" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E617" s="4" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F617" s="4" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11023,61 +11084,61 @@
     </row>
     <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="0" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C622" s="0" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="E622" s="8" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="F622" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G622" s="8"/>
       <c r="H622" s="6"/>
     </row>
     <row r="623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C623" s="9" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E623" s="8" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F623" s="6" t="s">
         <v>1004</v>
-      </c>
-      <c r="E623" s="8" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F623" s="6" t="s">
-        <v>1003</v>
       </c>
       <c r="G623" s="8"/>
       <c r="H623" s="6"/>
     </row>
     <row r="624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C624" s="9" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E624" s="8" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="F624" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G624" s="8"/>
       <c r="H624" s="6"/>
     </row>
     <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="0" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C625" s="0" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="E625" s="8" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="F625" s="4" t="s">
         <v>750</v>
@@ -11087,13 +11148,13 @@
     </row>
     <row r="626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C626" s="0" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="E626" s="8" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="F626" s="4" t="s">
         <v>750</v>
@@ -11103,96 +11164,96 @@
     </row>
     <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C627" s="0" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="E627" s="8" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="F627" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G627" s="8"/>
       <c r="H627" s="6"/>
     </row>
     <row r="628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C628" s="0" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="E628" s="8" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F628" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G628" s="8"/>
       <c r="H628" s="6"/>
     </row>
     <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C629" s="0" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="E629" s="8" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="F629" s="4" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G629" s="8"/>
       <c r="H629" s="4"/>
     </row>
     <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C630" s="0" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="E630" s="8" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="F630" s="4" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G630" s="8"/>
       <c r="H630" s="4"/>
     </row>
     <row r="631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C631" s="0" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="E631" s="10" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="F631" s="4" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G631" s="10"/>
       <c r="H631" s="4"/>
     </row>
     <row r="632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C632" s="0" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="E632" s="10" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="F632" s="4" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G632" s="10"/>
       <c r="H632" s="4"/>
@@ -11202,10 +11263,10 @@
         <v>712</v>
       </c>
       <c r="C634" s="0" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="E634" s="4" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="F634" s="4" t="s">
         <v>750</v>
@@ -11218,10 +11279,10 @@
         <v>712</v>
       </c>
       <c r="C635" s="0" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="E635" s="4" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F635" s="4" t="s">
         <v>750</v>
@@ -11234,10 +11295,10 @@
         <v>712</v>
       </c>
       <c r="C636" s="0" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E636" s="4" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="F636" s="4" t="s">
         <v>750</v>
@@ -11250,10 +11311,10 @@
         <v>712</v>
       </c>
       <c r="C637" s="0" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E637" s="4" t="s">
         <v>1031</v>
-      </c>
-      <c r="E637" s="4" t="s">
-        <v>1030</v>
       </c>
       <c r="F637" s="4" t="s">
         <v>750</v>
@@ -11263,13 +11324,13 @@
     </row>
     <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="0" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C638" s="0" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="E638" s="4" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F638" s="4" t="s">
         <v>750</v>
@@ -11279,13 +11340,13 @@
     </row>
     <row r="639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="0" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C639" s="0" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="E639" s="4" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="F639" s="4" t="s">
         <v>750</v>
@@ -11295,32 +11356,32 @@
     </row>
     <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C642" s="0" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="E642" s="4" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F642" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G642" s="4"/>
       <c r="H642" s="4"/>
     </row>
     <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C643" s="0" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="E643" s="4" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="F643" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G643" s="4"/>
       <c r="H643" s="4"/>
@@ -11328,96 +11389,96 @@
     </row>
     <row r="644" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C644" s="0" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="E644" s="4" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F644" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G644" s="4"/>
       <c r="H644" s="4"/>
     </row>
     <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C645" s="0" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="E645" s="4" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F645" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G645" s="4"/>
       <c r="H645" s="4"/>
     </row>
     <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C646" s="0" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="E646" s="4" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="F646" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G646" s="4"/>
       <c r="H646" s="4"/>
     </row>
     <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C647" s="0" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="E647" s="4" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="F647" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G647" s="4"/>
       <c r="H647" s="4"/>
     </row>
     <row r="648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C648" s="0" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="E648" s="4" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="F648" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G648" s="4"/>
       <c r="H648" s="4"/>
     </row>
     <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C649" s="0" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="E649" s="4" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="F649" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G649" s="4"/>
       <c r="H649" s="4"/>
@@ -11425,64 +11486,64 @@
     </row>
     <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C650" s="0" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="E650" s="4" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F650" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G650" s="4"/>
       <c r="H650" s="4"/>
     </row>
     <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C651" s="0" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E651" s="4" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="F651" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G651" s="4"/>
       <c r="H651" s="4"/>
     </row>
     <row r="652" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C652" s="0" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="E652" s="4" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="F652" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G652" s="4"/>
       <c r="H652" s="4"/>
     </row>
     <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C653" s="0" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="E653" s="4" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="F653" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G653" s="4"/>
       <c r="H653" s="4"/>
@@ -11490,125 +11551,125 @@
     </row>
     <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C654" s="0" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="E654" s="4" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="F654" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G654" s="4"/>
       <c r="H654" s="4"/>
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C655" s="0" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="E655" s="4" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="F655" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G655" s="4"/>
       <c r="H655" s="4"/>
     </row>
     <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C656" s="0" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="E656" s="4" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="F656" s="4" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="G656" s="4"/>
       <c r="H656" s="4"/>
     </row>
     <row r="657" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C657" s="0" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E657" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F657" s="4" t="s">
         <v>1068</v>
-      </c>
-      <c r="E657" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="F657" s="4" t="s">
-        <v>1067</v>
       </c>
       <c r="G657" s="4"/>
       <c r="H657" s="4"/>
     </row>
     <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C658" s="0" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="E658" s="4" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="F658" s="4" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="G658" s="4"/>
       <c r="H658" s="4"/>
     </row>
     <row r="659" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C659" s="0" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="E659" s="4" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="F659" s="4" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="G659" s="4"/>
       <c r="H659" s="4"/>
     </row>
     <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C660" s="0" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="E660" s="4" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="F660" s="4" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="G660" s="4"/>
       <c r="H660" s="4"/>
     </row>
     <row r="661" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="0" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C661" s="0" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="E661" s="4" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="F661" s="4" t="s">
         <v>750</v>
@@ -11618,13 +11679,13 @@
     </row>
     <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C662" s="0" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="E662" s="4" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="F662" s="4" t="s">
         <v>750</v>
@@ -11637,13 +11698,13 @@
         <v>712</v>
       </c>
       <c r="C663" s="0" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="E663" s="4" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="F663" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G663" s="4"/>
       <c r="H663" s="6"/>
@@ -11653,10 +11714,10 @@
         <v>712</v>
       </c>
       <c r="C664" s="0" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="E664" s="4" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="F664" s="4" t="s">
         <v>750</v>
@@ -11669,297 +11730,297 @@
         <v>712</v>
       </c>
       <c r="C665" s="0" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="E665" s="11" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="G665" s="11"/>
     </row>
     <row r="666" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C666" s="0" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="E666" s="4" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="F666" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G666" s="4"/>
       <c r="H666" s="6"/>
     </row>
     <row r="667" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C667" s="0" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="E667" s="4" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="F667" s="4" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G667" s="4"/>
       <c r="H667" s="4"/>
     </row>
     <row r="668" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C668" s="0" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="E668" s="4" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="F668" s="4" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G668" s="4"/>
       <c r="H668" s="4"/>
     </row>
     <row r="670" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C670" s="0" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="E670" s="4" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="F670" s="4" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="G670" s="4"/>
       <c r="H670" s="4"/>
     </row>
     <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C671" s="0" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E671" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F671" s="4" t="s">
         <v>1096</v>
-      </c>
-      <c r="E671" s="4" t="s">
-        <v>1097</v>
-      </c>
-      <c r="F671" s="4" t="s">
-        <v>1095</v>
       </c>
       <c r="G671" s="4"/>
       <c r="H671" s="4"/>
     </row>
     <row r="672" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C672" s="0" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="E672" s="4" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="F672" s="4" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G672" s="4"/>
       <c r="H672" s="4"/>
     </row>
     <row r="673" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C673" s="0" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="E673" s="4" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="F673" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G673" s="4"/>
       <c r="H673" s="4"/>
     </row>
     <row r="674" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C674" s="0" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="E674" s="4" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="F674" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G674" s="4"/>
       <c r="H674" s="4"/>
     </row>
     <row r="675" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C675" s="0" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="E675" s="4" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="F675" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G675" s="4"/>
       <c r="H675" s="4"/>
     </row>
     <row r="676" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C676" s="0" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="E676" s="4" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="F676" s="4" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="G676" s="4"/>
       <c r="H676" s="4"/>
     </row>
     <row r="677" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C677" s="0" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="E677" s="4" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="F677" s="4" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="G677" s="4"/>
       <c r="H677" s="4"/>
     </row>
     <row r="678" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="0" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C678" s="0" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="E678" s="4" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="F678" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G678" s="4"/>
       <c r="H678" s="6"/>
     </row>
     <row r="679" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="0" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C679" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E679" s="4" t="s">
         <v>1113</v>
       </c>
-      <c r="E679" s="4" t="s">
-        <v>1112</v>
-      </c>
       <c r="F679" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G679" s="4"/>
       <c r="H679" s="6"/>
     </row>
     <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C683" s="0" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="E683" s="4" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="F683" s="4" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="G683" s="4"/>
       <c r="H683" s="4"/>
     </row>
     <row r="684" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C684" s="0" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="E684" s="4" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="F684" s="4" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="G684" s="4"/>
       <c r="H684" s="4"/>
     </row>
     <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C685" s="0" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="E685" s="4" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="F685" s="4" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="G685" s="4"/>
       <c r="H685" s="4"/>
     </row>
     <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C686" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="E686" s="4" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="F686" s="4" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="G686" s="4"/>
       <c r="H686" s="4"/>
     </row>
     <row r="687" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C687" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="E687" s="4" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="F687" s="4" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="G687" s="4"/>
       <c r="H687" s="4"/>

</xml_diff>

<commit_message>
Identification step 3 VolMIP & LS3MIP variables #304: most are placed in pre ignored file, four LS3MIP variables went to pre identified missing file.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="1132">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3475,6 +3475,78 @@
   </si>
   <si>
     <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): coarse in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tsland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available: This coincides with skin temperature (code 235)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea Alessandri, Franco Catalano, Emanuel Dutra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature of the lower boundary of the atmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS3MIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy covered area percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available: Sum of [CVL (code: 27) + CVH (code: 28)] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea Alessandri, Franco Catalano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. 'Vegetation' means any plants e.g. trees, shrubs, grass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nudgincsm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nudging Increment of Water in Soil Mositure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg m-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to be saved: Have to be  made available via PEXTRA, upto now with some  non-defined or adhoc grib code. Nudincsm is, consistent with sm, saved for each of the four soil layers separately and has to be treated as sm. I am not sure, whether in the cmorization mrso is the total column of soil moisture, though. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emanuel Dutra, Wilhelm May, Thomas Reerink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 'nudging increment' refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. 'Content' indicates a quantity per unit area. 'Water' means water in all phases. The mass content of water in soil refers to the vertical integral from the surface down to the bottom of the soil model. The 'soil content' of a quantity refers to the vertical integral from the surface down to the bottom of the soil model. For the content between specified levels in the soil, standard names including 'content_of_soil_layer' are used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nudgincswe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nudging Increment of Water in Snow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to be saved: Have to be  made available via PEXTRA, upto now with some  non-defined or adhoc grib code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 'nudging increment' refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
   </si>
 </sst>
 </file>
@@ -3754,8 +3826,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A392" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A406" activeCellId="0" sqref="A406"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A661" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A678" activeCellId="0" sqref="678:682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3766,7 +3838,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="60.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.09"/>
@@ -11740,6 +11812,146 @@
       </c>
       <c r="J675" s="4"/>
       <c r="K675" s="4"/>
+    </row>
+    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A679" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B679" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C679" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D679" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E679" s="0" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F679" s="0" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G679" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H679" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="I679" s="0" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J679" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="K679" s="0" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A680" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B680" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C680" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D680" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E680" s="0" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F680" s="0" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G680" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H680" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="I680" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="J680" s="0" t="s">
+        <v>1121</v>
+      </c>
+      <c r="K680" s="0" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A681" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B681" s="0" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C681" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D681" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E681" s="0" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F681" s="0" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G681" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H681" s="0" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I681" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J681" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="K681" s="0" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A682" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B682" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C682" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D682" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E682" s="0" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F682" s="0" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G682" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H682" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="I682" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J682" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="K682" s="0" t="s">
+        <v>1115</v>
+      </c>
     </row>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
The missing variables which were still there after data request version 01.00.27 have now been identified, and are added to the ignored list and to the pre identified missing list #314.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1197">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3547,6 +3547,201 @@
   </si>
   <si>
     <t xml:space="preserve">A 'nudging increment' refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conccn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerosol Number Concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in TM5, though yet to be added by Tommi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommi Bergman, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Number concentration' means the number of particles or other specified objects per unit volume. 'Aerosol' means the system of suspended liquid or solid particles in air (except cloud droplets) and their carrier gas, the air itself. 'Ambient_aerosol' means that the aerosol is measured or modelled at the ambient state of pressure, temperature and relative humidity that exists in its immediate environment. 'Ambient aerosol particles' are aerosol particles that have taken up ambient water through hygroscopic growth. The extent of hygroscopic growth depends on the relative humidity and the composition of the particles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeoMIP,VIACSAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sconcss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Concentration of Seasalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg m-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mass concentration of seasalt dry aerosol in air in model lowest layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">talkos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Total Alkalinity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mol m-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlkaliniSFC_E3T / e3t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total alkalinity equivalent concentration (including carbonate, borate, phosphorus, silicon, and nitrogen components)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,OMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHSFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative log10 of hydrogen ion concentration with the concentration expressed as mol H kg-1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">po4os</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mole_concentration_of_dissolved_inorganic_phosphorous_in_sea_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PO4_E3T/e3t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole concentration means number of moles per unit volume, also called 'molarity', and is used in the construction 'mole_concentration_of_X_in_Y', where X is a material constituent of Y. A chemical or biological species denoted by X may be described by a single term such as 'nitrogen' or a phrase such as 'nox_expressed_as_nitrogen'. 'Dissolved inorganic phosphorus' means the sum of all inorganic phosphorus in solution (including phosphate, hydrogen phosphate, dihydrogen phosphate, and phosphoric acid).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Flux into Sea Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg m-2 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computed as the water  flux into the ocean divided by the area of the ocean portion of the grid cell.  This is the sum of the next two variables in this table.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CMIP,DAMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,OMIP,VIACSAB,VolMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zhalfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude olevel time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth Below Geoid of Interfaces Between Ocean Layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tpt_dep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth below geoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CFMIP,CMIP,DAMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,OMIP,VIACSAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intppcalc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Primary Mole Productivity of Carbon by Calcareous Phytoplankton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mol m-2 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTPCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Production of carbon' means the production of biomass expressed as the mass of carbon which it contains. Net primary production is the excess of gross primary production (rate of synthesis of biomass from inorganic precursors) by autotrophs ('producers'), for example, photosynthesis in plants or phytoplankton, over the rate at which the autotrophs themselves respire some of this biomass. 'Productivity' means production per unit area. Phytoplankton are autotrophic prokaryotic or eukaryotic algae that live near the water surface where there is sufficient light to support photosynthesis. 'Calcareous phytoplankton' are phytoplankton that produce calcite. The phrase 'expressed_as' is used in the construction A_expressed_as_B, where B is a chemical constituent of A. It means that the quantity indicated by the standard name is calculated solely with respect to the B contained in A, neglecting all other chemical constituents of A. Calcite is a mineral that is a polymorph of calcium carbonate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,OMIP,VIACSAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intpcalcite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcite Production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated calcite production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oclim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude olevel time2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raffaele Bernardello, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMIP,FAFMIP,HighResMIP,LUMIP,RFMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spco2nat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time depth0m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural Surface Aqueous Partial Pressure of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCO2sea (in uatm) in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings  are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The surface called 'surface' means the lower boundary of the atmosphere. The chemical formula for carbon dioxide is CO2. In ocean biogeochemistry models, a 'natural analogue' is used to simulate the effect on a modelled variable of imposing preindustrial atmospheric carbon dioxide concentrations, even when the model as a whole may be subjected to varying forcings. The partial pressure of a gaseous constituent of air is the pressure which it alone would exert with unchanged temperature and number of moles per unit volume. The partial pressure of a dissolved gas in sea water is the partial pressure in air with which it would be in equilibrium. The partial pressure difference between sea water and air is positive when the partial pressure of the dissolved gas in sea water is greater than the partial pressure in air.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oyr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dissicnat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural Dissolved Inorganic Carbon Concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIC_E3T/e3t in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings  are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dissolved inorganic carbon (CO3+HCO3+H2CO3) concentration at preindustrial atmospheric xCO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,CMIP,GeoMIP,LUMIP,OMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phnat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings  are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
   </si>
 </sst>
 </file>
@@ -3826,8 +4021,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A661" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A678" activeCellId="0" sqref="678:682"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A676" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A684" activeCellId="0" sqref="A684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11953,7 +12148,461 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A686" s="0" t="s">
+        <v>779</v>
+      </c>
+      <c r="B686" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C686" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D686" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="E686" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F686" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G686" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H686" s="0" t="s">
+        <v>1135</v>
+      </c>
+      <c r="I686" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="J686" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="K686" s="0" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A687" s="0" t="s">
+        <v>779</v>
+      </c>
+      <c r="B687" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C687" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D687" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E687" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F687" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G687" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H687" s="0" t="s">
+        <v>1135</v>
+      </c>
+      <c r="I687" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="J687" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="K687" s="0" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A691" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B691" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C691" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D691" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E691" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F691" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G691" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H691" s="0" t="s">
+        <v>1146</v>
+      </c>
+      <c r="I691" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J691" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="K691" s="0" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A692" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B692" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C692" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D692" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E692" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F692" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G692" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H692" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I692" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J692" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="K692" s="0" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A693" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B693" s="0" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C693" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D693" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E693" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F693" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G693" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H693" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I693" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J693" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="K693" s="0" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A694" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B694" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C694" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D694" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E694" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F694" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G694" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H694" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="I694" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J694" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="K694" s="0" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A695" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B695" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C695" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D695" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E695" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F695" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G695" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H695" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="I695" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J695" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K695" s="0" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A696" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B696" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C696" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D696" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E696" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F696" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G696" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H696" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I696" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J696" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="K696" s="0" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A697" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B697" s="0" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C697" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D697" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="E697" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F697" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G697" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H697" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I697" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J697" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="K697" s="0" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A699" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B699" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C699" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D699" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E699" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F699" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G699" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H699" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="I699" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="J699" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K699" s="0" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A702" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B702" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C702" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D702" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E702" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F702" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="G702" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H702" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="I702" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J702" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="K702" s="0" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A704" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B704" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C704" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D704" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E704" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F704" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G704" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H704" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I704" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J704" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K704" s="0" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A705" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B705" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C705" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D705" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E705" s="0" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F705" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G705" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H705" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="I705" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="J705" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="K705" s="0" t="s">
+        <v>1193</v>
+      </c>
+    </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Moving the variables: expn,expp,pso,intdoc,frn from pre ignored to pre identified missing file #314.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="1208">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3743,6 +3743,39 @@
   <si>
     <t xml:space="preserve">PH in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings  are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
   </si>
+  <si>
+    <t xml:space="preserve">expn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in PISCES: EXPC * (1/122). Not available inLPJ-GUESS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in PISCES: EXPC * (16/122). Not available inLPJ-GUESS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">botpres (dbar)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intdoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC_E3T * 12/1.e6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torben, Raffaele Bernardello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sdenit</t>
+  </si>
 </sst>
 </file>
 
@@ -3751,7 +3784,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3844,6 +3877,19 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFED1C24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3893,7 +3939,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3940,6 +3986,18 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4005,7 +4063,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -4021,8 +4079,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A676" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A684" activeCellId="0" sqref="A684"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A694" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A708" activeCellId="0" sqref="A708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12603,6 +12661,68 @@
         <v>1193</v>
       </c>
     </row>
+    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B708" s="12" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H708" s="13" t="s">
+        <v>1198</v>
+      </c>
+      <c r="I708" s="0" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B709" s="12" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H709" s="13" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I709" s="0" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B710" s="12" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H710" s="14" t="s">
+        <v>1202</v>
+      </c>
+      <c r="I710" s="0" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A711" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B711" s="0" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H711" s="14" t="s">
+        <v>1204</v>
+      </c>
+      <c r="I711" s="0" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A712" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="B712" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H712" s="14" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I712" s="0" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update for Shaconemo update from revision 270 to 274: these versions are in fact equivalent for ece2cmor3 #290.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">agessc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: Age_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: Age_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Reerink</t>
@@ -67,49 +67,49 @@
     <t xml:space="preserve">areacello</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: areacello</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: areacello</t>
   </si>
   <si>
     <t xml:space="preserve">basin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: basins</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: basins</t>
   </si>
   <si>
     <t xml:space="preserve">bigthetao</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: toce</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: toce</t>
   </si>
   <si>
     <t xml:space="preserve">bigthetaoga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sctemtot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sctemtot</t>
   </si>
   <si>
     <t xml:space="preserve">cfc11</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: CFC11_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: CFC11_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">cfc12</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: CFC12_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: CFC12_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">deptho</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: tpt_dep</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: tpt_dep</t>
   </si>
   <si>
     <t xml:space="preserve">diftrblo2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: aht2d_eiv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: aht2d_eiv</t>
   </si>
   <si>
     <t xml:space="preserve">diftrelo2d</t>
@@ -118,31 +118,31 @@
     <t xml:space="preserve">diftrxylo2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: aht2d</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: aht2d</t>
   </si>
   <si>
     <t xml:space="preserve">difvho</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: avt_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: avt_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvmo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: avm_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: avm_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvmto</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: av_wave_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: av_wave_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvso</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: avs_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: avs_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvtrto</t>
@@ -151,145 +151,145 @@
     <t xml:space="preserve">dispkevfo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: dispkevfo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: dispkevfo</t>
   </si>
   <si>
     <t xml:space="preserve">dispkexyfo2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: dispkexyfo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: dispkexyfo</t>
   </si>
   <si>
     <t xml:space="preserve">evs</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: evap_ao_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: evap_ao_cea</t>
   </si>
   <si>
     <t xml:space="preserve">fgcfc11</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: qtr_CFC11</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: qtr_CFC11</t>
   </si>
   <si>
     <t xml:space="preserve">fgcfc12</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: qtr_CFC12</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: qtr_CFC12</t>
   </si>
   <si>
     <t xml:space="preserve">fgsf6</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: qtr_SF6</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: qtr_SF6</t>
   </si>
   <si>
     <t xml:space="preserve">ficeberg2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: iceberg_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: iceberg_cea</t>
   </si>
   <si>
     <t xml:space="preserve">flandice</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: iceshelf_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: iceshelf_cea</t>
   </si>
   <si>
     <t xml:space="preserve">friver</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: runoffs</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: runoffs</t>
   </si>
   <si>
     <t xml:space="preserve">fsitherm</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: fmmflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: fmmflx</t>
   </si>
   <si>
     <t xml:space="preserve">hcont300</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: hc300</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: hc300</t>
   </si>
   <si>
     <t xml:space="preserve">hfbasin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sopht_vt_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sopht_vt_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">hfbasinpmadv</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sophteiv_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sophteiv_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">hfcorr</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: qrp</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: qrp</t>
   </si>
   <si>
     <t xml:space="preserve">hfds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: qt</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: qt</t>
   </si>
   <si>
     <t xml:space="preserve">hfevapds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: hflx_evap_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: hflx_evap_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfgeou</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: hfgeou</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: hfgeou</t>
   </si>
   <si>
     <t xml:space="preserve">hfibthermds2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: hflx_icb_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: hflx_icb_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfrainds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: hflx_rain_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: hflx_rain_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfrunoffds2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: hflx_rnf_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: hflx_rnf_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfsnthermds2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: hflx_snow_ao_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: hflx_snow_ao_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: uadv_heattr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: uadv_heattr</t>
   </si>
   <si>
     <t xml:space="preserve">hfy</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: vadv_heattr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: vadv_heattr</t>
   </si>
   <si>
     <t xml:space="preserve">htovgyre</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sophtove_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sophtove_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">htovovrt</t>
@@ -298,37 +298,37 @@
     <t xml:space="preserve">masscello</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: masscello</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: masscello</t>
   </si>
   <si>
     <t xml:space="preserve">masso</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: scmastot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: scmastot</t>
   </si>
   <si>
     <t xml:space="preserve">mfo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: transport_masse_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: transport_masse_transect</t>
   </si>
   <si>
     <t xml:space="preserve">mlotst</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: mldr10_3</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: mldr10_3</t>
   </si>
   <si>
     <t xml:space="preserve">mlotstmax</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: mldr10_3max</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: mldr10_3max</t>
   </si>
   <si>
     <t xml:space="preserve">mlotstmin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: mldr10_3min</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: mldr10_3min</t>
   </si>
   <si>
     <t xml:space="preserve">mlotstsq</t>
@@ -337,139 +337,139 @@
     <t xml:space="preserve">msftbarot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: uoce_e3u_vsum_e2u_cumul</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: uoce_e3u_vsum_e2u_cumul</t>
   </si>
   <si>
     <t xml:space="preserve">msftyz</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: zomsf_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: zomsf_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">obvfsq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: bn2_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: bn2_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontempdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: ttrd_zdfp_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: ttrd_zdfp_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemppadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: ttrd_eivad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: ttrd_eivad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemppmdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: ttrd_iso_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: ttrd_iso_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemprmadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: ttrd_totad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: ttrd_totad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemptend</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: ttrd_tot_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: ttrd_tot_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">omldamax</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: mldkz5</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: mldkz5</t>
   </si>
   <si>
     <t xml:space="preserve">osaltdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: strd_zdfp_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: strd_zdfp_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osaltpadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: strd_eivad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: strd_eivad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osaltpmdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: strd_iso_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: strd_iso_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osaltrmadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: strd_totad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: strd_totad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osalttend</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: strd_tot_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: strd_tot_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">pbo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: botpres</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: botpres</t>
   </si>
   <si>
     <t xml:space="preserve">rsdo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: qsr3d_e3t_SBC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: qsr3d_e3t_SBC</t>
   </si>
   <si>
     <t xml:space="preserve">rsntds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: qsr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: qsr</t>
   </si>
   <si>
     <t xml:space="preserve">sf6</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: SF6_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: SF6_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">sfdsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: saltflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: saltflx</t>
   </si>
   <si>
     <t xml:space="preserve">sftof</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: iceconc_pct</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: iceconc_pct</t>
   </si>
   <si>
     <t xml:space="preserve">sltbasin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sopst_vs_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sopst_vs_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">sltnortha</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sopst_atl</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sopst_atl</t>
   </si>
   <si>
     <t xml:space="preserve">sltovgyre</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sopstove_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sopstove_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">sltovovrt</t>
@@ -478,181 +478,181 @@
     <t xml:space="preserve">so</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: soce_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: soce_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">sob</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sbs_e3tb</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sbs_e3tb</t>
   </si>
   <si>
     <t xml:space="preserve">soga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: scsaltot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: scsaltot</t>
   </si>
   <si>
     <t xml:space="preserve">somint</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: somint</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: somint</t>
   </si>
   <si>
     <t xml:space="preserve">sos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sss</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sss</t>
   </si>
   <si>
     <t xml:space="preserve">sosga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: scssstot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: scssstot</t>
   </si>
   <si>
     <t xml:space="preserve">sossq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sss2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sss2</t>
   </si>
   <si>
     <t xml:space="preserve">t20d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: 20d</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: 20d</t>
   </si>
   <si>
     <t xml:space="preserve">tauuo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: utau</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: utau</t>
   </si>
   <si>
     <t xml:space="preserve">tauvo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: vtau</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: vtau</t>
   </si>
   <si>
     <t xml:space="preserve">thetao</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: toce_pot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: toce_pot</t>
   </si>
   <si>
     <t xml:space="preserve">thetaoga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sctemtotpot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sctemtotpot</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: toce_pot_vmean</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: toce_pot_vmean</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot2000</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: toce_pot_vmean2000</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: toce_pot_vmean2000</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot300</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: toce_pot_vmean300</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: toce_pot_vmean300</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot700</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: toce_pot_vmean700</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: toce_pot_vmean700</t>
   </si>
   <si>
     <t xml:space="preserve">thkcello</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: e3t</t>
   </si>
   <si>
     <t xml:space="preserve">tnkebto2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: eketrd_eiv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: eketrd_eiv</t>
   </si>
   <si>
     <t xml:space="preserve">tnpeo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: tnpeo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: tnpeo</t>
   </si>
   <si>
     <t xml:space="preserve">tob</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: toce_potb_e3tb</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: toce_potb_e3tb</t>
   </si>
   <si>
     <t xml:space="preserve">tos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sst_pot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sst_pot</t>
   </si>
   <si>
     <t xml:space="preserve">tosga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: scssttot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: scssttot</t>
   </si>
   <si>
     <t xml:space="preserve">tossq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sst_pot2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sst_pot2</t>
   </si>
   <si>
     <t xml:space="preserve">umo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: uocetr_eff</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: uocetr_eff</t>
   </si>
   <si>
     <t xml:space="preserve">uo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: uoce_e3u</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: uoce_e3u</t>
   </si>
   <si>
     <t xml:space="preserve">vmo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: vocetr_eff</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: vocetr_eff</t>
   </si>
   <si>
     <t xml:space="preserve">vo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: voce_e3v</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: voce_e3v</t>
   </si>
   <si>
     <t xml:space="preserve">volo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: scvoltot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: scvoltot</t>
   </si>
   <si>
     <t xml:space="preserve">wfcorr</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: erp</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: erp</t>
   </si>
   <si>
     <t xml:space="preserve">wfo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: empmr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: empmr</t>
   </si>
   <si>
     <t xml:space="preserve">wfonocorr</t>
@@ -661,85 +661,85 @@
     <t xml:space="preserve">wmo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: wocetr_eff</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: wocetr_eff</t>
   </si>
   <si>
     <t xml:space="preserve">wo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: woce</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: woce</t>
   </si>
   <si>
     <t xml:space="preserve">zos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sshdyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sshdyn</t>
   </si>
   <si>
     <t xml:space="preserve">zossq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: sshdyn2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: sshdyn2</t>
   </si>
   <si>
     <t xml:space="preserve">zostoga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocean ping file: scsshtst</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocean ping file: scsshtst</t>
   </si>
   <si>
     <t xml:space="preserve">bfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: BFe_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: BFe_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: BFeSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: BFeSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: GSi_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: GSi_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bsios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: GSiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: GSiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">calc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: CaCO3_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: CaCO3_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">calcos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: CaCO3SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: CaCO3SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chl</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NCHL_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NCHL_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chldiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DCHL_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DCHL_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chldiatos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DCHLSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DCHLSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chlmisc</t>
@@ -748,7 +748,7 @@
     <t xml:space="preserve">chlmiscos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NCHLSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NCHLSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chlos</t>
@@ -757,409 +757,409 @@
     <t xml:space="preserve">co3</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: CO3</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: CO3</t>
   </si>
   <si>
     <t xml:space="preserve">co3os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: CO3SFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: CO3SFC</t>
   </si>
   <si>
     <t xml:space="preserve">co3satcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: CO3sat</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: CO3sat</t>
   </si>
   <si>
     <t xml:space="preserve">co3satcalcos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: CO3satSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: CO3satSFC</t>
   </si>
   <si>
     <t xml:space="preserve">dcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DCAL</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DCAL</t>
   </si>
   <si>
     <t xml:space="preserve">detoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: POC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: POC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">detocos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: POCSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: POCSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: Fer_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Fer_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: FerSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: FerSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DIC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DIC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissicos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DICSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DICSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DOC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DOC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissocos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DOCSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DOCSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dpco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: Dpco2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Dpco2</t>
   </si>
   <si>
     <t xml:space="preserve">dpo2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: Dpo2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Dpo2</t>
   </si>
   <si>
     <t xml:space="preserve">epc100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EPC100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EPC100</t>
   </si>
   <si>
     <t xml:space="preserve">epcalc100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EPCAL100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EPCAL100</t>
   </si>
   <si>
     <t xml:space="preserve">epfe100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EPFE100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EPFE100</t>
   </si>
   <si>
     <t xml:space="preserve">epsi100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EPSI100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EPSI100</t>
   </si>
   <si>
     <t xml:space="preserve">expc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EXPC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EXPC</t>
   </si>
   <si>
     <t xml:space="preserve">expcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EXPCAL</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EXPCAL</t>
   </si>
   <si>
     <t xml:space="preserve">expfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EXPFE</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EXPFE</t>
   </si>
   <si>
     <t xml:space="preserve">expsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: EXPSI</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: EXPSI</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtalk</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTdtAlk</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTdtAlk</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTdtDIC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTdtDIC</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdife</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTdtFer</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTdtFer</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTdtDIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTdtDIN</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdip</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTdtDIP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTdtDIP</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdisi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTdtSil</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTdtSil</t>
   </si>
   <si>
     <t xml:space="preserve">fgco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: Cflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Cflx</t>
   </si>
   <si>
     <t xml:space="preserve">fgo2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: Oflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Oflx</t>
   </si>
   <si>
     <t xml:space="preserve">fric</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: SedCal</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: SedCal</t>
   </si>
   <si>
     <t xml:space="preserve">froc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: SedC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: SedC</t>
   </si>
   <si>
     <t xml:space="preserve">fsfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: IronSupply</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: IronSupply</t>
   </si>
   <si>
     <t xml:space="preserve">fsn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NitrSupply</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NitrSupply</t>
   </si>
   <si>
     <t xml:space="preserve">graz</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: GRAZ1</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: GRAZ1</t>
   </si>
   <si>
     <t xml:space="preserve">intdic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTDIC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTDIC</t>
   </si>
   <si>
     <t xml:space="preserve">intpbfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTPBFE</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPBFE</t>
   </si>
   <si>
     <t xml:space="preserve">intpbsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTPBSI</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPBSI</t>
   </si>
   <si>
     <t xml:space="preserve">intpn2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTNFIX</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTNFIX</t>
   </si>
   <si>
     <t xml:space="preserve">intpp</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTPP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPP</t>
   </si>
   <si>
     <t xml:space="preserve">intppdiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTPPPHY2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPPPHY2</t>
   </si>
   <si>
     <t xml:space="preserve">intppmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTPPPHY</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">intppnitrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: INTPNEW</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: INTPNEW</t>
   </si>
   <si>
     <t xml:space="preserve">limfediat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: LDFeSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: LDFeSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limfemisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: LNFeSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: LNFeSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limirrdiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: LDlightSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: LDlightSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limirrmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: LNlightSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: LNlightSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limndiaz</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: LDnutSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: LDnutSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limnmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: &lt;LNnutSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: &lt;LNnutSFC</t>
   </si>
   <si>
     <t xml:space="preserve">nh4</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NH4_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NH4_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">nh4os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NH4SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NH4SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">no3</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NO3_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NO3_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">no3os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NO3SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NO3SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">o2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: O2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: O2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">o2min</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: O2MIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: O2MIN</t>
   </si>
   <si>
     <t xml:space="preserve">o2os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: O2SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: O2SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pbfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PFeN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PFeN</t>
   </si>
   <si>
     <t xml:space="preserve">pbsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PBSi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PBSi</t>
   </si>
   <si>
     <t xml:space="preserve">pcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PCAL</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PCAL</t>
   </si>
   <si>
     <t xml:space="preserve">ph</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PH</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PH</t>
   </si>
   <si>
     <t xml:space="preserve">phos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PHSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PHSFC</t>
   </si>
   <si>
     <t xml:space="preserve">phyc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PHY_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PHY_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phycos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PHYSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PHYSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phydiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PHY2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PHY2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phydiatos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PHY2SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PHY2SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phyfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NFe_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NFe_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phyfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: NFeSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: NFeSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phymisc</t>
@@ -1171,121 +1171,121 @@
     <t xml:space="preserve">physi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DSi_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DSi_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">physios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: DSiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DSiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pnitrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: TPNEW</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: TPNEW</t>
   </si>
   <si>
     <t xml:space="preserve">po4</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PO4_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PO4_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">po4os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PO4SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PO4SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pp</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: TPP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: TPP</t>
   </si>
   <si>
     <t xml:space="preserve">ppdiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PPPHY2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PPPHY2</t>
   </si>
   <si>
     <t xml:space="preserve">ppmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: PPPHY</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: PPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">ppos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: TPPSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: TPPSFC</t>
   </si>
   <si>
     <t xml:space="preserve">remoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: REMIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: REMIN</t>
   </si>
   <si>
     <t xml:space="preserve">si</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: Si_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Si_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">sios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: SiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: SiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">spco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: pCO2sea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: pCO2sea</t>
   </si>
   <si>
     <t xml:space="preserve">talk</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: Alkalini_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Alkalini_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">talkos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: AlkaliniSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: AlkaliniSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmeso</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: ZOO2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: ZOO2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmesoos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: ZOO2SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: ZOO2SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmicro</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: ZOO_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: ZOO_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmicroos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: ZOOSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: ZOOSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zo2min</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) ocnBgchem ping file: ZO2MIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: ZO2MIN</t>
   </si>
   <si>
     <t xml:space="preserve">zooc</t>
@@ -1297,409 +1297,409 @@
     <t xml:space="preserve">siage</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: iceage</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: iceage</t>
   </si>
   <si>
     <t xml:space="preserve">siareaacrossline</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: transport_siarea_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: transport_siarea_transect</t>
   </si>
   <si>
     <t xml:space="preserve">siarean</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: NH_sc_icearea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: NH_sc_icearea</t>
   </si>
   <si>
     <t xml:space="preserve">siareas</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: SH_sc_icearea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: SH_sc_icearea</t>
   </si>
   <si>
     <t xml:space="preserve">sicompstren</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icestr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icestr</t>
   </si>
   <si>
     <t xml:space="preserve">siconc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: iceconc_pct</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: iceconc_pct</t>
   </si>
   <si>
     <t xml:space="preserve">sidconcdyn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: afxdyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: afxdyn</t>
   </si>
   <si>
     <t xml:space="preserve">sidconcth</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: afxthd</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: afxthd</t>
   </si>
   <si>
     <t xml:space="preserve">sidivvel</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: idive</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: idive</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassdyn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmidyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmidyn</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassevapsubl</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmisub</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmisub</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassgrowthbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmibog</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmibog</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassgrowthwat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmiopw</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmiopw</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassmeltbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmibom</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmibom</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassmelttop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmisum</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmisum</t>
   </si>
   <si>
     <t xml:space="preserve">sidmasssi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmisni</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmisni</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassth</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmithd</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmithd</t>
   </si>
   <si>
     <t xml:space="preserve">sidmasstranx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: xmtrptot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: xmtrptot</t>
   </si>
   <si>
     <t xml:space="preserve">sidmasstrany</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: ymtrptot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: ymtrptot</t>
   </si>
   <si>
     <t xml:space="preserve">siextentn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: NH_sc_iceextt</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: NH_sc_iceextt</t>
   </si>
   <si>
     <t xml:space="preserve">siextents</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: SH_sc_iceextt</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: SH_sc_iceextt</t>
   </si>
   <si>
     <t xml:space="preserve">sifb</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icefb</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icefb</t>
   </si>
   <si>
     <t xml:space="preserve">siflcondbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: hfxconbo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: hfxconbo</t>
   </si>
   <si>
     <t xml:space="preserve">siflcondtop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: hfxconsu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: hfxconsu</t>
   </si>
   <si>
     <t xml:space="preserve">siflfwbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: wfxtot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: wfxtot</t>
   </si>
   <si>
     <t xml:space="preserve">siflfwdrain</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: wfxsum</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: wfxsum</t>
   </si>
   <si>
     <t xml:space="preserve">siflsensupbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: hfxsenso</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: hfxsenso</t>
   </si>
   <si>
     <t xml:space="preserve">siforcecoriolx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: corstrx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: corstrx</t>
   </si>
   <si>
     <t xml:space="preserve">siforcecorioly</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: corstry</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: corstry</t>
   </si>
   <si>
     <t xml:space="preserve">siforceintstrx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: intstrx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: intstrx</t>
   </si>
   <si>
     <t xml:space="preserve">siforceintstry</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: intstry</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: intstry</t>
   </si>
   <si>
     <t xml:space="preserve">siforcetiltx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dssh_dx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dssh_dx</t>
   </si>
   <si>
     <t xml:space="preserve">siforcetilty</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dssh_dy</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dssh_dy</t>
   </si>
   <si>
     <t xml:space="preserve">sihc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icehcneg</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icehcneg</t>
   </si>
   <si>
     <t xml:space="preserve">siitdconc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: iceconc_cat_pct_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: iceconc_cat_pct_mv</t>
   </si>
   <si>
     <t xml:space="preserve">siitdsnthick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: snowthic_cat_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: snowthic_cat_mv</t>
   </si>
   <si>
     <t xml:space="preserve">siitdthick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icethic_cat_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icethic_cat_mv</t>
   </si>
   <si>
     <t xml:space="preserve">simass</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icemass</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icemass</t>
   </si>
   <si>
     <t xml:space="preserve">simassacrossline</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: transport_simasse_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: transport_simasse_transect</t>
   </si>
   <si>
     <t xml:space="preserve">sisali</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icesal</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icesal</t>
   </si>
   <si>
     <t xml:space="preserve">sisaltmass</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icesmass</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icesmass</t>
   </si>
   <si>
     <t xml:space="preserve">sishevel</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: ishear</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: ishear</t>
   </si>
   <si>
     <t xml:space="preserve">sisnhc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: isnhcneg</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: isnhcneg</t>
   </si>
   <si>
     <t xml:space="preserve">sisnmass</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: snomass</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: snomass</t>
   </si>
   <si>
     <t xml:space="preserve">sisnthick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: snothic</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: snothic</t>
   </si>
   <si>
     <t xml:space="preserve">sispeed</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icevel_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icevel_mv</t>
   </si>
   <si>
     <t xml:space="preserve">sistremax</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: sheastr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: sheastr</t>
   </si>
   <si>
     <t xml:space="preserve">sistresave</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: normstr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: normstr</t>
   </si>
   <si>
     <t xml:space="preserve">sistrxdtop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: utau_ice</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: utau_ice</t>
   </si>
   <si>
     <t xml:space="preserve">sistrxubot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: utau_oi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: utau_oi</t>
   </si>
   <si>
     <t xml:space="preserve">sistrydtop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: vtau_ice</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: vtau_ice</t>
   </si>
   <si>
     <t xml:space="preserve">sistryubot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: vtau_oi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: vtau_oi</t>
   </si>
   <si>
     <t xml:space="preserve">sitempbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icebotK</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icebotK</t>
   </si>
   <si>
     <t xml:space="preserve">sitempsnic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icesntK</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icesntK</t>
   </si>
   <si>
     <t xml:space="preserve">sitemptop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icestK</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icestK</t>
   </si>
   <si>
     <t xml:space="preserve">sithick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icethic</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icethic</t>
   </si>
   <si>
     <t xml:space="preserve">sitimefrac</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icepres</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icepres</t>
   </si>
   <si>
     <t xml:space="preserve">siu</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: uice_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: uice_mv</t>
   </si>
   <si>
     <t xml:space="preserve">siv</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: vice_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: vice_mv</t>
   </si>
   <si>
     <t xml:space="preserve">sivol</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: icevolu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: icevolu</t>
   </si>
   <si>
     <t xml:space="preserve">sivoln</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: NH_sc_icevolu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: NH_sc_icevolu</t>
   </si>
   <si>
     <t xml:space="preserve">sivols</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: SH_sc_icevolu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: SH_sc_icevolu</t>
   </si>
   <si>
     <t xml:space="preserve">sndmassdyn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmsdyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmsdyn</t>
   </si>
   <si>
     <t xml:space="preserve">sndmassmelt</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmsmel</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmsmel</t>
   </si>
   <si>
     <t xml:space="preserve">sndmasssi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmsssi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmsssi</t>
   </si>
   <si>
     <t xml:space="preserve">sndmasssnf</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmsspr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmsspr</t>
   </si>
   <si>
     <t xml:space="preserve">sndmasssubl</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: dmssub</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: dmssub</t>
   </si>
   <si>
     <t xml:space="preserve">snmassacrossline</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r270) seaIce ping file: transport_snmasse_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) seaIce ping file: transport_snmasse_transect</t>
   </si>
   <si>
     <t xml:space="preserve">dissicnatos</t>
@@ -4139,8 +4139,8 @@
   </sheetPr>
   <dimension ref="A1:L727"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A254" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H256" activeCellId="0" sqref="H3:H282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update due to data request chages: et --> det and ec --> dec #326 #330.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -2983,13 +2983,13 @@
     <t xml:space="preserve">Available in LPJ-GUESS, but the field will be the same precipitation over crops as for the rest of the gridcell. Available in LPJ-GUESS, but the field will be the same precipitation over crops as for the rest of the gridcell.</t>
   </si>
   <si>
-    <t xml:space="preserve">et</t>
+    <t xml:space="preserve">det</t>
   </si>
   <si>
     <t xml:space="preserve">Available in LPJ-GUESS. Is now implemented as a monthly output from LPJ-GUESS.</t>
   </si>
   <si>
-    <t xml:space="preserve">ec</t>
+    <t xml:space="preserve">dec</t>
   </si>
   <si>
     <t xml:space="preserve">Available in LPJ-GUESS.  Already exist as - evspsblveg - Total Evaporation of intercepted water from Canopy [kg m-2 s-1]</t>
@@ -4139,8 +4139,8 @@
   </sheetPr>
   <dimension ref="A1:L727"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H256" activeCellId="0" sqref="H3:H282"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A568" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D595" activeCellId="0" sqref="D595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add again fco2antt and fco2nat: available in LPJ-GUESS #188. They accidentally dropped out with the recompilation of lpjgpar.json for the new approach in #330.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="1233">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2999,6 +2999,21 @@
   </si>
   <si>
     <t xml:space="preserve">Available in LPJ-GUESS.  Is now implemented as a monthly output from LPJ-GUESS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2antt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, will be cmorized by Peter Anthoni &amp; Lars Nieradzik.  Previous: Not available in the AOGCM, neither in TM5. TM5 can only provide total fluxes. Maybe sum the land use in LPJ-GUESS + fossil fuel from CEDS? This means it then has to be added in an additional post processing step.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind, Tommi Bergman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2nat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in LPJ-GUESS, will be cmorized by Peter Anthoni &amp; Lars Nieradzik.  Previous: Not available in the AOGCM, neither in TM5. TM5 can only provide total fluxes. It is not clear to us if this variable includes the contribution from land use. This variable can be calculated from the total CO2 flux provided by TM5 and the contributions from CEDS and land use from LPJ-GUESS. This "Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources" could be provided by LPJ-GUESS but its definition is very vague... Should we include emissions from managed forests? Cropland? Pasture? Any managed land? If a land has a history of being managed, but now is "natural"?</t>
   </si>
   <si>
     <t xml:space="preserve">Not available in LPJ-GUESS.  Available in PISCES: expfe</t>
@@ -4137,10 +4152,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L727"/>
+  <dimension ref="A1:L729"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A708" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H723" activeCellId="0" sqref="H723"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A572" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I597" activeCellId="0" sqref="I597:I598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11136,131 +11151,131 @@
         <v>818</v>
       </c>
     </row>
+    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B597" s="0" t="s">
+        <v>977</v>
+      </c>
+      <c r="H597" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="I597" s="0" t="s">
+        <v>979</v>
+      </c>
+    </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B598" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="H598" s="2" t="s">
-        <v>977</v>
+        <v>980</v>
+      </c>
+      <c r="H598" s="0" t="s">
+        <v>981</v>
       </c>
       <c r="I598" s="0" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B599" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="H599" s="0" t="s">
         <v>979</v>
-      </c>
-      <c r="I599" s="0" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B600" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="H600" s="0" t="s">
-        <v>980</v>
+        <v>286</v>
+      </c>
+      <c r="H600" s="2" t="s">
+        <v>982</v>
       </c>
       <c r="I600" s="0" t="s">
-        <v>978</v>
+        <v>983</v>
       </c>
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B601" s="0" t="s">
-        <v>394</v>
+        <v>288</v>
       </c>
       <c r="H601" s="0" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
       <c r="I601" s="0" t="s">
-        <v>978</v>
+        <v>983</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B602" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="H602" s="0" t="s">
+        <v>985</v>
+      </c>
+      <c r="I602" s="0" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B603" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="H603" s="0" t="s">
+        <v>986</v>
+      </c>
+      <c r="I603" s="0" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B604" s="0" t="s">
         <v>396</v>
       </c>
-      <c r="H602" s="0" t="s">
-        <v>981</v>
-      </c>
-      <c r="I602" s="0" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="604" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A604" s="2" t="s">
-        <v>982</v>
-      </c>
-      <c r="B604" s="2" t="s">
+      <c r="H604" s="0" t="s">
+        <v>986</v>
+      </c>
+      <c r="I604" s="0" t="s">
         <v>983</v>
       </c>
-      <c r="H604" s="4" t="s">
-        <v>984</v>
-      </c>
-      <c r="I604" s="4" t="s">
-        <v>985</v>
-      </c>
-      <c r="J604" s="4"/>
-      <c r="K604" s="4"/>
-    </row>
-    <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="606" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A606" s="2" t="s">
+        <v>987</v>
+      </c>
       <c r="B606" s="2" t="s">
-        <v>986</v>
-      </c>
-      <c r="C606" s="2"/>
-      <c r="D606" s="2"/>
+        <v>988</v>
+      </c>
       <c r="H606" s="4" t="s">
-        <v>987</v>
-      </c>
-      <c r="I606" s="6" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B607" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="H607" s="4" t="s">
         <v>989</v>
       </c>
-      <c r="I607" s="6" t="s">
+      <c r="I606" s="4" t="s">
         <v>990</v>
       </c>
+      <c r="J606" s="4"/>
+      <c r="K606" s="4"/>
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B608" s="0" t="s">
+      <c r="B608" s="2" t="s">
         <v>991</v>
       </c>
+      <c r="C608" s="2"/>
+      <c r="D608" s="2"/>
       <c r="H608" s="4" t="s">
         <v>992</v>
       </c>
       <c r="I608" s="6" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B614" s="0" t="s">
         <v>993</v>
       </c>
-      <c r="H614" s="4" t="s">
+    </row>
+    <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B609" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="H609" s="4" t="s">
         <v>994</v>
       </c>
-      <c r="I614" s="4" t="s">
+      <c r="I609" s="6" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B615" s="0" t="s">
+    <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B610" s="0" t="s">
         <v>996</v>
       </c>
-      <c r="H615" s="7" t="s">
+      <c r="H610" s="4" t="s">
         <v>997</v>
       </c>
-      <c r="I615" s="4" t="s">
+      <c r="I610" s="6" t="s">
         <v>995</v>
       </c>
     </row>
@@ -11268,222 +11283,212 @@
       <c r="B616" s="0" t="s">
         <v>998</v>
       </c>
-      <c r="H616" s="7" t="s">
+      <c r="H616" s="4" t="s">
         <v>999</v>
       </c>
       <c r="I616" s="4" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B617" s="0" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H617" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I617" s="4" t="s">
         <v>1000</v>
-      </c>
-      <c r="H617" s="4" t="s">
-        <v>1001</v>
-      </c>
-      <c r="I617" s="4" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B618" s="0" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H618" s="4" t="s">
         <v>1003</v>
       </c>
+      <c r="H618" s="7" t="s">
+        <v>1004</v>
+      </c>
       <c r="I618" s="4" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B619" s="0" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="H619" s="4" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I619" s="4" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B620" s="0" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="H620" s="4" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="I620" s="4" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H624" s="8"/>
-    </row>
-    <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A625" s="0" t="s">
-        <v>1008</v>
-      </c>
-      <c r="B625" s="0" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B621" s="0" t="s">
         <v>1009</v>
       </c>
-      <c r="H625" s="8" t="s">
+      <c r="H621" s="4" t="s">
         <v>1010</v>
       </c>
-      <c r="I625" s="6" t="s">
+      <c r="I621" s="4" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B622" s="0" t="s">
         <v>1011</v>
       </c>
-      <c r="J625" s="8"/>
-      <c r="K625" s="6"/>
-    </row>
-    <row r="626" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A626" s="0" t="s">
-        <v>968</v>
-      </c>
-      <c r="B626" s="9" t="s">
+      <c r="H622" s="4" t="s">
         <v>1012</v>
       </c>
-      <c r="C626" s="9"/>
-      <c r="D626" s="9"/>
-      <c r="H626" s="8" t="s">
+      <c r="I622" s="4" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H626" s="8"/>
+    </row>
+    <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A627" s="0" t="s">
         <v>1013</v>
       </c>
-      <c r="I626" s="6" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J626" s="8"/>
-      <c r="K626" s="6"/>
-    </row>
-    <row r="627" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A627" s="0" t="s">
-        <v>968</v>
-      </c>
-      <c r="B627" s="9" t="s">
+      <c r="B627" s="0" t="s">
         <v>1014</v>
       </c>
-      <c r="C627" s="9"/>
-      <c r="D627" s="9"/>
       <c r="H627" s="8" t="s">
         <v>1015</v>
       </c>
       <c r="I627" s="6" t="s">
-        <v>1011</v>
+        <v>1016</v>
       </c>
       <c r="J627" s="8"/>
       <c r="K627" s="6"/>
     </row>
-    <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="628" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="0" t="s">
-        <v>1016</v>
-      </c>
-      <c r="B628" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B628" s="9" t="s">
         <v>1017</v>
       </c>
+      <c r="C628" s="9"/>
+      <c r="D628" s="9"/>
       <c r="H628" s="8" t="s">
         <v>1018</v>
       </c>
-      <c r="I628" s="4" t="s">
-        <v>771</v>
+      <c r="I628" s="6" t="s">
+        <v>1016</v>
       </c>
       <c r="J628" s="8"/>
-      <c r="K628" s="4"/>
-    </row>
-    <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K628" s="6"/>
+    </row>
+    <row r="629" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="0" t="s">
-        <v>803</v>
-      </c>
-      <c r="B629" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B629" s="9" t="s">
         <v>1019</v>
       </c>
+      <c r="C629" s="9"/>
+      <c r="D629" s="9"/>
       <c r="H629" s="8" t="s">
         <v>1020</v>
       </c>
-      <c r="I629" s="4" t="s">
-        <v>771</v>
+      <c r="I629" s="6" t="s">
+        <v>1016</v>
       </c>
       <c r="J629" s="8"/>
-      <c r="K629" s="4"/>
+      <c r="K629" s="6"/>
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="0" t="s">
-        <v>803</v>
+        <v>1021</v>
       </c>
       <c r="B630" s="0" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="H630" s="8" t="s">
-        <v>1022</v>
-      </c>
-      <c r="I630" s="6" t="s">
-        <v>1011</v>
+        <v>1023</v>
+      </c>
+      <c r="I630" s="4" t="s">
+        <v>771</v>
       </c>
       <c r="J630" s="8"/>
-      <c r="K630" s="6"/>
+      <c r="K630" s="4"/>
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="0" t="s">
         <v>803</v>
       </c>
       <c r="B631" s="0" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="H631" s="8" t="s">
-        <v>1024</v>
-      </c>
-      <c r="I631" s="6" t="s">
-        <v>1011</v>
+        <v>1025</v>
+      </c>
+      <c r="I631" s="4" t="s">
+        <v>771</v>
       </c>
       <c r="J631" s="8"/>
-      <c r="K631" s="6"/>
+      <c r="K631" s="4"/>
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="0" t="s">
         <v>803</v>
       </c>
       <c r="B632" s="0" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="H632" s="8" t="s">
-        <v>1026</v>
-      </c>
-      <c r="I632" s="4" t="s">
-        <v>1011</v>
+        <v>1027</v>
+      </c>
+      <c r="I632" s="6" t="s">
+        <v>1016</v>
       </c>
       <c r="J632" s="8"/>
-      <c r="K632" s="4"/>
+      <c r="K632" s="6"/>
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="0" t="s">
         <v>803</v>
       </c>
       <c r="B633" s="0" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="H633" s="8" t="s">
-        <v>1028</v>
-      </c>
-      <c r="I633" s="4" t="s">
-        <v>1011</v>
+        <v>1029</v>
+      </c>
+      <c r="I633" s="6" t="s">
+        <v>1016</v>
       </c>
       <c r="J633" s="8"/>
-      <c r="K633" s="4"/>
+      <c r="K633" s="6"/>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="0" t="s">
         <v>803</v>
       </c>
       <c r="B634" s="0" t="s">
-        <v>1029</v>
-      </c>
-      <c r="H634" s="10" t="s">
         <v>1030</v>
       </c>
+      <c r="H634" s="8" t="s">
+        <v>1031</v>
+      </c>
       <c r="I634" s="4" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J634" s="10"/>
+        <v>1016</v>
+      </c>
+      <c r="J634" s="8"/>
       <c r="K634" s="4"/>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11491,58 +11496,58 @@
         <v>803</v>
       </c>
       <c r="B635" s="0" t="s">
-        <v>1031</v>
-      </c>
-      <c r="H635" s="10" t="s">
         <v>1032</v>
       </c>
+      <c r="H635" s="8" t="s">
+        <v>1033</v>
+      </c>
       <c r="I635" s="4" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J635" s="10"/>
+        <v>1016</v>
+      </c>
+      <c r="J635" s="8"/>
       <c r="K635" s="4"/>
+    </row>
+    <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A636" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="B636" s="0" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H636" s="10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I636" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J636" s="10"/>
+      <c r="K636" s="4"/>
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="0" t="s">
-        <v>733</v>
+        <v>803</v>
       </c>
       <c r="B637" s="0" t="s">
-        <v>1033</v>
-      </c>
-      <c r="H637" s="4" t="s">
-        <v>1034</v>
+        <v>1036</v>
+      </c>
+      <c r="H637" s="10" t="s">
+        <v>1037</v>
       </c>
       <c r="I637" s="4" t="s">
-        <v>771</v>
-      </c>
-      <c r="J637" s="4"/>
+        <v>1016</v>
+      </c>
+      <c r="J637" s="10"/>
       <c r="K637" s="4"/>
-    </row>
-    <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A638" s="0" t="s">
-        <v>733</v>
-      </c>
-      <c r="B638" s="0" t="s">
-        <v>1035</v>
-      </c>
-      <c r="H638" s="4" t="s">
-        <v>1036</v>
-      </c>
-      <c r="I638" s="4" t="s">
-        <v>771</v>
-      </c>
-      <c r="J638" s="4"/>
-      <c r="K638" s="4"/>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="0" t="s">
         <v>733</v>
       </c>
       <c r="B639" s="0" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="H639" s="4" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="I639" s="4" t="s">
         <v>771</v>
@@ -11555,10 +11560,10 @@
         <v>733</v>
       </c>
       <c r="B640" s="0" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="H640" s="4" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="I640" s="4" t="s">
         <v>771</v>
@@ -11568,13 +11573,13 @@
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="0" t="s">
-        <v>1008</v>
+        <v>733</v>
       </c>
       <c r="B641" s="0" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="H641" s="4" t="s">
-        <v>1036</v>
+        <v>1043</v>
       </c>
       <c r="I641" s="4" t="s">
         <v>771</v>
@@ -11584,13 +11589,13 @@
     </row>
     <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="0" t="s">
-        <v>1008</v>
+        <v>733</v>
       </c>
       <c r="B642" s="0" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
       <c r="H642" s="4" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="I642" s="4" t="s">
         <v>771</v>
@@ -11598,236 +11603,236 @@
       <c r="J642" s="4"/>
       <c r="K642" s="4"/>
     </row>
-    <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A645" s="0" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B645" s="0" t="s">
-        <v>1044</v>
-      </c>
-      <c r="H645" s="4" t="s">
+    <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A643" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B643" s="0" t="s">
         <v>1045</v>
       </c>
-      <c r="I645" s="4" t="s">
-        <v>988</v>
-      </c>
-      <c r="J645" s="4"/>
-      <c r="K645" s="4"/>
-    </row>
-    <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A646" s="0" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B646" s="0" t="s">
+      <c r="H643" s="4" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I643" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="J643" s="4"/>
+      <c r="K643" s="4"/>
+    </row>
+    <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A644" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B644" s="0" t="s">
         <v>1046</v>
       </c>
-      <c r="H646" s="4" t="s">
+      <c r="H644" s="4" t="s">
         <v>1047</v>
       </c>
-      <c r="I646" s="4" t="s">
-        <v>988</v>
-      </c>
-      <c r="J646" s="4"/>
-      <c r="K646" s="4"/>
-      <c r="L646" s="4"/>
-    </row>
-    <row r="647" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I644" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="J644" s="4"/>
+      <c r="K644" s="4"/>
+    </row>
+    <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B647" s="0" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="H647" s="4" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="I647" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J647" s="4"/>
       <c r="K647" s="4"/>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B648" s="0" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="H648" s="4" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="I648" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J648" s="4"/>
       <c r="K648" s="4"/>
-    </row>
-    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L648" s="4"/>
+    </row>
+    <row r="649" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B649" s="0" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="H649" s="4" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="I649" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J649" s="4"/>
       <c r="K649" s="4"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B650" s="0" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="H650" s="4" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="I650" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J650" s="4"/>
       <c r="K650" s="4"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B651" s="0" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="H651" s="4" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="I651" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J651" s="4"/>
       <c r="K651" s="4"/>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B652" s="0" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="H652" s="4" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="I652" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J652" s="4"/>
       <c r="K652" s="4"/>
-      <c r="L652" s="4"/>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B653" s="0" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="H653" s="4" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="I653" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J653" s="4"/>
       <c r="K653" s="4"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B654" s="0" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="H654" s="4" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="I654" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J654" s="4"/>
       <c r="K654" s="4"/>
+      <c r="L654" s="4"/>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B655" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="H655" s="4" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="I655" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J655" s="4"/>
       <c r="K655" s="4"/>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B656" s="0" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="H656" s="4" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="I656" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J656" s="4"/>
       <c r="K656" s="4"/>
-      <c r="L656" s="4"/>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B657" s="0" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="H657" s="4" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="I657" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J657" s="4"/>
       <c r="K657" s="4"/>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B658" s="0" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="H658" s="4" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="I658" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J658" s="4"/>
       <c r="K658" s="4"/>
+      <c r="L658" s="4"/>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>1072</v>
+        <v>1048</v>
       </c>
       <c r="B659" s="0" t="s">
         <v>1073</v>
@@ -11836,30 +11841,30 @@
         <v>1074</v>
       </c>
       <c r="I659" s="4" t="s">
-        <v>1075</v>
+        <v>993</v>
       </c>
       <c r="J659" s="4"/>
       <c r="K659" s="4"/>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="0" t="s">
-        <v>1072</v>
+        <v>1048</v>
       </c>
       <c r="B660" s="0" t="s">
+        <v>1075</v>
+      </c>
+      <c r="H660" s="4" t="s">
         <v>1076</v>
       </c>
-      <c r="H660" s="4" t="s">
-        <v>1077</v>
-      </c>
       <c r="I660" s="4" t="s">
-        <v>1075</v>
+        <v>993</v>
       </c>
       <c r="J660" s="4"/>
       <c r="K660" s="4"/>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="0" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="B661" s="0" t="s">
         <v>1078</v>
@@ -11868,100 +11873,100 @@
         <v>1079</v>
       </c>
       <c r="I661" s="4" t="s">
-        <v>1075</v>
+        <v>1080</v>
       </c>
       <c r="J661" s="4"/>
       <c r="K661" s="4"/>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="B662" s="0" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H662" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="I662" s="4" t="s">
         <v>1080</v>
-      </c>
-      <c r="H662" s="4" t="s">
-        <v>1081</v>
-      </c>
-      <c r="I662" s="4" t="s">
-        <v>1075</v>
       </c>
       <c r="J662" s="4"/>
       <c r="K662" s="4"/>
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="0" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
       <c r="B663" s="0" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="H663" s="4" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="I663" s="4" t="s">
-        <v>1075</v>
+        <v>1080</v>
       </c>
       <c r="J663" s="4"/>
       <c r="K663" s="4"/>
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="0" t="s">
-        <v>1084</v>
+        <v>1077</v>
       </c>
       <c r="B664" s="0" t="s">
-        <v>1076</v>
+        <v>1085</v>
       </c>
       <c r="H664" s="4" t="s">
-        <v>1077</v>
+        <v>1086</v>
       </c>
       <c r="I664" s="4" t="s">
-        <v>771</v>
+        <v>1080</v>
       </c>
       <c r="J664" s="4"/>
       <c r="K664" s="4"/>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="s">
-        <v>1085</v>
+        <v>1077</v>
       </c>
       <c r="B665" s="0" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="H665" s="4" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="I665" s="4" t="s">
-        <v>771</v>
+        <v>1080</v>
       </c>
       <c r="J665" s="4"/>
       <c r="K665" s="4"/>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
-        <v>733</v>
+        <v>1089</v>
       </c>
       <c r="B666" s="0" t="s">
-        <v>1088</v>
+        <v>1081</v>
       </c>
       <c r="H666" s="4" t="s">
-        <v>1089</v>
-      </c>
-      <c r="I666" s="6" t="s">
-        <v>1011</v>
+        <v>1082</v>
+      </c>
+      <c r="I666" s="4" t="s">
+        <v>771</v>
       </c>
       <c r="J666" s="4"/>
-      <c r="K666" s="6"/>
+      <c r="K666" s="4"/>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
-        <v>733</v>
+        <v>1090</v>
       </c>
       <c r="B667" s="0" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="H667" s="4" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="I667" s="4" t="s">
         <v>771</v>
@@ -11974,96 +11979,96 @@
         <v>733</v>
       </c>
       <c r="B668" s="0" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H668" s="11" t="s">
         <v>1093</v>
       </c>
-      <c r="J668" s="11"/>
+      <c r="H668" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I668" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J668" s="4"/>
+      <c r="K668" s="6"/>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>968</v>
+        <v>733</v>
       </c>
       <c r="B669" s="0" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="H669" s="4" t="s">
-        <v>1095</v>
-      </c>
-      <c r="I669" s="6" t="s">
-        <v>1011</v>
+        <v>1096</v>
+      </c>
+      <c r="I669" s="4" t="s">
+        <v>771</v>
       </c>
       <c r="J669" s="4"/>
-      <c r="K669" s="6"/>
+      <c r="K669" s="4"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>803</v>
+        <v>733</v>
       </c>
       <c r="B670" s="0" t="s">
-        <v>1096</v>
-      </c>
-      <c r="H670" s="4" t="s">
         <v>1097</v>
       </c>
-      <c r="I670" s="4" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J670" s="4"/>
-      <c r="K670" s="4"/>
+      <c r="H670" s="11" t="s">
+        <v>1098</v>
+      </c>
+      <c r="J670" s="11"/>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B671" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H671" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="I671" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J671" s="4"/>
+      <c r="K671" s="6"/>
+    </row>
+    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A672" s="0" t="s">
         <v>803</v>
       </c>
-      <c r="B671" s="0" t="s">
-        <v>1098</v>
-      </c>
-      <c r="H671" s="4" t="s">
-        <v>1099</v>
-      </c>
-      <c r="I671" s="4" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J671" s="4"/>
-      <c r="K671" s="4"/>
+      <c r="B672" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H672" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I672" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J672" s="4"/>
+      <c r="K672" s="4"/>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
-        <v>1100</v>
+        <v>803</v>
       </c>
       <c r="B673" s="0" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="H673" s="4" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="I673" s="4" t="s">
-        <v>1103</v>
+        <v>1016</v>
       </c>
       <c r="J673" s="4"/>
       <c r="K673" s="4"/>
     </row>
-    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A674" s="0" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B674" s="0" t="s">
-        <v>1104</v>
-      </c>
-      <c r="H674" s="4" t="s">
-        <v>1105</v>
-      </c>
-      <c r="I674" s="4" t="s">
-        <v>1103</v>
-      </c>
-      <c r="J674" s="4"/>
-      <c r="K674" s="4"/>
-    </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="0" t="s">
-        <v>1100</v>
+        <v>1105</v>
       </c>
       <c r="B675" s="0" t="s">
         <v>1106</v>
@@ -12072,94 +12077,94 @@
         <v>1107</v>
       </c>
       <c r="I675" s="4" t="s">
-        <v>1011</v>
+        <v>1108</v>
       </c>
       <c r="J675" s="4"/>
       <c r="K675" s="4"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="0" t="s">
-        <v>1043</v>
+        <v>1105</v>
       </c>
       <c r="B676" s="0" t="s">
+        <v>1109</v>
+      </c>
+      <c r="H676" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="I676" s="4" t="s">
         <v>1108</v>
-      </c>
-      <c r="H676" s="4" t="s">
-        <v>1109</v>
-      </c>
-      <c r="I676" s="4" t="s">
-        <v>988</v>
       </c>
       <c r="J676" s="4"/>
       <c r="K676" s="4"/>
     </row>
-    <row r="677" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>1043</v>
+        <v>1105</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="H677" s="4" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="I677" s="4" t="s">
-        <v>988</v>
+        <v>1016</v>
       </c>
       <c r="J677" s="4"/>
       <c r="K677" s="4"/>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B678" s="0" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="H678" s="4" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="I678" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J678" s="4"/>
       <c r="K678" s="4"/>
     </row>
-    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="679" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="0" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="B679" s="0" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="H679" s="4" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="I679" s="4" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="J679" s="4"/>
       <c r="K679" s="4"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>1072</v>
+        <v>1048</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="H680" s="4" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="I680" s="4" t="s">
-        <v>1075</v>
+        <v>993</v>
       </c>
       <c r="J680" s="4"/>
       <c r="K680" s="4"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
-        <v>1118</v>
+        <v>1048</v>
       </c>
       <c r="B681" s="0" t="s">
         <v>1119</v>
@@ -12167,184 +12172,146 @@
       <c r="H681" s="4" t="s">
         <v>1120</v>
       </c>
-      <c r="I681" s="6" t="s">
-        <v>1011</v>
+      <c r="I681" s="4" t="s">
+        <v>993</v>
       </c>
       <c r="J681" s="4"/>
-      <c r="K681" s="6"/>
+      <c r="K681" s="4"/>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="0" t="s">
-        <v>1118</v>
+        <v>1077</v>
       </c>
       <c r="B682" s="0" t="s">
         <v>1121</v>
       </c>
       <c r="H682" s="4" t="s">
-        <v>1120</v>
-      </c>
-      <c r="I682" s="6" t="s">
-        <v>1011</v>
+        <v>1122</v>
+      </c>
+      <c r="I682" s="4" t="s">
+        <v>1080</v>
       </c>
       <c r="J682" s="4"/>
-      <c r="K682" s="6"/>
-    </row>
-    <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A686" s="0" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B686" s="0" t="s">
-        <v>1122</v>
-      </c>
-      <c r="H686" s="4" t="s">
+      <c r="K682" s="4"/>
+    </row>
+    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A683" s="0" t="s">
         <v>1123</v>
       </c>
-      <c r="I686" s="4" t="s">
-        <v>1103</v>
-      </c>
-      <c r="J686" s="4"/>
-      <c r="K686" s="4"/>
-    </row>
-    <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A687" s="0" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B687" s="0" t="s">
+      <c r="B683" s="0" t="s">
         <v>1124</v>
       </c>
-      <c r="H687" s="4" t="s">
+      <c r="H683" s="4" t="s">
         <v>1125</v>
       </c>
-      <c r="I687" s="4" t="s">
-        <v>1103</v>
-      </c>
-      <c r="J687" s="4"/>
-      <c r="K687" s="4"/>
+      <c r="I683" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J683" s="4"/>
+      <c r="K683" s="6"/>
+    </row>
+    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A684" s="0" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B684" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H684" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I684" s="6" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J684" s="4"/>
+      <c r="K684" s="6"/>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="0" t="s">
-        <v>1100</v>
+        <v>1105</v>
       </c>
       <c r="B688" s="0" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="H688" s="4" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="I688" s="4" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="J688" s="4"/>
       <c r="K688" s="4"/>
     </row>
     <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="0" t="s">
-        <v>1100</v>
+        <v>1105</v>
       </c>
       <c r="B689" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="H689" s="4" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="I689" s="4" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="J689" s="4"/>
       <c r="K689" s="4"/>
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="0" t="s">
-        <v>1100</v>
+        <v>1105</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="H690" s="4" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="I690" s="4" t="s">
-        <v>1103</v>
+        <v>1108</v>
       </c>
       <c r="J690" s="4"/>
       <c r="K690" s="4"/>
     </row>
-    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A694" s="0" t="s">
-        <v>968</v>
-      </c>
-      <c r="B694" s="0" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C694" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D694" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="E694" s="0" t="s">
+    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A691" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B691" s="0" t="s">
         <v>1133</v>
       </c>
-      <c r="F694" s="0" t="s">
+      <c r="H691" s="4" t="s">
         <v>1134</v>
       </c>
-      <c r="G694" s="0" t="s">
+      <c r="I691" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J691" s="4"/>
+      <c r="K691" s="4"/>
+    </row>
+    <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A692" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B692" s="0" t="s">
         <v>1135</v>
       </c>
-      <c r="H694" s="0" t="s">
+      <c r="H692" s="4" t="s">
         <v>1136</v>
       </c>
-      <c r="I694" s="0" t="s">
-        <v>1137</v>
-      </c>
-      <c r="J694" s="0" t="s">
-        <v>1138</v>
-      </c>
-      <c r="K694" s="0" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A695" s="0" t="s">
-        <v>968</v>
-      </c>
-      <c r="B695" s="0" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C695" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D695" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="E695" s="0" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F695" s="0" t="s">
-        <v>1142</v>
-      </c>
-      <c r="G695" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H695" s="0" t="s">
-        <v>1143</v>
-      </c>
-      <c r="I695" s="0" t="s">
-        <v>1144</v>
-      </c>
-      <c r="J695" s="0" t="s">
-        <v>1145</v>
-      </c>
-      <c r="K695" s="0" t="s">
-        <v>1139</v>
-      </c>
+      <c r="I692" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J692" s="4"/>
+      <c r="K692" s="4"/>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="0" t="s">
         <v>968</v>
       </c>
       <c r="B696" s="0" t="s">
-        <v>1146</v>
+        <v>1137</v>
       </c>
       <c r="C696" s="0" t="n">
         <v>1</v>
@@ -12353,25 +12320,25 @@
         <v>594</v>
       </c>
       <c r="E696" s="0" t="s">
-        <v>1147</v>
+        <v>1138</v>
       </c>
       <c r="F696" s="0" t="s">
-        <v>1148</v>
+        <v>1139</v>
       </c>
       <c r="G696" s="0" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="H696" s="0" t="s">
-        <v>1149</v>
+        <v>1141</v>
       </c>
       <c r="I696" s="0" t="s">
-        <v>1150</v>
+        <v>1142</v>
       </c>
       <c r="J696" s="0" t="s">
-        <v>1151</v>
+        <v>1143</v>
       </c>
       <c r="K696" s="0" t="s">
-        <v>1139</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12379,7 +12346,7 @@
         <v>968</v>
       </c>
       <c r="B697" s="0" t="s">
-        <v>1152</v>
+        <v>1145</v>
       </c>
       <c r="C697" s="0" t="n">
         <v>1</v>
@@ -12388,165 +12355,165 @@
         <v>594</v>
       </c>
       <c r="E697" s="0" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F697" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G697" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H697" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="I697" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="J697" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="K697" s="0" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A698" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B698" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C698" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D698" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="E698" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F698" s="0" t="s">
         <v>1153</v>
       </c>
-      <c r="F697" s="0" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G697" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H697" s="0" t="s">
+      <c r="G698" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H698" s="0" t="s">
         <v>1154</v>
       </c>
-      <c r="I697" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="J697" s="0" t="s">
+      <c r="I698" s="0" t="s">
         <v>1155</v>
       </c>
-      <c r="K697" s="0" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A701" s="0" t="s">
+      <c r="J698" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="K698" s="0" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A699" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B699" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C699" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D699" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="E699" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F699" s="0" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G699" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H699" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="I699" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="J699" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="K699" s="0" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A703" s="0" t="s">
         <v>803</v>
       </c>
-      <c r="B701" s="0" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C701" s="0" t="n">
+      <c r="B703" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C703" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D701" s="0" t="s">
+      <c r="D703" s="0" t="s">
         <v>603</v>
       </c>
-      <c r="E701" s="0" t="s">
-        <v>1157</v>
-      </c>
-      <c r="F701" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="G701" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H701" s="0" t="s">
-        <v>1159</v>
-      </c>
-      <c r="I701" s="0" t="s">
-        <v>1160</v>
-      </c>
-      <c r="J701" s="0" t="s">
-        <v>1161</v>
-      </c>
-      <c r="K701" s="0" t="s">
+      <c r="E703" s="0" t="s">
         <v>1162</v>
       </c>
-    </row>
-    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A702" s="0" t="s">
+      <c r="F703" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G703" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H703" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="I703" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J703" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="K703" s="0" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A704" s="0" t="s">
         <v>803</v>
       </c>
-      <c r="B702" s="0" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C702" s="0" t="n">
+      <c r="B704" s="0" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C704" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D702" s="0" t="s">
+      <c r="D704" s="0" t="s">
         <v>594</v>
       </c>
-      <c r="E702" s="0" t="s">
+      <c r="E704" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F704" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="G704" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H704" s="0" t="s">
         <v>1164</v>
       </c>
-      <c r="F702" s="0" t="s">
+      <c r="I704" s="0" t="s">
         <v>1165</v>
       </c>
-      <c r="G702" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H702" s="0" t="s">
-        <v>1159</v>
-      </c>
-      <c r="I702" s="0" t="s">
-        <v>1160</v>
-      </c>
-      <c r="J702" s="0" t="s">
-        <v>1166</v>
-      </c>
-      <c r="K702" s="0" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A706" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="B706" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="C706" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D706" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="E706" s="0" t="s">
+      <c r="J704" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="K704" s="0" t="s">
         <v>1167</v>
-      </c>
-      <c r="F706" s="0" t="s">
-        <v>1168</v>
-      </c>
-      <c r="G706" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H706" s="0" t="s">
-        <v>1169</v>
-      </c>
-      <c r="I706" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="J706" s="0" t="s">
-        <v>1170</v>
-      </c>
-      <c r="K706" s="0" t="s">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A707" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="B707" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="C707" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D707" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="E707" s="0" t="s">
-        <v>1172</v>
-      </c>
-      <c r="F707" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G707" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H707" s="0" t="s">
-        <v>1173</v>
-      </c>
-      <c r="I707" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="J707" s="0" t="s">
-        <v>1174</v>
-      </c>
-      <c r="K707" s="0" t="s">
-        <v>1171</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12554,7 +12521,7 @@
         <v>568</v>
       </c>
       <c r="B708" s="0" t="s">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="C708" s="0" t="n">
         <v>1</v>
@@ -12563,25 +12530,25 @@
         <v>594</v>
       </c>
       <c r="E708" s="0" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="F708" s="0" t="s">
-        <v>1168</v>
+        <v>1173</v>
       </c>
       <c r="G708" s="0" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="H708" s="0" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="I708" s="0" t="s">
         <v>562</v>
       </c>
       <c r="J708" s="0" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="K708" s="0" t="s">
-        <v>1171</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12589,34 +12556,34 @@
         <v>568</v>
       </c>
       <c r="B709" s="0" t="s">
-        <v>209</v>
+        <v>366</v>
       </c>
       <c r="C709" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D709" s="0" t="s">
         <v>594</v>
       </c>
       <c r="E709" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F709" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G709" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H709" s="0" t="s">
         <v>1178</v>
-      </c>
-      <c r="F709" s="0" t="s">
-        <v>1179</v>
-      </c>
-      <c r="G709" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H709" s="0" t="s">
-        <v>209</v>
       </c>
       <c r="I709" s="0" t="s">
         <v>562</v>
       </c>
       <c r="J709" s="0" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K709" s="0" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12624,34 +12591,34 @@
         <v>568</v>
       </c>
       <c r="B710" s="0" t="s">
-        <v>1182</v>
+        <v>390</v>
       </c>
       <c r="C710" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D710" s="0" t="s">
-        <v>1183</v>
+        <v>594</v>
       </c>
       <c r="E710" s="0" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="F710" s="0" t="s">
-        <v>1185</v>
+        <v>1173</v>
       </c>
       <c r="G710" s="0" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="H710" s="0" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="I710" s="0" t="s">
         <v>562</v>
       </c>
       <c r="J710" s="0" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="K710" s="0" t="s">
-        <v>1188</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12659,34 +12626,34 @@
         <v>568</v>
       </c>
       <c r="B711" s="0" t="s">
-        <v>1189</v>
+        <v>209</v>
       </c>
       <c r="C711" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D711" s="0" t="s">
         <v>594</v>
       </c>
       <c r="E711" s="0" t="s">
-        <v>1190</v>
+        <v>1183</v>
       </c>
       <c r="F711" s="0" t="s">
-        <v>1191</v>
+        <v>1184</v>
       </c>
       <c r="G711" s="0" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="H711" s="0" t="s">
-        <v>1192</v>
+        <v>209</v>
       </c>
       <c r="I711" s="0" t="s">
         <v>562</v>
       </c>
       <c r="J711" s="0" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
       <c r="K711" s="0" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12694,127 +12661,162 @@
         <v>568</v>
       </c>
       <c r="B712" s="0" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
       <c r="C712" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D712" s="0" t="s">
-        <v>594</v>
+        <v>1188</v>
       </c>
       <c r="E712" s="0" t="s">
-        <v>1196</v>
+        <v>1189</v>
       </c>
       <c r="F712" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G712" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H712" s="0" t="s">
         <v>1191</v>
-      </c>
-      <c r="G712" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H712" s="0" t="s">
-        <v>1192</v>
       </c>
       <c r="I712" s="0" t="s">
         <v>562</v>
       </c>
       <c r="J712" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K712" s="0" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A713" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="B713" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C713" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D713" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="E713" s="0" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F713" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G713" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H713" s="0" t="s">
         <v>1197</v>
       </c>
-      <c r="K712" s="0" t="s">
-        <v>1194</v>
+      <c r="I713" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="J713" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="K713" s="0" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="0" t="s">
-        <v>1198</v>
+        <v>568</v>
       </c>
       <c r="B714" s="0" t="s">
-        <v>1182</v>
+        <v>1200</v>
       </c>
       <c r="C714" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D714" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="E714" s="0" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F714" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G714" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H714" s="0" t="s">
+        <v>1197</v>
+      </c>
+      <c r="I714" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="J714" s="0" t="s">
+        <v>1202</v>
+      </c>
+      <c r="K714" s="0" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A716" s="0" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B716" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C716" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D714" s="0" t="s">
-        <v>1199</v>
-      </c>
-      <c r="E714" s="0" t="s">
-        <v>1184</v>
-      </c>
-      <c r="F714" s="0" t="s">
-        <v>1185</v>
-      </c>
-      <c r="G714" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H714" s="0" t="s">
-        <v>1186</v>
-      </c>
-      <c r="I714" s="0" t="s">
-        <v>1200</v>
-      </c>
-      <c r="J714" s="0" t="s">
-        <v>1187</v>
-      </c>
-      <c r="K714" s="0" t="s">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A717" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="B717" s="0" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C717" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D717" s="0" t="s">
-        <v>1203</v>
-      </c>
-      <c r="E717" s="0" t="s">
+      <c r="D716" s="0" t="s">
         <v>1204</v>
       </c>
-      <c r="F717" s="0" t="s">
+      <c r="E716" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F716" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G716" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H716" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I716" s="0" t="s">
         <v>1205</v>
       </c>
-      <c r="G717" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H717" s="0" t="s">
+      <c r="J716" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K716" s="0" t="s">
         <v>1206</v>
-      </c>
-      <c r="I717" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="J717" s="0" t="s">
-        <v>1207</v>
-      </c>
-      <c r="K717" s="0" t="s">
-        <v>1171</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="0" t="s">
-        <v>1208</v>
+        <v>568</v>
       </c>
       <c r="B719" s="0" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C719" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D719" s="0" t="s">
-        <v>1183</v>
+        <v>1208</v>
       </c>
       <c r="E719" s="0" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F719" s="0" t="s">
         <v>1210</v>
       </c>
-      <c r="F719" s="0" t="s">
-        <v>1168</v>
-      </c>
       <c r="G719" s="0" t="s">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="H719" s="0" t="s">
         <v>1211</v>
@@ -12826,103 +12828,138 @@
         <v>1212</v>
       </c>
       <c r="K719" s="0" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A721" s="0" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A720" s="0" t="s">
-        <v>1208</v>
-      </c>
-      <c r="B720" s="0" t="s">
+      <c r="B721" s="0" t="s">
         <v>1214</v>
       </c>
-      <c r="C720" s="0" t="n">
+      <c r="C721" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D720" s="0" t="s">
-        <v>1183</v>
-      </c>
-      <c r="E720" s="0" t="s">
+      <c r="D721" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E721" s="0" t="s">
         <v>1215</v>
       </c>
-      <c r="F720" s="0" t="n">
+      <c r="F721" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G721" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H721" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="I721" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="J721" s="0" t="s">
+        <v>1217</v>
+      </c>
+      <c r="K721" s="0" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A722" s="0" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B722" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C722" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G720" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H720" s="0" t="s">
-        <v>1216</v>
-      </c>
-      <c r="I720" s="0" t="s">
+      <c r="D722" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E722" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F722" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G722" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H722" s="0" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I722" s="0" t="s">
         <v>562</v>
       </c>
-      <c r="J720" s="0" t="s">
-        <v>1174</v>
-      </c>
-      <c r="K720" s="0" t="s">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B723" s="12" t="s">
-        <v>1217</v>
-      </c>
-      <c r="H723" s="13" t="s">
+      <c r="J722" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="K722" s="0" t="s">
         <v>1218</v>
-      </c>
-      <c r="I723" s="0" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B724" s="12" t="s">
-        <v>1219</v>
-      </c>
-      <c r="H724" s="13" t="s">
-        <v>1220</v>
-      </c>
-      <c r="I724" s="0" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B725" s="12" t="s">
-        <v>1221</v>
-      </c>
-      <c r="H725" s="14" t="s">
         <v>1222</v>
       </c>
+      <c r="H725" s="13" t="s">
+        <v>1223</v>
+      </c>
       <c r="I725" s="0" t="s">
-        <v>562</v>
+        <v>983</v>
       </c>
     </row>
     <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A726" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="B726" s="0" t="s">
-        <v>1223</v>
-      </c>
-      <c r="H726" s="14" t="s">
+      <c r="B726" s="12" t="s">
         <v>1224</v>
       </c>
+      <c r="H726" s="13" t="s">
+        <v>1225</v>
+      </c>
       <c r="I726" s="0" t="s">
-        <v>1225</v>
+        <v>983</v>
       </c>
     </row>
     <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A727" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="B727" s="0" t="s">
+      <c r="B727" s="12" t="s">
         <v>1226</v>
       </c>
       <c r="H727" s="14" t="s">
         <v>1227</v>
       </c>
       <c r="I727" s="0" t="s">
-        <v>1225</v>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A728" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="B728" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="H728" s="14" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I728" s="0" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A729" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="B729" s="0" t="s">
+        <v>1231</v>
+      </c>
+      <c r="H729" s="14" t="s">
+        <v>1232</v>
+      </c>
+      <c r="I729" s="0" t="s">
+        <v>1230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move the variables tauupbl & tauvpbl from the pre identified missing file to the pre ignored file and modify comment #191 #143 #346.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="1243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="1239">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3173,56 +3173,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gijs &amp; Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tauupbl</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF007FFF"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Available in IFS: Eastward turbulent surface stress (grib 128.180) plus the Eastward gravity wave surface stress (grib 128.195).  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Check with data request or DynVar people if this is indeed what is asked here.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">tauvpbl</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF007FFF"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Available in IFS: Northward turbulent surface stress (grib 128.181) plus the Northward gravity wave surface stress (grib 128.196).  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Cambria"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Check with data request or DynVar people if this is indeed what is asked here.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">E3hr</t>
@@ -3963,15 +3913,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Cambria"/>
+      <color rgb="FF007FFF"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF007FFF"/>
-      <name val="Arial"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -4044,7 +3994,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4081,11 +4031,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4182,10 +4128,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L746"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E266" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I282" activeCellId="0" sqref="I282:I297"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A630" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A645" activeCellId="0" sqref="A645"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11581,45 +11527,41 @@
       <c r="J644" s="8"/>
       <c r="K644" s="6"/>
     </row>
-    <row r="645" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B645" s="9" t="s">
         <v>1035</v>
       </c>
-      <c r="C645" s="9"/>
-      <c r="D645" s="9"/>
+      <c r="B645" s="0" t="s">
+        <v>1036</v>
+      </c>
       <c r="H645" s="8" t="s">
-        <v>1036</v>
-      </c>
-      <c r="I645" s="6" t="s">
-        <v>1034</v>
+        <v>1037</v>
+      </c>
+      <c r="I645" s="4" t="s">
+        <v>789</v>
       </c>
       <c r="J645" s="8"/>
-      <c r="K645" s="6"/>
-    </row>
-    <row r="646" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K645" s="4"/>
+    </row>
+    <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B646" s="9" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C646" s="9"/>
-      <c r="D646" s="9"/>
+        <v>821</v>
+      </c>
+      <c r="B646" s="0" t="s">
+        <v>1038</v>
+      </c>
       <c r="H646" s="8" t="s">
-        <v>1038</v>
-      </c>
-      <c r="I646" s="6" t="s">
-        <v>1034</v>
+        <v>1039</v>
+      </c>
+      <c r="I646" s="4" t="s">
+        <v>789</v>
       </c>
       <c r="J646" s="8"/>
-      <c r="K646" s="6"/>
+      <c r="K646" s="4"/>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
-        <v>1039</v>
+        <v>821</v>
       </c>
       <c r="B647" s="0" t="s">
         <v>1040</v>
@@ -11627,11 +11569,11 @@
       <c r="H647" s="8" t="s">
         <v>1041</v>
       </c>
-      <c r="I647" s="4" t="s">
-        <v>789</v>
+      <c r="I647" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J647" s="8"/>
-      <c r="K647" s="4"/>
+      <c r="K647" s="6"/>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="0" t="s">
@@ -11643,11 +11585,11 @@
       <c r="H648" s="8" t="s">
         <v>1043</v>
       </c>
-      <c r="I648" s="4" t="s">
-        <v>789</v>
+      <c r="I648" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J648" s="8"/>
-      <c r="K648" s="4"/>
+      <c r="K648" s="6"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
@@ -11659,11 +11601,11 @@
       <c r="H649" s="8" t="s">
         <v>1045</v>
       </c>
-      <c r="I649" s="6" t="s">
+      <c r="I649" s="4" t="s">
         <v>1034</v>
       </c>
       <c r="J649" s="8"/>
-      <c r="K649" s="6"/>
+      <c r="K649" s="4"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
@@ -11675,11 +11617,11 @@
       <c r="H650" s="8" t="s">
         <v>1047</v>
       </c>
-      <c r="I650" s="6" t="s">
+      <c r="I650" s="4" t="s">
         <v>1034</v>
       </c>
       <c r="J650" s="8"/>
-      <c r="K650" s="6"/>
+      <c r="K650" s="4"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
@@ -11688,13 +11630,13 @@
       <c r="B651" s="0" t="s">
         <v>1048</v>
       </c>
-      <c r="H651" s="8" t="s">
+      <c r="H651" s="9" t="s">
         <v>1049</v>
       </c>
       <c r="I651" s="4" t="s">
         <v>1034</v>
       </c>
-      <c r="J651" s="8"/>
+      <c r="J651" s="9"/>
       <c r="K651" s="4"/>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11704,46 +11646,46 @@
       <c r="B652" s="0" t="s">
         <v>1050</v>
       </c>
-      <c r="H652" s="8" t="s">
+      <c r="H652" s="9" t="s">
         <v>1051</v>
       </c>
       <c r="I652" s="4" t="s">
         <v>1034</v>
       </c>
-      <c r="J652" s="8"/>
+      <c r="J652" s="9"/>
       <c r="K652" s="4"/>
-    </row>
-    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A653" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B653" s="0" t="s">
-        <v>1052</v>
-      </c>
-      <c r="H653" s="10" t="s">
-        <v>1053</v>
-      </c>
-      <c r="I653" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J653" s="10"/>
-      <c r="K653" s="4"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>821</v>
+        <v>751</v>
       </c>
       <c r="B654" s="0" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H654" s="4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="I654" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="J654" s="4"/>
+      <c r="K654" s="4"/>
+    </row>
+    <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A655" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="B655" s="0" t="s">
         <v>1054</v>
       </c>
-      <c r="H654" s="10" t="s">
+      <c r="H655" s="4" t="s">
         <v>1055</v>
       </c>
-      <c r="I654" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J654" s="10"/>
-      <c r="K654" s="4"/>
+      <c r="I655" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="J655" s="4"/>
+      <c r="K655" s="4"/>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
@@ -11769,7 +11711,7 @@
         <v>1058</v>
       </c>
       <c r="H657" s="4" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="I657" s="4" t="s">
         <v>789</v>
@@ -11779,13 +11721,13 @@
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
-        <v>751</v>
+        <v>1031</v>
       </c>
       <c r="B658" s="0" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="H658" s="4" t="s">
-        <v>1061</v>
+        <v>1055</v>
       </c>
       <c r="I658" s="4" t="s">
         <v>789</v>
@@ -11795,10 +11737,10 @@
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>751</v>
+        <v>1031</v>
       </c>
       <c r="B659" s="0" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="H659" s="4" t="s">
         <v>1061</v>
@@ -11809,41 +11751,42 @@
       <c r="J659" s="4"/>
       <c r="K659" s="4"/>
     </row>
-    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A660" s="0" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B660" s="0" t="s">
+    <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A662" s="0" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B662" s="0" t="s">
         <v>1063</v>
       </c>
-      <c r="H660" s="4" t="s">
-        <v>1059</v>
-      </c>
-      <c r="I660" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="J660" s="4"/>
-      <c r="K660" s="4"/>
-    </row>
-    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A661" s="0" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B661" s="0" t="s">
+      <c r="H662" s="4" t="s">
         <v>1064</v>
       </c>
-      <c r="H661" s="4" t="s">
+      <c r="I662" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J662" s="4"/>
+      <c r="K662" s="4"/>
+    </row>
+    <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A663" s="0" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B663" s="0" t="s">
         <v>1065</v>
       </c>
-      <c r="I661" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="J661" s="4"/>
-      <c r="K661" s="4"/>
-    </row>
-    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H663" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I663" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J663" s="4"/>
+      <c r="K663" s="4"/>
+      <c r="L663" s="4"/>
+    </row>
+    <row r="664" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B664" s="0" t="s">
         <v>1067</v>
@@ -11859,7 +11802,7 @@
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B665" s="0" t="s">
         <v>1069</v>
@@ -11872,11 +11815,10 @@
       </c>
       <c r="J665" s="4"/>
       <c r="K665" s="4"/>
-      <c r="L665" s="4"/>
-    </row>
-    <row r="666" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B666" s="0" t="s">
         <v>1071</v>
@@ -11892,7 +11834,7 @@
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B667" s="0" t="s">
         <v>1073</v>
@@ -11908,7 +11850,7 @@
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B668" s="0" t="s">
         <v>1075</v>
@@ -11924,7 +11866,7 @@
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B669" s="0" t="s">
         <v>1077</v>
@@ -11937,10 +11879,11 @@
       </c>
       <c r="J669" s="4"/>
       <c r="K669" s="4"/>
+      <c r="L669" s="4"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B670" s="0" t="s">
         <v>1079</v>
@@ -11956,7 +11899,7 @@
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B671" s="0" t="s">
         <v>1081</v>
@@ -11969,11 +11912,10 @@
       </c>
       <c r="J671" s="4"/>
       <c r="K671" s="4"/>
-      <c r="L671" s="4"/>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B672" s="0" t="s">
         <v>1083</v>
@@ -11989,7 +11931,7 @@
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B673" s="0" t="s">
         <v>1085</v>
@@ -12002,10 +11944,11 @@
       </c>
       <c r="J673" s="4"/>
       <c r="K673" s="4"/>
+      <c r="L673" s="4"/>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B674" s="0" t="s">
         <v>1087</v>
@@ -12021,7 +11964,7 @@
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B675" s="0" t="s">
         <v>1089</v>
@@ -12034,59 +11977,58 @@
       </c>
       <c r="J675" s="4"/>
       <c r="K675" s="4"/>
-      <c r="L675" s="4"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="0" t="s">
-        <v>1066</v>
+        <v>1091</v>
       </c>
       <c r="B676" s="0" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="H676" s="4" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="I676" s="4" t="s">
-        <v>1011</v>
+        <v>1094</v>
       </c>
       <c r="J676" s="4"/>
       <c r="K676" s="4"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>1066</v>
+        <v>1091</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="H677" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I677" s="4" t="s">
         <v>1094</v>
-      </c>
-      <c r="I677" s="4" t="s">
-        <v>1011</v>
       </c>
       <c r="J677" s="4"/>
       <c r="K677" s="4"/>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="0" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B678" s="0" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="H678" s="4" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="I678" s="4" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="J678" s="4"/>
       <c r="K678" s="4"/>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="0" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B679" s="0" t="s">
         <v>1099</v>
@@ -12095,14 +12037,14 @@
         <v>1100</v>
       </c>
       <c r="I679" s="4" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="J679" s="4"/>
       <c r="K679" s="4"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B680" s="0" t="s">
         <v>1101</v>
@@ -12111,30 +12053,30 @@
         <v>1102</v>
       </c>
       <c r="I680" s="4" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="J680" s="4"/>
       <c r="K680" s="4"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B681" s="0" t="s">
         <v>1095</v>
       </c>
-      <c r="B681" s="0" t="s">
-        <v>1103</v>
-      </c>
       <c r="H681" s="4" t="s">
-        <v>1104</v>
+        <v>1096</v>
       </c>
       <c r="I681" s="4" t="s">
-        <v>1098</v>
+        <v>789</v>
       </c>
       <c r="J681" s="4"/>
       <c r="K681" s="4"/>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="0" t="s">
-        <v>1095</v>
+        <v>1104</v>
       </c>
       <c r="B682" s="0" t="s">
         <v>1105</v>
@@ -12143,30 +12085,30 @@
         <v>1106</v>
       </c>
       <c r="I682" s="4" t="s">
-        <v>1098</v>
+        <v>789</v>
       </c>
       <c r="J682" s="4"/>
       <c r="K682" s="4"/>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="B683" s="0" t="s">
         <v>1107</v>
       </c>
-      <c r="B683" s="0" t="s">
-        <v>1099</v>
-      </c>
       <c r="H683" s="4" t="s">
-        <v>1100</v>
-      </c>
-      <c r="I683" s="4" t="s">
-        <v>789</v>
+        <v>1108</v>
+      </c>
+      <c r="I683" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J683" s="4"/>
-      <c r="K683" s="4"/>
+      <c r="K683" s="6"/>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="0" t="s">
-        <v>1108</v>
+        <v>751</v>
       </c>
       <c r="B684" s="0" t="s">
         <v>1109</v>
@@ -12187,18 +12129,14 @@
       <c r="B685" s="0" t="s">
         <v>1111</v>
       </c>
-      <c r="H685" s="4" t="s">
+      <c r="H685" s="10" t="s">
         <v>1112</v>
       </c>
-      <c r="I685" s="6" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J685" s="4"/>
-      <c r="K685" s="6"/>
+      <c r="J685" s="10"/>
     </row>
     <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="0" t="s">
-        <v>751</v>
+        <v>987</v>
       </c>
       <c r="B686" s="0" t="s">
         <v>1113</v>
@@ -12206,27 +12144,31 @@
       <c r="H686" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="I686" s="4" t="s">
-        <v>789</v>
+      <c r="I686" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J686" s="4"/>
-      <c r="K686" s="4"/>
+      <c r="K686" s="6"/>
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="0" t="s">
-        <v>751</v>
+        <v>821</v>
       </c>
       <c r="B687" s="0" t="s">
         <v>1115</v>
       </c>
-      <c r="H687" s="11" t="s">
+      <c r="H687" s="4" t="s">
         <v>1116</v>
       </c>
-      <c r="J687" s="11"/>
+      <c r="I687" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J687" s="4"/>
+      <c r="K687" s="4"/>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="0" t="s">
-        <v>987</v>
+        <v>821</v>
       </c>
       <c r="B688" s="0" t="s">
         <v>1117</v>
@@ -12234,63 +12176,63 @@
       <c r="H688" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="I688" s="6" t="s">
+      <c r="I688" s="4" t="s">
         <v>1034</v>
       </c>
       <c r="J688" s="4"/>
-      <c r="K688" s="6"/>
-    </row>
-    <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A689" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B689" s="0" t="s">
-        <v>1119</v>
-      </c>
-      <c r="H689" s="4" t="s">
-        <v>1120</v>
-      </c>
-      <c r="I689" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J689" s="4"/>
-      <c r="K689" s="4"/>
+      <c r="K688" s="4"/>
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="0" t="s">
-        <v>821</v>
+        <v>1119</v>
       </c>
       <c r="B690" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="H690" s="4" t="s">
         <v>1121</v>
       </c>
-      <c r="H690" s="4" t="s">
+      <c r="I690" s="4" t="s">
         <v>1122</v>
-      </c>
-      <c r="I690" s="4" t="s">
-        <v>1034</v>
       </c>
       <c r="J690" s="4"/>
       <c r="K690" s="4"/>
     </row>
+    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A691" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B691" s="0" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H691" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I691" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J691" s="4"/>
+      <c r="K691" s="4"/>
+    </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="0" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="B692" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="H692" s="4" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="I692" s="4" t="s">
-        <v>1126</v>
+        <v>1034</v>
       </c>
       <c r="J692" s="4"/>
       <c r="K692" s="4"/>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="0" t="s">
-        <v>1123</v>
+        <v>1062</v>
       </c>
       <c r="B693" s="0" t="s">
         <v>1127</v>
@@ -12299,14 +12241,14 @@
         <v>1128</v>
       </c>
       <c r="I693" s="4" t="s">
-        <v>1126</v>
+        <v>1011</v>
       </c>
       <c r="J693" s="4"/>
       <c r="K693" s="4"/>
     </row>
-    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="694" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A694" s="0" t="s">
-        <v>1123</v>
+        <v>1062</v>
       </c>
       <c r="B694" s="0" t="s">
         <v>1129</v>
@@ -12315,14 +12257,14 @@
         <v>1130</v>
       </c>
       <c r="I694" s="4" t="s">
-        <v>1034</v>
+        <v>1011</v>
       </c>
       <c r="J694" s="4"/>
       <c r="K694" s="4"/>
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B695" s="0" t="s">
         <v>1131</v>
@@ -12336,9 +12278,9 @@
       <c r="J695" s="4"/>
       <c r="K695" s="4"/>
     </row>
-    <row r="696" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="0" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B696" s="0" t="s">
         <v>1133</v>
@@ -12354,7 +12296,7 @@
     </row>
     <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A697" s="0" t="s">
-        <v>1066</v>
+        <v>1091</v>
       </c>
       <c r="B697" s="0" t="s">
         <v>1135</v>
@@ -12363,78 +12305,78 @@
         <v>1136</v>
       </c>
       <c r="I697" s="4" t="s">
-        <v>1011</v>
+        <v>1094</v>
       </c>
       <c r="J697" s="4"/>
       <c r="K697" s="4"/>
     </row>
     <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="0" t="s">
-        <v>1066</v>
+        <v>1137</v>
       </c>
       <c r="B698" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="H698" s="4" t="s">
-        <v>1138</v>
-      </c>
-      <c r="I698" s="4" t="s">
-        <v>1011</v>
+        <v>1139</v>
+      </c>
+      <c r="I698" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J698" s="4"/>
-      <c r="K698" s="4"/>
+      <c r="K698" s="6"/>
     </row>
     <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A699" s="0" t="s">
-        <v>1095</v>
+        <v>1137</v>
       </c>
       <c r="B699" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H699" s="4" t="s">
         <v>1139</v>
       </c>
-      <c r="H699" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="I699" s="4" t="s">
-        <v>1098</v>
+      <c r="I699" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J699" s="4"/>
-      <c r="K699" s="4"/>
-    </row>
-    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A700" s="0" t="s">
+      <c r="K699" s="6"/>
+    </row>
+    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A703" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B703" s="0" t="s">
         <v>1141</v>
       </c>
-      <c r="B700" s="0" t="s">
+      <c r="H703" s="4" t="s">
         <v>1142</v>
       </c>
-      <c r="H700" s="4" t="s">
+      <c r="I703" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J703" s="4"/>
+      <c r="K703" s="4"/>
+    </row>
+    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A704" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B704" s="0" t="s">
         <v>1143</v>
       </c>
-      <c r="I700" s="6" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J700" s="4"/>
-      <c r="K700" s="6"/>
-    </row>
-    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A701" s="0" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B701" s="0" t="s">
+      <c r="H704" s="4" t="s">
         <v>1144</v>
       </c>
-      <c r="H701" s="4" t="s">
-        <v>1143</v>
-      </c>
-      <c r="I701" s="6" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J701" s="4"/>
-      <c r="K701" s="6"/>
+      <c r="I704" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="J704" s="4"/>
+      <c r="K704" s="4"/>
     </row>
     <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="0" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="B705" s="0" t="s">
         <v>1145</v>
@@ -12443,14 +12385,14 @@
         <v>1146</v>
       </c>
       <c r="I705" s="4" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="J705" s="4"/>
       <c r="K705" s="4"/>
     </row>
     <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="0" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="B706" s="0" t="s">
         <v>1147</v>
@@ -12459,14 +12401,14 @@
         <v>1148</v>
       </c>
       <c r="I706" s="4" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="J706" s="4"/>
       <c r="K706" s="4"/>
     </row>
     <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A707" s="0" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="B707" s="0" t="s">
         <v>1149</v>
@@ -12475,49 +12417,87 @@
         <v>1150</v>
       </c>
       <c r="I707" s="4" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="J707" s="4"/>
       <c r="K707" s="4"/>
     </row>
-    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A708" s="0" t="s">
-        <v>1123</v>
-      </c>
-      <c r="B708" s="0" t="s">
+    <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A711" s="0" t="s">
+        <v>987</v>
+      </c>
+      <c r="B711" s="0" t="s">
         <v>1151</v>
       </c>
-      <c r="H708" s="4" t="s">
+      <c r="C711" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D711" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E711" s="0" t="s">
         <v>1152</v>
       </c>
-      <c r="I708" s="4" t="s">
-        <v>1126</v>
-      </c>
-      <c r="J708" s="4"/>
-      <c r="K708" s="4"/>
-    </row>
-    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="0" t="s">
-        <v>1123</v>
-      </c>
-      <c r="B709" s="0" t="s">
+      <c r="F711" s="0" t="s">
         <v>1153</v>
       </c>
-      <c r="H709" s="4" t="s">
+      <c r="G711" s="0" t="s">
         <v>1154</v>
       </c>
-      <c r="I709" s="4" t="s">
-        <v>1126</v>
-      </c>
-      <c r="J709" s="4"/>
-      <c r="K709" s="4"/>
+      <c r="H711" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I711" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="J711" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="K711" s="0" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A712" s="0" t="s">
+        <v>987</v>
+      </c>
+      <c r="B712" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C712" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D712" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E712" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F712" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G712" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H712" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="I712" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="J712" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="K712" s="0" t="s">
+        <v>1158</v>
+      </c>
     </row>
     <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="0" t="s">
         <v>987</v>
       </c>
       <c r="B713" s="0" t="s">
-        <v>1155</v>
+        <v>1165</v>
       </c>
       <c r="C713" s="0" t="n">
         <v>1</v>
@@ -12526,25 +12506,25 @@
         <v>612</v>
       </c>
       <c r="E713" s="0" t="s">
-        <v>1156</v>
+        <v>1166</v>
       </c>
       <c r="F713" s="0" t="s">
-        <v>1157</v>
+        <v>1167</v>
       </c>
       <c r="G713" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H713" s="0" t="s">
+        <v>1168</v>
+      </c>
+      <c r="I713" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="J713" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K713" s="0" t="s">
         <v>1158</v>
-      </c>
-      <c r="H713" s="0" t="s">
-        <v>1159</v>
-      </c>
-      <c r="I713" s="0" t="s">
-        <v>1160</v>
-      </c>
-      <c r="J713" s="0" t="s">
-        <v>1161</v>
-      </c>
-      <c r="K713" s="0" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12552,7 +12532,7 @@
         <v>987</v>
       </c>
       <c r="B714" s="0" t="s">
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="C714" s="0" t="n">
         <v>1</v>
@@ -12561,165 +12541,165 @@
         <v>612</v>
       </c>
       <c r="E714" s="0" t="s">
-        <v>1164</v>
+        <v>1172</v>
       </c>
       <c r="F714" s="0" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="G714" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H714" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I714" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="J714" s="0" t="s">
+        <v>1174</v>
+      </c>
+      <c r="K714" s="0" t="s">
         <v>1158</v>
       </c>
-      <c r="H714" s="0" t="s">
-        <v>1166</v>
-      </c>
-      <c r="I714" s="0" t="s">
-        <v>1167</v>
-      </c>
-      <c r="J714" s="0" t="s">
-        <v>1168</v>
-      </c>
-      <c r="K714" s="0" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A715" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B715" s="0" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C715" s="0" t="n">
+    </row>
+    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A718" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B718" s="0" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C718" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D715" s="0" t="s">
+      <c r="D718" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="E718" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F718" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G718" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H718" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I718" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J718" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="K718" s="0" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A719" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B719" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C719" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D719" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E715" s="0" t="s">
-        <v>1170</v>
-      </c>
-      <c r="F715" s="0" t="s">
-        <v>1171</v>
-      </c>
-      <c r="G715" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H715" s="0" t="s">
-        <v>1172</v>
-      </c>
-      <c r="I715" s="0" t="s">
-        <v>1173</v>
-      </c>
-      <c r="J715" s="0" t="s">
-        <v>1174</v>
-      </c>
-      <c r="K715" s="0" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A716" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B716" s="0" t="s">
-        <v>1175</v>
-      </c>
-      <c r="C716" s="0" t="n">
+      <c r="E719" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F719" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G719" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H719" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I719" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J719" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="K719" s="0" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A723" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B723" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C723" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D716" s="0" t="s">
+      <c r="D723" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E716" s="0" t="s">
-        <v>1176</v>
-      </c>
-      <c r="F716" s="0" t="s">
-        <v>1171</v>
-      </c>
-      <c r="G716" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H716" s="0" t="s">
-        <v>1177</v>
-      </c>
-      <c r="I716" s="0" t="s">
-        <v>1173</v>
-      </c>
-      <c r="J716" s="0" t="s">
-        <v>1178</v>
-      </c>
-      <c r="K716" s="0" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A720" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B720" s="0" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C720" s="0" t="n">
+      <c r="E723" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F723" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G723" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H723" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I723" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J723" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="K723" s="0" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A724" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B724" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C724" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D724" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E724" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F724" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D720" s="0" t="s">
-        <v>621</v>
-      </c>
-      <c r="E720" s="0" t="s">
-        <v>1180</v>
-      </c>
-      <c r="F720" s="0" t="s">
-        <v>1181</v>
-      </c>
-      <c r="G720" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H720" s="0" t="s">
-        <v>1182</v>
-      </c>
-      <c r="I720" s="0" t="s">
-        <v>1183</v>
-      </c>
-      <c r="J720" s="0" t="s">
-        <v>1184</v>
-      </c>
-      <c r="K720" s="0" t="s">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A721" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B721" s="0" t="s">
-        <v>1186</v>
-      </c>
-      <c r="C721" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D721" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E721" s="0" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F721" s="0" t="s">
-        <v>1188</v>
-      </c>
-      <c r="G721" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H721" s="0" t="s">
-        <v>1182</v>
-      </c>
-      <c r="I721" s="0" t="s">
-        <v>1183</v>
-      </c>
-      <c r="J721" s="0" t="s">
-        <v>1189</v>
-      </c>
-      <c r="K721" s="0" t="s">
-        <v>1185</v>
+      <c r="G724" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H724" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="I724" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J724" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="K724" s="0" t="s">
+        <v>1190</v>
       </c>
     </row>
     <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12727,7 +12707,7 @@
         <v>590</v>
       </c>
       <c r="B725" s="0" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="C725" s="0" t="n">
         <v>1</v>
@@ -12736,25 +12716,25 @@
         <v>612</v>
       </c>
       <c r="E725" s="0" t="s">
-        <v>1190</v>
+        <v>1194</v>
       </c>
       <c r="F725" s="0" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="G725" s="0" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="H725" s="0" t="s">
-        <v>1192</v>
+        <v>1195</v>
       </c>
       <c r="I725" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J725" s="0" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="K725" s="0" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12762,34 +12742,34 @@
         <v>590</v>
       </c>
       <c r="B726" s="0" t="s">
-        <v>386</v>
+        <v>218</v>
       </c>
       <c r="C726" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D726" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E726" s="0" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F726" s="0" t="n">
-        <v>1</v>
+        <v>1197</v>
+      </c>
+      <c r="F726" s="0" t="s">
+        <v>1198</v>
       </c>
       <c r="G726" s="0" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="H726" s="0" t="s">
-        <v>1196</v>
+        <v>218</v>
       </c>
       <c r="I726" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J726" s="0" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="K726" s="0" t="s">
-        <v>1194</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12797,34 +12777,34 @@
         <v>590</v>
       </c>
       <c r="B727" s="0" t="s">
-        <v>410</v>
+        <v>225</v>
       </c>
       <c r="C727" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D727" s="0" t="s">
-        <v>612</v>
+        <v>1201</v>
       </c>
       <c r="E727" s="0" t="s">
-        <v>1198</v>
+        <v>1202</v>
       </c>
       <c r="F727" s="0" t="s">
-        <v>1191</v>
+        <v>1203</v>
       </c>
       <c r="G727" s="0" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="H727" s="0" t="s">
-        <v>1199</v>
+        <v>1204</v>
       </c>
       <c r="I727" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J727" s="0" t="s">
-        <v>1200</v>
+        <v>1205</v>
       </c>
       <c r="K727" s="0" t="s">
-        <v>1194</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12832,34 +12812,34 @@
         <v>590</v>
       </c>
       <c r="B728" s="0" t="s">
-        <v>218</v>
+        <v>345</v>
       </c>
       <c r="C728" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D728" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E728" s="0" t="s">
-        <v>1201</v>
+        <v>1207</v>
       </c>
       <c r="F728" s="0" t="s">
-        <v>1202</v>
+        <v>1208</v>
       </c>
       <c r="G728" s="0" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="H728" s="0" t="s">
-        <v>218</v>
+        <v>1209</v>
       </c>
       <c r="I728" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J728" s="0" t="s">
-        <v>1203</v>
+        <v>1210</v>
       </c>
       <c r="K728" s="0" t="s">
-        <v>1204</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12867,307 +12847,239 @@
         <v>590</v>
       </c>
       <c r="B729" s="0" t="s">
-        <v>225</v>
+        <v>339</v>
       </c>
       <c r="C729" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D729" s="0" t="s">
-        <v>1205</v>
+        <v>612</v>
       </c>
       <c r="E729" s="0" t="s">
-        <v>1206</v>
+        <v>1212</v>
       </c>
       <c r="F729" s="0" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="G729" s="0" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="H729" s="0" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="I729" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J729" s="0" t="s">
-        <v>1209</v>
+        <v>1213</v>
       </c>
       <c r="K729" s="0" t="s">
-        <v>1210</v>
-      </c>
-    </row>
-    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A730" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B730" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C730" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D730" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E730" s="0" t="s">
         <v>1211</v>
-      </c>
-      <c r="F730" s="0" t="s">
-        <v>1212</v>
-      </c>
-      <c r="G730" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H730" s="0" t="s">
-        <v>1213</v>
-      </c>
-      <c r="I730" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J730" s="0" t="s">
-        <v>1214</v>
-      </c>
-      <c r="K730" s="0" t="s">
-        <v>1215</v>
       </c>
     </row>
     <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="0" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B731" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C731" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D731" s="0" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E731" s="0" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F731" s="0" t="s">
+        <v>1203</v>
+      </c>
+      <c r="G731" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H731" s="0" t="s">
+        <v>1204</v>
+      </c>
+      <c r="I731" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="J731" s="0" t="s">
+        <v>1205</v>
+      </c>
+      <c r="K731" s="0" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A734" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B731" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C731" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D731" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E731" s="0" t="s">
-        <v>1216</v>
-      </c>
-      <c r="F731" s="0" t="s">
-        <v>1212</v>
-      </c>
-      <c r="G731" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H731" s="0" t="s">
-        <v>1213</v>
-      </c>
-      <c r="I731" s="0" t="s">
+      <c r="B734" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C734" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D734" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E734" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F734" s="0" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G734" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H734" s="0" t="s">
+        <v>1222</v>
+      </c>
+      <c r="I734" s="0" t="s">
         <v>585</v>
       </c>
-      <c r="J731" s="0" t="s">
-        <v>1217</v>
-      </c>
-      <c r="K731" s="0" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A733" s="0" t="s">
-        <v>1218</v>
-      </c>
-      <c r="B733" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C733" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D733" s="0" t="s">
-        <v>1219</v>
-      </c>
-      <c r="E733" s="0" t="s">
-        <v>1206</v>
-      </c>
-      <c r="F733" s="0" t="s">
-        <v>1207</v>
-      </c>
-      <c r="G733" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H733" s="0" t="s">
-        <v>1208</v>
-      </c>
-      <c r="I733" s="0" t="s">
-        <v>1220</v>
-      </c>
-      <c r="J733" s="0" t="s">
-        <v>1209</v>
-      </c>
-      <c r="K733" s="0" t="s">
-        <v>1221</v>
+      <c r="J734" s="0" t="s">
+        <v>1223</v>
+      </c>
+      <c r="K734" s="0" t="s">
+        <v>1190</v>
       </c>
     </row>
     <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="0" t="s">
-        <v>590</v>
+        <v>1224</v>
       </c>
       <c r="B736" s="0" t="s">
-        <v>1222</v>
+        <v>1225</v>
       </c>
       <c r="C736" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D736" s="0" t="s">
-        <v>1223</v>
+        <v>1201</v>
       </c>
       <c r="E736" s="0" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="F736" s="0" t="s">
-        <v>1225</v>
+        <v>1187</v>
       </c>
       <c r="G736" s="0" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="H736" s="0" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="I736" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J736" s="0" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="K736" s="0" t="s">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A738" s="0" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B738" s="0" t="s">
         <v>1229</v>
       </c>
-      <c r="C738" s="0" t="n">
+    </row>
+    <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A737" s="0" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B737" s="0" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C737" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D738" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="E738" s="0" t="s">
-        <v>1230</v>
-      </c>
-      <c r="F738" s="0" t="s">
-        <v>1191</v>
-      </c>
-      <c r="G738" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H738" s="0" t="s">
+      <c r="D737" s="0" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E737" s="0" t="s">
         <v>1231</v>
       </c>
-      <c r="I738" s="0" t="s">
+      <c r="F737" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G737" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H737" s="0" t="s">
+        <v>1232</v>
+      </c>
+      <c r="I737" s="0" t="s">
         <v>585</v>
       </c>
-      <c r="J738" s="0" t="s">
-        <v>1232</v>
-      </c>
-      <c r="K738" s="0" t="s">
+      <c r="J737" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="K737" s="0" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B740" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="H740" s="12" t="s">
         <v>1233</v>
       </c>
-    </row>
-    <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A739" s="0" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B739" s="0" t="s">
+      <c r="I740" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B741" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="H741" s="12" t="s">
         <v>1234</v>
       </c>
-      <c r="C739" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D739" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="E739" s="0" t="s">
+      <c r="I741" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B742" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H742" s="13" t="s">
         <v>1235</v>
       </c>
-      <c r="F739" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G739" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="H739" s="0" t="s">
+      <c r="I742" s="0" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A743" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B743" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="H743" s="13" t="s">
         <v>1236</v>
       </c>
-      <c r="I739" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J739" s="0" t="s">
-        <v>1197</v>
-      </c>
-      <c r="K739" s="0" t="s">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B742" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="H742" s="13" t="s">
+      <c r="I743" s="0" t="s">
         <v>1237</v>
       </c>
-      <c r="I742" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B743" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="H743" s="13" t="s">
+    </row>
+    <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A744" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B744" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="H744" s="13" t="s">
         <v>1238</v>
       </c>
-      <c r="I743" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B744" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H744" s="14" t="s">
-        <v>1239</v>
-      </c>
       <c r="I744" s="0" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A745" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B745" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="H745" s="14" t="s">
-        <v>1240</v>
-      </c>
-      <c r="I745" s="0" t="s">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A746" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B746" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="H746" s="14" t="s">
-        <v>1242</v>
-      </c>
-      <c r="I746" s="0" t="s">
-        <v>1241</v>
-      </c>
-    </row>
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Move the variables spco2nat, dissicnat and phnat from the pre identified missing to the ignored file because the will be only manually added for OMIP #381.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="1224">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3767,51 +3767,6 @@
   </si>
   <si>
     <t xml:space="preserve">CMIP,FAFMIP,HighResMIP,LUMIP,RFMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spco2nat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time depth0m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural Surface Aqueous Partial Pressure of CO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pCO2sea (in uatm) in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings  are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The surface called 'surface' means the lower boundary of the atmosphere. The chemical formula for carbon dioxide is CO2. In ocean biogeochemistry models, a 'natural analogue' is used to simulate the effect on a modelled variable of imposing preindustrial atmospheric carbon dioxide concentrations, even when the model as a whole may be subjected to varying forcings. The partial pressure of a gaseous constituent of air is the pressure which it alone would exert with unchanged temperature and number of moles per unit volume. The partial pressure of a dissolved gas in sea water is the partial pressure in air with which it would be in equilibrium. The partial pressure difference between sea water and air is positive when the partial pressure of the dissolved gas in sea water is greater than the partial pressure in air.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oyr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dissicnat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural Dissolved Inorganic Carbon Concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIC_E3T/e3t in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings  are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolved inorganic carbon (CO3+HCO3+H2CO3) concentration at preindustrial atmospheric xCO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CMIP,GeoMIP,LUMIP,OMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phnat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH in simulation where ocean biogeochemistry sees preindustrial atmospheric pCO2 but initial conditions and forcings  are identical to historical. This variable will be delivered for OMIP but seems unlikely to be delivered for C4MIP. This is because it requires running twice simulations.</t>
   </si>
   <si>
     <t xml:space="preserve">Available in PISCES: EXPC * (16/122). Not available inLPJ-GUESS.</t>
@@ -4130,8 +4085,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A630" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A645" activeCellId="0" sqref="A645"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A718" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A732" activeCellId="0" sqref="A732"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12913,171 +12868,72 @@
       </c>
     </row>
     <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A734" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B734" s="0" t="s">
+      <c r="B734" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="H734" s="12" t="s">
         <v>1218</v>
       </c>
-      <c r="C734" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D734" s="0" t="s">
+      <c r="I734" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B735" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="H735" s="12" t="s">
         <v>1219</v>
       </c>
-      <c r="E734" s="0" t="s">
+      <c r="I735" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B736" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H736" s="13" t="s">
         <v>1220</v>
-      </c>
-      <c r="F734" s="0" t="s">
-        <v>1221</v>
-      </c>
-      <c r="G734" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H734" s="0" t="s">
-        <v>1222</v>
-      </c>
-      <c r="I734" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J734" s="0" t="s">
-        <v>1223</v>
-      </c>
-      <c r="K734" s="0" t="s">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A736" s="0" t="s">
-        <v>1224</v>
-      </c>
-      <c r="B736" s="0" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C736" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D736" s="0" t="s">
-        <v>1201</v>
-      </c>
-      <c r="E736" s="0" t="s">
-        <v>1226</v>
-      </c>
-      <c r="F736" s="0" t="s">
-        <v>1187</v>
-      </c>
-      <c r="G736" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H736" s="0" t="s">
-        <v>1227</v>
       </c>
       <c r="I736" s="0" t="s">
         <v>585</v>
       </c>
-      <c r="J736" s="0" t="s">
-        <v>1228</v>
-      </c>
-      <c r="K736" s="0" t="s">
-        <v>1229</v>
-      </c>
     </row>
     <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="0" t="s">
-        <v>1224</v>
+        <v>590</v>
       </c>
       <c r="B737" s="0" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C737" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D737" s="0" t="s">
-        <v>1201</v>
-      </c>
-      <c r="E737" s="0" t="s">
-        <v>1231</v>
-      </c>
-      <c r="F737" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G737" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H737" s="0" t="s">
-        <v>1232</v>
+        <v>334</v>
+      </c>
+      <c r="H737" s="13" t="s">
+        <v>1221</v>
       </c>
       <c r="I737" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J737" s="0" t="s">
-        <v>1193</v>
-      </c>
-      <c r="K737" s="0" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B740" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="H740" s="12" t="s">
-        <v>1233</v>
-      </c>
-      <c r="I740" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B741" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="H741" s="12" t="s">
-        <v>1234</v>
-      </c>
-      <c r="I741" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B742" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H742" s="13" t="s">
-        <v>1235</v>
-      </c>
-      <c r="I742" s="0" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A743" s="0" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A738" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B743" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="H743" s="13" t="s">
-        <v>1236</v>
-      </c>
-      <c r="I743" s="0" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B744" s="0" t="s">
+      <c r="B738" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="H744" s="13" t="s">
-        <v>1238</v>
-      </c>
-      <c r="I744" s="0" t="s">
-        <v>1237</v>
-      </c>
-    </row>
+      <c r="H738" s="13" t="s">
+        <v>1223</v>
+      </c>
+      <c r="I738" s="0" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Move the variables rsutcsaf, rsdscsaf and rsuscsaf from the pre identified missing to the ignored file, these are variables which finally have been identified in the PEXTRA list (see shared PEXTRA overview) #143 #368 #346.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="1224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="1220">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3242,18 +3242,6 @@
   </si>
   <si>
     <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #403   aerosol free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsutcsaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsdscsaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsuscsaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #405</t>
   </si>
   <si>
     <t xml:space="preserve">LImon</t>
@@ -4085,8 +4073,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A718" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A732" activeCellId="0" sqref="A732"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A641" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A657" activeCellId="0" sqref="A657"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11658,63 +11646,64 @@
       <c r="J656" s="4"/>
       <c r="K656" s="4"/>
     </row>
-    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A657" s="0" t="s">
-        <v>751</v>
-      </c>
-      <c r="B657" s="0" t="s">
-        <v>1058</v>
-      </c>
-      <c r="H657" s="4" t="s">
-        <v>1057</v>
-      </c>
-      <c r="I657" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="J657" s="4"/>
-      <c r="K657" s="4"/>
-    </row>
-    <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A658" s="0" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B658" s="0" t="s">
-        <v>1059</v>
-      </c>
-      <c r="H658" s="4" t="s">
-        <v>1055</v>
-      </c>
-      <c r="I658" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="J658" s="4"/>
-      <c r="K658" s="4"/>
-    </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>1031</v>
+        <v>1058</v>
       </c>
       <c r="B659" s="0" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H659" s="4" t="s">
         <v>1060</v>
       </c>
-      <c r="H659" s="4" t="s">
-        <v>1061</v>
-      </c>
       <c r="I659" s="4" t="s">
-        <v>789</v>
+        <v>1011</v>
       </c>
       <c r="J659" s="4"/>
       <c r="K659" s="4"/>
     </row>
+    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A660" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B660" s="0" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H660" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="I660" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J660" s="4"/>
+      <c r="K660" s="4"/>
+      <c r="L660" s="4"/>
+    </row>
+    <row r="661" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A661" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B661" s="0" t="s">
+        <v>1063</v>
+      </c>
+      <c r="H661" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I661" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J661" s="4"/>
+      <c r="K661" s="4"/>
+    </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B662" s="0" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="H662" s="4" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="I662" s="4" t="s">
         <v>1011</v>
@@ -11724,30 +11713,29 @@
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B663" s="0" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="H663" s="4" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="I663" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J663" s="4"/>
       <c r="K663" s="4"/>
-      <c r="L663" s="4"/>
-    </row>
-    <row r="664" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B664" s="0" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="H664" s="4" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="I664" s="4" t="s">
         <v>1011</v>
@@ -11757,13 +11745,13 @@
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B665" s="0" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="H665" s="4" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="I665" s="4" t="s">
         <v>1011</v>
@@ -11773,29 +11761,30 @@
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B666" s="0" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="H666" s="4" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="I666" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J666" s="4"/>
       <c r="K666" s="4"/>
+      <c r="L666" s="4"/>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B667" s="0" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="H667" s="4" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="I667" s="4" t="s">
         <v>1011</v>
@@ -11805,13 +11794,13 @@
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B668" s="0" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="H668" s="4" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="I668" s="4" t="s">
         <v>1011</v>
@@ -11821,46 +11810,46 @@
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B669" s="0" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="H669" s="4" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="I669" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J669" s="4"/>
       <c r="K669" s="4"/>
-      <c r="L669" s="4"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B670" s="0" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="H670" s="4" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="I670" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J670" s="4"/>
       <c r="K670" s="4"/>
+      <c r="L670" s="4"/>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B671" s="0" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="H671" s="4" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="I671" s="4" t="s">
         <v>1011</v>
@@ -11870,13 +11859,13 @@
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B672" s="0" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="H672" s="4" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="I672" s="4" t="s">
         <v>1011</v>
@@ -11886,142 +11875,141 @@
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
-        <v>1062</v>
+        <v>1087</v>
       </c>
       <c r="B673" s="0" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
       <c r="H673" s="4" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
       <c r="I673" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J673" s="4"/>
       <c r="K673" s="4"/>
-      <c r="L673" s="4"/>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>1062</v>
+        <v>1087</v>
       </c>
       <c r="B674" s="0" t="s">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c r="H674" s="4" t="s">
-        <v>1088</v>
+        <v>1092</v>
       </c>
       <c r="I674" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J674" s="4"/>
       <c r="K674" s="4"/>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="0" t="s">
-        <v>1062</v>
+        <v>1087</v>
       </c>
       <c r="B675" s="0" t="s">
-        <v>1089</v>
+        <v>1093</v>
       </c>
       <c r="H675" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I675" s="4" t="s">
         <v>1090</v>
-      </c>
-      <c r="I675" s="4" t="s">
-        <v>1011</v>
       </c>
       <c r="J675" s="4"/>
       <c r="K675" s="4"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="0" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="B676" s="0" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="H676" s="4" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
       <c r="I676" s="4" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="J676" s="4"/>
       <c r="K676" s="4"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="H677" s="4" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="I677" s="4" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="J677" s="4"/>
       <c r="K677" s="4"/>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B678" s="0" t="s">
         <v>1091</v>
       </c>
-      <c r="B678" s="0" t="s">
-        <v>1097</v>
-      </c>
       <c r="H678" s="4" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="I678" s="4" t="s">
-        <v>1094</v>
+        <v>789</v>
       </c>
       <c r="J678" s="4"/>
       <c r="K678" s="4"/>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="0" t="s">
-        <v>1091</v>
+        <v>1100</v>
       </c>
       <c r="B679" s="0" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="H679" s="4" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="I679" s="4" t="s">
-        <v>1094</v>
+        <v>789</v>
       </c>
       <c r="J679" s="4"/>
       <c r="K679" s="4"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>1091</v>
+        <v>751</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="H680" s="4" t="s">
-        <v>1102</v>
-      </c>
-      <c r="I680" s="4" t="s">
-        <v>1094</v>
+        <v>1104</v>
+      </c>
+      <c r="I680" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J680" s="4"/>
-      <c r="K680" s="4"/>
+      <c r="K680" s="6"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
-        <v>1103</v>
+        <v>751</v>
       </c>
       <c r="B681" s="0" t="s">
-        <v>1095</v>
+        <v>1105</v>
       </c>
       <c r="H681" s="4" t="s">
-        <v>1096</v>
+        <v>1106</v>
       </c>
       <c r="I681" s="4" t="s">
         <v>789</v>
@@ -12031,29 +12019,25 @@
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="0" t="s">
-        <v>1104</v>
+        <v>751</v>
       </c>
       <c r="B682" s="0" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H682" s="4" t="s">
-        <v>1106</v>
-      </c>
-      <c r="I682" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="J682" s="4"/>
-      <c r="K682" s="4"/>
+        <v>1107</v>
+      </c>
+      <c r="H682" s="10" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J682" s="10"/>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
-        <v>751</v>
+        <v>987</v>
       </c>
       <c r="B683" s="0" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="H683" s="4" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="I683" s="6" t="s">
         <v>1034</v>
@@ -12063,137 +12047,141 @@
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="0" t="s">
-        <v>751</v>
+        <v>821</v>
       </c>
       <c r="B684" s="0" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="H684" s="4" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="I684" s="4" t="s">
-        <v>789</v>
+        <v>1034</v>
       </c>
       <c r="J684" s="4"/>
       <c r="K684" s="4"/>
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="0" t="s">
-        <v>751</v>
+        <v>821</v>
       </c>
       <c r="B685" s="0" t="s">
-        <v>1111</v>
-      </c>
-      <c r="H685" s="10" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J685" s="10"/>
-    </row>
-    <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A686" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B686" s="0" t="s">
         <v>1113</v>
       </c>
-      <c r="H686" s="4" t="s">
+      <c r="H685" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="I686" s="6" t="s">
+      <c r="I685" s="4" t="s">
         <v>1034</v>
       </c>
-      <c r="J686" s="4"/>
-      <c r="K686" s="6"/>
+      <c r="J685" s="4"/>
+      <c r="K685" s="4"/>
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="0" t="s">
-        <v>821</v>
+        <v>1115</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="H687" s="4" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="I687" s="4" t="s">
-        <v>1034</v>
+        <v>1118</v>
       </c>
       <c r="J687" s="4"/>
       <c r="K687" s="4"/>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="0" t="s">
-        <v>821</v>
+        <v>1115</v>
       </c>
       <c r="B688" s="0" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="H688" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I688" s="4" t="s">
         <v>1118</v>
-      </c>
-      <c r="I688" s="4" t="s">
-        <v>1034</v>
       </c>
       <c r="J688" s="4"/>
       <c r="K688" s="4"/>
     </row>
+    <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A689" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B689" s="0" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H689" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="I689" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J689" s="4"/>
+      <c r="K689" s="4"/>
+    </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="0" t="s">
-        <v>1119</v>
+        <v>1058</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>1120</v>
+        <v>1123</v>
       </c>
       <c r="H690" s="4" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
       <c r="I690" s="4" t="s">
-        <v>1122</v>
+        <v>1011</v>
       </c>
       <c r="J690" s="4"/>
       <c r="K690" s="4"/>
     </row>
-    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="691" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="0" t="s">
-        <v>1119</v>
+        <v>1058</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="H691" s="4" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="I691" s="4" t="s">
-        <v>1122</v>
+        <v>1011</v>
       </c>
       <c r="J691" s="4"/>
       <c r="K691" s="4"/>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="0" t="s">
-        <v>1119</v>
+        <v>1058</v>
       </c>
       <c r="B692" s="0" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="H692" s="4" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="I692" s="4" t="s">
-        <v>1034</v>
+        <v>1011</v>
       </c>
       <c r="J692" s="4"/>
       <c r="K692" s="4"/>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="0" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B693" s="0" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="H693" s="4" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="I693" s="4" t="s">
         <v>1011</v>
@@ -12201,188 +12189,245 @@
       <c r="J693" s="4"/>
       <c r="K693" s="4"/>
     </row>
-    <row r="694" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A694" s="0" t="s">
-        <v>1062</v>
+        <v>1087</v>
       </c>
       <c r="B694" s="0" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="H694" s="4" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="I694" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J694" s="4"/>
       <c r="K694" s="4"/>
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="0" t="s">
-        <v>1062</v>
+        <v>1133</v>
       </c>
       <c r="B695" s="0" t="s">
-        <v>1131</v>
+        <v>1134</v>
       </c>
       <c r="H695" s="4" t="s">
-        <v>1132</v>
-      </c>
-      <c r="I695" s="4" t="s">
-        <v>1011</v>
+        <v>1135</v>
+      </c>
+      <c r="I695" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J695" s="4"/>
-      <c r="K695" s="4"/>
+      <c r="K695" s="6"/>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="0" t="s">
-        <v>1062</v>
+        <v>1133</v>
       </c>
       <c r="B696" s="0" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="H696" s="4" t="s">
-        <v>1134</v>
-      </c>
-      <c r="I696" s="4" t="s">
-        <v>1011</v>
+        <v>1135</v>
+      </c>
+      <c r="I696" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J696" s="4"/>
-      <c r="K696" s="4"/>
-    </row>
-    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A697" s="0" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B697" s="0" t="s">
-        <v>1135</v>
-      </c>
-      <c r="H697" s="4" t="s">
-        <v>1136</v>
-      </c>
-      <c r="I697" s="4" t="s">
-        <v>1094</v>
-      </c>
-      <c r="J697" s="4"/>
-      <c r="K697" s="4"/>
-    </row>
-    <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A698" s="0" t="s">
+      <c r="K696" s="6"/>
+    </row>
+    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A700" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B700" s="0" t="s">
         <v>1137</v>
       </c>
-      <c r="B698" s="0" t="s">
+      <c r="H700" s="4" t="s">
         <v>1138</v>
       </c>
-      <c r="H698" s="4" t="s">
+      <c r="I700" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J700" s="4"/>
+      <c r="K700" s="4"/>
+    </row>
+    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A701" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B701" s="0" t="s">
         <v>1139</v>
       </c>
-      <c r="I698" s="6" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J698" s="4"/>
-      <c r="K698" s="6"/>
-    </row>
-    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A699" s="0" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B699" s="0" t="s">
+      <c r="H701" s="4" t="s">
         <v>1140</v>
       </c>
-      <c r="H699" s="4" t="s">
-        <v>1139</v>
-      </c>
-      <c r="I699" s="6" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J699" s="4"/>
-      <c r="K699" s="6"/>
+      <c r="I701" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J701" s="4"/>
+      <c r="K701" s="4"/>
+    </row>
+    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A702" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B702" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H702" s="4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I702" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J702" s="4"/>
+      <c r="K702" s="4"/>
     </row>
     <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="0" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="B703" s="0" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="H703" s="4" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="I703" s="4" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="J703" s="4"/>
       <c r="K703" s="4"/>
     </row>
     <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="0" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="B704" s="0" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="H704" s="4" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="I704" s="4" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="J704" s="4"/>
       <c r="K704" s="4"/>
     </row>
-    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A705" s="0" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B705" s="0" t="s">
-        <v>1145</v>
-      </c>
-      <c r="H705" s="4" t="s">
-        <v>1146</v>
-      </c>
-      <c r="I705" s="4" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J705" s="4"/>
-      <c r="K705" s="4"/>
-    </row>
-    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A706" s="0" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B706" s="0" t="s">
+    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A708" s="0" t="s">
+        <v>987</v>
+      </c>
+      <c r="B708" s="0" t="s">
         <v>1147</v>
       </c>
-      <c r="H706" s="4" t="s">
+      <c r="C708" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D708" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E708" s="0" t="s">
         <v>1148</v>
       </c>
-      <c r="I706" s="4" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J706" s="4"/>
-      <c r="K706" s="4"/>
-    </row>
-    <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A707" s="0" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B707" s="0" t="s">
+      <c r="F708" s="0" t="s">
         <v>1149</v>
       </c>
-      <c r="H707" s="4" t="s">
+      <c r="G708" s="0" t="s">
         <v>1150</v>
       </c>
-      <c r="I707" s="4" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J707" s="4"/>
-      <c r="K707" s="4"/>
+      <c r="H708" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I708" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="J708" s="0" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K708" s="0" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A709" s="0" t="s">
+        <v>987</v>
+      </c>
+      <c r="B709" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C709" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D709" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E709" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F709" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G709" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H709" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="I709" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="J709" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="K709" s="0" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A710" s="0" t="s">
+        <v>987</v>
+      </c>
+      <c r="B710" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C710" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D710" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E710" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F710" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G710" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H710" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="I710" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J710" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="K710" s="0" t="s">
+        <v>1154</v>
+      </c>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A711" s="0" t="s">
         <v>987</v>
       </c>
       <c r="B711" s="0" t="s">
-        <v>1151</v>
+        <v>1167</v>
       </c>
       <c r="C711" s="0" t="n">
         <v>1</v>
@@ -12391,200 +12436,200 @@
         <v>612</v>
       </c>
       <c r="E711" s="0" t="s">
-        <v>1152</v>
+        <v>1168</v>
       </c>
       <c r="F711" s="0" t="s">
-        <v>1153</v>
+        <v>1163</v>
       </c>
       <c r="G711" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H711" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I711" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J711" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K711" s="0" t="s">
         <v>1154</v>
       </c>
-      <c r="H711" s="0" t="s">
-        <v>1155</v>
-      </c>
-      <c r="I711" s="0" t="s">
-        <v>1156</v>
-      </c>
-      <c r="J711" s="0" t="s">
-        <v>1157</v>
-      </c>
-      <c r="K711" s="0" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A712" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B712" s="0" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C712" s="0" t="n">
+    </row>
+    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A715" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B715" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C715" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D712" s="0" t="s">
+      <c r="D715" s="0" t="s">
+        <v>621</v>
+      </c>
+      <c r="E715" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F715" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G715" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H715" s="0" t="s">
+        <v>1174</v>
+      </c>
+      <c r="I715" s="0" t="s">
+        <v>1175</v>
+      </c>
+      <c r="J715" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="K715" s="0" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A716" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B716" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C716" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D716" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E712" s="0" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F712" s="0" t="s">
-        <v>1161</v>
-      </c>
-      <c r="G712" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H712" s="0" t="s">
-        <v>1162</v>
-      </c>
-      <c r="I712" s="0" t="s">
-        <v>1163</v>
-      </c>
-      <c r="J712" s="0" t="s">
-        <v>1164</v>
-      </c>
-      <c r="K712" s="0" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A713" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B713" s="0" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C713" s="0" t="n">
+      <c r="E716" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F716" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G716" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H716" s="0" t="s">
+        <v>1174</v>
+      </c>
+      <c r="I716" s="0" t="s">
+        <v>1175</v>
+      </c>
+      <c r="J716" s="0" t="s">
+        <v>1181</v>
+      </c>
+      <c r="K716" s="0" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A720" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B720" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C720" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D713" s="0" t="s">
+      <c r="D720" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E713" s="0" t="s">
-        <v>1166</v>
-      </c>
-      <c r="F713" s="0" t="s">
-        <v>1167</v>
-      </c>
-      <c r="G713" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H713" s="0" t="s">
-        <v>1168</v>
-      </c>
-      <c r="I713" s="0" t="s">
-        <v>1169</v>
-      </c>
-      <c r="J713" s="0" t="s">
-        <v>1170</v>
-      </c>
-      <c r="K713" s="0" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A714" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B714" s="0" t="s">
-        <v>1171</v>
-      </c>
-      <c r="C714" s="0" t="n">
+      <c r="E720" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F720" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G720" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H720" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="I720" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J720" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="K720" s="0" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A721" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B721" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C721" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D721" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E721" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F721" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D714" s="0" t="s">
+      <c r="G721" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H721" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I721" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J721" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="K721" s="0" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A722" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B722" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C722" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D722" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E714" s="0" t="s">
-        <v>1172</v>
-      </c>
-      <c r="F714" s="0" t="s">
-        <v>1167</v>
-      </c>
-      <c r="G714" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H714" s="0" t="s">
-        <v>1173</v>
-      </c>
-      <c r="I714" s="0" t="s">
-        <v>1169</v>
-      </c>
-      <c r="J714" s="0" t="s">
-        <v>1174</v>
-      </c>
-      <c r="K714" s="0" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A718" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B718" s="0" t="s">
-        <v>1175</v>
-      </c>
-      <c r="C718" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D718" s="0" t="s">
-        <v>621</v>
-      </c>
-      <c r="E718" s="0" t="s">
-        <v>1176</v>
-      </c>
-      <c r="F718" s="0" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G718" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H718" s="0" t="s">
-        <v>1178</v>
-      </c>
-      <c r="I718" s="0" t="s">
-        <v>1179</v>
-      </c>
-      <c r="J718" s="0" t="s">
-        <v>1180</v>
-      </c>
-      <c r="K718" s="0" t="s">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A719" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B719" s="0" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C719" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D719" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E719" s="0" t="s">
+      <c r="E722" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F722" s="0" t="s">
         <v>1183</v>
       </c>
-      <c r="F719" s="0" t="s">
-        <v>1184</v>
-      </c>
-      <c r="G719" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H719" s="0" t="s">
-        <v>1178</v>
-      </c>
-      <c r="I719" s="0" t="s">
-        <v>1179</v>
-      </c>
-      <c r="J719" s="0" t="s">
-        <v>1185</v>
-      </c>
-      <c r="K719" s="0" t="s">
-        <v>1181</v>
+      <c r="G722" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H722" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I722" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J722" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K722" s="0" t="s">
+        <v>1186</v>
       </c>
     </row>
     <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12592,7 +12637,7 @@
         <v>590</v>
       </c>
       <c r="B723" s="0" t="s">
-        <v>432</v>
+        <v>218</v>
       </c>
       <c r="C723" s="0" t="n">
         <v>1</v>
@@ -12601,25 +12646,25 @@
         <v>612</v>
       </c>
       <c r="E723" s="0" t="s">
-        <v>1186</v>
+        <v>1193</v>
       </c>
       <c r="F723" s="0" t="s">
-        <v>1187</v>
+        <v>1194</v>
       </c>
       <c r="G723" s="0" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="H723" s="0" t="s">
-        <v>1188</v>
+        <v>218</v>
       </c>
       <c r="I723" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J723" s="0" t="s">
-        <v>1189</v>
+        <v>1195</v>
       </c>
       <c r="K723" s="0" t="s">
-        <v>1190</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12627,34 +12672,34 @@
         <v>590</v>
       </c>
       <c r="B724" s="0" t="s">
-        <v>386</v>
+        <v>225</v>
       </c>
       <c r="C724" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D724" s="0" t="s">
-        <v>612</v>
+        <v>1197</v>
       </c>
       <c r="E724" s="0" t="s">
-        <v>1191</v>
-      </c>
-      <c r="F724" s="0" t="n">
-        <v>1</v>
+        <v>1198</v>
+      </c>
+      <c r="F724" s="0" t="s">
+        <v>1199</v>
       </c>
       <c r="G724" s="0" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="H724" s="0" t="s">
-        <v>1192</v>
+        <v>1200</v>
       </c>
       <c r="I724" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J724" s="0" t="s">
-        <v>1193</v>
+        <v>1201</v>
       </c>
       <c r="K724" s="0" t="s">
-        <v>1190</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12662,34 +12707,34 @@
         <v>590</v>
       </c>
       <c r="B725" s="0" t="s">
-        <v>410</v>
+        <v>345</v>
       </c>
       <c r="C725" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D725" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E725" s="0" t="s">
-        <v>1194</v>
+        <v>1203</v>
       </c>
       <c r="F725" s="0" t="s">
-        <v>1187</v>
+        <v>1204</v>
       </c>
       <c r="G725" s="0" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="H725" s="0" t="s">
-        <v>1195</v>
+        <v>1205</v>
       </c>
       <c r="I725" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J725" s="0" t="s">
-        <v>1196</v>
+        <v>1206</v>
       </c>
       <c r="K725" s="0" t="s">
-        <v>1190</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12697,237 +12742,135 @@
         <v>590</v>
       </c>
       <c r="B726" s="0" t="s">
-        <v>218</v>
+        <v>339</v>
       </c>
       <c r="C726" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D726" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E726" s="0" t="s">
-        <v>1197</v>
+        <v>1208</v>
       </c>
       <c r="F726" s="0" t="s">
-        <v>1198</v>
+        <v>1204</v>
       </c>
       <c r="G726" s="0" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="H726" s="0" t="s">
-        <v>218</v>
+        <v>1205</v>
       </c>
       <c r="I726" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J726" s="0" t="s">
-        <v>1199</v>
+        <v>1209</v>
       </c>
       <c r="K726" s="0" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A727" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B727" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C727" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D727" s="0" t="s">
-        <v>1201</v>
-      </c>
-      <c r="E727" s="0" t="s">
-        <v>1202</v>
-      </c>
-      <c r="F727" s="0" t="s">
-        <v>1203</v>
-      </c>
-      <c r="G727" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H727" s="0" t="s">
-        <v>1204</v>
-      </c>
-      <c r="I727" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J727" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="K727" s="0" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A728" s="0" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B728" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C728" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D728" s="0" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E728" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F728" s="0" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G728" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H728" s="0" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I728" s="0" t="s">
+        <v>1212</v>
+      </c>
+      <c r="J728" s="0" t="s">
+        <v>1201</v>
+      </c>
+      <c r="K728" s="0" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B731" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="H731" s="12" t="s">
+        <v>1214</v>
+      </c>
+      <c r="I731" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B732" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="H732" s="12" t="s">
+        <v>1215</v>
+      </c>
+      <c r="I732" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B733" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H733" s="13" t="s">
+        <v>1216</v>
+      </c>
+      <c r="I733" s="0" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A734" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B728" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C728" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D728" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E728" s="0" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F728" s="0" t="s">
-        <v>1208</v>
-      </c>
-      <c r="G728" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H728" s="0" t="s">
-        <v>1209</v>
-      </c>
-      <c r="I728" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J728" s="0" t="s">
-        <v>1210</v>
-      </c>
-      <c r="K728" s="0" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A729" s="0" t="s">
+      <c r="B734" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="H734" s="13" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I734" s="0" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A735" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B729" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C729" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D729" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E729" s="0" t="s">
-        <v>1212</v>
-      </c>
-      <c r="F729" s="0" t="s">
-        <v>1208</v>
-      </c>
-      <c r="G729" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H729" s="0" t="s">
-        <v>1209</v>
-      </c>
-      <c r="I729" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J729" s="0" t="s">
-        <v>1213</v>
-      </c>
-      <c r="K729" s="0" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A731" s="0" t="s">
-        <v>1214</v>
-      </c>
-      <c r="B731" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C731" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D731" s="0" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E731" s="0" t="s">
-        <v>1202</v>
-      </c>
-      <c r="F731" s="0" t="s">
-        <v>1203</v>
-      </c>
-      <c r="G731" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="H731" s="0" t="s">
-        <v>1204</v>
-      </c>
-      <c r="I731" s="0" t="s">
-        <v>1216</v>
-      </c>
-      <c r="J731" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="K731" s="0" t="s">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B734" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="H734" s="12" t="s">
+      <c r="B735" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="H735" s="13" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I735" s="0" t="s">
         <v>1218</v>
       </c>
-      <c r="I734" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B735" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="H735" s="12" t="s">
-        <v>1219</v>
-      </c>
-      <c r="I735" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B736" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H736" s="13" t="s">
-        <v>1220</v>
-      </c>
-      <c r="I736" s="0" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A737" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B737" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="H737" s="13" t="s">
-        <v>1221</v>
-      </c>
-      <c r="I737" s="0" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A738" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B738" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="H738" s="13" t="s">
-        <v>1223</v>
-      </c>
-      <c r="I738" s="0" t="s">
-        <v>1222</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Move Emon conccn & sconcss from pre identified missing to pre ignored file #384.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2399" uniqueCount="1209">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3626,39 +3626,6 @@
   </si>
   <si>
     <t xml:space="preserve">A 'nudging increment' refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conccn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aerosol Number Concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in TM5, though yet to be added by Tommi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tommi Bergman, Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Number concentration' means the number of particles or other specified objects per unit volume. 'Aerosol' means the system of suspended liquid or solid particles in air (except cloud droplets) and their carrier gas, the air itself. 'Ambient_aerosol' means that the aerosol is measured or modelled at the ambient state of pressure, temperature and relative humidity that exists in its immediate environment. 'Ambient aerosol particles' are aerosol particles that have taken up ambient water through hygroscopic growth. The extent of hygroscopic growth depends on the relative humidity and the composition of the particles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeoMIP,VIACSAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sconcss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Concentration of Seasalt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg m-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mass concentration of seasalt dry aerosol in air in model lowest layer</t>
   </si>
   <si>
     <t xml:space="preserve">Surface Total Alkalinity</t>
@@ -4073,8 +4040,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A641" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A657" activeCellId="0" sqref="A657"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A699" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A714" activeCellId="0" sqref="A714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12457,47 +12424,12 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A715" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B715" s="0" t="s">
-        <v>1171</v>
-      </c>
-      <c r="C715" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D715" s="0" t="s">
-        <v>621</v>
-      </c>
-      <c r="E715" s="0" t="s">
-        <v>1172</v>
-      </c>
-      <c r="F715" s="0" t="s">
-        <v>1173</v>
-      </c>
-      <c r="G715" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H715" s="0" t="s">
-        <v>1174</v>
-      </c>
-      <c r="I715" s="0" t="s">
-        <v>1175</v>
-      </c>
-      <c r="J715" s="0" t="s">
-        <v>1176</v>
-      </c>
-      <c r="K715" s="0" t="s">
-        <v>1177</v>
-      </c>
-    </row>
     <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="0" t="s">
-        <v>821</v>
+        <v>590</v>
       </c>
       <c r="B716" s="0" t="s">
-        <v>1178</v>
+        <v>432</v>
       </c>
       <c r="C716" s="0" t="n">
         <v>1</v>
@@ -12506,25 +12438,130 @@
         <v>612</v>
       </c>
       <c r="E716" s="0" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
       <c r="F716" s="0" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
       <c r="G716" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H716" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I716" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J716" s="0" t="s">
         <v>1174</v>
       </c>
-      <c r="I716" s="0" t="s">
+      <c r="K716" s="0" t="s">
         <v>1175</v>
       </c>
-      <c r="J716" s="0" t="s">
+    </row>
+    <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A717" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B717" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C717" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D717" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E717" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F717" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G717" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H717" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I717" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J717" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="K717" s="0" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A718" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B718" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C718" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D718" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E718" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F718" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G718" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H718" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="I718" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J718" s="0" t="s">
         <v>1181</v>
       </c>
-      <c r="K716" s="0" t="s">
-        <v>1177</v>
+      <c r="K718" s="0" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A719" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B719" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C719" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D719" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E719" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F719" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G719" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H719" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="I719" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J719" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K719" s="0" t="s">
+        <v>1185</v>
       </c>
     </row>
     <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12532,34 +12569,34 @@
         <v>590</v>
       </c>
       <c r="B720" s="0" t="s">
-        <v>432</v>
+        <v>225</v>
       </c>
       <c r="C720" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D720" s="0" t="s">
-        <v>612</v>
+        <v>1186</v>
       </c>
       <c r="E720" s="0" t="s">
-        <v>1182</v>
+        <v>1187</v>
       </c>
       <c r="F720" s="0" t="s">
-        <v>1183</v>
+        <v>1188</v>
       </c>
       <c r="G720" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H720" s="0" t="s">
-        <v>1184</v>
+        <v>1189</v>
       </c>
       <c r="I720" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J720" s="0" t="s">
-        <v>1185</v>
+        <v>1190</v>
       </c>
       <c r="K720" s="0" t="s">
-        <v>1186</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12567,34 +12604,34 @@
         <v>590</v>
       </c>
       <c r="B721" s="0" t="s">
-        <v>386</v>
+        <v>345</v>
       </c>
       <c r="C721" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D721" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E721" s="0" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F721" s="0" t="n">
-        <v>1</v>
+        <v>1192</v>
+      </c>
+      <c r="F721" s="0" t="s">
+        <v>1193</v>
       </c>
       <c r="G721" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H721" s="0" t="s">
-        <v>1188</v>
+        <v>1194</v>
       </c>
       <c r="I721" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J721" s="0" t="s">
-        <v>1189</v>
+        <v>1195</v>
       </c>
       <c r="K721" s="0" t="s">
-        <v>1186</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12602,74 +12639,39 @@
         <v>590</v>
       </c>
       <c r="B722" s="0" t="s">
-        <v>410</v>
+        <v>339</v>
       </c>
       <c r="C722" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D722" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E722" s="0" t="s">
-        <v>1190</v>
+        <v>1197</v>
       </c>
       <c r="F722" s="0" t="s">
-        <v>1183</v>
+        <v>1193</v>
       </c>
       <c r="G722" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H722" s="0" t="s">
-        <v>1191</v>
+        <v>1194</v>
       </c>
       <c r="I722" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J722" s="0" t="s">
-        <v>1192</v>
+        <v>1198</v>
       </c>
       <c r="K722" s="0" t="s">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A723" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B723" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="C723" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D723" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E723" s="0" t="s">
-        <v>1193</v>
-      </c>
-      <c r="F723" s="0" t="s">
-        <v>1194</v>
-      </c>
-      <c r="G723" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H723" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="I723" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J723" s="0" t="s">
-        <v>1195</v>
-      </c>
-      <c r="K723" s="0" t="s">
         <v>1196</v>
       </c>
     </row>
     <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="0" t="s">
-        <v>590</v>
+        <v>1199</v>
       </c>
       <c r="B724" s="0" t="s">
         <v>225</v>
@@ -12678,196 +12680,95 @@
         <v>1</v>
       </c>
       <c r="D724" s="0" t="s">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="E724" s="0" t="s">
-        <v>1198</v>
+        <v>1187</v>
       </c>
       <c r="F724" s="0" t="s">
-        <v>1199</v>
+        <v>1188</v>
       </c>
       <c r="G724" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H724" s="0" t="s">
-        <v>1200</v>
+        <v>1189</v>
       </c>
       <c r="I724" s="0" t="s">
-        <v>585</v>
+        <v>1201</v>
       </c>
       <c r="J724" s="0" t="s">
-        <v>1201</v>
+        <v>1190</v>
       </c>
       <c r="K724" s="0" t="s">
         <v>1202</v>
       </c>
     </row>
-    <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A725" s="0" t="s">
+    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B727" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="H727" s="12" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I727" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B728" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="H728" s="12" t="s">
+        <v>1204</v>
+      </c>
+      <c r="I728" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B729" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H729" s="13" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I729" s="0" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A730" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B725" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C725" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D725" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E725" s="0" t="s">
-        <v>1203</v>
-      </c>
-      <c r="F725" s="0" t="s">
-        <v>1204</v>
-      </c>
-      <c r="G725" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H725" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I725" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J725" s="0" t="s">
+      <c r="B730" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="H730" s="13" t="s">
         <v>1206</v>
       </c>
-      <c r="K725" s="0" t="s">
+      <c r="I730" s="0" t="s">
         <v>1207</v>
       </c>
     </row>
-    <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A726" s="0" t="s">
+    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A731" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B726" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C726" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D726" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E726" s="0" t="s">
+      <c r="B731" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="H731" s="13" t="s">
         <v>1208</v>
       </c>
-      <c r="F726" s="0" t="s">
-        <v>1204</v>
-      </c>
-      <c r="G726" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H726" s="0" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I726" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J726" s="0" t="s">
-        <v>1209</v>
-      </c>
-      <c r="K726" s="0" t="s">
+      <c r="I731" s="0" t="s">
         <v>1207</v>
       </c>
     </row>
-    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A728" s="0" t="s">
-        <v>1210</v>
-      </c>
-      <c r="B728" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C728" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D728" s="0" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E728" s="0" t="s">
-        <v>1198</v>
-      </c>
-      <c r="F728" s="0" t="s">
-        <v>1199</v>
-      </c>
-      <c r="G728" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H728" s="0" t="s">
-        <v>1200</v>
-      </c>
-      <c r="I728" s="0" t="s">
-        <v>1212</v>
-      </c>
-      <c r="J728" s="0" t="s">
-        <v>1201</v>
-      </c>
-      <c r="K728" s="0" t="s">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B731" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="H731" s="12" t="s">
-        <v>1214</v>
-      </c>
-      <c r="I731" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B732" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="H732" s="12" t="s">
-        <v>1215</v>
-      </c>
-      <c r="I732" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B733" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H733" s="13" t="s">
-        <v>1216</v>
-      </c>
-      <c r="I733" s="0" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A734" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B734" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="H734" s="13" t="s">
-        <v>1217</v>
-      </c>
-      <c r="I734" s="0" t="s">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A735" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B735" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="H735" s="13" t="s">
-        <v>1219</v>
-      </c>
-      <c r="I735" s="0" t="s">
-        <v>1218</v>
-      </c>
-    </row>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update comment for COSP variables in pre idetified missing file #368.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -3118,49 +3118,49 @@
     <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
   </si>
   <si>
+    <t xml:space="preserve">cllcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clmcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clhcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
+  </si>
+  <si>
     <t xml:space="preserve">cltisccp</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: ISCCP total cloud area, CVEXTRA(5)='94 ISCCP_TOTALCLDAREA'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klaus</t>
+    <t xml:space="preserve">grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pctisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
   </si>
   <si>
     <t xml:space="preserve">albisccp</t>
   </si>
   <si>
-    <t xml:space="preserve">COSP: ISCCP cloud albedo, CVEXTRA(7)='96 ISCCP_MEANALBEDOCLD'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pctisccp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP: ISCCP cloud top pressure, CVEXTRA(6)='95 ISCCP_MEANPTOP'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cltcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP: CALIPSO total cloud cover, CVEXTRA(4)='93 CALIPSO_CLDLAYER TOTAL'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cllcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP: CALIPSO low cloud cover, CVEXTRA(1)='90 CALIPSO_CLDLAYER LOW'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clmcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP: CALIPSO mid cloud cover, CVEXTRA(2)='91 CALIPSO_CLDLAYER MID'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clhcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP: CALIPSO high cloud cover, CVEXTRA(3)='92 CALIPSO_CLDLAYER HIGH'</t>
+    <t xml:space="preserve">grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
   </si>
   <si>
     <t xml:space="preserve">E3hrPt</t>
@@ -3749,7 +3749,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3804,13 +3804,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -3904,7 +3897,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3933,31 +3926,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4040,8 +4029,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A699" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A714" activeCellId="0" sqref="A714"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A620" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A629" activeCellId="0" sqref="A629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11341,116 +11330,200 @@
         <v>1013</v>
       </c>
     </row>
+    <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H629" s="4"/>
+      <c r="I629" s="4"/>
+    </row>
+    <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B630" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="H630" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I630" s="4" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B631" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H631" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I631" s="4" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B632" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H632" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I632" s="4" t="s">
+        <v>1018</v>
+      </c>
+    </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B633" s="0" t="s">
-        <v>1016</v>
+      <c r="B633" s="3" t="s">
+        <v>1023</v>
       </c>
       <c r="H633" s="4" t="s">
-        <v>1017</v>
+        <v>1024</v>
       </c>
       <c r="I633" s="4" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B634" s="0" t="s">
-        <v>1019</v>
-      </c>
-      <c r="H634" s="7" t="s">
-        <v>1020</v>
+      <c r="B634" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H634" s="4" t="s">
+        <v>1026</v>
       </c>
       <c r="I634" s="4" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B635" s="0" t="s">
-        <v>1021</v>
-      </c>
-      <c r="H635" s="7" t="s">
-        <v>1022</v>
+      <c r="B635" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H635" s="0" t="s">
+        <v>1028</v>
       </c>
       <c r="I635" s="4" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B636" s="0" t="s">
-        <v>1023</v>
-      </c>
-      <c r="H636" s="4" t="s">
-        <v>1024</v>
+      <c r="B636" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H636" s="0" t="s">
+        <v>1030</v>
       </c>
       <c r="I636" s="4" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B637" s="0" t="s">
-        <v>1025</v>
-      </c>
-      <c r="H637" s="4" t="s">
-        <v>1026</v>
-      </c>
-      <c r="I637" s="4" t="s">
-        <v>1018</v>
-      </c>
-    </row>
     <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B638" s="0" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H638" s="4" t="s">
-        <v>1028</v>
-      </c>
-      <c r="I638" s="4" t="s">
-        <v>1018</v>
-      </c>
+      <c r="H638" s="7"/>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A639" s="0" t="s">
+        <v>1031</v>
+      </c>
       <c r="B639" s="0" t="s">
-        <v>1029</v>
-      </c>
-      <c r="H639" s="4" t="s">
-        <v>1030</v>
-      </c>
-      <c r="I639" s="4" t="s">
-        <v>1018</v>
-      </c>
+        <v>1032</v>
+      </c>
+      <c r="H639" s="7" t="s">
+        <v>1033</v>
+      </c>
+      <c r="I639" s="6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J639" s="7"/>
+      <c r="K639" s="6"/>
+    </row>
+    <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A640" s="0" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B640" s="0" t="s">
+        <v>1036</v>
+      </c>
+      <c r="H640" s="7" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I640" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="J640" s="7"/>
+      <c r="K640" s="4"/>
+    </row>
+    <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A641" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B641" s="0" t="s">
+        <v>1038</v>
+      </c>
+      <c r="H641" s="7" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I641" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="J641" s="7"/>
+      <c r="K641" s="4"/>
+    </row>
+    <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A642" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B642" s="0" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H642" s="7" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I642" s="6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J642" s="7"/>
+      <c r="K642" s="6"/>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H643" s="8"/>
+      <c r="A643" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="B643" s="0" t="s">
+        <v>1042</v>
+      </c>
+      <c r="H643" s="7" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I643" s="6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="J643" s="7"/>
+      <c r="K643" s="6"/>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="0" t="s">
-        <v>1031</v>
+        <v>821</v>
       </c>
       <c r="B644" s="0" t="s">
-        <v>1032</v>
-      </c>
-      <c r="H644" s="8" t="s">
-        <v>1033</v>
-      </c>
-      <c r="I644" s="6" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H644" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="I644" s="4" t="s">
         <v>1034</v>
       </c>
-      <c r="J644" s="8"/>
-      <c r="K644" s="6"/>
+      <c r="J644" s="7"/>
+      <c r="K644" s="4"/>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="0" t="s">
-        <v>1035</v>
+        <v>821</v>
       </c>
       <c r="B645" s="0" t="s">
-        <v>1036</v>
-      </c>
-      <c r="H645" s="8" t="s">
-        <v>1037</v>
+        <v>1046</v>
+      </c>
+      <c r="H645" s="7" t="s">
+        <v>1047</v>
       </c>
       <c r="I645" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="J645" s="8"/>
+        <v>1034</v>
+      </c>
+      <c r="J645" s="7"/>
       <c r="K645" s="4"/>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11458,13 +11531,13 @@
         <v>821</v>
       </c>
       <c r="B646" s="0" t="s">
-        <v>1038</v>
+        <v>1048</v>
       </c>
       <c r="H646" s="8" t="s">
-        <v>1039</v>
+        <v>1049</v>
       </c>
       <c r="I646" s="4" t="s">
-        <v>789</v>
+        <v>1034</v>
       </c>
       <c r="J646" s="8"/>
       <c r="K646" s="4"/>
@@ -11474,154 +11547,155 @@
         <v>821</v>
       </c>
       <c r="B647" s="0" t="s">
-        <v>1040</v>
+        <v>1050</v>
       </c>
       <c r="H647" s="8" t="s">
-        <v>1041</v>
-      </c>
-      <c r="I647" s="6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I647" s="4" t="s">
         <v>1034</v>
       </c>
       <c r="J647" s="8"/>
-      <c r="K647" s="6"/>
-    </row>
-    <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A648" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B648" s="0" t="s">
-        <v>1042</v>
-      </c>
-      <c r="H648" s="8" t="s">
-        <v>1043</v>
-      </c>
-      <c r="I648" s="6" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J648" s="8"/>
-      <c r="K648" s="6"/>
+      <c r="K647" s="4"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
-        <v>821</v>
+        <v>751</v>
       </c>
       <c r="B649" s="0" t="s">
-        <v>1044</v>
-      </c>
-      <c r="H649" s="8" t="s">
-        <v>1045</v>
+        <v>1052</v>
+      </c>
+      <c r="H649" s="4" t="s">
+        <v>1053</v>
       </c>
       <c r="I649" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J649" s="8"/>
+        <v>789</v>
+      </c>
+      <c r="J649" s="4"/>
       <c r="K649" s="4"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
-        <v>821</v>
+        <v>751</v>
       </c>
       <c r="B650" s="0" t="s">
-        <v>1046</v>
-      </c>
-      <c r="H650" s="8" t="s">
-        <v>1047</v>
+        <v>1054</v>
+      </c>
+      <c r="H650" s="4" t="s">
+        <v>1055</v>
       </c>
       <c r="I650" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J650" s="8"/>
+        <v>789</v>
+      </c>
+      <c r="J650" s="4"/>
       <c r="K650" s="4"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
-        <v>821</v>
+        <v>751</v>
       </c>
       <c r="B651" s="0" t="s">
-        <v>1048</v>
-      </c>
-      <c r="H651" s="9" t="s">
-        <v>1049</v>
+        <v>1056</v>
+      </c>
+      <c r="H651" s="4" t="s">
+        <v>1057</v>
       </c>
       <c r="I651" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J651" s="9"/>
+        <v>789</v>
+      </c>
+      <c r="J651" s="4"/>
       <c r="K651" s="4"/>
-    </row>
-    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A652" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="B652" s="0" t="s">
-        <v>1050</v>
-      </c>
-      <c r="H652" s="9" t="s">
-        <v>1051</v>
-      </c>
-      <c r="I652" s="4" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J652" s="9"/>
-      <c r="K652" s="4"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>751</v>
+        <v>1058</v>
       </c>
       <c r="B654" s="0" t="s">
-        <v>1052</v>
+        <v>1059</v>
       </c>
       <c r="H654" s="4" t="s">
-        <v>1053</v>
+        <v>1060</v>
       </c>
       <c r="I654" s="4" t="s">
-        <v>789</v>
+        <v>1011</v>
       </c>
       <c r="J654" s="4"/>
       <c r="K654" s="4"/>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="0" t="s">
-        <v>751</v>
+        <v>1058</v>
       </c>
       <c r="B655" s="0" t="s">
-        <v>1054</v>
+        <v>1061</v>
       </c>
       <c r="H655" s="4" t="s">
-        <v>1055</v>
+        <v>1062</v>
       </c>
       <c r="I655" s="4" t="s">
-        <v>789</v>
+        <v>1011</v>
       </c>
       <c r="J655" s="4"/>
       <c r="K655" s="4"/>
-    </row>
-    <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L655" s="4"/>
+    </row>
+    <row r="656" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
-        <v>751</v>
+        <v>1058</v>
       </c>
       <c r="B656" s="0" t="s">
-        <v>1056</v>
+        <v>1063</v>
       </c>
       <c r="H656" s="4" t="s">
-        <v>1057</v>
+        <v>1064</v>
       </c>
       <c r="I656" s="4" t="s">
-        <v>789</v>
+        <v>1011</v>
       </c>
       <c r="J656" s="4"/>
       <c r="K656" s="4"/>
+    </row>
+    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A657" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B657" s="0" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H657" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I657" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J657" s="4"/>
+      <c r="K657" s="4"/>
+    </row>
+    <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A658" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B658" s="0" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H658" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="I658" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J658" s="4"/>
+      <c r="K658" s="4"/>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
         <v>1058</v>
       </c>
       <c r="B659" s="0" t="s">
-        <v>1059</v>
+        <v>1069</v>
       </c>
       <c r="H659" s="4" t="s">
-        <v>1060</v>
+        <v>1070</v>
       </c>
       <c r="I659" s="4" t="s">
         <v>1011</v>
@@ -11634,43 +11708,43 @@
         <v>1058</v>
       </c>
       <c r="B660" s="0" t="s">
-        <v>1061</v>
+        <v>1071</v>
       </c>
       <c r="H660" s="4" t="s">
-        <v>1062</v>
+        <v>1072</v>
       </c>
       <c r="I660" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J660" s="4"/>
       <c r="K660" s="4"/>
-      <c r="L660" s="4"/>
-    </row>
-    <row r="661" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="0" t="s">
         <v>1058</v>
       </c>
       <c r="B661" s="0" t="s">
-        <v>1063</v>
+        <v>1073</v>
       </c>
       <c r="H661" s="4" t="s">
-        <v>1064</v>
+        <v>1074</v>
       </c>
       <c r="I661" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J661" s="4"/>
       <c r="K661" s="4"/>
+      <c r="L661" s="4"/>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
         <v>1058</v>
       </c>
       <c r="B662" s="0" t="s">
-        <v>1065</v>
+        <v>1075</v>
       </c>
       <c r="H662" s="4" t="s">
-        <v>1066</v>
+        <v>1076</v>
       </c>
       <c r="I662" s="4" t="s">
         <v>1011</v>
@@ -11683,10 +11757,10 @@
         <v>1058</v>
       </c>
       <c r="B663" s="0" t="s">
-        <v>1067</v>
+        <v>1077</v>
       </c>
       <c r="H663" s="4" t="s">
-        <v>1068</v>
+        <v>1078</v>
       </c>
       <c r="I663" s="4" t="s">
         <v>1011</v>
@@ -11699,10 +11773,10 @@
         <v>1058</v>
       </c>
       <c r="B664" s="0" t="s">
-        <v>1069</v>
+        <v>1079</v>
       </c>
       <c r="H664" s="4" t="s">
-        <v>1070</v>
+        <v>1080</v>
       </c>
       <c r="I664" s="4" t="s">
         <v>1011</v>
@@ -11715,43 +11789,43 @@
         <v>1058</v>
       </c>
       <c r="B665" s="0" t="s">
-        <v>1071</v>
+        <v>1081</v>
       </c>
       <c r="H665" s="4" t="s">
-        <v>1072</v>
+        <v>1082</v>
       </c>
       <c r="I665" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J665" s="4"/>
       <c r="K665" s="4"/>
+      <c r="L665" s="4"/>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
         <v>1058</v>
       </c>
       <c r="B666" s="0" t="s">
-        <v>1073</v>
+        <v>1083</v>
       </c>
       <c r="H666" s="4" t="s">
-        <v>1074</v>
+        <v>1084</v>
       </c>
       <c r="I666" s="4" t="s">
         <v>1011</v>
       </c>
       <c r="J666" s="4"/>
       <c r="K666" s="4"/>
-      <c r="L666" s="4"/>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
         <v>1058</v>
       </c>
       <c r="B667" s="0" t="s">
-        <v>1075</v>
+        <v>1085</v>
       </c>
       <c r="H667" s="4" t="s">
-        <v>1076</v>
+        <v>1086</v>
       </c>
       <c r="I667" s="4" t="s">
         <v>1011</v>
@@ -11761,266 +11835,249 @@
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="0" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="B668" s="0" t="s">
-        <v>1077</v>
+        <v>1088</v>
       </c>
       <c r="H668" s="4" t="s">
-        <v>1078</v>
+        <v>1089</v>
       </c>
       <c r="I668" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J668" s="4"/>
       <c r="K668" s="4"/>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="B669" s="0" t="s">
-        <v>1079</v>
+        <v>1091</v>
       </c>
       <c r="H669" s="4" t="s">
-        <v>1080</v>
+        <v>1092</v>
       </c>
       <c r="I669" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J669" s="4"/>
       <c r="K669" s="4"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="0" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="B670" s="0" t="s">
-        <v>1081</v>
+        <v>1093</v>
       </c>
       <c r="H670" s="4" t="s">
-        <v>1082</v>
+        <v>1094</v>
       </c>
       <c r="I670" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J670" s="4"/>
       <c r="K670" s="4"/>
-      <c r="L670" s="4"/>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="B671" s="0" t="s">
-        <v>1083</v>
+        <v>1095</v>
       </c>
       <c r="H671" s="4" t="s">
-        <v>1084</v>
+        <v>1096</v>
       </c>
       <c r="I671" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J671" s="4"/>
       <c r="K671" s="4"/>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="B672" s="0" t="s">
-        <v>1085</v>
+        <v>1097</v>
       </c>
       <c r="H672" s="4" t="s">
-        <v>1086</v>
+        <v>1098</v>
       </c>
       <c r="I672" s="4" t="s">
-        <v>1011</v>
+        <v>1090</v>
       </c>
       <c r="J672" s="4"/>
       <c r="K672" s="4"/>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
       <c r="B673" s="0" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
       <c r="H673" s="4" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="I673" s="4" t="s">
-        <v>1090</v>
+        <v>789</v>
       </c>
       <c r="J673" s="4"/>
       <c r="K673" s="4"/>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>1087</v>
+        <v>1100</v>
       </c>
       <c r="B674" s="0" t="s">
-        <v>1091</v>
+        <v>1101</v>
       </c>
       <c r="H674" s="4" t="s">
-        <v>1092</v>
+        <v>1102</v>
       </c>
       <c r="I674" s="4" t="s">
-        <v>1090</v>
+        <v>789</v>
       </c>
       <c r="J674" s="4"/>
       <c r="K674" s="4"/>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="0" t="s">
-        <v>1087</v>
+        <v>751</v>
       </c>
       <c r="B675" s="0" t="s">
-        <v>1093</v>
+        <v>1103</v>
       </c>
       <c r="H675" s="4" t="s">
-        <v>1094</v>
-      </c>
-      <c r="I675" s="4" t="s">
-        <v>1090</v>
+        <v>1104</v>
+      </c>
+      <c r="I675" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J675" s="4"/>
-      <c r="K675" s="4"/>
+      <c r="K675" s="6"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="0" t="s">
-        <v>1087</v>
+        <v>751</v>
       </c>
       <c r="B676" s="0" t="s">
-        <v>1095</v>
+        <v>1105</v>
       </c>
       <c r="H676" s="4" t="s">
-        <v>1096</v>
+        <v>1106</v>
       </c>
       <c r="I676" s="4" t="s">
-        <v>1090</v>
+        <v>789</v>
       </c>
       <c r="J676" s="4"/>
       <c r="K676" s="4"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>1087</v>
+        <v>751</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1097</v>
-      </c>
-      <c r="H677" s="4" t="s">
-        <v>1098</v>
-      </c>
-      <c r="I677" s="4" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J677" s="4"/>
-      <c r="K677" s="4"/>
+        <v>1107</v>
+      </c>
+      <c r="H677" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J677" s="9"/>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="0" t="s">
-        <v>1099</v>
+        <v>987</v>
       </c>
       <c r="B678" s="0" t="s">
-        <v>1091</v>
+        <v>1109</v>
       </c>
       <c r="H678" s="4" t="s">
-        <v>1092</v>
-      </c>
-      <c r="I678" s="4" t="s">
-        <v>789</v>
+        <v>1110</v>
+      </c>
+      <c r="I678" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J678" s="4"/>
-      <c r="K678" s="4"/>
+      <c r="K678" s="6"/>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="0" t="s">
-        <v>1100</v>
+        <v>821</v>
       </c>
       <c r="B679" s="0" t="s">
-        <v>1101</v>
+        <v>1111</v>
       </c>
       <c r="H679" s="4" t="s">
-        <v>1102</v>
+        <v>1112</v>
       </c>
       <c r="I679" s="4" t="s">
-        <v>789</v>
+        <v>1034</v>
       </c>
       <c r="J679" s="4"/>
       <c r="K679" s="4"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>751</v>
+        <v>821</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1103</v>
+        <v>1113</v>
       </c>
       <c r="H680" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="I680" s="6" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I680" s="4" t="s">
         <v>1034</v>
       </c>
       <c r="J680" s="4"/>
-      <c r="K680" s="6"/>
-    </row>
-    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A681" s="0" t="s">
-        <v>751</v>
-      </c>
-      <c r="B681" s="0" t="s">
-        <v>1105</v>
-      </c>
-      <c r="H681" s="4" t="s">
-        <v>1106</v>
-      </c>
-      <c r="I681" s="4" t="s">
-        <v>789</v>
-      </c>
-      <c r="J681" s="4"/>
-      <c r="K681" s="4"/>
+      <c r="K680" s="4"/>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="0" t="s">
-        <v>751</v>
+        <v>1115</v>
       </c>
       <c r="B682" s="0" t="s">
-        <v>1107</v>
-      </c>
-      <c r="H682" s="10" t="s">
-        <v>1108</v>
-      </c>
-      <c r="J682" s="10"/>
+        <v>1116</v>
+      </c>
+      <c r="H682" s="4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I682" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J682" s="4"/>
+      <c r="K682" s="4"/>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
-        <v>987</v>
+        <v>1115</v>
       </c>
       <c r="B683" s="0" t="s">
-        <v>1109</v>
+        <v>1119</v>
       </c>
       <c r="H683" s="4" t="s">
-        <v>1110</v>
-      </c>
-      <c r="I683" s="6" t="s">
-        <v>1034</v>
+        <v>1120</v>
+      </c>
+      <c r="I683" s="4" t="s">
+        <v>1118</v>
       </c>
       <c r="J683" s="4"/>
-      <c r="K683" s="6"/>
+      <c r="K683" s="4"/>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="0" t="s">
-        <v>821</v>
+        <v>1115</v>
       </c>
       <c r="B684" s="0" t="s">
-        <v>1111</v>
+        <v>1121</v>
       </c>
       <c r="H684" s="4" t="s">
-        <v>1112</v>
+        <v>1122</v>
       </c>
       <c r="I684" s="4" t="s">
         <v>1034</v>
@@ -12030,371 +12087,342 @@
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="0" t="s">
-        <v>821</v>
+        <v>1058</v>
       </c>
       <c r="B685" s="0" t="s">
-        <v>1113</v>
+        <v>1123</v>
       </c>
       <c r="H685" s="4" t="s">
-        <v>1114</v>
+        <v>1124</v>
       </c>
       <c r="I685" s="4" t="s">
-        <v>1034</v>
+        <v>1011</v>
       </c>
       <c r="J685" s="4"/>
       <c r="K685" s="4"/>
     </row>
+    <row r="686" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A686" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B686" s="0" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H686" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I686" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J686" s="4"/>
+      <c r="K686" s="4"/>
+    </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="0" t="s">
-        <v>1115</v>
+        <v>1058</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>1116</v>
+        <v>1127</v>
       </c>
       <c r="H687" s="4" t="s">
-        <v>1117</v>
+        <v>1128</v>
       </c>
       <c r="I687" s="4" t="s">
-        <v>1118</v>
+        <v>1011</v>
       </c>
       <c r="J687" s="4"/>
       <c r="K687" s="4"/>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="0" t="s">
-        <v>1115</v>
+        <v>1058</v>
       </c>
       <c r="B688" s="0" t="s">
-        <v>1119</v>
+        <v>1129</v>
       </c>
       <c r="H688" s="4" t="s">
-        <v>1120</v>
+        <v>1130</v>
       </c>
       <c r="I688" s="4" t="s">
-        <v>1118</v>
+        <v>1011</v>
       </c>
       <c r="J688" s="4"/>
       <c r="K688" s="4"/>
     </row>
     <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="0" t="s">
-        <v>1115</v>
+        <v>1087</v>
       </c>
       <c r="B689" s="0" t="s">
-        <v>1121</v>
+        <v>1131</v>
       </c>
       <c r="H689" s="4" t="s">
-        <v>1122</v>
+        <v>1132</v>
       </c>
       <c r="I689" s="4" t="s">
-        <v>1034</v>
+        <v>1090</v>
       </c>
       <c r="J689" s="4"/>
       <c r="K689" s="4"/>
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="0" t="s">
-        <v>1058</v>
+        <v>1133</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>1123</v>
+        <v>1134</v>
       </c>
       <c r="H690" s="4" t="s">
-        <v>1124</v>
-      </c>
-      <c r="I690" s="4" t="s">
-        <v>1011</v>
+        <v>1135</v>
+      </c>
+      <c r="I690" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J690" s="4"/>
-      <c r="K690" s="4"/>
-    </row>
-    <row r="691" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K690" s="6"/>
+    </row>
+    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="0" t="s">
-        <v>1058</v>
+        <v>1133</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>1125</v>
+        <v>1136</v>
       </c>
       <c r="H691" s="4" t="s">
-        <v>1126</v>
-      </c>
-      <c r="I691" s="4" t="s">
-        <v>1011</v>
+        <v>1135</v>
+      </c>
+      <c r="I691" s="6" t="s">
+        <v>1034</v>
       </c>
       <c r="J691" s="4"/>
-      <c r="K691" s="4"/>
-    </row>
-    <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A692" s="0" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B692" s="0" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H692" s="4" t="s">
-        <v>1128</v>
-      </c>
-      <c r="I692" s="4" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J692" s="4"/>
-      <c r="K692" s="4"/>
-    </row>
-    <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A693" s="0" t="s">
-        <v>1058</v>
-      </c>
-      <c r="B693" s="0" t="s">
-        <v>1129</v>
-      </c>
-      <c r="H693" s="4" t="s">
-        <v>1130</v>
-      </c>
-      <c r="I693" s="4" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J693" s="4"/>
-      <c r="K693" s="4"/>
-    </row>
-    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A694" s="0" t="s">
-        <v>1087</v>
-      </c>
-      <c r="B694" s="0" t="s">
-        <v>1131</v>
-      </c>
-      <c r="H694" s="4" t="s">
-        <v>1132</v>
-      </c>
-      <c r="I694" s="4" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J694" s="4"/>
-      <c r="K694" s="4"/>
+      <c r="K691" s="6"/>
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="0" t="s">
-        <v>1133</v>
+        <v>1115</v>
       </c>
       <c r="B695" s="0" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="H695" s="4" t="s">
-        <v>1135</v>
-      </c>
-      <c r="I695" s="6" t="s">
-        <v>1034</v>
+        <v>1138</v>
+      </c>
+      <c r="I695" s="4" t="s">
+        <v>1118</v>
       </c>
       <c r="J695" s="4"/>
-      <c r="K695" s="6"/>
+      <c r="K695" s="4"/>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="0" t="s">
-        <v>1133</v>
+        <v>1115</v>
       </c>
       <c r="B696" s="0" t="s">
-        <v>1136</v>
+        <v>1139</v>
       </c>
       <c r="H696" s="4" t="s">
-        <v>1135</v>
-      </c>
-      <c r="I696" s="6" t="s">
-        <v>1034</v>
+        <v>1140</v>
+      </c>
+      <c r="I696" s="4" t="s">
+        <v>1118</v>
       </c>
       <c r="J696" s="4"/>
-      <c r="K696" s="6"/>
-    </row>
-    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A700" s="0" t="s">
+      <c r="K696" s="4"/>
+    </row>
+    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A697" s="0" t="s">
         <v>1115</v>
       </c>
-      <c r="B700" s="0" t="s">
-        <v>1137</v>
-      </c>
-      <c r="H700" s="4" t="s">
-        <v>1138</v>
-      </c>
-      <c r="I700" s="4" t="s">
+      <c r="B697" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H697" s="4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I697" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="J700" s="4"/>
-      <c r="K700" s="4"/>
-    </row>
-    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A701" s="0" t="s">
+      <c r="J697" s="4"/>
+      <c r="K697" s="4"/>
+    </row>
+    <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A698" s="0" t="s">
         <v>1115</v>
       </c>
-      <c r="B701" s="0" t="s">
-        <v>1139</v>
-      </c>
-      <c r="H701" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="I701" s="4" t="s">
+      <c r="B698" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="H698" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I698" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="J701" s="4"/>
-      <c r="K701" s="4"/>
-    </row>
-    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A702" s="0" t="s">
+      <c r="J698" s="4"/>
+      <c r="K698" s="4"/>
+    </row>
+    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A699" s="0" t="s">
         <v>1115</v>
       </c>
-      <c r="B702" s="0" t="s">
-        <v>1141</v>
-      </c>
-      <c r="H702" s="4" t="s">
-        <v>1142</v>
-      </c>
-      <c r="I702" s="4" t="s">
+      <c r="B699" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="H699" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="I699" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="J702" s="4"/>
-      <c r="K702" s="4"/>
+      <c r="J699" s="4"/>
+      <c r="K699" s="4"/>
     </row>
     <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="0" t="s">
-        <v>1115</v>
+        <v>987</v>
       </c>
       <c r="B703" s="0" t="s">
-        <v>1143</v>
-      </c>
-      <c r="H703" s="4" t="s">
-        <v>1144</v>
-      </c>
-      <c r="I703" s="4" t="s">
-        <v>1118</v>
-      </c>
-      <c r="J703" s="4"/>
-      <c r="K703" s="4"/>
+        <v>1147</v>
+      </c>
+      <c r="C703" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D703" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E703" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F703" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G703" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H703" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I703" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="J703" s="0" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K703" s="0" t="s">
+        <v>1154</v>
+      </c>
     </row>
     <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="0" t="s">
-        <v>1115</v>
+        <v>987</v>
       </c>
       <c r="B704" s="0" t="s">
-        <v>1145</v>
-      </c>
-      <c r="H704" s="4" t="s">
-        <v>1146</v>
-      </c>
-      <c r="I704" s="4" t="s">
-        <v>1118</v>
-      </c>
-      <c r="J704" s="4"/>
-      <c r="K704" s="4"/>
-    </row>
-    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A708" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C704" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D704" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E704" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F704" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G704" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H704" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="I704" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="J704" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="K704" s="0" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A705" s="0" t="s">
         <v>987</v>
       </c>
-      <c r="B708" s="0" t="s">
-        <v>1147</v>
-      </c>
-      <c r="C708" s="0" t="n">
+      <c r="B705" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C705" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D708" s="0" t="s">
+      <c r="D705" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E708" s="0" t="s">
-        <v>1148</v>
-      </c>
-      <c r="F708" s="0" t="s">
-        <v>1149</v>
-      </c>
-      <c r="G708" s="0" t="s">
+      <c r="E705" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F705" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G705" s="0" t="s">
         <v>1150</v>
       </c>
-      <c r="H708" s="0" t="s">
-        <v>1151</v>
-      </c>
-      <c r="I708" s="0" t="s">
-        <v>1152</v>
-      </c>
-      <c r="J708" s="0" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K708" s="0" t="s">
+      <c r="H705" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="I705" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J705" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="K705" s="0" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="0" t="s">
+    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A706" s="0" t="s">
         <v>987</v>
       </c>
-      <c r="B709" s="0" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C709" s="0" t="n">
+      <c r="B706" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C706" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D709" s="0" t="s">
+      <c r="D706" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E709" s="0" t="s">
-        <v>1156</v>
-      </c>
-      <c r="F709" s="0" t="s">
-        <v>1157</v>
-      </c>
-      <c r="G709" s="0" t="s">
+      <c r="E706" s="0" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F706" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G706" s="0" t="s">
         <v>1150</v>
       </c>
-      <c r="H709" s="0" t="s">
-        <v>1158</v>
-      </c>
-      <c r="I709" s="0" t="s">
-        <v>1159</v>
-      </c>
-      <c r="J709" s="0" t="s">
-        <v>1160</v>
-      </c>
-      <c r="K709" s="0" t="s">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A710" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="B710" s="0" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C710" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D710" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E710" s="0" t="s">
-        <v>1162</v>
-      </c>
-      <c r="F710" s="0" t="s">
-        <v>1163</v>
-      </c>
-      <c r="G710" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H710" s="0" t="s">
-        <v>1164</v>
-      </c>
-      <c r="I710" s="0" t="s">
+      <c r="H706" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I706" s="0" t="s">
         <v>1165</v>
       </c>
-      <c r="J710" s="0" t="s">
-        <v>1166</v>
-      </c>
-      <c r="K710" s="0" t="s">
+      <c r="J706" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K706" s="0" t="s">
         <v>1154</v>
       </c>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A711" s="0" t="s">
-        <v>987</v>
+        <v>590</v>
       </c>
       <c r="B711" s="0" t="s">
-        <v>1167</v>
+        <v>432</v>
       </c>
       <c r="C711" s="0" t="n">
         <v>1</v>
@@ -12403,25 +12431,165 @@
         <v>612</v>
       </c>
       <c r="E711" s="0" t="s">
-        <v>1168</v>
+        <v>1171</v>
       </c>
       <c r="F711" s="0" t="s">
-        <v>1163</v>
+        <v>1172</v>
       </c>
       <c r="G711" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H711" s="0" t="s">
-        <v>1169</v>
+        <v>1173</v>
       </c>
       <c r="I711" s="0" t="s">
-        <v>1165</v>
+        <v>585</v>
       </c>
       <c r="J711" s="0" t="s">
-        <v>1170</v>
+        <v>1174</v>
       </c>
       <c r="K711" s="0" t="s">
-        <v>1154</v>
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A712" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B712" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C712" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D712" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E712" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F712" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G712" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H712" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="I712" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J712" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="K712" s="0" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A713" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B713" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C713" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D713" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E713" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F713" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G713" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H713" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="I713" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J713" s="0" t="s">
+        <v>1181</v>
+      </c>
+      <c r="K713" s="0" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A714" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B714" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C714" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D714" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="E714" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F714" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G714" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H714" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="I714" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J714" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K714" s="0" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A715" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B715" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C715" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D715" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E715" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F715" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G715" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H715" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I715" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="J715" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="K715" s="0" t="s">
+        <v>1191</v>
       </c>
     </row>
     <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12429,34 +12597,34 @@
         <v>590</v>
       </c>
       <c r="B716" s="0" t="s">
-        <v>432</v>
+        <v>345</v>
       </c>
       <c r="C716" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D716" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E716" s="0" t="s">
-        <v>1171</v>
+        <v>1192</v>
       </c>
       <c r="F716" s="0" t="s">
-        <v>1172</v>
+        <v>1193</v>
       </c>
       <c r="G716" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H716" s="0" t="s">
-        <v>1173</v>
+        <v>1194</v>
       </c>
       <c r="I716" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J716" s="0" t="s">
-        <v>1174</v>
+        <v>1195</v>
       </c>
       <c r="K716" s="0" t="s">
-        <v>1175</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12464,307 +12632,137 @@
         <v>590</v>
       </c>
       <c r="B717" s="0" t="s">
-        <v>386</v>
+        <v>339</v>
       </c>
       <c r="C717" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D717" s="0" t="s">
         <v>612</v>
       </c>
       <c r="E717" s="0" t="s">
-        <v>1176</v>
-      </c>
-      <c r="F717" s="0" t="n">
-        <v>1</v>
+        <v>1197</v>
+      </c>
+      <c r="F717" s="0" t="s">
+        <v>1193</v>
       </c>
       <c r="G717" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H717" s="0" t="s">
-        <v>1177</v>
+        <v>1194</v>
       </c>
       <c r="I717" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J717" s="0" t="s">
-        <v>1178</v>
+        <v>1198</v>
       </c>
       <c r="K717" s="0" t="s">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A718" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B718" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="C718" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D718" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E718" s="0" t="s">
-        <v>1179</v>
-      </c>
-      <c r="F718" s="0" t="s">
-        <v>1172</v>
-      </c>
-      <c r="G718" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H718" s="0" t="s">
-        <v>1180</v>
-      </c>
-      <c r="I718" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J718" s="0" t="s">
-        <v>1181</v>
-      </c>
-      <c r="K718" s="0" t="s">
-        <v>1175</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="0" t="s">
-        <v>590</v>
+        <v>1199</v>
       </c>
       <c r="B719" s="0" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="C719" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D719" s="0" t="s">
-        <v>612</v>
+        <v>1200</v>
       </c>
       <c r="E719" s="0" t="s">
-        <v>1182</v>
+        <v>1187</v>
       </c>
       <c r="F719" s="0" t="s">
-        <v>1183</v>
+        <v>1188</v>
       </c>
       <c r="G719" s="0" t="s">
         <v>1150</v>
       </c>
       <c r="H719" s="0" t="s">
-        <v>218</v>
+        <v>1189</v>
       </c>
       <c r="I719" s="0" t="s">
+        <v>1201</v>
+      </c>
+      <c r="J719" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="K719" s="0" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B722" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="H722" s="11" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I722" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B723" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="H723" s="11" t="s">
+        <v>1204</v>
+      </c>
+      <c r="I723" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B724" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H724" s="12" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I724" s="0" t="s">
         <v>585</v>
       </c>
-      <c r="J719" s="0" t="s">
-        <v>1184</v>
-      </c>
-      <c r="K719" s="0" t="s">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A720" s="0" t="s">
+    </row>
+    <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A725" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B720" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C720" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D720" s="0" t="s">
-        <v>1186</v>
-      </c>
-      <c r="E720" s="0" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F720" s="0" t="s">
-        <v>1188</v>
-      </c>
-      <c r="G720" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H720" s="0" t="s">
-        <v>1189</v>
-      </c>
-      <c r="I720" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J720" s="0" t="s">
-        <v>1190</v>
-      </c>
-      <c r="K720" s="0" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A721" s="0" t="s">
+      <c r="B725" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="H725" s="12" t="s">
+        <v>1206</v>
+      </c>
+      <c r="I725" s="0" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A726" s="0" t="s">
         <v>590</v>
       </c>
-      <c r="B721" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C721" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D721" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E721" s="0" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F721" s="0" t="s">
-        <v>1193</v>
-      </c>
-      <c r="G721" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H721" s="0" t="s">
-        <v>1194</v>
-      </c>
-      <c r="I721" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J721" s="0" t="s">
-        <v>1195</v>
-      </c>
-      <c r="K721" s="0" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A722" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B722" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C722" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D722" s="0" t="s">
-        <v>612</v>
-      </c>
-      <c r="E722" s="0" t="s">
-        <v>1197</v>
-      </c>
-      <c r="F722" s="0" t="s">
-        <v>1193</v>
-      </c>
-      <c r="G722" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H722" s="0" t="s">
-        <v>1194</v>
-      </c>
-      <c r="I722" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="J722" s="0" t="s">
-        <v>1198</v>
-      </c>
-      <c r="K722" s="0" t="s">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A724" s="0" t="s">
-        <v>1199</v>
-      </c>
-      <c r="B724" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="C724" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D724" s="0" t="s">
-        <v>1200</v>
-      </c>
-      <c r="E724" s="0" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F724" s="0" t="s">
-        <v>1188</v>
-      </c>
-      <c r="G724" s="0" t="s">
-        <v>1150</v>
-      </c>
-      <c r="H724" s="0" t="s">
-        <v>1189</v>
-      </c>
-      <c r="I724" s="0" t="s">
-        <v>1201</v>
-      </c>
-      <c r="J724" s="0" t="s">
-        <v>1190</v>
-      </c>
-      <c r="K724" s="0" t="s">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B727" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="H727" s="12" t="s">
-        <v>1203</v>
-      </c>
-      <c r="I727" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B728" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="H728" s="12" t="s">
-        <v>1204</v>
-      </c>
-      <c r="I728" s="0" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B729" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H729" s="13" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I729" s="0" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A730" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B730" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="H730" s="13" t="s">
-        <v>1206</v>
-      </c>
-      <c r="I730" s="0" t="s">
+      <c r="B726" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="H726" s="12" t="s">
+        <v>1208</v>
+      </c>
+      <c r="I726" s="0" t="s">
         <v>1207</v>
       </c>
     </row>
-    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A731" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="B731" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="H731" s="13" t="s">
-        <v>1208</v>
-      </c>
-      <c r="I731" s="0" t="s">
-        <v>1207</v>
-      </c>
-    </row>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Adjust cdnc comment, add COSP label to COSP variables in pre idetified missing file #143.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -2434,7 +2434,7 @@
     <t xml:space="preserve">cdnc</t>
   </si>
   <si>
-    <t xml:space="preserve">In runtime/classic/ctrl/namelist.ifs.cloudact+diag.sh CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
+    <t xml:space="preserve">Grib 126.20 / 126.22  in namelist.ifs.cloudact+diag.sh  CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
   </si>
   <si>
     <t xml:space="preserve">Twan &amp; Thomas</t>
@@ -3121,7 +3121,7 @@
     <t xml:space="preserve">cllcalipso</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
+    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
   </si>
   <si>
     <t xml:space="preserve">Klaus</t>
@@ -3130,37 +3130,37 @@
     <t xml:space="preserve">clmcalipso</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
+    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
   </si>
   <si>
     <t xml:space="preserve">clhcalipso</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
+    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
   </si>
   <si>
     <t xml:space="preserve">cltcalipso</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
+    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
   </si>
   <si>
     <t xml:space="preserve">cltisccp</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
+    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
   </si>
   <si>
     <t xml:space="preserve">pctisccp</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
+    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
   </si>
   <si>
     <t xml:space="preserve">albisccp</t>
   </si>
   <si>
-    <t xml:space="preserve">grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
+    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
   </si>
   <si>
     <t xml:space="preserve">E3hrPt</t>
@@ -4029,8 +4029,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A620" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A629" activeCellId="0" sqref="A629"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A400" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B416" activeCellId="0" sqref="B416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add recent proper comment #143.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2399" uniqueCount="1209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2399" uniqueCount="1210">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3229,19 +3229,19 @@
     <t xml:space="preserve">rlutaf</t>
   </si>
   <si>
-    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #403</t>
+    <t xml:space="preserve">grib 126.73                      Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">rlutcsaf</t>
   </si>
   <si>
-    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #404</t>
+    <t xml:space="preserve">grib 126.72                       Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">rsutaf</t>
   </si>
   <si>
-    <t xml:space="preserve">Available from double radiation call in IFS. See also PEXTRA issue #403   aerosol free</t>
+    <t xml:space="preserve">grib 128.212-126.069  Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
   </si>
   <si>
     <t xml:space="preserve">LImon</t>
@@ -3355,7 +3355,7 @@
     <t xml:space="preserve">tntr</t>
   </si>
   <si>
-    <t xml:space="preserve">Available in IFS: T-tendency from radiation: grib 128.95</t>
+    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
   </si>
   <si>
     <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
@@ -3364,28 +3364,31 @@
     <t xml:space="preserve">tntc</t>
   </si>
   <si>
+    <t xml:space="preserve">grib 126.105                                                              Available in IFS: T-tendency from convection : grib 128.105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110  Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.106                                                              Available in IFS: q-tendency from convection: grib 128.106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                      Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmonZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Available in IFS: T-tendency from convection : grib 128.105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhusc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in IFS: q-tendency from convection: grib 128.106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhusmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EmonZ</t>
   </si>
   <si>
     <t xml:space="preserve">6hrPlev</t>
@@ -4029,8 +4032,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A400" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B416" activeCellId="0" sqref="B416"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A652" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H669" activeCellId="0" sqref="H669"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11921,7 +11924,7 @@
         <v>1091</v>
       </c>
       <c r="H673" s="4" t="s">
-        <v>1092</v>
+        <v>1100</v>
       </c>
       <c r="I673" s="4" t="s">
         <v>789</v>
@@ -11931,13 +11934,13 @@
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B674" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="H674" s="4" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="I674" s="4" t="s">
         <v>789</v>
@@ -11950,10 +11953,10 @@
         <v>751</v>
       </c>
       <c r="B675" s="0" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="H675" s="4" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="I675" s="6" t="s">
         <v>1034</v>
@@ -11966,10 +11969,10 @@
         <v>751</v>
       </c>
       <c r="B676" s="0" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="H676" s="4" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="I676" s="4" t="s">
         <v>789</v>
@@ -11982,10 +11985,10 @@
         <v>751</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="H677" s="9" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="J677" s="9"/>
     </row>
@@ -11994,10 +11997,10 @@
         <v>987</v>
       </c>
       <c r="B678" s="0" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="H678" s="4" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="I678" s="6" t="s">
         <v>1034</v>
@@ -12010,10 +12013,10 @@
         <v>821</v>
       </c>
       <c r="B679" s="0" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="H679" s="4" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="I679" s="4" t="s">
         <v>1034</v>
@@ -12026,10 +12029,10 @@
         <v>821</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="H680" s="4" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="I680" s="4" t="s">
         <v>1034</v>
@@ -12039,45 +12042,45 @@
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B682" s="0" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="H682" s="4" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="I682" s="4" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J682" s="4"/>
       <c r="K682" s="4"/>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B683" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="H683" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="I683" s="4" t="s">
         <v>1119</v>
-      </c>
-      <c r="H683" s="4" t="s">
-        <v>1120</v>
-      </c>
-      <c r="I683" s="4" t="s">
-        <v>1118</v>
       </c>
       <c r="J683" s="4"/>
       <c r="K683" s="4"/>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B684" s="0" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="H684" s="4" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="I684" s="4" t="s">
         <v>1034</v>
@@ -12090,10 +12093,10 @@
         <v>1058</v>
       </c>
       <c r="B685" s="0" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="H685" s="4" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="I685" s="4" t="s">
         <v>1011</v>
@@ -12106,10 +12109,10 @@
         <v>1058</v>
       </c>
       <c r="B686" s="0" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="H686" s="4" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="I686" s="4" t="s">
         <v>1011</v>
@@ -12122,10 +12125,10 @@
         <v>1058</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="H687" s="4" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="I687" s="4" t="s">
         <v>1011</v>
@@ -12138,10 +12141,10 @@
         <v>1058</v>
       </c>
       <c r="B688" s="0" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="H688" s="4" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="I688" s="4" t="s">
         <v>1011</v>
@@ -12154,10 +12157,10 @@
         <v>1087</v>
       </c>
       <c r="B689" s="0" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="H689" s="4" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="I689" s="4" t="s">
         <v>1090</v>
@@ -12167,13 +12170,13 @@
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="0" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="H690" s="4" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="I690" s="6" t="s">
         <v>1034</v>
@@ -12183,13 +12186,13 @@
     </row>
     <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="0" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B691" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="H691" s="4" t="s">
         <v>1136</v>
-      </c>
-      <c r="H691" s="4" t="s">
-        <v>1135</v>
       </c>
       <c r="I691" s="6" t="s">
         <v>1034</v>
@@ -12199,80 +12202,80 @@
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B695" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="H695" s="4" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="I695" s="4" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J695" s="4"/>
       <c r="K695" s="4"/>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B696" s="0" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="H696" s="4" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="I696" s="4" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J696" s="4"/>
       <c r="K696" s="4"/>
     </row>
     <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A697" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B697" s="0" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="H697" s="4" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="I697" s="4" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J697" s="4"/>
       <c r="K697" s="4"/>
     </row>
     <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B698" s="0" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="H698" s="4" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="I698" s="4" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J698" s="4"/>
       <c r="K698" s="4"/>
     </row>
     <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A699" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B699" s="0" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="H699" s="4" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="I699" s="4" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="J699" s="4"/>
       <c r="K699" s="4"/>
@@ -12282,7 +12285,7 @@
         <v>987</v>
       </c>
       <c r="B703" s="0" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="C703" s="0" t="n">
         <v>1</v>
@@ -12291,25 +12294,25 @@
         <v>612</v>
       </c>
       <c r="E703" s="0" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="F703" s="0" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="G703" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H703" s="0" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="I703" s="0" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="J703" s="0" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="K703" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12317,7 +12320,7 @@
         <v>987</v>
       </c>
       <c r="B704" s="0" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C704" s="0" t="n">
         <v>1</v>
@@ -12326,25 +12329,25 @@
         <v>612</v>
       </c>
       <c r="E704" s="0" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="F704" s="0" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="G704" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H704" s="0" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="I704" s="0" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="J704" s="0" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="K704" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12352,7 +12355,7 @@
         <v>987</v>
       </c>
       <c r="B705" s="0" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C705" s="0" t="n">
         <v>1</v>
@@ -12361,25 +12364,25 @@
         <v>612</v>
       </c>
       <c r="E705" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="F705" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="G705" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H705" s="0" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="I705" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="J705" s="0" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="K705" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12387,7 +12390,7 @@
         <v>987</v>
       </c>
       <c r="B706" s="0" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="C706" s="0" t="n">
         <v>1</v>
@@ -12396,25 +12399,25 @@
         <v>612</v>
       </c>
       <c r="E706" s="0" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="F706" s="0" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="G706" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H706" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="I706" s="0" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="J706" s="0" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="K706" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12431,25 +12434,25 @@
         <v>612</v>
       </c>
       <c r="E711" s="0" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="F711" s="0" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="G711" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H711" s="0" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="I711" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J711" s="0" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="K711" s="0" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12466,25 +12469,25 @@
         <v>612</v>
       </c>
       <c r="E712" s="0" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="F712" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G712" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H712" s="0" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="I712" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J712" s="0" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="K712" s="0" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12501,25 +12504,25 @@
         <v>612</v>
       </c>
       <c r="E713" s="0" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="F713" s="0" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="G713" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H713" s="0" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="I713" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J713" s="0" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="K713" s="0" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12536,13 +12539,13 @@
         <v>612</v>
       </c>
       <c r="E714" s="0" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="F714" s="0" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="G714" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H714" s="0" t="s">
         <v>218</v>
@@ -12551,10 +12554,10 @@
         <v>585</v>
       </c>
       <c r="J714" s="0" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="K714" s="0" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12568,28 +12571,28 @@
         <v>1</v>
       </c>
       <c r="D715" s="0" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="E715" s="0" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="F715" s="0" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="G715" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H715" s="0" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="I715" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J715" s="0" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="K715" s="0" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12606,25 +12609,25 @@
         <v>612</v>
       </c>
       <c r="E716" s="0" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="F716" s="0" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="G716" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H716" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="I716" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J716" s="0" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="K716" s="0" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12641,30 +12644,30 @@
         <v>612</v>
       </c>
       <c r="E717" s="0" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="F717" s="0" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="G717" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H717" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="I717" s="0" t="s">
         <v>585</v>
       </c>
       <c r="J717" s="0" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="K717" s="0" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="0" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B719" s="0" t="s">
         <v>225</v>
@@ -12673,28 +12676,28 @@
         <v>1</v>
       </c>
       <c r="D719" s="0" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="E719" s="0" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="F719" s="0" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="G719" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="H719" s="0" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="I719" s="0" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J719" s="0" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="K719" s="0" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12702,7 +12705,7 @@
         <v>300</v>
       </c>
       <c r="H722" s="11" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="I722" s="0" t="s">
         <v>1002</v>
@@ -12713,7 +12716,7 @@
         <v>301</v>
       </c>
       <c r="H723" s="11" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="I723" s="0" t="s">
         <v>1002</v>
@@ -12724,7 +12727,7 @@
         <v>140</v>
       </c>
       <c r="H724" s="12" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="I724" s="0" t="s">
         <v>585</v>
@@ -12738,10 +12741,10 @@
         <v>334</v>
       </c>
       <c r="H725" s="12" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="I725" s="0" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12752,10 +12755,10 @@
         <v>322</v>
       </c>
       <c r="H726" s="12" t="s">
+        <v>1209</v>
+      </c>
+      <c r="I726" s="0" t="s">
         <v>1208</v>
-      </c>
-      <c r="I726" s="0" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Remove last identified IFS variables from the pre identified missing list. Move Oman prra to the pre ignored list. Update the ignored and identified lists #450.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="126">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -67,21 +67,15 @@
     <t xml:space="preserve">Twan &amp; Thomas</t>
   </si>
   <si>
-    <t xml:space="preserve">prra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large-scale precipitation (rain+snow) + Convective precipitation (rain+snow) - Snowfall: grib 128.142 + 128.143 - 128.144</t>
+    <t xml:space="preserve">mrroLi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
   </si>
   <si>
     <t xml:space="preserve">Shuting, Thomas</t>
   </si>
   <si>
-    <t xml:space="preserve">mrroLi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
-  </si>
-  <si>
     <t xml:space="preserve">sza</t>
   </si>
   <si>
@@ -133,235 +127,229 @@
     <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the U component of wind (grib 128.131) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
   </si>
   <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This site lon,lat is specifed by the experiment we guess, and should be available in the netcdf file. So far it doesn't seem to be specified in the data request: in the CMIP6_coordinate.json table file the requested": "" is empty for site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tsland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available: This coincides with skin temperature (code 235)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea Alessandri, Franco Catalano, Emanuel Dutra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature of the lower boundary of the atmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS3MIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy covered area percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available: Sum of [CVL (code: 27) + CVH (code: 28)] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea Alessandri, Franco Catalano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. 'Vegetation' means any plants e.g. trees, shrubs, grass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wilt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilting point is defined in HTESSEL as a fraction (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128) of field capacity. (Alessandri A.: an Effective Wilting Point can be defined ... same as below discussion for the field capacity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea &amp; Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fldcapacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum amount of water the soil can hold (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128). It is constant map in time in H-TESSEL (Alessandri A.: an Effective Field Capacity can be defined for coupling analysis pourpouses that will change with the effective vegetation cover; as soon as we have daily effective vegetation cover in the outputs we can compute as well the Effective Field capacity).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clayfrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): very fine (&amp; fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siltfrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): medium (&amp; medium fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandfrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): coarse in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ksat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture  (not in the output; no grib code associated).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rootdsl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture (not in the output, no grib code associated).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slthick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS: independent of lon, lat. Top soil layer: 0-7 cm, Soil layer 2: 7-28 cm, Soil layer 3: 28-100 cm, Soil layer 4: 100-289 cm, added as issue #126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cllcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clmcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clhcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltcalipso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cltisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pctisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">albisccp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlutaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.73                      Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlutcsaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.72                       Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsutaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 128.212-126.069  Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grib 126.20 / 126.22  in namelist.ifs.cloudact+diag.sh  CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tntc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.105                                                              Available in IFS: T-tendency from convection : grib 128.105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110  Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.106                                                              Available in IFS: q-tendency from convection: grib 128.106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tnhusmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                      Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
+  </si>
+  <si>
     <t xml:space="preserve">LImon</t>
   </si>
   <si>
-    <t xml:space="preserve">orogIs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is grib 128.129 at surface. But be aware not missing up with the grib 128.129 for free atmospehre.</t>
+    <t xml:space="preserve">sftgrf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Greenland this is the same as above sftgif. We do not have Antarctic ice sheet.</t>
   </si>
   <si>
     <t xml:space="preserve">Shuting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This site lon,lat is specifed by the experiment we guess, and should be available in the netcdf file. So far it doesn't seem to be specified in the data request: in the CMIP6_coordinate.json table file the requested": "" is empty for site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tsland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available: This coincides with skin temperature (code 235)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea Alessandri, Franco Catalano, Emanuel Dutra </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature of the lower boundary of the atmosphere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LS3MIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cnc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canopy covered area percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available: Sum of [CVL (code: 27) + CVH (code: 28)] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea Alessandri, Franco Catalano </t>
-  </si>
-  <si>
-    <t xml:space="preserve">X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. 'Vegetation' means any plants e.g. trees, shrubs, grass.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wilt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wilting point is defined in HTESSEL as a fraction (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128) of field capacity. (Alessandri A.: an Effective Wilting Point can be defined ... same as below discussion for the field capacity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea &amp; Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fldcapacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum amount of water the soil can hold (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128). It is constant map in time in H-TESSEL (Alessandri A.: an Effective Field Capacity can be defined for coupling analysis pourpouses that will change with the effective vegetation cover; as soon as we have daily effective vegetation cover in the outputs we can compute as well the Effective Field capacity).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clayfrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): very fine (&amp; fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">siltfrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): medium (&amp; medium fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sandfrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): coarse in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ksat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture  (not in the output; no grib code associated).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rootdsl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture (not in the output, no grib code associated).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slthick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in IFS: independent of lon, lat. Top soil layer: 0-7 cm, Soil layer 2: 7-28 cm, Soil layer 3: 28-100 cm, Soil layer 4: 100-289 cm, added as issue #126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cllcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.40   CVEXTR2(1)='CALIPSO_LCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klaus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clmcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.41   CVEXTR2(2)='CALIPSO_MCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clhcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.42   CVEXTR2(3)='CALIPSO_HCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cltcalipso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.43   CVEXTR2(4)='CALIPSO_TCC'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cltisccp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.44   CVEXTR2(5)='ISCCP_TOTALCLD'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pctisccp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.45   CVEXTR2(6)='ISCCP_MEANPTOP'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">albisccp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSP grib 126.46   CVEXTR2(7)='ISCCP_MEANALBCLD'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rlutaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.73                      Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rlutcsaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.72                       Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsutaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 128.212-126.069  Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cdnc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grib 126.20 / 126.22  in namelist.ifs.cloudact+diag.sh  CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tntr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.95                                                                Available in IFS: T-tendency from radiation: grib 128.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twan, Thomas &amp; Gijs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tntc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.105                                                              Available in IFS: T-tendency from convection : grib 128.105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grib 126.94 + 126.99 + 126.106 + 126.110  Adding all the q-tendencies, thus: grib 128.94 + 128.99 + 128.106 + 128.110.  Alternatively, in IFS: just estimating the delta q per month. So far no direct grib code for the totoal q-tendency found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhusc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.106                                                              Available in IFS: q-tendency from convection: grib 128.106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tnhusmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                      Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sftgrf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For Greenland this is the same as above sftgif. We do not have Antarctic ice sheet.</t>
   </si>
   <si>
     <t xml:space="preserve">sncIs</t>
@@ -709,8 +697,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -791,32 +779,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H8" s="4"/>
+      <c r="I8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="s">
@@ -825,11 +815,11 @@
       <c r="H10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>14</v>
+      <c r="I10" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="2"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
@@ -839,7 +829,7 @@
         <v>26</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="3"/>
@@ -851,11 +841,11 @@
       <c r="H12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>22</v>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="J12" s="4"/>
-      <c r="K12" s="3"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5" t="s">
@@ -865,7 +855,7 @@
         <v>30</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="2"/>
@@ -874,13 +864,13 @@
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="6" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="J14" s="6"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,357 +881,354 @@
         <v>34</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="2"/>
+      <c r="I18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="B19" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="3"/>
       <c r="J20" s="2"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="I22" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="J22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="D23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="0" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="B26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="H26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="0" t="s">
+      <c r="I26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="H27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K25" s="0" t="s">
-        <v>53</v>
-      </c>
+      <c r="I27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="H28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="I28" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>72</v>
+        <v>54</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="8" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="2" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="9" t="s">
+      <c r="H38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="I39" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="10" t="s">
+      <c r="I46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="H44" s="0" t="s">
+      <c r="H47" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="I47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>14</v>
@@ -1249,114 +1236,120 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10"/>
+      <c r="B51" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="H51" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
+      <c r="I54" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10" t="s">
+      <c r="H55" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="H53" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>14</v>
-      </c>
+      <c r="I55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="I56" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I62" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>112</v>
@@ -1365,126 +1358,96 @@
         <v>113</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="11" t="s">
         <v>114</v>
       </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
       <c r="H64" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="I64" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-    </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="H65" s="2" t="s">
+      <c r="E101" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="F101" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H101" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I101" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J101" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="K101" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="11" t="s">
+      <c r="E102" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F102" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="H66" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B103" s="0" t="s">
+      <c r="G102" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H102" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I102" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C103" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D103" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E103" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F103" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="G103" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H103" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I103" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="J103" s="0" t="s">
+      <c r="J102" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="K103" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B104" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="C104" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D104" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E104" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F104" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="G104" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H104" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="I104" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="J104" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K104" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
+      <c r="K102" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Move the Efx variables fldcapacity, ksat, rootdsl, wilt from the identified missing list to the ignored list #394. And add the identified Eday variables mrsow, tsland to the identified missing list #443.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -187,27 +187,15 @@
     <t xml:space="preserve">Efx</t>
   </si>
   <si>
-    <t xml:space="preserve">wilt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wilting point is defined in HTESSEL as a fraction (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128) of field capacity. (Alessandri A.: an Effective Wilting Point can be defined ... same as below discussion for the field capacity)</t>
+    <t xml:space="preserve">clayfrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): very fine (&amp; fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
   </si>
   <si>
     <t xml:space="preserve">Andrea &amp; Thomas</t>
   </si>
   <si>
-    <t xml:space="preserve">fldcapacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum amount of water the soil can hold (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128). It is constant map in time in H-TESSEL (Alessandri A.: an Effective Field Capacity can be defined for coupling analysis pourpouses that will change with the effective vegetation cover; as soon as we have daily effective vegetation cover in the outputs we can compute as well the Effective Field capacity).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clayfrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): very fine (&amp; fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
-  </si>
-  <si>
     <t xml:space="preserve">siltfrac</t>
   </si>
   <si>
@@ -220,18 +208,6 @@
     <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): coarse in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
   </si>
   <si>
-    <t xml:space="preserve">ksat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture  (not in the output; no grib code associated).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rootdsl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-TESSEL parameters inside the model that is prescribed for each dominant soil texture (not in the output, no grib code associated).</t>
-  </si>
-  <si>
     <t xml:space="preserve">cllcalipso</t>
   </si>
   <si>
@@ -332,6 +308,30 @@
   </si>
   <si>
     <t xml:space="preserve">grib 126.99 + 126.106 + 126.110                           part of MFP3D        Adding all the q-tendencies without advection, thus: grib 128.99 + 128.106 + 128.110.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrsow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Soil Wetness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrsow=swvl1*0.07+swvl2*0.21+swvl3*0.72+swvl4*1.89 note: NOT divided by maximum allowable soil moisture above wilting point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea Alessandri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated soil moisture divided by maximum allowable soil moisture above wilting point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land Surface Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available by IFS: grib code 235 but it needs masking out the ocean points: thus add in ifspar.json the entry "masked": "land"</t>
   </si>
   <si>
     <t xml:space="preserve">LImon</t>
@@ -492,9 +492,6 @@
   </si>
   <si>
     <t xml:space="preserve">nudgincsm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">Nudging Increment of Water in Soil Moisture</t>
@@ -589,7 +586,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -677,6 +674,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFCE181E"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -731,7 +734,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -769,6 +772,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -849,10 +856,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="53:56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1190,278 +1197,312 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="7" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="I31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="2" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="H32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="7" t="s">
+      <c r="H33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="H34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="B35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>76</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="8" t="s">
+      <c r="I40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="8" t="s">
+      <c r="I41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="H41" s="0" t="s">
+      <c r="H42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="8" t="s">
+      <c r="I42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="H45" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="I45" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="I48" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="H49" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8" t="s">
+      <c r="H50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="H50" s="0" t="s">
+      <c r="I50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="I50" s="0" t="s">
-        <v>14</v>
-      </c>
+      <c r="H51" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B55" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>98</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>99</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B56" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I56" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J56" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>104</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>107</v>
@@ -1469,15 +1510,15 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>104</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>107</v>
@@ -1485,33 +1526,56 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>110</v>
-      </c>
+    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
       <c r="H62" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I62" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I62" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="H63" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>107</v>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I63" s="10"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G65" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/01c8c41a-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,177 +1583,37 @@
         <v>38</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>40</v>
       </c>
       <c r="E66" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F66" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F66" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="G66" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/01c8c41a-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0abbdddc-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H66" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="I66" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="I66" s="0" t="s">
-        <v>119</v>
-      </c>
       <c r="J66" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="K66" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="G67" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0abbdddc-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H67" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I67" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="J67" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="K67" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Taking off clayfrac, siltfrac & sandfrac from the pre identified missing file as well, so it does not get disabled during a reidentification session #443 #500 point 5 #526.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="116">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -182,30 +182,6 @@
   </si>
   <si>
     <t xml:space="preserve">X_area_fraction' means the fraction of horizontal area occupied by X. 'X_area' means the horizontal area occupied by X within the grid cell. 'Vegetation' means any plants e.g. trees, shrubs, grass.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clayfrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): very fine (&amp; fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea &amp; Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">siltfrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): medium (&amp; medium fine?) in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sandfrac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil texture (could be derived by soil HTESSEL soil types [1-6]: variable slt grib code 43 - Table 128): coarse in H-TESSEL boundary condition constant in time. It is available in a kind of mask: for each type a number 1-6 if this type at a lon,lat location the number corresponding with this type is in the mask. (No grib code we think.)</t>
   </si>
   <si>
     <t xml:space="preserve">cllcalipso</t>
@@ -586,7 +562,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -653,13 +629,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFF58220"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFCE181E"/>
       <name val="Cambria"/>
       <family val="0"/>
@@ -671,12 +640,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -734,7 +697,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -763,19 +726,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,7 +789,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFF58220"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -856,10 +811,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="53:56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1150,470 +1105,426 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="H27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="2" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="H28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="H29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="8" t="s">
-        <v>62</v>
+      <c r="B31" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="0" t="s">
         <v>68</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="8" t="s">
+      <c r="I36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="8" t="s">
+      <c r="I37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="H38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="8" t="s">
+      <c r="I38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H37" s="0" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="H41" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
+      <c r="I41" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="I44" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="H45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8" t="s">
+      <c r="H46" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="H45" s="0" t="s">
+      <c r="I46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="I45" s="0" t="s">
-        <v>14</v>
-      </c>
+      <c r="H47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B51" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="J51" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+      <c r="K51" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B52" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>94</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="H58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I59" s="8"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B55" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D55" s="0" t="s">
+      <c r="B61" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G55" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I59" s="2" t="s">
+      <c r="E61" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B60" s="0" t="s">
+      <c r="F61" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-    </row>
-    <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-    </row>
-    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="H62" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I63" s="10"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="G65" s="0" t="str">
+      <c r="G61" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/01c8c41a-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H65" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="K65" s="0" t="s">
+      <c r="H61" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="K61" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" s="0" t="s">
+      <c r="B62" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="G66" s="0" t="str">
+      <c r="E62" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G62" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0abbdddc-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H66" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="K66" s="0" t="s">
+      <c r="H62" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K62" s="0" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>